<commit_message>
Fluxo de tratamento de .xls - remoção de imagem dos arquivos.
</commit_message>
<xml_diff>
--- a/src/data/uploads/Project Room (Jira).xlsx
+++ b/src/data/uploads/Project Room (Jira).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/paulo_vieira_d_silva_accenture_com/Documents/Desktop/Automação_v3/src/data/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1AE3755-7109-4414-A82D-6F68FFB8675A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C8A17F8-3516-49AA-AD7C-725DA47B78CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B14E7F1B-C2CF-4F8C-8FD7-706B78DB2A55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3BFA2687-D76A-45EE-91A0-139B4961BFD7}"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -10304,72 +10304,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2049" name="Picture 1" descr="Project Room (Jira)">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4957DC-10C6-34C2-E80E-256129BB06E5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:link="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1371600" cy="571500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -10686,7 +10620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F5C6E0-41F1-4431-BC4C-EFF19AF62E96}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C4E895-4723-4AB2-884A-B6DEB348F755}">
   <dimension ref="A1:AR578"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -66621,583 +66555,583 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{48917178-2994-4010-A7F0-2C5AB43BCCC3}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{45072F55-AA05-4A09-8EF9-A5BA0BA460D5}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{EA921CE9-1F86-432A-8879-09A1315169A9}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{B642EEC1-C8C8-4130-93F9-04D912E67947}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{30FC037F-BAD4-4D2E-BE7F-732C1A17BDCD}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{0DB46F79-E0F9-4B11-AA86-2C29CF88C015}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{9CCF15B6-F86A-44B5-A5F4-1B94CDF39DD9}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{130B8D6E-B146-4F98-AC20-AE968D8909C0}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{B658F511-46EA-4A1A-8A6F-16E2C67CBD18}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{2346E366-4CDF-4168-B886-24A12BBC834E}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{6A992A61-5F3D-40AA-8DFB-55B84A62E83F}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{BD53130B-98D3-49CA-9552-CBC3C27C5552}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{8995C1B3-FB74-4926-B1CA-EDFFD3966D7F}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{AA9C8762-A71E-4B96-AC62-5BED09DCFB8E}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{26BDDABC-17C6-47DB-861D-E9120367EE41}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{48D88C2B-A6CC-4F9C-83D8-38881CD24525}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{9E9146E4-2727-46D5-8A01-D532CE305296}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{9375641F-46AA-4418-9FEE-3223DF88103A}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{EAF46FC3-93E0-46AE-B398-556E5E787257}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{C318F2E7-4372-479E-BA2C-F84450A5CA61}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{B3124975-20EA-426A-B7AA-FCC65BFFE7CF}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{467CB07E-94E0-4E5B-A973-6F595F1AC982}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{A3D912A7-BF81-4ACD-8E86-1E7017CB9ED1}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{0148806A-71A5-4140-BC67-F926C6AE5E05}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{C4F78E88-E811-40ED-A936-669E775D24A1}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{46F1DE3B-5046-48F7-A67E-EDE0EF4F5CDB}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{E298C9AC-736C-447F-8509-4F4B83075501}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{1BE64E2A-BD7E-42B7-B69B-C78F92D5CA03}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{DE036F24-9345-420F-AEAE-5E7177EC2E81}"/>
-    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{5615AA01-75FC-4E90-AF95-5853B1E689B5}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{32316FF6-CA08-4CBF-9D4E-F418B1EE6A7D}"/>
-    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{7D3212BD-E03E-4B9C-9D79-961DB64130CA}"/>
-    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{AF3770C5-FB67-415A-9872-4FA1309F0EDC}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{3AF91D0B-43EF-4B43-875C-C14E17AEE735}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{3754AD77-1775-4713-9DFB-13136409F464}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{C74F3008-7BDA-486E-820F-7E8AA2829888}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{E96C3542-9A75-4177-B71E-269A8324C3FA}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{77575AAF-2A9B-4CA1-8F1E-8D04B577208E}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{0B4D1448-8019-417F-9007-90B0012FF1A5}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{0F556A30-3955-4A49-A5CE-B5E8E0D0D9FD}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{21EC08E3-8192-4877-979B-4C145988A0C3}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{63A5D342-1021-434F-9F9A-E06779B8DF6C}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{E03982E1-4105-4184-A4D6-551CC2CEFBA1}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{DA5AAEF7-4159-401D-AA5B-33EBCFD04297}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{5C4FBC18-422D-4B6E-845D-AC48276BDA94}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{7205A06C-2404-4850-9B9A-F70C52238022}"/>
-    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{D1A12289-9FAB-49A6-B85E-FDE5745969CE}"/>
-    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{80371AEA-2DBB-46E6-B424-6E1C82E1E2F4}"/>
-    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{129ABFD1-016D-4D12-B788-94DA6DA62BAE}"/>
-    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{011EA164-1262-4B73-A8C6-E7BD1EC8A4B2}"/>
-    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{0811A199-E3B8-49BA-9098-B402081C8424}"/>
-    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{6EEB0430-8A11-4E7E-A2A6-99424F3A95D1}"/>
-    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{26C1459B-3618-463A-9928-E684D57D383E}"/>
-    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{585A66A7-4947-419C-A643-E1E26922BDDD}"/>
-    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{D709FCA0-433F-4D78-9C6F-E7FF1797E1DD}"/>
-    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{49B87C17-E613-483D-971F-6BD90BE06DBB}"/>
-    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{BEA4D7BC-ED65-4927-83DC-E72ECBF50066}"/>
-    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{101D66A3-DCEA-400D-90FD-79BFCCB5D853}"/>
-    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{F17B4F9F-C2A5-43D0-8A14-66AAF2EF0FAC}"/>
-    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{3E212C39-2998-4607-BB30-804EF73F2893}"/>
-    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{3A71B595-A798-4711-A799-2B5E3E7966D9}"/>
-    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{929ECB3E-525B-461C-A846-F36987F5C176}"/>
-    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{B07F8116-8014-4407-86AD-F268F56D0A22}"/>
-    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{3C6EAF86-381D-4D8E-B6B8-D23E71E1E40C}"/>
-    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{043C958F-FF80-4271-A619-9E77432EE83B}"/>
-    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{D06C9724-8D10-49CD-AA8D-7078D7368CAE}"/>
-    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{63EA28D7-6519-4C54-9621-223B7F934326}"/>
-    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{E1254E7B-6A90-47BE-BF56-8DC13ED172C4}"/>
-    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{49F0BB92-FCCC-49C2-94E9-69F1E18D49C5}"/>
-    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{DF83FE81-9F31-4FE2-900B-8D6BDA5D218F}"/>
-    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{FB3A9A29-967B-40ED-AB4B-FBB04DF31488}"/>
-    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{66C8D6E7-BA86-4400-A2C9-133D74AAC20D}"/>
-    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{E4172A22-3272-45CC-8871-765072574E43}"/>
-    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{00D08BFF-DE4F-444A-A87A-91E1D0E0E886}"/>
-    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{829E5E75-4643-4C8B-82F8-6B8B18B78F9D}"/>
-    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{E816AD76-0341-4CAF-B963-745C22903A57}"/>
-    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{199F114E-B050-417C-ACFC-E84667E592AD}"/>
-    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{BCC744EB-618B-49DB-945B-65B38D1A3BF1}"/>
-    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{060335A7-4684-46DC-85E7-6B529370C6B5}"/>
-    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{4180DAF9-D223-41DD-B032-87814C7E6427}"/>
-    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{2F97A066-595E-4153-BA9A-8B5C9D705ACF}"/>
-    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{5D862D13-BF8A-4364-BD12-0E7268ACCEB7}"/>
-    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{87C52DA3-E717-4400-BB80-4CBF0C590E00}"/>
-    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{0ED51F50-2E88-40DE-9F9F-4BB255FADF73}"/>
-    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{02E77872-DCC9-4FBA-8C0B-16D380ABB8A1}"/>
-    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{183529D2-98B6-4593-8F6D-C820713D9419}"/>
-    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{B74335FC-4CF4-4C32-B04F-179B52F44728}"/>
-    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{5FB6F2E9-70D5-4C3C-A483-103CAD729A48}"/>
-    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{33DEC4B5-5941-42A7-8BA4-FCC9BD2095E2}"/>
-    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{1B5CFD17-791F-4320-8F25-71DC202E6C03}"/>
-    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{69C64C22-3E44-4F11-AE76-D3C7DB70BD66}"/>
-    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{2DF6F6BD-0CF0-445A-B962-96BD3D60C4B2}"/>
-    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{C2020676-7347-4047-92A9-46C83DFF8AAA}"/>
-    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{0D774614-88B5-4832-AFFD-246479520012}"/>
-    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{B54028C3-CA80-47EE-8086-0D18BD71D074}"/>
-    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{5E66C12C-ECF2-4B02-BB67-4DEA6D0006C7}"/>
-    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{D10BEF66-69F0-433A-BC32-E4A3C45C55CA}"/>
-    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{4B4825C6-8473-4048-AE3D-E0FA5846A5A8}"/>
-    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{C85CAA39-C68E-45BB-A3FD-180198B410CF}"/>
-    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{8EBEB22C-AEA8-45BA-BE9D-2A54C4C35934}"/>
-    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{30700A25-EACA-43CB-BA86-EFBBC7528BC1}"/>
-    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{06722D96-1A88-4EEF-9BA3-7E21E3F6E72C}"/>
-    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{741D473A-07A2-4D2C-A35F-2E6B4F850AA4}"/>
-    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{190D1D01-1A89-4F4D-866C-AE5867E88A47}"/>
-    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{F16D4303-8479-4C97-9427-9E73DB76E61A}"/>
-    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{2FB7F046-1F0A-4693-BAD1-DCFC20700562}"/>
-    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{F4D9F95B-2563-44CC-9EBC-16FA4A4720D3}"/>
-    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{28DB164B-DDE8-41F1-918F-94B296CCE61C}"/>
-    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{D0788FE4-8999-474D-A4FB-83914AE6AB49}"/>
-    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{B5662363-4A12-4DE6-9E7D-2FF5F0059426}"/>
-    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{33A661E9-19F8-486D-BE12-5C3840CF831A}"/>
-    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{7BD237F3-655A-4C20-8760-5396A3E33B13}"/>
-    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{D250CD52-4E67-4EDD-AA68-C3704E624718}"/>
-    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{9532A1E6-8905-431B-AB05-0315AD33DAAD}"/>
-    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{006EF322-3CF1-4427-B327-F971FA5FD288}"/>
-    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{03C2B028-EF09-4600-B77B-9D23CFC50AE3}"/>
-    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{414D24EC-DEE4-4E03-8C73-3D988FF79EFC}"/>
-    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{0B8A242E-D4D6-4626-BDE1-17CAD4535E5B}"/>
-    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{9AB32760-FD01-47DC-BC90-3B022FE8B796}"/>
-    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{50BBA60F-85C7-4A17-A31F-5FBC9F5D85A0}"/>
-    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{BE17A3E9-444B-48BC-B9B9-6F5405231A72}"/>
-    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{52FA9526-60E1-4661-96A0-6FDBF3728D17}"/>
-    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{5853E814-7FA0-4C0B-A5F9-A0A3761D3013}"/>
-    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{B00CF8FA-AEDF-4EE5-9BB0-72ACF8FE55D3}"/>
-    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{5F840ABC-FF80-4357-82F5-E45D6381930B}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{898F23D0-8F93-479F-B506-804DDF7352A8}"/>
-    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{F32774A7-8698-4874-8721-C6A7BF9C69D3}"/>
-    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{0F6AB2FD-BB75-4B76-AB2D-A0B8438700AF}"/>
-    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{288304CE-6B01-4305-8DE3-EF02B689FC61}"/>
-    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{B7E6350A-C5AE-4650-9142-D6797240683F}"/>
-    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{936F3367-53C7-4684-84DB-456D3A3269EA}"/>
-    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{05C5FDD5-1982-4A10-B0A2-73B5CA3296A2}"/>
-    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{414A72FB-5EB3-447C-9261-A42E8C084D48}"/>
-    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{68216BE0-1183-4626-8145-27164D25A439}"/>
-    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{B6077945-9464-4982-9F7E-6B5A111E286A}"/>
-    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{5A23F016-4C6F-4C26-82AD-C6A036491092}"/>
-    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{EDE7B3AA-51DA-4EA2-97DD-FD3BC9135A26}"/>
-    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{9B4CEA90-7035-4AD0-98F2-1FACAB1AC2D3}"/>
-    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{EA74742E-3F1E-4E83-B34F-AF5A9AA4C1A8}"/>
-    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{CFE22ED4-AF02-4A52-B236-58F54C90E00D}"/>
-    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{E12B8CF6-4294-454B-B0CD-0A84649A4858}"/>
-    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{7F9457EF-B687-4D3B-9215-1600DD718683}"/>
-    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{F5FDADD0-C6D4-424A-A34D-F0C2C6998164}"/>
-    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{76A2131A-7287-4F83-A65D-6FBBA5057B87}"/>
-    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{4417F264-2E18-4D94-A23B-925CABE048ED}"/>
-    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{4FD0B733-F50E-43ED-BD8E-D80DD82246C6}"/>
-    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{B8069DA1-C1C4-4555-B4E4-7AA599C9EC1D}"/>
-    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{2B25932D-316F-45FB-9A33-108431D8FF5E}"/>
-    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{0DACCAC8-EA05-4F03-A3E2-481EF620FEA5}"/>
-    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{FFF37478-6F89-4A11-AFB5-310B9361AD70}"/>
-    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{D7E43015-5632-4299-B143-153F4B8E82AE}"/>
-    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{3E4D23DB-AFC0-41AA-937E-8B3E3FCB1809}"/>
-    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{E0073132-3400-41D5-B2CA-85526B0F67C7}"/>
-    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{38FD4D75-3D67-4D52-BB20-FFE3FE820F86}"/>
-    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{1BE47FD4-1469-4BD3-95C2-1FF1DA70DDBA}"/>
-    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{78313917-0612-4B66-AA4C-AF87C4B3354C}"/>
-    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{C4F8C1E5-BB2C-4CD7-860E-36E0B4A9CF55}"/>
-    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{576E3739-BF0C-4D5A-A0B5-CE9386C96B28}"/>
-    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{11589B09-785E-487E-B679-A8A47E67CD51}"/>
-    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{A36734D4-2704-44A6-BE1B-8008A2B87614}"/>
-    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{1381EE25-B004-4478-A6F1-02D273959D3A}"/>
-    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{AB03D4E0-AEBC-4E90-90FD-FBFD156A28D2}"/>
-    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{9DFCA900-4D47-489D-BEE0-B5A6B1606C4F}"/>
-    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{E5C815D9-8EEB-4730-9308-27ACF40C9CB6}"/>
-    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{238D5385-3556-41E3-9BF0-071E2FD89E8B}"/>
-    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{67B194BC-3134-4604-9DD4-EBFE82B2488D}"/>
-    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{CB66DF6D-822E-4597-B503-C3C48676F906}"/>
-    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{8180F84D-84F9-4946-9249-7105362C0D9C}"/>
-    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{8AA38B19-142B-40F4-8AC5-AD17F4D37A19}"/>
-    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{1F35C29A-A79E-44C7-A667-01966DDF10CB}"/>
-    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{939CD594-3C0F-4D39-810E-D6D9ED7AD198}"/>
-    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{4CCDB604-764A-4D99-A141-126CE6EBBD4E}"/>
-    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{619684C6-8647-4D01-BF2F-B583C88B5519}"/>
-    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{3CD7144E-9C5D-4C68-9B7F-878B0B5B9FAC}"/>
-    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{1ED700BE-AFBB-47CB-A721-EA8BA9E61040}"/>
-    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{7B5316B0-C430-4541-94B4-2A86B71F87AB}"/>
-    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{72BCB0B1-139B-4844-BEED-2494640E7EA3}"/>
-    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{0EB52381-9FFC-428F-BDDB-8678EA649B9C}"/>
-    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{ABEC6961-DDFD-41CA-BA16-610A13DF887C}"/>
-    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{CC0A3A77-BE17-49E1-8F22-FBEF58EFF685}"/>
-    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{40FE2550-F4D0-411A-A8B0-346EDFC2DE51}"/>
-    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{97A47865-F46E-4C11-9316-A4ABDCD4B685}"/>
-    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{C3C5DA2A-27FB-4251-9507-A1A4A6002566}"/>
-    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{A26DE1EA-E326-4E75-AD94-23B8986125A8}"/>
-    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{6180F98E-9622-4C88-9999-23585413C02B}"/>
-    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{7CD508B0-FEF0-4913-978A-5DB22C596A2D}"/>
-    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{1D0A4CCD-2216-4FB3-BA6A-C703724E133A}"/>
-    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{02922A9D-43B5-4F67-9577-5A094BA10E8B}"/>
-    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{4B058B21-DD0A-4C3C-B8E1-63B1034BFA49}"/>
-    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{C8C6DF1F-D1A1-4889-9452-AF9AA9EE8484}"/>
-    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{F41DF2E2-2909-43AB-96E5-9BE4F5D914DE}"/>
-    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{BAA86007-C1E5-44A3-9860-7A3BC12BBD7E}"/>
-    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{28B07C59-9737-4B41-95EB-787D14C64D32}"/>
-    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{9C5AD9DB-22FB-4699-BCFC-E37B6B4ADF01}"/>
-    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{3EA5F6BE-0842-4677-AAC4-24A467CFB265}"/>
-    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{A7BCF66B-45CA-499A-8595-859E7C6DC983}"/>
-    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{18CA0B37-320B-4383-8617-A17CF68ECF1A}"/>
-    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{26A057DA-84F8-48F8-9417-B8B84F27EBCD}"/>
-    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{EF10964D-482D-4DEF-B89D-F889A6D6A359}"/>
-    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{C37D7524-E49E-41D4-99B0-871736872FF2}"/>
-    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{30680B7C-1714-4A32-971F-91E5DE59FC8E}"/>
-    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{71FDCF30-F6D5-4E5F-A12B-A818DC6B9FD0}"/>
-    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{E5CD3F59-00C6-41E6-9B0B-6A547EC8A0AE}"/>
-    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{65C67997-AFEA-45C6-8AA5-31325C606630}"/>
-    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{D0A94586-D476-42BE-A2D4-FA0DEBC34621}"/>
-    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{142CCA27-518C-4C18-B4E2-80BC63B0FC3E}"/>
-    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{617B9E05-BE59-4B9F-AC2A-8350DB75C0CF}"/>
-    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{6F98C296-02DF-459D-B44D-83BA30DD8896}"/>
-    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{4C994EAD-04B9-45E0-A72C-F84739AA4790}"/>
-    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{5981D2FB-197D-434F-8ECD-2F37BE384720}"/>
-    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{FB5C1B31-6C11-47DD-9BEB-0E96F428240E}"/>
-    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{42AC09CC-4A3E-44DC-AB31-205D879DB173}"/>
-    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{059CE529-5982-4C3C-B4E8-E798B3715A5B}"/>
-    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{8EB3DFD1-9144-45DA-8134-D4743B50B349}"/>
-    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{D4CE801F-0B7D-45C9-AA4C-0EF93B75C0E2}"/>
-    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{4EF6BF38-42C5-4881-9ABE-F6D839CCC6A5}"/>
-    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{98C6C31B-3DC2-4A8A-8023-BA029D13AEF5}"/>
-    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{3C7AD335-4379-434A-91D8-C4B76A6FD8C9}"/>
-    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{ED0E2A4B-B63E-4071-8B75-6D04418E0621}"/>
-    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{0CFBE5B1-E7B7-4970-9C9C-1B02D672CD84}"/>
-    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{991E54FF-0B64-4AE9-BADE-DDD62D679F05}"/>
-    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{A424A5B7-926D-4094-9E7F-6A48B6883806}"/>
-    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{D1ACD9F9-FC4C-4A53-AE3C-15884282893D}"/>
-    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{802E1615-8549-4778-A695-C662F1E24EE5}"/>
-    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{A94F3F3B-81BA-4155-BF02-E8C50FA5AB44}"/>
-    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{B1EEC1DE-0E8B-48D6-BEE9-9781ECCD2278}"/>
-    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{29AB1EC0-08A4-4C40-A764-3EDD48715ABD}"/>
-    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{C2575228-E1E9-4088-A417-4A1E3FA45A87}"/>
-    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{F25141F1-2A1A-4157-A6AF-D54F20D26D6B}"/>
-    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{A562A1AD-EEBD-4343-B797-3DEC186BD57A}"/>
-    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{817D573A-4E2E-4DE3-AC64-6E885FEF3E8E}"/>
-    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{FD683E96-73F8-42F4-8EC8-BF7C913B02FF}"/>
-    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{18B54511-43E8-45E9-9FD7-5BCC45417F33}"/>
-    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{D3AA4A7A-4691-402A-B447-478BC506CF04}"/>
-    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{111CA10C-F9A7-4DBE-9EAA-786D59C5EA5D}"/>
-    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{F5C5F894-F32F-4394-B8D0-531D5299723D}"/>
-    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{8C612EF4-121E-401D-9DB4-01E65AC75DFB}"/>
-    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{53C7CBE6-D286-462C-902A-DD0E5DEE333F}"/>
-    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{841951E4-CBE1-4D55-9FAE-38EE63CA4DBC}"/>
-    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{C19883DA-C27B-4334-802F-996EA919C3FF}"/>
-    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{B4DCE4D5-3BEB-4E20-B05E-2B1054A28638}"/>
-    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{CD9F5247-4E8E-4FEC-8DB3-E40CE8AA5BF8}"/>
-    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{7FAD398C-FC75-4914-A303-730CB923B550}"/>
-    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{4505B386-6110-4B1A-9013-EDB69413EC34}"/>
-    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{750115CC-BCB5-4F9D-90A3-8A5994703DB1}"/>
-    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{F5E55E18-51D8-48F5-A400-DD7DB9BFD254}"/>
-    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{CBFEF3B3-2476-49E0-82E1-2AA432500783}"/>
-    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{3277FBC0-829D-4960-89CD-DA9C980D01CB}"/>
-    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{C3203BAD-23E7-4D27-9F68-02EA9E5E7CF7}"/>
-    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{8882BAC3-8A54-4D2E-B771-9C8FB58DCE53}"/>
-    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{077B69C0-8F25-473B-82D9-558639D513F7}"/>
-    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{9998ADD3-2DA9-4668-BCC9-896BFAE1D9FD}"/>
-    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{68EC9BC7-649D-4EAD-92D6-E85E12964DAE}"/>
-    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{FFAC9C4C-22F0-46A6-98D3-1099267E2B91}"/>
-    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{357C418E-4CE4-4023-B101-C9B19ED1C51D}"/>
-    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{85DF6A6A-5122-488F-91E9-BA4C7843F038}"/>
-    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{D45DC5C8-0F61-4C06-9AA0-50EC512E8F34}"/>
-    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{6C96299F-D031-416A-9768-550F91B6A913}"/>
-    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{09303433-6DF3-47FB-A293-395A1136F829}"/>
-    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{057A3F60-D4CD-43EF-AB96-42A0D8609C9D}"/>
-    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{B675AE30-EA63-458E-B6CA-322C2505ECD1}"/>
-    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{DC8206E9-88B5-4A88-8256-0F795823B19B}"/>
-    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{9F10AF62-43C9-49F1-8492-011300D51B1C}"/>
-    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{BF3B2A31-A121-4D68-BB9D-477A7B2D6B6F}"/>
-    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{A1C1E0D7-E259-45F8-A37D-0E63639ED714}"/>
-    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{1AE10A72-DFFD-49F4-A7EA-E3AE93581633}"/>
-    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{A3D94A67-E4B7-4214-AB94-0E5CCEA98E7E}"/>
-    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{4B1B9903-C06E-4C53-A453-555175AD66CB}"/>
-    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{E5B7E136-F1E8-447D-8ABE-A26CAF554C63}"/>
-    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{BF1ED14C-518D-4455-8B61-16B1BA0BFA39}"/>
-    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{1D2BF9DA-8294-4B1F-ACA1-88702E6367D1}"/>
-    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{4546EE46-C2A3-4F78-9867-6453381436F5}"/>
-    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{97635C78-C3A9-449C-B120-733FA06A33C5}"/>
-    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{5888879D-6016-40D8-A34F-44FA7F21D23D}"/>
-    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{BC4B803B-BA76-49D1-8804-44791E5152A2}"/>
-    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{927DBDCC-5179-40FD-BB35-31FC3F899986}"/>
-    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{34783F2F-1F89-4CB8-B994-2D83BC2133D2}"/>
-    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{3E52E9D7-ADAC-44DB-AA6E-8BCEB9FAD368}"/>
-    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{5FC272A3-049B-4CCD-A3D6-5DEF4B54A4A9}"/>
-    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{A7E13522-C40E-42DA-9EFD-FCBBE467FCDF}"/>
-    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{03991E79-5EA8-4769-8483-2F89A356BF45}"/>
-    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{85F238A3-590D-4EF4-9F39-787F77809A7B}"/>
-    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{D2F8066E-989B-4515-ACD0-FB26DA166BEA}"/>
-    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{5E4CF3F4-34B4-4D59-BED9-F66DBD5A95E1}"/>
-    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{B3122686-2C98-4892-952D-6847EA73788D}"/>
-    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{05A8F2A7-8192-4E61-A98A-BA17796ADFE2}"/>
-    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{107FE89E-14D4-4BFC-B7F6-BD09DCDC7E1A}"/>
-    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{D10FBBE9-6C08-4B9D-A0F2-C0DDA2AD6BA9}"/>
-    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{68A45235-741B-4990-88F6-5D2318200BE5}"/>
-    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{BC4B8489-73F4-4C70-B3EC-2CE84555E127}"/>
-    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{05DA43B0-167C-4BC9-B1A5-8302E920859B}"/>
-    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{7D9E845F-061F-4403-A6A1-0A77AC09A973}"/>
-    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{361D0CD4-C818-468E-B271-8C57400BE48F}"/>
-    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{83DD75FA-FE60-4D98-8A5D-3E97E2913213}"/>
-    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{0FD91E73-4D8D-44D5-8A29-3030F4EEF7D2}"/>
-    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{B22FAEBF-548B-4821-A7A4-2DB841B36C44}"/>
-    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{2961864A-D0CA-4817-8864-BB8E6D27A46D}"/>
-    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{31D5953B-32A0-4547-B8FF-019ECF450367}"/>
-    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{F3A13C34-63C5-45C8-A571-0A31B88479A1}"/>
-    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{A4E3B05A-731B-4352-8E87-9FC0E721C211}"/>
-    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{3690DB75-4259-4C67-A7CF-A4170BFCC73A}"/>
-    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{736C3021-C148-407A-B282-D6AFB28E2B36}"/>
-    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{18CE6C95-7D60-4D0F-B92B-BDAE9C5EBF44}"/>
-    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{AFE52139-DDF7-4971-915D-0004CDB25604}"/>
-    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{CABED0E0-F562-46C6-92C5-5706CE483FF0}"/>
-    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{74107D83-775C-4921-8CBF-7B6AB57FA847}"/>
-    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{07E3F77C-1089-45D7-ACD6-EB940D8319E0}"/>
-    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{693F065C-BA5D-4C4A-8C44-4CCA149BB7D7}"/>
-    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{94C5DBC9-466E-4670-870A-7E0F445B9C36}"/>
-    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{405A0F19-F6FE-41C4-A4F0-44D0456BBCDB}"/>
-    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{EFDE35CA-13CA-423C-8ED2-760C22E0E7D8}"/>
-    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{C6AB01F7-707D-4C79-AE90-67D8E8CA0FA3}"/>
-    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{9B983409-6C73-41A2-A503-F37DA6F6AC32}"/>
-    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{9195D426-E137-4924-8BE8-B36DEA82E497}"/>
-    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{8045E7C9-7E78-4ACC-AAAB-AC6B6DED218A}"/>
-    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{3B23ED67-13ED-4A9B-892A-514130A4370C}"/>
-    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{EAF82799-C14B-4049-9F3A-8AAB0692838F}"/>
-    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{A3ECCEBA-FD07-4F82-B836-814CEC23CA52}"/>
-    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{518E0780-7371-49D7-AD33-25AB44DAEF08}"/>
-    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{00E77F37-2C04-4030-B0D5-2FE97F3A0EA6}"/>
-    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{98EBEBB1-137D-451B-9594-6E96721EA12A}"/>
-    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{2C19815E-6BAF-455C-848C-2F8F0AB051EC}"/>
-    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{898E8029-94EE-4EBE-9245-D2533450D447}"/>
-    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{2D7D7CB3-707E-462D-A849-3424199BA070}"/>
-    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{08BF4BE9-274D-4747-BA6F-3DFD257A6573}"/>
-    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{4F9BBB9E-E495-4AFD-8468-E4EBA2DB7CB0}"/>
-    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{769CEDAF-8183-4F75-9770-19A1679EDFA7}"/>
-    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{A8B737E5-17A5-4C40-847B-34129CDEC2CB}"/>
-    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{FBFB72F1-59FD-4701-8014-D1EE3D78C5FC}"/>
-    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{9B470F38-DCC9-4024-BBB8-3960C072083C}"/>
-    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{2C9245F5-048C-429A-BED8-14B8836D0B6B}"/>
-    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{B6D432A8-7EFC-4A96-8FA1-B076A3489940}"/>
-    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{44DF3B6A-BF1C-4DD3-98AB-B3F9B580FF54}"/>
-    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{BAE7038E-FC1F-41A9-9C80-BD1C3622C96D}"/>
-    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{B461388C-D847-418A-A183-184F444940FF}"/>
-    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{FA87FCBE-0C39-4FD1-AA26-4E35F31C23D3}"/>
-    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{7E3F0096-D2BD-4B75-AEF2-1FDABE2BDA6B}"/>
-    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{6F2503FB-A6DB-4E36-9C77-AB77EA1B30B7}"/>
-    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{7AF23A93-F7FE-42E6-8FFA-5E8A3D4CAF8D}"/>
-    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{707179C2-48B8-49D0-A4D6-1344A9BD6F5D}"/>
-    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{42FAF839-18EC-4516-90C1-04858A56627C}"/>
-    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{A17C0520-021C-436E-AF89-264FC5412693}"/>
-    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{67BAA32D-39E8-49E8-95BE-E4FCFB42DAF5}"/>
-    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{D8C538D6-27AF-444E-9805-A90C77FA547C}"/>
-    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{D21DC3A8-1ABF-4E36-8B6D-0883CA69D1F4}"/>
-    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{437D836B-4289-4C59-8AD2-24084E0D3D71}"/>
-    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{50A6A663-3F34-4016-9FFC-F48ABF655A6C}"/>
-    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{1FF1E3B2-F399-40FF-8A05-D2281C788AD6}"/>
-    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{485565BF-D832-48A2-82AA-5585273CDE5E}"/>
-    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{A9398CE6-ACB3-4C68-B53E-470A08168D4F}"/>
-    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{05859A7B-A8EB-4CAD-963E-82181E3678EA}"/>
-    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{03A29973-9B2B-4E04-9B57-7386A46937B9}"/>
-    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{2F762429-33B1-4894-B698-6AA7E7B59435}"/>
-    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{E21202FE-BBEC-4C3A-AC76-6D9729E6CAF4}"/>
-    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{F58C8CF9-A657-42B1-817E-E2F00753C7DE}"/>
-    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{7639B4CF-25ED-4A3F-A570-BC79DC4840B6}"/>
-    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{D47D8423-3EDA-47A3-BEF1-54673E38C4D4}"/>
-    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{9BD63E23-C5B9-4E2E-8BCF-F9F0AF5AEFB2}"/>
-    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{CEFD6486-D0FB-4D11-882F-9FFCBBBE603E}"/>
-    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{4659728A-9FA1-4CFE-8B15-72C439543776}"/>
-    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{54103DA5-132D-4490-8ACB-31F1A56AD2C5}"/>
-    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{40F4FF9B-1FAB-45FE-B2C0-211F676D4203}"/>
-    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{3B341349-2FA8-4BE6-887E-4346DDAB0716}"/>
-    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{41B417DF-7BC9-4CC1-A86C-6B9CF20EE1B7}"/>
-    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{00D200DD-E86D-42FA-93AB-D76A39B8567F}"/>
-    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{F0159DB3-C4FF-4409-A96C-822F299A774F}"/>
-    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{CCDE9928-60E7-41D3-A7D0-2B8B90647296}"/>
-    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{5531F0E6-3619-4D42-85A0-874E8E95AF32}"/>
-    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{250FD988-F965-4D4B-A629-E8F7EAAEB714}"/>
-    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{2FBA145D-58F3-48C9-9917-3998DAD547E2}"/>
-    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{868252EA-7F39-43BE-96E5-64A21C860DEB}"/>
-    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{F7DFCD4F-1A8B-4F0F-9AC3-78A3E0787387}"/>
-    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{A37EC796-8E63-424E-8AE0-1CF11E0BF765}"/>
-    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{2BC31810-0236-4980-AD70-67902EC3671E}"/>
-    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{947462D8-8B9D-4D54-B536-0D24E8735067}"/>
-    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{9B09D246-052F-4C3A-B4C7-3C9687DD35D5}"/>
-    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{4A4971AC-2602-4810-A178-28AE3D21E01A}"/>
-    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{77B984C6-C056-4F4A-A6F1-1BB437D830BD}"/>
-    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{90099561-07BC-45AA-B7A1-13F8A5853EA8}"/>
-    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{86DA776E-68BA-47EB-B40E-3CED41C3EF78}"/>
-    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{6B6AA6F1-9C1B-4790-AB76-DFDA662B0D44}"/>
-    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{4F40EAB5-0441-452F-BF25-09CBDB7E7982}"/>
-    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{53739F5E-C3E8-4A2B-8E36-79316706DC9C}"/>
-    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{41FCBD72-CB13-4DDF-817C-A4E971E1A05B}"/>
-    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{2895D44A-3B39-4798-86E5-F3523CAA12A4}"/>
-    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{A2619D00-2015-4264-B7B5-1CDEFA3AF84A}"/>
-    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{B07D027E-EDE0-4884-984B-5D2BD41C8692}"/>
-    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{0E56CF29-C92B-445B-87B6-F7EF5B3D7F44}"/>
-    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{EC95B16E-D18A-4071-A53A-D6C12595EAE0}"/>
-    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{DEA96C40-B04C-4832-A6A0-65E4CD319280}"/>
-    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{23D2E1B5-9C29-4E39-9892-49D6C820A184}"/>
-    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{AA0059F6-6A13-41E4-B9C2-93A6785ECE62}"/>
-    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{0BCC515F-01B5-4101-BBAC-93E6D002E1C0}"/>
-    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{567B729E-6404-4712-96B8-24A46487BB02}"/>
-    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{76C3DEAA-DD5D-4040-A5B8-570A2B582CE7}"/>
-    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{6D4ADA83-7649-4CC1-8416-41E8A38713B7}"/>
-    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{EFB4807B-1AB6-414B-A615-BD39596DEB1A}"/>
-    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{6AFF259C-045E-43F6-A82F-6FDEF7774F2B}"/>
-    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{EF7129A5-FFC2-42C5-ADC8-5E029C452A33}"/>
-    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{8F973322-F917-4CB9-81DA-1E46150B144B}"/>
-    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{DFF1EE5C-3E28-4901-A49F-F1D897E1D389}"/>
-    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{4DED3E53-40BD-497D-9EEF-855FE45848D2}"/>
-    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{0F32BEB4-EEDC-4212-80C7-AC0DD7B043D3}"/>
-    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{ECA33CED-4CBE-43ED-A22F-B11650C577A7}"/>
-    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{C45A91ED-8982-4AD8-8738-59F06BD44536}"/>
-    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{30A5E8DC-474B-497E-91C9-56E057CAAF5B}"/>
-    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{2BC09CFD-10F9-4178-9BC2-AA7E91C039F6}"/>
-    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{DFF1E992-5AAC-42EF-A96E-19D9CF9BC9B1}"/>
-    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{D31393C8-6058-4C7A-890D-34428D9534D9}"/>
-    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{070C593A-8593-4F89-934B-88690B270EDA}"/>
-    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{0899ED88-5B7D-405A-B3DC-013AA5CDF370}"/>
-    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{3D900CFC-907B-4A30-8AD1-72E0CF5B880A}"/>
-    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{A75B2B1B-0B63-499C-B30C-AFE4B545EABA}"/>
-    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{4E8F2A8A-4D7B-479F-BC44-ECB829C24189}"/>
-    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{CEE9AFE0-2612-4BC4-A3C4-B056C3F4A73A}"/>
-    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{C219B386-CB33-44F9-955A-A653329CDA68}"/>
-    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{0D80E769-582B-4A49-84EE-DB25E1A9C413}"/>
-    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{892998B6-F589-46F7-A020-40A7068DDACD}"/>
-    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{E3C70C71-FA96-4FB5-B8C7-C07D1F4B4F2F}"/>
-    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{F429E7F0-D56B-4241-9A61-9359CEB09AB4}"/>
-    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{05278B88-92F3-4604-B525-9FAA3D3BC2A0}"/>
-    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{D95E78E0-7A7A-4EF6-B17E-127B767C9D50}"/>
-    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{966B732E-DCCB-4C01-BD1D-8D88F1E749F7}"/>
-    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{D7516294-CFD8-4834-9C85-79544C4C5542}"/>
-    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{C79EF5F6-2D2F-4770-8051-2F1439D30E54}"/>
-    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{4FB460A0-3A2E-47EF-A4C1-DB62D39D5C03}"/>
-    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{99D1361D-3E54-4A58-827F-CAEF78A418A6}"/>
-    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{93A24B7F-18BD-4739-BFD9-05CD49B1B271}"/>
-    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{380FA9BF-EBD6-4392-A997-4DAEAD11F05B}"/>
-    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{7B94E33E-AA67-4C0C-81F1-D1354A583F45}"/>
-    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{E1C24387-3612-4596-843D-8EE7226A1188}"/>
-    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{DE2948CC-4A2E-47DD-9591-D0726BD39B8B}"/>
-    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{050082B3-A8F8-43BB-9C1E-C328B53CB344}"/>
-    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{4F957744-CC21-4938-80C1-1AA7FF78870D}"/>
-    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{59C33909-B569-4C48-8C08-E0781E2EB210}"/>
-    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{61D96615-6DD9-4231-A95F-4DB71BFDD14E}"/>
-    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{80202EC0-2CA7-4AFE-BCFF-A2720749679B}"/>
-    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{3DACC6B8-2ED5-4342-A7B4-84160DFBDB63}"/>
-    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{841E7B1A-DA0A-4A8C-B62B-F8FF0B8B5A73}"/>
-    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{738F530E-8A61-420B-8308-9E87AD393FD5}"/>
-    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{E16DA4E0-8E91-4A5E-8C62-388C731FC9ED}"/>
-    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{40FA7469-7EFA-406F-8C16-3D7B7DF9DFBA}"/>
-    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{5B9F393B-0ADF-48AA-8BA1-8D009E6A8A44}"/>
-    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{593726CA-BF86-4579-B36B-10826FEF67F5}"/>
-    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{76CE75DC-1BF8-49AE-8D4F-50532DF14362}"/>
-    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{EA7C6C34-B2D7-477B-8FBB-3173E0422284}"/>
-    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{EACFAFAB-A210-4BC8-B304-B67FE6B0E373}"/>
-    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{2D429A81-8139-4117-AD59-0293570721DE}"/>
-    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{14F169DB-7A76-4C56-B759-B02F1C56447F}"/>
-    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{8252C522-26F5-4537-A2AC-E0FF50E5A8C6}"/>
-    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{1E7EDF23-4C6C-44D5-B7DC-00A4A306482E}"/>
-    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{047D50D4-523A-49A8-A009-1034D16F51B3}"/>
-    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{86D04CF7-E754-4701-B063-13FF684E5CA3}"/>
-    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{D1E7FE28-6042-4EC4-9067-4ED3225AFE6A}"/>
-    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{8364BA44-21B1-4DD1-A82D-051B09A0A1E6}"/>
-    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{5AECB991-76FB-48DB-B3D9-3FC0041B6424}"/>
-    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{8C5D740F-78E4-4606-81F0-4344B7100198}"/>
-    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{C5625E7D-48AC-4B59-B3F0-C41729B909BA}"/>
-    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{B2339C55-670A-437C-9ADA-4F43D4F1335E}"/>
-    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{00505909-3BA5-47AE-8332-00C19204435C}"/>
-    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{0D61342F-D09A-4157-8672-B59B70AEAD58}"/>
-    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{E8500DFE-5CD7-450E-8C35-70EE24ED93E1}"/>
-    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{2ACA6F22-4283-46D7-8F0E-F63A9A35CD07}"/>
-    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{60B23B70-A0D0-4839-AAB2-15BACDEC2447}"/>
-    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{1A223BB5-F7B1-4DB7-91A4-5F6F3A0EA06A}"/>
-    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{C213ED2B-53A7-4C23-9849-F69B431E28F5}"/>
-    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{C77AEDF9-5AAB-44C0-A05C-9D7868C85B38}"/>
-    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{FC911F8B-C60E-43FC-9227-ABD73D74E772}"/>
-    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{5A764E82-7E02-4E1A-AC1A-BE0929CB6971}"/>
-    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{BD45781E-E053-4EBC-AF72-F33F7BA7D52C}"/>
-    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{DB4AA7BC-8DEC-4B7E-B8CB-FFE386A25877}"/>
-    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{49B4FFD7-D850-44B7-ABBD-92F1E1AE876B}"/>
-    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{16559992-2E5A-4C07-8F75-1C8B40512A8A}"/>
-    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{6F6D2767-FF9F-497E-9DA7-F4550F62DDC1}"/>
-    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{80CCE185-2EB9-4D03-9A6F-563BF3E215E9}"/>
-    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{AD90749A-110B-4C6E-B0B7-658CB120E97F}"/>
-    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{2B8F061B-6DF9-4944-80BA-EC8D0446F6BB}"/>
-    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{2CDF3B0E-A8F0-425A-AFDB-2D71EE2E6632}"/>
-    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{9DA6A9A8-7C68-45E4-B695-A4451089DB4E}"/>
-    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{44F194B6-31AE-49BD-B91E-8B70805F4111}"/>
-    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{AC7F9E35-F8A0-42A1-AF1F-1B3861B97CA6}"/>
-    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{9D512D66-A2A5-4C49-AE6A-A916F9772611}"/>
-    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{EF28AC45-4F57-450A-A3AC-008EAB907875}"/>
-    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{8F7F1BCF-B3F3-4D82-883C-0CC94E180A90}"/>
-    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{980B17DF-4E5B-4DE0-A7AB-5D05ACCBBF32}"/>
-    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{7DD4F744-7F81-4C47-A3E3-B1CD7B5A3DA7}"/>
-    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{4C9B23FB-EB54-4EBB-B772-FB9CD9C8E650}"/>
-    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{2CEC3CAB-0348-4435-9F65-A49864F99BFA}"/>
-    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{58A79C7A-CBD1-4E22-9D91-C5A2A5AAC8ED}"/>
-    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{00723527-E121-402B-8351-2A401C849188}"/>
-    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{8E4E1274-FDA0-40B0-946C-91B902F4A5BD}"/>
-    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{E0D01E63-D487-45C4-8457-69CEFB7FF732}"/>
-    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{1F137146-0586-4264-B0D5-2CB2A022385A}"/>
-    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{0741228F-EC21-47E3-B3B6-4E8B470B6901}"/>
-    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{6DE3CFE1-0CCE-4217-86FB-DE5C332C0F2F}"/>
-    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{DCD5A7F5-6587-4F6C-96F1-A457F2940209}"/>
-    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{23027AEF-B335-4232-9815-55882D6C1BFD}"/>
-    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{73B36F37-0D44-4DF1-B21E-4BED7CFDA46A}"/>
-    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{9036990E-D854-4702-8C98-A989FC483745}"/>
-    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{025158CA-4380-4A51-A186-DCBD7B252124}"/>
-    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{91B8B71F-9DEB-4630-80BA-A2541E124D49}"/>
-    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{EC40C022-7764-4D6B-89CA-1EF499858E5C}"/>
-    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{0E3BE111-F844-4E90-8F76-08846D8DFFE9}"/>
-    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{8E52DB15-67F1-4601-A5DC-B056461F26CA}"/>
-    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{31B1199A-80AD-4433-B8A8-051BBE2F938E}"/>
-    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{CB0F3E27-40A5-45E8-8B42-EB853F2D223C}"/>
-    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{3BB6F0A4-9BEF-4244-AF44-E0673D75695E}"/>
-    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{52FE4B70-2DE9-4B32-8E17-FC0CE3E11FEC}"/>
-    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{9EF1A63D-F950-46E2-96E8-24CDEA2F3C0B}"/>
-    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{6810904C-EA36-4B49-BD10-165DBD2A69BE}"/>
-    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{7D1EAEF9-5761-466D-89E2-39EB4DF0C610}"/>
-    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{D2EB1636-16E3-4D14-8B86-F0DFA536C170}"/>
-    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{0517372B-EC36-4808-963E-AB386E3DE966}"/>
-    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{803DAD50-9461-415F-84DA-906B99748413}"/>
-    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{31477E27-7D5C-4DF4-84B6-770243E700D0}"/>
-    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{A0A17232-F947-46DC-8A27-1B8BBCDE0267}"/>
-    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{2F78C896-63D7-4FDB-9EF7-1FF48CE88BE0}"/>
-    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{1B5C6DB9-2C8A-42D0-8D6A-A5CC442D3BF3}"/>
-    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{15CDAB22-98DD-483F-8EB4-29D957DC7090}"/>
-    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{89831428-98A9-45F4-92E6-1914B8D7D74C}"/>
-    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{1CF901F0-A2FE-4931-BCF1-23A6108D6587}"/>
-    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{01FB9AB7-428D-489D-80C1-0C1CE3CACC94}"/>
-    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{1BA410E4-0532-4BC4-83B1-2CD46517B2AD}"/>
-    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{8EA29A9B-529A-4D24-B649-DF2903E7D491}"/>
-    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{02205BA3-7D4B-42CE-84AD-2669FBB5A4B2}"/>
-    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{8580DA61-EA64-4123-8B23-E2C42675D133}"/>
-    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{C6FF47FE-7206-431D-95BA-ACA677EC6969}"/>
-    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{6B2AE59E-3B9C-4616-836B-75A493A546CF}"/>
-    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{A1CCD124-0C50-4EFA-9C2B-4B2026F7F2EF}"/>
-    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{A4C5C78B-1C0D-48DF-8175-45D14255DF3E}"/>
-    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{240A2C4A-B247-4978-A0BA-01DEEC63C8E1}"/>
-    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{703866F3-031F-4E81-B2F4-7D1E0033771F}"/>
-    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{DB44416D-FC1F-4889-B09F-F36AED2442ED}"/>
-    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{A7B25192-2EAE-4D94-94FD-576B29BA6D38}"/>
-    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{57940B61-8C52-4C85-B7F4-1F660AC02EBE}"/>
-    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{5087E42F-5512-484B-A39E-A7E79793D7E8}"/>
-    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{6C7CD7B1-46A9-4FC3-96C4-CE9A29A2606F}"/>
-    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{94A107E0-4D0D-49AE-BB64-D76B9CF2C965}"/>
-    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{01BE0737-5F82-4007-BA81-F4F659D86B3E}"/>
-    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{AAE7FA79-1240-4401-8001-890BB2C5C1A9}"/>
-    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{31AAF33D-E0CC-4347-886C-863BC0C4EBC3}"/>
-    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{E3E2BD2C-FE11-49CF-874F-6132192F71A4}"/>
-    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{D8E34B6F-EC9A-4569-951C-4D47BC090B88}"/>
-    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{71EB4EA6-02DC-43D3-AA78-DA669CED5511}"/>
-    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{BE709898-4C16-427B-9558-ED7EE2D74CE2}"/>
-    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{0C8124A6-A0F3-43FD-857B-002B20A6C096}"/>
-    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{21ACA1A2-CE78-414F-B403-4037453A0422}"/>
-    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{AB69D8F1-EA67-45EB-8FDD-112741D4004A}"/>
-    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{8C603AD6-A9C7-47A1-B14C-A2A4FE39680A}"/>
-    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{A55B5EE4-D20D-407A-9DC9-8054FDB800E7}"/>
-    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{91FF72A7-77BB-4F13-86EB-FA85BE1BFB6E}"/>
-    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{9FEBC35C-8F2A-4D70-A95F-3EBFE207E6C6}"/>
-    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{3F347239-F478-4AAD-B8C7-D2CD283F10B2}"/>
-    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{B7F9D7C8-B3CA-4246-87FC-BEED2CF7129B}"/>
-    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{5B9EDD68-C88B-48A2-B2B0-39EE33DF117A}"/>
-    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{695DBFE3-4ABD-4562-B429-186FDBFC30DF}"/>
-    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{D0A86A63-EFB0-4B1D-8CDF-40FB41B0B9FA}"/>
-    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{EC811C8F-6702-481C-8E7D-4B59F844DA10}"/>
-    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{A618691F-490F-41D2-9442-51E9995BDC42}"/>
-    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{2FBEFF2E-FD0C-4671-87ED-E57662A437A9}"/>
-    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{F3B2D0EF-BC45-41E6-B917-052879108D4C}"/>
-    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{B1145ACE-2113-45BE-B200-94667838B3B5}"/>
-    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{EE3F90DD-F6F3-41F6-8F36-C50670E3E0A1}"/>
-    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{0987E8B1-306F-4640-ABD5-49AC7732E240}"/>
-    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{F65DAEE8-F57A-4025-A92A-A3A6246BE519}"/>
-    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{112976F6-9541-4D02-AE2B-DD74645ADA7F}"/>
-    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{8376073B-4BCE-448D-B1C6-C64E1ED67B3E}"/>
-    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{BA8E4758-06A4-4201-834D-4036E5A621D5}"/>
-    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{D3972A93-F67F-4C76-9922-6C387EB1F2DF}"/>
-    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{48355588-1837-4C63-B519-1AFFFB51E775}"/>
-    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{A7E02C0F-BE4B-4C9F-93CE-F2FDE54BFAF6}"/>
-    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{97DD071E-28E3-4AE4-9D75-75A817BEBB20}"/>
-    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{E334457E-01B3-4A6D-B98C-1A74009B0107}"/>
-    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{1F1E09AC-1CD9-4FC4-9AC8-0BD99EF01CE6}"/>
-    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{EDB1C3F9-D85A-45A0-887C-DB1EEEC5B918}"/>
-    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{3054FF1A-EB1E-40D0-95D8-BDEBA41A7A0A}"/>
-    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{88CB0CD2-3B34-4262-B91C-9F0F7C6868AC}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{5C84C89C-EC66-4BE9-8433-6FEE878CC6AA}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{7B06E4BD-B247-4999-A3E0-AAD4D5B0475B}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{CE815206-5C5D-4BB8-9B07-3DA04828BE01}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{AC328FFC-09E7-4FF7-A26B-74D4C9CAB15F}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{B18368CC-8497-4BB5-AEAD-D2598F91E2CB}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{0D713C12-61D6-478A-93C8-134A13BD6484}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{280E36FF-9DA8-49C3-9732-2895BF18C202}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{CA4C7E49-798E-48A0-BE91-89AC9043E5E6}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{6263329D-55CE-474F-ADEF-08D16B9DE210}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{3EE66B21-EEDE-45FF-A407-1AE4BF3791DC}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{3BCDA23C-563F-4C76-8E9A-C83DDF361713}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{33459195-98E3-4DB8-853F-03798A690216}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{521A79C8-F71D-46EF-99C2-093A50D4CE72}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{E7ADDAC1-DB8D-4D5B-8E44-460A2B2E794A}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{80B7B620-E6A4-48B5-8F2A-7242C5A3CA52}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{9E503973-36C3-4C4F-8931-AEA4399D4E11}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{CB8C7DBE-D747-4C29-A2B7-FCF78D5102B2}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{914256F0-5514-44B7-A0A7-94E24C1F88B6}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{594BF5E6-5323-41D6-AA27-D08647C6C347}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{9B3EB5B0-26E4-4909-9622-7AB21D6BF9F5}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{D4E325AC-8129-42AF-A17F-DAEFC40467BF}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{E2BE28F1-79B9-48EF-990E-51F862666079}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{5D5E0C47-61C7-46A4-B70E-FDABCDC53B1F}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{5F8F6963-5AE5-4866-8908-00E8DD1EAC59}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{D3B10734-7AF5-4641-8559-63FE7C2848DD}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{66BE6C87-57A0-4385-8906-AECF54021AAA}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{E34C81A2-A89D-484A-BC93-03574752F126}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{201917BB-A36C-4DA4-908A-8D962EDFB6CC}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{1E9642C7-09B4-4159-9811-CA085ECAFFE5}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{9C25F095-8A7B-4299-8571-08D9ED461B72}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{85EEEAAC-F0E2-4569-A941-4C7484EFB069}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{ED9CF52F-E820-4E8C-8124-5A065B01CE2C}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{001F4AF1-B2F2-4375-8F76-08C1BBFAADE0}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{E0FE9AC2-E123-4EA9-834B-4A97A9AE1C62}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{4EE12511-02CC-42FB-B5E1-3F01A8B7A843}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{4F3308D6-8E5C-482E-81EB-BD33C6265068}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{254E9B17-A0A7-4FC1-BB7E-91A3D30DB295}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{2F5C8044-4F54-4E67-BF60-4F2A518D6281}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{3F24C275-5A06-45A0-A0E9-702A3A8690BF}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{5FE9EE38-EFA2-4C20-9F3C-E78F796C49CE}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{B5CAAF8C-8B40-4F98-953D-55963B525F60}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{C77D7477-309F-4831-BA74-2968066DBC3B}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{21E49855-9F8C-4C4D-AE49-B213633E4B4F}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{3A5F7DF9-872B-49EE-A1AB-6346652F8357}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{D4A1EBE0-A83E-4874-8585-D1A43D9C27BD}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{89816DFC-57A8-421A-BF2B-489A260A2A60}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{F99FC190-63AE-4D75-98B7-921D605B87FE}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{CB795A44-69FB-49DD-A849-B0A3AD0A7633}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{2F459AAB-1C38-46CF-A5C9-1490FDFEBC7D}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{04146260-3849-4E51-8A86-D3B4932DF372}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{BF1533EF-D0A6-47AE-8FF4-CA9539802964}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{EFCE3167-8296-4032-B68E-DDF6BCD4219B}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{7B7FE882-99AF-4FD4-858B-6F0BDB59A2BB}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{21FCE30D-3646-4192-9222-983CB0E212BE}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{35B2F997-737D-418D-A451-7351E79EDD21}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{711F4C3D-DBAD-4D4A-88C5-75F267E008CA}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{EADD91AE-E1FE-4E4C-857D-B6B9AE3C285B}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{82392A22-0457-4965-BCBF-7CA059A92B16}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{FE90417E-4F63-4DE9-9054-32896CF5B88D}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{37D77441-48D9-4FAC-BB99-EA2559DFBBDF}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{40066A73-FC92-44CA-A367-1B2012556A08}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{FA2514EC-89A0-4F40-A2A5-AC64D16D391B}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{E729D86C-98D3-453A-BFB1-65A73F8E8877}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{026BE6C8-01CC-45B8-A699-174E0EE8D54E}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{175A977F-3240-4570-8513-D8C2D0AF0429}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{780CB63D-B702-46DE-ABA9-FBF581BE4622}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{9CCD9DD5-8009-49E7-B920-0DA11FD32AE7}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{B5FDA060-4373-4619-9E99-4ADC74D26460}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{53B2BE56-2873-405D-BEB1-7661B8CF8E6F}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{B2CC6130-EC71-4848-88EE-F92DD6BE1DFC}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{72894EA9-DFCE-46A0-B3B3-BAD9E5F62BDC}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{89339090-EA66-4FBC-8423-D514528BE12F}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{C2CEB6C2-0F0B-4EB1-8988-447EBB5BD576}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{BA1B4F82-2EA7-4F8F-8099-95FB432D9C32}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{74C1DDED-A18E-4EE4-BC03-88EDC8E22F98}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{8CA1B7BD-5852-4F03-AA26-10145DADB5C1}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{357D2664-30E1-4596-8A3D-4204FBD2C722}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{C5887AEA-9A3F-4B52-A4D3-511F41C6FB78}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{F938ADF6-A6F1-402C-8E2A-EAD0AE1AF360}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{7281DE4D-359F-457E-B3CF-6534950B0F0A}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{629F586C-2448-4E2F-9D81-22C9871C4FB9}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{48A48B11-387B-4590-95F2-A936BEBED106}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{4D1C98C9-D138-41F0-969D-D0BCA827FE0F}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{1C3E3F79-4DA3-4945-B9CC-3137F624769F}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{12146C4B-8A9B-4A23-B1EE-A04CE9852FA6}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{C9B3CB89-7E1E-4A9E-B5F1-B0CCEF5262DB}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{C52E55E0-1651-4D43-A2B3-77F83CD4A066}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{0CB4A77F-6657-4875-954C-9FD427F1545B}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{E1133A33-752E-4685-90A1-78AC100A1A6A}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{FE45B744-86AB-4B87-86C1-5080362EF175}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{9BA99935-B8A8-49B3-97BC-221D7B740CE5}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{962EE0A5-7EE1-487D-AC5B-3C0B36B0E66A}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{3A9783CF-0872-4779-8B04-F145AF7DA61D}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{29DFCC34-9D02-4D27-AAE5-DD172751CFAB}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{AEF486CC-697E-452C-B8CD-C235D2062A23}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{CF50B4DC-7787-4369-8AA3-EEC5175891C8}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{49A17C12-CF02-4C2D-8591-DD12561F26AB}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{9EB0AAF7-F8A1-440B-A9EC-F7ACB43DC484}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{29E2EC0E-4C6C-4950-AFEA-C89DD459A5DA}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{70692CEF-78ED-4A2D-ACF5-A35A6B58655E}"/>
+    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{57C4FBB6-A92E-488A-92EB-59578036A88A}"/>
+    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{C4D8016B-A707-4F85-8987-AFAFB84EF298}"/>
+    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{293DB7B9-3DFF-433C-93A9-DA049B1CF77E}"/>
+    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{B7F3CB49-8D73-40DE-939B-C85E6FA3CE10}"/>
+    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{3CC20C99-2C93-4EC7-A657-2045ECB0DBCC}"/>
+    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{9FEA57C0-9399-4D4D-B7D2-EE479821B247}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{F277B3FE-6A81-44A9-BBBE-594C7E10BAF7}"/>
+    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{99C173A3-8147-4680-9B36-C4E804B560BE}"/>
+    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{275459FC-AEA7-4EB4-B0C8-DE677E893E47}"/>
+    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{125E7FBA-75FB-4EFE-8379-8B4D7C18B1FD}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{02762AB4-4B35-4E1F-8228-5A2B6907F0ED}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{21192263-6F93-4458-AB7C-2C41B24D1F51}"/>
+    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{FDD074FA-6CD5-4BB3-8462-2C6F9B604D6D}"/>
+    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{18015AB0-7875-4BF7-BC65-15998EF86ACB}"/>
+    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{900B0E52-8155-4838-893E-5BD6FBE5C860}"/>
+    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{1CAD854B-09AB-4EBD-81CB-6A75662E7E56}"/>
+    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{C9EB53B7-F8AE-490E-A03E-993A68A15D4C}"/>
+    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{7E55AE27-3E83-4CF9-8253-77F568087BE6}"/>
+    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{C9C8DA10-DC45-4211-A96E-80DDDDCB9439}"/>
+    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{11B210D0-855E-45EF-9FF5-D0BD6C3A48FC}"/>
+    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{490B6F03-4DC2-4865-AC88-3D12453768DD}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{DC6A6C14-8CA3-4BCC-96AC-8F1F6794515E}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{E3C9CDE2-7911-42E0-8BEE-B48546BAB575}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{08E189E4-1C01-41E0-80E1-697EEF8DC3F9}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{40C3D8FB-DA48-4B75-B9C2-E2B8B7477707}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{6CA89123-C8C6-4663-A5B1-9FEB9F6D73E4}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{2F11A377-4523-4A69-BF66-8186D31902A1}"/>
+    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{1F6BB93B-1816-4F17-9629-9FEC9DF1A167}"/>
+    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{CF1B9E94-6C93-4D38-B2B2-B4AC3AF22718}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{70AE736D-EBAD-4E85-8656-CBD5A5DEF8B5}"/>
+    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{C7073AAC-787F-49E9-8AF7-1A75FDDBC94E}"/>
+    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{3CA717DB-9F3E-4AF5-B09F-C63CD525EA9F}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{12AF662E-1763-49BE-B33E-3EDB2F75DB81}"/>
+    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{23041EA9-4BCD-4BE9-884A-F8A4EF6D4CE0}"/>
+    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{BE41C7CE-6D4C-4BE4-B0B9-4AA9186B2BEB}"/>
+    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{2858237B-CE56-4FCC-A9E7-32F04BCFB2D0}"/>
+    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{686717AC-31B1-482E-AEE6-8EFB199D4B54}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{F9D98A64-65FB-45E0-8DBD-FE301663AFD7}"/>
+    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{47B62886-8D42-4551-ABD3-BD57792E18B3}"/>
+    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{04DE8955-BDB5-434E-B070-E852BD2E5AEF}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{4C411850-E1BC-4C5B-A658-81AD8B065F17}"/>
+    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{0D69F557-0402-45E7-889B-FBCA0A57EC6C}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{4697794B-35E9-4EDE-8566-FD9944018FC9}"/>
+    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{12A343D9-DF9F-4407-BAB4-99930B2ECFBF}"/>
+    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{1AFFE813-1966-4E81-B97B-DA2DA9CF1D65}"/>
+    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{72EA8357-63C4-4773-91F3-865C8BB8BBCE}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{BC726F0B-D7BA-4DF4-9042-CB03212D47DD}"/>
+    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{44A98665-17B2-4545-BCB0-897F5EA182AB}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{81843F54-2F08-4DB6-8145-D822913C42C9}"/>
+    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{1EC04B7E-91B6-445E-8AE8-3A4CC6C28015}"/>
+    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{4CA94B10-41A0-4775-9A5E-7E2A6EF5582F}"/>
+    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{12585966-0F09-4045-9672-9906D51FA335}"/>
+    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{25BD4E51-0232-48FE-8AF1-3E0C71FF7EF0}"/>
+    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{D9D84557-B66C-446D-BDDE-BAB4F6A385B8}"/>
+    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{03E0EBFA-38F4-42AC-838F-E098A1811068}"/>
+    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{FE55EFBD-7099-4221-A7ED-06A049057E6C}"/>
+    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{B2144A6B-C20D-415A-A6CE-532FE7F0ED2C}"/>
+    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{C1FA2635-5C4B-4D5A-9D5C-F503FFBFF2D0}"/>
+    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{7469D590-F56E-462D-BBB5-9D732F988771}"/>
+    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{478BDA3A-5B17-4050-9035-A8D63D8C506D}"/>
+    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{FB5111A0-E838-4F46-A69F-282C6329392E}"/>
+    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{F54BD6DA-4729-4B23-B558-8DDB2A98E651}"/>
+    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{3758A706-F1A1-4A6D-98D3-41F7E0754372}"/>
+    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{94ADA259-F120-47E5-B48D-229A5D54D155}"/>
+    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{B5F05259-384E-432C-839D-BEBF4424D6A5}"/>
+    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{7D1060EF-4B34-4995-8115-94F28F2FEDF9}"/>
+    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{6618E98D-1727-4EFC-9E26-98C627C646D9}"/>
+    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{E51E89C0-DC85-4BA6-B06B-40C6A8057CFF}"/>
+    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{BBF70E11-604E-4168-BC01-750A3A8526E7}"/>
+    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{DDC6899F-2573-40BC-9E5F-F4CB3B0BD344}"/>
+    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{439C56DC-E64D-4514-B1FA-615A20718BF2}"/>
+    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{E7287DB5-E25F-4808-88C9-CA9EA885AADA}"/>
+    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{2C1F2860-952E-491A-BF01-C61E95F89B8B}"/>
+    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{7F1A7924-8454-45D7-B664-15F9E0BBC998}"/>
+    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{A26FDE9D-29B4-4BAB-A232-F307AD51879B}"/>
+    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{34CEB2C0-3A52-4A14-92EB-F2C6AD2C33F6}"/>
+    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{27700E61-3A15-48CD-898E-150A377882E5}"/>
+    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{2AE57E0E-92EA-4A31-B6A0-1DE5B9C941D2}"/>
+    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{944BA521-29A1-4063-974A-14B538F981DE}"/>
+    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{07AA365D-42D1-4C47-B7EF-F858DE815E5B}"/>
+    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{8F1881F5-1652-43E8-9042-A55439890964}"/>
+    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{4DF1A851-2B07-4B9B-A18F-10D4D50A5D73}"/>
+    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{C42B8024-5C2F-4517-A1F2-6138E4A3A266}"/>
+    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{BFF8AA93-AFCD-47B0-A841-5CB9B6AF7891}"/>
+    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{096E0E38-6976-4060-B67A-CA0E22EAFC26}"/>
+    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{60580C2E-5085-4470-9B45-4AF27E51C3B0}"/>
+    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{F05A7762-5160-4737-B880-1BE1A79B5961}"/>
+    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{27DBA3D9-29C2-495F-8163-F7D2BF3CFCA0}"/>
+    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{1CA86324-FD3C-40B2-9A61-F356802EFB2B}"/>
+    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{5C1B7B1B-B175-4DBE-807F-A4462854968D}"/>
+    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{DEC27BC4-5434-4AFE-93D3-A4402D8D7759}"/>
+    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{04924825-A94A-447D-96E4-031B5FF0504F}"/>
+    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{478F207C-20D3-4F4B-A08C-DAE3B6B529C4}"/>
+    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{2B2D9877-9557-4B12-9396-DF14CCC4DD58}"/>
+    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{19A2CBD3-2CA3-48F1-8F60-B6AC0EE60C11}"/>
+    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{9ADA1E1B-1978-4A8E-808C-2DB76A14B48D}"/>
+    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{A9A501C9-664E-47DF-850C-36A687E8D19B}"/>
+    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{A6D1B241-50F4-445A-A730-120FE415623B}"/>
+    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{A7562668-4717-46DC-8D23-FE31F8A8C302}"/>
+    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{32787952-AF3B-4FC8-B26D-27DF63D78438}"/>
+    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{28B74272-E223-4547-BE19-CBA0102D347B}"/>
+    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{FFD7A4C2-1132-4C29-BDF6-9B42402D348C}"/>
+    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{CF7AA2EF-8A09-48AA-B5A7-273601086615}"/>
+    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{82EDDB09-CC7E-4FA0-BC2D-FD29F47634E4}"/>
+    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{4DBDD9B3-4DC0-4C49-8995-C02E08A032BE}"/>
+    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{ECDCE062-CE7F-4CEE-A193-B7E937D035B9}"/>
+    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{CBC933BE-34E1-4506-B0B5-031BDAC53D1A}"/>
+    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{FF2F6AF9-EA17-4D6A-A284-3FF875AE567E}"/>
+    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{7606A263-ED32-4DA8-A33A-5CA14B44F733}"/>
+    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{A1255457-70A6-4A55-BB2A-C97E38F5D565}"/>
+    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{E3681523-AC26-4253-AD1D-A58D47DAF179}"/>
+    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{7D0C889F-46A3-4081-9CF7-572B71B58C45}"/>
+    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{A6F8E3E3-C7A8-4CFA-81E6-80C50750459A}"/>
+    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{12D67002-FED7-41EE-A476-C3FCCF95C5F2}"/>
+    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{D6705D1C-7463-42FF-B412-53BF5AAE2DD6}"/>
+    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{F011CC62-EEC7-4813-8EA9-1BF1E042F596}"/>
+    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{D9D3E851-2792-4861-AF35-AAFDB80FDB96}"/>
+    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{21D9C6AF-0424-4B6D-99C1-D4BB74368E7F}"/>
+    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{A7E5FA1C-F51D-4133-9311-BC4FAAF6C567}"/>
+    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{2A8A3E4D-B404-43FA-BC9F-F76F5BDB2B1F}"/>
+    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{A3987FD0-3DC2-4D31-B96E-FE4BB94691E5}"/>
+    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{A69B9C66-E89E-4E42-A06B-491FF0AC4515}"/>
+    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{8B811928-532D-4D48-82A2-A7B4AF2728E4}"/>
+    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{8A8DDA16-67CC-401E-853A-61D672502EA2}"/>
+    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{78A89724-4785-47E2-8655-F438C0EFF925}"/>
+    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{A5B4E085-1ADB-48D7-AB04-E4E9E13AF297}"/>
+    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{D4EC9CFC-A51E-465F-BD49-45297DC4964E}"/>
+    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{BA196D1A-A908-46FC-AF40-B3963E35FF5C}"/>
+    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{B7233543-5054-4B77-9EA8-F307F7C84438}"/>
+    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{CDF1F468-D221-46BA-83F5-CFB0DA4E0FD5}"/>
+    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{C1FFAD3A-1C56-43BD-B811-1EEB0B68D56F}"/>
+    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{8ABD8642-FDA1-492B-85D9-9C4119052163}"/>
+    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{2AEB00D6-82DB-48A4-87C4-FF794C7F4E03}"/>
+    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{B44611E8-6597-46CB-ADB7-752BE96EA5B5}"/>
+    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{3255FD6F-7825-4F6F-8153-2786118BBF4A}"/>
+    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{23CF815B-2449-4984-BD6F-A649F581F2FF}"/>
+    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{7CE553A2-4716-44EE-B116-690B3F21B758}"/>
+    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{E6C3AF01-060D-4869-9D42-72117C7E3159}"/>
+    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{1237DD09-F151-42DE-AFF7-E91355D867B6}"/>
+    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{3CA2E917-FDCC-4E02-94A4-540A95D6EB26}"/>
+    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{5EB998B2-B1BB-4D3C-AB53-C9BBE430ABBB}"/>
+    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{F86A8862-EB5C-4AF8-90C9-38C7E9398F07}"/>
+    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{A18FE846-877E-4817-9693-BC3A6FFD5B6D}"/>
+    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{D60E5709-7BE5-4E2A-9CA3-2C190AC7E0B6}"/>
+    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{0C42DD3D-9E47-440E-9D2D-C56C46E82C8A}"/>
+    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{8FFFB991-6DFA-40BA-8B8C-12A8C92A8254}"/>
+    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{9B9CFA47-5D1D-4848-B3D5-9950D40EA332}"/>
+    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{3ACE965A-9551-416F-8DB2-73AC013E064C}"/>
+    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{0BB9B3E5-B5CC-4601-997D-F3B4DCCEA712}"/>
+    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{BC202FEB-DF85-40AB-BBC8-6D44A60822DC}"/>
+    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{64E75BCF-1FDD-4F51-82CA-A98A35B54B78}"/>
+    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{5A35EB4B-5F8A-48FE-A451-0A5339E6F74C}"/>
+    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{0F820133-A41B-46C9-BCE5-9993146F0A33}"/>
+    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{7AD5A673-437B-443B-ADA6-C1A1EF68E181}"/>
+    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{4C09E369-123B-4574-B9A8-AF27BC31B793}"/>
+    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{06EC3B0E-E0D9-48F2-8023-1A2251FE5EF8}"/>
+    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{714BA9DC-2FD8-41D8-A256-DD26DE079321}"/>
+    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{4E6BEA0C-10A2-45B5-98AD-7699EDF4B8E5}"/>
+    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{E2B4417F-8380-45B7-A327-ED7E648E63C1}"/>
+    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{C642B823-4987-47EE-B2E9-B824EE3240EA}"/>
+    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{1AB61509-5E51-4ED9-91BC-5B4688AA2208}"/>
+    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{4EB3C5CF-26E1-49B8-90FD-193C0604EACC}"/>
+    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{480F8578-486A-400C-9B35-0A1399AC8010}"/>
+    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{39CFDC98-1409-433F-AD98-804F792D85B5}"/>
+    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{E1589BC1-ED76-435E-B1BB-21C44D0F8917}"/>
+    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{6B83A216-1832-47D6-A877-A4A940F742E2}"/>
+    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{D06DBCA3-6A5E-4F0B-A630-C27D4A157240}"/>
+    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{0AD80330-DB7A-4C55-A53B-E9CC8C53A46A}"/>
+    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{E38B68C4-4BB3-4796-B054-D539DC715ED5}"/>
+    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{FA71A184-3A69-4DAE-9848-5D5277C66052}"/>
+    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{D8E07BDB-8509-40C1-A768-3696B347E1A2}"/>
+    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{9975C54B-1978-4FEE-A240-480F22732376}"/>
+    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{CE32B67F-A4F6-4A79-A698-CA724FEF6BC7}"/>
+    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{C1065885-3775-4924-B32E-71540E14E4F0}"/>
+    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{B73AB7D3-6E05-4165-90C3-2A208782189C}"/>
+    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{FC48011B-872F-4E1B-AA1D-83310C6E6E13}"/>
+    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{F83DB681-D261-425B-84BF-86B81FA21B7B}"/>
+    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{B0BC0C1D-CEA1-49E8-87F2-6FE228366F4C}"/>
+    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{EA078A04-14A1-4A9E-BB59-B50699F4A5EE}"/>
+    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{0A9DCBE3-16B8-435A-8F1E-8DDF67D16E38}"/>
+    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{2C9EA3AE-337A-42CA-B702-2806FE8A3324}"/>
+    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{9C923AA1-BCF6-49A6-8807-BE67CBA79862}"/>
+    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{4B13D682-B098-4F4B-BFC5-596A6BBB1EA1}"/>
+    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{E2DFD4B1-275C-4176-A5BA-08A86A344C2D}"/>
+    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{1C5AE7CC-3D8D-4000-BF8E-4658FC1BF6C0}"/>
+    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{90AB284E-B0E1-4B32-B22A-2BFEEC28E80E}"/>
+    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{3E480A5F-ED65-42AB-93C3-B985365C7A14}"/>
+    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{B85FC8A7-31DC-43F7-8ADA-9F117C3647A5}"/>
+    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{2DA83086-8D29-4606-8E40-DA006C854032}"/>
+    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{D6BBBC5F-2481-4659-8AC7-342F38EF875A}"/>
+    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{0EF044F4-90D3-417C-BD96-5BC6768121B2}"/>
+    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{DED02D02-5BE2-4AB8-9FAB-A42FC7C76841}"/>
+    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{07D87658-D4F3-4C73-B840-9F99952F710B}"/>
+    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{4EA01B06-B305-4BB5-9C10-941D5560CBE4}"/>
+    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{057500BC-A8E0-4E32-A362-E7C67AA25980}"/>
+    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{89B71737-4C85-4F93-9F9C-93C1E03030F9}"/>
+    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{4EE26A8A-6854-42F5-A1AB-58FEBE9A6FA6}"/>
+    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{0BFE2223-65E5-446C-B53C-CD7C930F721D}"/>
+    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{85FBD4A4-A05B-4075-8ACB-55A292B4E370}"/>
+    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{57D0FDC9-0BF2-412F-AB0E-2554FBBE779E}"/>
+    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{0CE1557F-F2C0-422D-A94D-020F246D791D}"/>
+    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{7E295E41-BCFD-446C-8C0F-D88295FF6FE3}"/>
+    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{AF8219B3-BC18-46A1-85D8-D43593454770}"/>
+    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{B206BD3F-DB55-4179-92F3-F0F5F89A384E}"/>
+    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{F69A0EBB-38F3-4AB1-898C-6D0968E145D2}"/>
+    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{D81E92AD-DAF3-4D08-BCC9-BB4958CC101D}"/>
+    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{F3043AED-3EA4-4D12-B753-95F9B7455703}"/>
+    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{955B7A09-701B-4942-AF59-84875971A0F5}"/>
+    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{FE927F87-8811-4392-957A-D2F557D8425D}"/>
+    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{688F7334-922F-4E37-916D-A3B16014205A}"/>
+    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{8C76F9E8-1D18-47A6-A965-A1C0568F0409}"/>
+    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{E091E0D2-9E29-48E6-8C50-F2CFD8841AB5}"/>
+    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{6BC0259A-3DD7-4BC1-B020-1609EDD8EF87}"/>
+    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{B047E7CC-982E-4F96-B627-D761659B9384}"/>
+    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{BDC0FB9B-CACA-4059-8C89-E4ACD2141A0A}"/>
+    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{6B814CBA-CA65-4E81-8D19-971C7DD7EEBA}"/>
+    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{291CB43B-8877-468A-A91E-B91D2BAF3DC2}"/>
+    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{98ADC4EE-D5C0-40F8-B6D2-29ABA1507189}"/>
+    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{E5CBAF55-BADE-44AE-85DF-595A9ACDE186}"/>
+    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{6E0962C1-4B48-45E5-B0D7-F83CBC838715}"/>
+    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{97A4CFBE-D49C-4400-95D9-468F7EAF9731}"/>
+    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{1672AB97-B7E1-44C8-BB1A-B6B1A95A41CA}"/>
+    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{2EAEA243-CFA8-477E-9578-4699073E1871}"/>
+    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{66EF3882-8BA8-4E54-A2E4-3D440ECBC175}"/>
+    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{E590453C-F482-4F8D-BA78-DA264A698FAD}"/>
+    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{21F48C64-6B21-4CB0-8C7B-1752485E9FB0}"/>
+    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{223AE4CA-A202-4F59-A06D-1F9EC4400F66}"/>
+    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{26FFE85C-8D57-4F55-97CB-B1AE18A3740F}"/>
+    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{D4282466-5011-460B-BB9E-DF0A299A33FD}"/>
+    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{5953EBF0-18FC-4938-B785-A0CDA2424628}"/>
+    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{B2E867C1-A0D0-498B-8672-F3A271D0CDAD}"/>
+    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{72E30063-BD30-4F2B-97F2-294BEBB4A9D1}"/>
+    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{F7173FEA-D649-4B9C-95B1-2A31F41C55B1}"/>
+    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{9B1B5C15-4518-4747-BC4B-5F5A4AC60E41}"/>
+    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{296C744C-6E91-448E-A03C-5F05C497A019}"/>
+    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{6656630D-159C-43A4-8A30-0E5352811642}"/>
+    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{C2C767B5-6A91-4180-A72B-1625FCAD0CA0}"/>
+    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{119A5BD4-21B4-4C53-BF74-BDBEA9AEC1AB}"/>
+    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{EFA57F33-D4FE-4634-AA63-FE185162FCA8}"/>
+    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{75171705-F5B6-4B0B-8583-6173235D4D25}"/>
+    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{FC92D2F3-7F2C-4812-A56E-3CD891FE6AAB}"/>
+    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{F1B00700-7709-467D-8FD7-354B24141F72}"/>
+    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{97418F87-019F-489D-A6AB-FCACC0E58D54}"/>
+    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{4D384525-2DFB-4234-B942-B37C5E6319E7}"/>
+    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{A0011565-3F71-40F4-A1D1-424B451458F5}"/>
+    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{0317A3FF-09CB-4BC3-A31F-A651D497C2CB}"/>
+    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{8AC48587-E3F9-44BA-9EA5-43EF91C96CB7}"/>
+    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{7433C4AA-E65E-4AE0-9E05-B1DAB1FA3D68}"/>
+    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{35BB7AC4-9FA7-4900-B7A2-39A298844DBE}"/>
+    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{BFC21C75-961B-408B-9259-1449C829A313}"/>
+    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{52B9D160-D230-48DE-8999-0B1BD765DFC2}"/>
+    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{E4B64F11-0330-4D8B-BDCB-239E0A7472DB}"/>
+    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{3B9A4EEF-BBBD-47A1-97FF-D8F0389944E7}"/>
+    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{7110405C-510F-41B3-9990-F9CF69ED8218}"/>
+    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{70BB09E1-6671-4761-869D-528812A65B90}"/>
+    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{79620E42-2BB8-4AAE-9555-E28B277242E7}"/>
+    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{AAA6136D-31A0-49C1-AEE6-0BA47EA9874B}"/>
+    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{0F08FECE-0BB4-4648-8131-04E041494607}"/>
+    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{E9BFE642-E622-4A46-8831-C3FC9EBCF377}"/>
+    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{18FC112C-B063-4DF5-8E46-B1FCFBF58C11}"/>
+    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{CA62425F-8D73-467F-A69A-5DF36A059714}"/>
+    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{A92FD45E-35F0-426A-A916-FF6BA3EBAF58}"/>
+    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{AF59E558-ADC2-432A-92AA-FED84FB91834}"/>
+    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{9ABC1356-8CA7-4A56-A06C-04DA3EE19AC7}"/>
+    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{7C38BA93-2C9B-424F-B79D-51E736AC38B2}"/>
+    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{99E05172-D8BE-48F9-A276-767714008C97}"/>
+    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{EA96A598-FDA7-4210-9E67-1E2651093A55}"/>
+    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{8DB66287-38B3-4A12-BA5C-BD3215B4A1C2}"/>
+    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{62C3F883-1821-4F6E-937D-A2E546C8FFC7}"/>
+    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{0319B7F6-6A7B-4C3F-A699-AFF03984E82B}"/>
+    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{1F45F644-8389-4764-A7AE-6A8CC77F64BC}"/>
+    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{245C787C-49EA-47CE-AD73-A61832672F22}"/>
+    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{B7B7FBF9-96DA-4800-A5C3-43AD4C39B2B6}"/>
+    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{1E7D980A-10B6-4BFC-AAB0-8B4BB7F482FB}"/>
+    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{74A84635-214E-46DC-83C0-02CF359D0E43}"/>
+    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{FDAE85B8-800C-4454-A52A-053F75FA4179}"/>
+    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{C13EC8AD-9AA6-4994-AA7A-25064526D95B}"/>
+    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{F0BD1C14-3D2A-4F0E-A393-0FF58D0D1C10}"/>
+    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{85F0D3F7-E55E-4610-9E84-3FEA15F10DCE}"/>
+    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{CAB49B15-DE05-4886-BFB6-7E02FB3F032E}"/>
+    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{D4404E7D-6692-4320-A3E0-C0C3519FB335}"/>
+    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{D30F78AC-4132-4AE8-9E1C-F3BAEAEAE000}"/>
+    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{52B2EDEA-D35A-404F-B6C2-F3E86D15C3DC}"/>
+    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{0489156A-69B6-4BA9-BFFA-43201F63318C}"/>
+    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{FCCA01AB-D516-43BD-B24B-A395D4C09DFF}"/>
+    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{5B7A5521-61FD-4B5E-B079-C7ECAB5A24F8}"/>
+    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{0B36707C-E6C7-437A-A7D5-F967818FA030}"/>
+    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{0ADBFAF9-3743-4BC6-A7EF-DAF9E3C0E7BE}"/>
+    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{7AB71FC9-1375-492E-B1DA-7DDEDEDFD298}"/>
+    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{9C18E681-F905-4E7A-BACA-0B4F99908B0A}"/>
+    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{48F795CA-C0A8-46A6-B899-20CA2647AD8F}"/>
+    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{352E3A15-F3C4-4882-B031-FB1B401E5986}"/>
+    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{806869A3-D167-41A8-A392-3B24B128EF2B}"/>
+    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{84A2273B-A6E5-4B0D-B72B-D81D2E7979D1}"/>
+    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{F57E48A7-D873-4A77-B869-0BFD9033DF5F}"/>
+    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{3BEBAC2D-D02A-4A0D-A97C-AC748113D290}"/>
+    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{70122600-3A0F-48F5-873F-D7B3416BE735}"/>
+    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{EA9988A5-9E91-4D42-B4DC-23011D2FE641}"/>
+    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{BDF7A08D-1E0E-41D0-A6B3-F160C8DFA997}"/>
+    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{EDA7746A-9E39-45AC-AF79-D726E27C7881}"/>
+    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{33F1C9F7-FA6C-4F8B-B0DF-DD81B1F022B3}"/>
+    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{E2FCEE6A-E3D4-4D5E-9AAE-62DC371F6071}"/>
+    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{92AA383B-C6FD-443D-ADAF-3DFF9CFA1EF3}"/>
+    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{7A4522C1-B488-4799-9DF4-67991AD23A62}"/>
+    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{CEEB2429-1793-4EDA-801A-E5686A3A3C55}"/>
+    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{7AD41E70-7A51-42B6-9380-2E2BF365191B}"/>
+    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{9E741FB4-93D7-4B9C-A138-30DE232C4574}"/>
+    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{E23849CA-E205-4D20-86E9-3FA84C0E0FAA}"/>
+    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{D41DFA2D-B710-429F-95DD-4BF5E0702F22}"/>
+    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{EA450FEE-C442-4986-B609-61786CF987EC}"/>
+    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{E972AEB2-AEDE-4523-8061-817170880667}"/>
+    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{277B90A3-6E21-444F-A1BE-EDB50E3FEC1A}"/>
+    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{685B5B1A-EB97-490D-9B31-C0CFA3855CAA}"/>
+    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{B9837D0A-F816-4094-BA91-F8C223053BA2}"/>
+    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{535343F5-72CD-4F16-BDB0-6B9C549EDD63}"/>
+    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{85EDAEFB-5FDB-476C-8933-1931B4554496}"/>
+    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{0BC136E3-317A-4586-8137-AF3A52D2EB70}"/>
+    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{FCF0DF09-957C-4A96-89FE-24BDADDF3E1F}"/>
+    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{ACD44E04-6A6B-459F-BB80-A771867C4916}"/>
+    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{23F728A8-A5A9-40E3-93F8-E805B49A12C9}"/>
+    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{A28F56D2-C3ED-495D-8B68-0F744CD45A45}"/>
+    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{31196837-6659-4098-A8E1-85627D286142}"/>
+    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{3DA8EB30-3C6A-4954-9CF4-67FFF8D38035}"/>
+    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{943DF90B-6B2F-46F2-BE54-7FAF6C18A4B1}"/>
+    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{4FC19FB4-320D-4F3F-A811-453B9899D720}"/>
+    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{DDC841EE-C0FA-4980-9A8E-25306622331D}"/>
+    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{BFC792CF-E7E5-48D0-99E2-343E22FAB80C}"/>
+    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{F6B74E18-0764-4F7D-819C-1DC94337A5DC}"/>
+    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{EAECB7D8-3424-4BEC-9377-9EAA8F33AD4F}"/>
+    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{43A31073-D220-48A0-8189-79160B8EE051}"/>
+    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{C46D35E2-6B47-40DA-9779-6798621BEE3B}"/>
+    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{F3EBD67A-37BD-44C9-B840-49D5C46011E9}"/>
+    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{39D4A7C0-6F93-4316-A1BB-B3996719743F}"/>
+    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{BBE15010-5DCB-43B8-A7D3-E5BB8549C331}"/>
+    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{4C62BD72-D45C-4B14-BABF-C9339C81C066}"/>
+    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{D1E9ED8F-F83F-4FE2-B3F8-297EA58313CA}"/>
+    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{0779C52F-DBD2-4857-AB2E-FCB6DA6CA9E8}"/>
+    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{E2DFF156-8890-49E4-A8B0-21394C3EC6FC}"/>
+    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{22CBAF9F-D601-4489-9B04-11EDE7858A26}"/>
+    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{A88A001B-1B46-44AC-B02D-8BC2DD5634CE}"/>
+    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{551114BB-24C1-4FD6-A79E-AD20BB33CE15}"/>
+    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{88EFAD6F-FC4A-4A47-B8FD-07ECA8DB9778}"/>
+    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{0399FBB3-13AD-4486-8623-7AECAC6CCA70}"/>
+    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{5B5ECE7F-5738-42E8-8455-180524B17AB2}"/>
+    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{94ABB820-37BB-4333-9885-B6D6ED8328B6}"/>
+    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{42E929AA-4861-4F76-AFB7-B072239423B0}"/>
+    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{187DFB87-D784-4E89-8369-75A688659BE2}"/>
+    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{65191927-BDB0-4A2C-8680-04D0889B0BB8}"/>
+    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{823EB12A-5F4F-4B98-BF5B-5D883D0E7935}"/>
+    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{97F0AEF4-1885-48BF-9201-DE33E5247F76}"/>
+    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{A6273080-8C65-4DCB-9139-3F2F87FFF8F8}"/>
+    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{6B94AFE7-C111-4E5A-8EB8-BF223E81583D}"/>
+    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{C33BB8F6-966D-4D27-9C11-BAD9EF8E4874}"/>
+    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{230ADC0F-FA20-481E-8CCF-0B0E2927FE94}"/>
+    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{A12B8585-01BB-4623-993C-5FB15448E4A5}"/>
+    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{9501D82D-73CC-4468-B63F-9D68B5F48FA8}"/>
+    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{A33DC336-C01A-4009-BCE2-4C68F059B501}"/>
+    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{FA3BFFC0-3E8A-4461-99C3-424203C89743}"/>
+    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{87C428C6-FC49-4BF2-AB46-F8DBEB4118E2}"/>
+    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{F7A6BEF2-DEAF-41C7-9125-A8D91933267D}"/>
+    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{ACCB82A8-CDDB-4FF0-B24C-39B91E1D339F}"/>
+    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{33EE5E6D-001B-47FA-8321-FB548F5DE22E}"/>
+    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{673E33D2-17AA-45C3-8C53-7FEF125C82B9}"/>
+    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{574861DD-75A0-4699-84B0-08DEEF484A6D}"/>
+    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{FDAB81F1-7AE2-4F55-8B08-B39677E224F8}"/>
+    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{25C87BB1-7ADA-4666-8117-AE43224F42C0}"/>
+    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{D5FC2253-958C-4A0B-BF32-F591BE87A023}"/>
+    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{8A4BD246-D2CE-4083-B8A1-F3BBD9504EC1}"/>
+    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{581B044D-1F94-48A4-8C46-E8FFEE7D115F}"/>
+    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{E3089137-313D-4295-958C-8040BEBB1F7C}"/>
+    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{2170C333-4869-443D-A13F-1E1E923C8B47}"/>
+    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{1B103262-0E5A-4DE0-B286-F84958B9CABA}"/>
+    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{3C69B0EB-F531-43E4-A6FB-31965A8CC703}"/>
+    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{7EE36BCA-3E01-4C7A-9F01-BECB2CCDF45D}"/>
+    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{2EFDD92A-2AA1-4B89-A835-D0CB0C055218}"/>
+    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{2D1790D0-09DD-4677-865A-F203877B1090}"/>
+    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{C1785384-28CB-4005-93DF-EEBB20E6165E}"/>
+    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{E40690FE-79FA-4DE7-A875-EC688D655CE1}"/>
+    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{107A6236-6A6D-4A0C-8A5C-9AF95DD03EA7}"/>
+    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{381B2790-478B-4D7C-BFE3-E30FEF6EE46C}"/>
+    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{1C81D2D9-DBDE-460D-B22F-FF312779AE5B}"/>
+    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{B53552F9-A082-4D91-A9D9-468097E73DB8}"/>
+    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{4948C465-0376-4E41-875F-96176C67C898}"/>
+    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{004CC30E-5887-4566-BE3C-77E7A633961C}"/>
+    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{80573F9D-CFF0-41A3-8306-C7D050A8DFA4}"/>
+    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{0B4F2CDF-8587-4602-92C3-05AEA11AEEB3}"/>
+    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{5BE905C9-BB06-41E5-B957-6431F65FD323}"/>
+    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{EA3FA0D0-3DCB-4FD9-A5FD-0B7A85E5001E}"/>
+    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{8B150839-BC30-411E-818F-542768D04030}"/>
+    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{7E2DF5CD-4D94-4D79-9A95-AEF29E0F800B}"/>
+    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{DD723BE3-E9DD-487D-B5D0-23ECFEACC398}"/>
+    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{ADC6ED00-E4F9-41FB-83BA-5D56F7489A20}"/>
+    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{30F66D74-2F27-4317-A4DD-272E810FF763}"/>
+    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{7F04130A-5855-4D81-8270-C1FA5959F96E}"/>
+    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{172FC913-E4B2-477B-A759-82EE395A157E}"/>
+    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{2214DBE3-A556-4746-A80A-183AAD397CA0}"/>
+    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{442E1F4F-34AE-4EB7-BF37-E894552345E3}"/>
+    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{096DFEF5-9FF3-434A-AE47-FC2B5D7F5DF2}"/>
+    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{23EEE56C-C63D-41BB-89EE-D4EB9B9FC626}"/>
+    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{5D029458-C6EC-4E34-A464-1241D1FF44BD}"/>
+    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{0FDBBEC4-809A-468F-AEC6-CABE731017FA}"/>
+    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{91AEF8DB-6C70-4572-B0D2-567722EE47F7}"/>
+    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{D47A2B42-CCB1-4BB2-8FF6-F26803C132BE}"/>
+    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{075525A0-3B3C-4E3E-993E-1B8A515C76E8}"/>
+    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{5538B0D5-A85D-4406-8754-6C4A6831D2D2}"/>
+    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{D32C31CB-FB5C-4808-A340-BB1AEB6BD061}"/>
+    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{F4DFE4BA-3BA7-4057-9CE1-C93A92841C3B}"/>
+    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{EF0ECF1B-076D-452C-82B4-FAAC2345BB41}"/>
+    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{5C343CB7-8EB6-4A53-BFCE-0B350DD2E538}"/>
+    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{9F1BAADA-1177-42CF-B4F2-60F4BBAB4748}"/>
+    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{54FEA7DD-DA10-4248-859B-995A8928FB62}"/>
+    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{06011912-CC4F-42AB-9CF7-5F89D209675E}"/>
+    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{8A6C7319-3130-47B2-8E47-7EDD1FD1619E}"/>
+    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{7C1719A2-F5B5-4132-9AFF-C16DD8770415}"/>
+    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{58508B58-F472-4D43-87B3-21B99228BA98}"/>
+    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{F5E43C5F-88C9-4570-95CB-CBFCD00CDABE}"/>
+    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{F85E97A2-6B2A-417B-B0E5-2C38192C238C}"/>
+    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{D1BA79EA-D3A3-42B9-A888-4DB562A29A5E}"/>
+    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{87A76DBF-AF06-4F19-8452-91A1980C4AB9}"/>
+    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{4BBC5F9D-4EAB-45AC-8DB5-6D6634A8DCEC}"/>
+    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{75DF7A42-1126-46DF-8277-DE0B663F9C04}"/>
+    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{8C952D5F-C1CC-445F-99BA-79C8D63E9B59}"/>
+    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{B748FFC2-21C1-4CB6-8FC6-9F84542F6806}"/>
+    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{52A6C161-022B-416A-90E3-95BDF04846FF}"/>
+    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{A8B6AFF7-D08D-405C-BD68-C53802A4D3F6}"/>
+    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{AD927349-D35D-4BE8-B4E0-0BE6CFCAF2A5}"/>
+    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{38108639-FDCE-42C6-A65A-D5F31BB9AC19}"/>
+    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{5F633499-49B1-4D56-B95F-2BCEA44C857F}"/>
+    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{2BF85C1C-CE8D-4D09-BB23-B741F02A1478}"/>
+    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{CA66F850-9948-40D6-8436-309AB05F7D7C}"/>
+    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{211FCA0B-3B73-471A-AAA4-9E7251A21470}"/>
+    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{95014C38-31E8-424E-B8DE-7BD6E2326E19}"/>
+    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{2543FE5B-00BF-4A74-8249-41C9A2311325}"/>
+    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{312CB4E1-8C4A-448D-8A04-0CC9C5D0039A}"/>
+    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{931DFE9B-E7E6-416C-A42E-C77059FFF6C6}"/>
+    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{C6DB6FE3-7C75-4596-B1DE-8F95B29A4B37}"/>
+    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{BFC5B372-62A4-44E7-A7A5-89E03CA4AE49}"/>
+    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{ED2B8CB5-02D5-4EC4-B29C-03C94E2714A3}"/>
+    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{911BCF39-908B-4932-BDF6-5A33146B4788}"/>
+    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{9DCB96E3-B9EA-411B-AECE-456E9EB2154B}"/>
+    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{B0F93B41-3D8A-4F88-8805-9042E91A2F2A}"/>
+    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{BEC8811A-9C5C-44EF-8B64-1FFB99E0226D}"/>
+    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{88C28F6F-2B89-4245-AAA3-F627BEA2E851}"/>
+    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{5204C48C-86AD-4479-BEA2-283088FD8AD8}"/>
+    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{33B052B1-532B-41F4-9717-15AFB88BB5EB}"/>
+    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{FBC40021-AFEC-4DB3-ACAD-DB72C5DCF847}"/>
+    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{30770019-123D-43B6-A030-9941137D9927}"/>
+    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{F62CB21B-2334-4ACA-A6A2-5935FACF2ED5}"/>
+    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{C85A3A7D-1BC3-4025-A728-6F057905B04A}"/>
+    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{91AA869C-D777-4449-881C-5B0ABD8B0A2A}"/>
+    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{F70444C5-5155-4D1B-88EA-74C8CE49D216}"/>
+    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{ECAE748F-2F4A-446E-BB79-0A407FDD191C}"/>
+    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{7CE28ACE-9B7C-4D12-AE32-C7930F30A5C4}"/>
+    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{B8C7C9C1-F03B-4962-996A-122B644F062B}"/>
+    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{12FEDC41-DD15-4FD7-A19D-ACB967BB8F85}"/>
+    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{AE4ECB53-96D4-44EF-8A9C-690B488F501E}"/>
+    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{DCD5FD87-0055-40A7-AA64-DEE944633160}"/>
+    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{9C91BDF9-056E-480A-AEB1-21382CEFB431}"/>
+    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{EF591625-0283-4F3F-B790-C1814B9FEB5C}"/>
+    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{4F909526-A268-4617-A609-F337332EC7D8}"/>
+    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{DE3F0F9D-FFB0-4748-A02D-C0F0637E5A88}"/>
+    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{FE491598-F0C3-41DF-9908-4A6A4F4DCF3A}"/>
+    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{194DF245-ED1A-4377-8949-D9E8FE2CAD92}"/>
+    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{F813F25F-1537-40E4-83B9-6AF1BD51B4EA}"/>
+    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{E97BF132-13E1-463B-8DEE-3E711494CEE2}"/>
+    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{4923A6AC-D035-4B61-9686-CB94C04C9F2C}"/>
+    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{583170B2-7905-4B79-93FD-621D7F96CEB3}"/>
+    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{9731B73A-5F53-4FEE-AC3B-A4756196DE2B}"/>
+    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{563F69F6-1A34-4187-891F-C4DDC09237C7}"/>
+    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{D01CF549-68D7-4801-B63B-6B6A57587865}"/>
+    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{FF97D89E-4275-41D2-8ACB-025B736527A7}"/>
+    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{601AAEED-B404-42C1-9A51-3785117B121D}"/>
+    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{2FC3AA56-1D22-4BF8-8ED5-4EB317DA15E9}"/>
+    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{D10A210B-61C6-4841-9CB3-F74200AAC7C3}"/>
+    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{CC7F03E1-163B-4BAE-86A7-8C78C2B91700}"/>
+    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{EA633B60-C7A0-4302-A639-9662196BEE9A}"/>
+    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{56185330-4761-41CD-A93D-D0BFA7E51FA2}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>
@@ -67205,7 +67139,6 @@
   <headerFooter>
     <oddFooter>&amp;R&amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId578"/>
-  <legacyDrawing r:id="rId579"/>
+  <legacyDrawing r:id="rId578"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fluxo - Tratamento dos .xls - Relatório de Garantias - Relatório de Project Room
</commit_message>
<xml_diff>
--- a/src/data/uploads/Project Room (Jira).xlsx
+++ b/src/data/uploads/Project Room (Jira).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/paulo_vieira_d_silva_accenture_com/Documents/Desktop/Automação_v3/src/data/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C8A17F8-3516-49AA-AD7C-725DA47B78CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35D7498F-00B4-4AFF-A755-8A9E1A83145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3BFA2687-D76A-45EE-91A0-139B4961BFD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D86CF08D-308C-4181-A076-5BE61EE2D276}"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -10620,7 +10620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C4E895-4723-4AB2-884A-B6DEB348F755}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DD4AC3-1407-4A9D-B827-6B3E926823BD}">
   <dimension ref="A1:AR578"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -66555,583 +66555,583 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{5C84C89C-EC66-4BE9-8433-6FEE878CC6AA}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{7B06E4BD-B247-4999-A3E0-AAD4D5B0475B}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{CE815206-5C5D-4BB8-9B07-3DA04828BE01}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{AC328FFC-09E7-4FF7-A26B-74D4C9CAB15F}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{B18368CC-8497-4BB5-AEAD-D2598F91E2CB}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{0D713C12-61D6-478A-93C8-134A13BD6484}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{280E36FF-9DA8-49C3-9732-2895BF18C202}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{CA4C7E49-798E-48A0-BE91-89AC9043E5E6}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{6263329D-55CE-474F-ADEF-08D16B9DE210}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{3EE66B21-EEDE-45FF-A407-1AE4BF3791DC}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{3BCDA23C-563F-4C76-8E9A-C83DDF361713}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{33459195-98E3-4DB8-853F-03798A690216}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{521A79C8-F71D-46EF-99C2-093A50D4CE72}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{E7ADDAC1-DB8D-4D5B-8E44-460A2B2E794A}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{80B7B620-E6A4-48B5-8F2A-7242C5A3CA52}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{9E503973-36C3-4C4F-8931-AEA4399D4E11}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{CB8C7DBE-D747-4C29-A2B7-FCF78D5102B2}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{914256F0-5514-44B7-A0A7-94E24C1F88B6}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{594BF5E6-5323-41D6-AA27-D08647C6C347}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{9B3EB5B0-26E4-4909-9622-7AB21D6BF9F5}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{D4E325AC-8129-42AF-A17F-DAEFC40467BF}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{E2BE28F1-79B9-48EF-990E-51F862666079}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{5D5E0C47-61C7-46A4-B70E-FDABCDC53B1F}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{5F8F6963-5AE5-4866-8908-00E8DD1EAC59}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{D3B10734-7AF5-4641-8559-63FE7C2848DD}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{66BE6C87-57A0-4385-8906-AECF54021AAA}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{E34C81A2-A89D-484A-BC93-03574752F126}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{201917BB-A36C-4DA4-908A-8D962EDFB6CC}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{1E9642C7-09B4-4159-9811-CA085ECAFFE5}"/>
-    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{9C25F095-8A7B-4299-8571-08D9ED461B72}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{85EEEAAC-F0E2-4569-A941-4C7484EFB069}"/>
-    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{ED9CF52F-E820-4E8C-8124-5A065B01CE2C}"/>
-    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{001F4AF1-B2F2-4375-8F76-08C1BBFAADE0}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{E0FE9AC2-E123-4EA9-834B-4A97A9AE1C62}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{4EE12511-02CC-42FB-B5E1-3F01A8B7A843}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{4F3308D6-8E5C-482E-81EB-BD33C6265068}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{254E9B17-A0A7-4FC1-BB7E-91A3D30DB295}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{2F5C8044-4F54-4E67-BF60-4F2A518D6281}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{3F24C275-5A06-45A0-A0E9-702A3A8690BF}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{5FE9EE38-EFA2-4C20-9F3C-E78F796C49CE}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{B5CAAF8C-8B40-4F98-953D-55963B525F60}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{C77D7477-309F-4831-BA74-2968066DBC3B}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{21E49855-9F8C-4C4D-AE49-B213633E4B4F}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{3A5F7DF9-872B-49EE-A1AB-6346652F8357}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{D4A1EBE0-A83E-4874-8585-D1A43D9C27BD}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{89816DFC-57A8-421A-BF2B-489A260A2A60}"/>
-    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{F99FC190-63AE-4D75-98B7-921D605B87FE}"/>
-    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{CB795A44-69FB-49DD-A849-B0A3AD0A7633}"/>
-    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{2F459AAB-1C38-46CF-A5C9-1490FDFEBC7D}"/>
-    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{04146260-3849-4E51-8A86-D3B4932DF372}"/>
-    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{BF1533EF-D0A6-47AE-8FF4-CA9539802964}"/>
-    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{EFCE3167-8296-4032-B68E-DDF6BCD4219B}"/>
-    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{7B7FE882-99AF-4FD4-858B-6F0BDB59A2BB}"/>
-    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{21FCE30D-3646-4192-9222-983CB0E212BE}"/>
-    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{35B2F997-737D-418D-A451-7351E79EDD21}"/>
-    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{711F4C3D-DBAD-4D4A-88C5-75F267E008CA}"/>
-    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{EADD91AE-E1FE-4E4C-857D-B6B9AE3C285B}"/>
-    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{82392A22-0457-4965-BCBF-7CA059A92B16}"/>
-    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{FE90417E-4F63-4DE9-9054-32896CF5B88D}"/>
-    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{37D77441-48D9-4FAC-BB99-EA2559DFBBDF}"/>
-    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{40066A73-FC92-44CA-A367-1B2012556A08}"/>
-    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{FA2514EC-89A0-4F40-A2A5-AC64D16D391B}"/>
-    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{E729D86C-98D3-453A-BFB1-65A73F8E8877}"/>
-    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{026BE6C8-01CC-45B8-A699-174E0EE8D54E}"/>
-    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{175A977F-3240-4570-8513-D8C2D0AF0429}"/>
-    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{780CB63D-B702-46DE-ABA9-FBF581BE4622}"/>
-    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{9CCD9DD5-8009-49E7-B920-0DA11FD32AE7}"/>
-    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{B5FDA060-4373-4619-9E99-4ADC74D26460}"/>
-    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{53B2BE56-2873-405D-BEB1-7661B8CF8E6F}"/>
-    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{B2CC6130-EC71-4848-88EE-F92DD6BE1DFC}"/>
-    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{72894EA9-DFCE-46A0-B3B3-BAD9E5F62BDC}"/>
-    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{89339090-EA66-4FBC-8423-D514528BE12F}"/>
-    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{C2CEB6C2-0F0B-4EB1-8988-447EBB5BD576}"/>
-    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{BA1B4F82-2EA7-4F8F-8099-95FB432D9C32}"/>
-    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{74C1DDED-A18E-4EE4-BC03-88EDC8E22F98}"/>
-    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{8CA1B7BD-5852-4F03-AA26-10145DADB5C1}"/>
-    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{357D2664-30E1-4596-8A3D-4204FBD2C722}"/>
-    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{C5887AEA-9A3F-4B52-A4D3-511F41C6FB78}"/>
-    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{F938ADF6-A6F1-402C-8E2A-EAD0AE1AF360}"/>
-    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{7281DE4D-359F-457E-B3CF-6534950B0F0A}"/>
-    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{629F586C-2448-4E2F-9D81-22C9871C4FB9}"/>
-    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{48A48B11-387B-4590-95F2-A936BEBED106}"/>
-    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{4D1C98C9-D138-41F0-969D-D0BCA827FE0F}"/>
-    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{1C3E3F79-4DA3-4945-B9CC-3137F624769F}"/>
-    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{12146C4B-8A9B-4A23-B1EE-A04CE9852FA6}"/>
-    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{C9B3CB89-7E1E-4A9E-B5F1-B0CCEF5262DB}"/>
-    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{C52E55E0-1651-4D43-A2B3-77F83CD4A066}"/>
-    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{0CB4A77F-6657-4875-954C-9FD427F1545B}"/>
-    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{E1133A33-752E-4685-90A1-78AC100A1A6A}"/>
-    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{FE45B744-86AB-4B87-86C1-5080362EF175}"/>
-    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{9BA99935-B8A8-49B3-97BC-221D7B740CE5}"/>
-    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{962EE0A5-7EE1-487D-AC5B-3C0B36B0E66A}"/>
-    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{3A9783CF-0872-4779-8B04-F145AF7DA61D}"/>
-    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{29DFCC34-9D02-4D27-AAE5-DD172751CFAB}"/>
-    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{AEF486CC-697E-452C-B8CD-C235D2062A23}"/>
-    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{CF50B4DC-7787-4369-8AA3-EEC5175891C8}"/>
-    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{49A17C12-CF02-4C2D-8591-DD12561F26AB}"/>
-    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{9EB0AAF7-F8A1-440B-A9EC-F7ACB43DC484}"/>
-    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{29E2EC0E-4C6C-4950-AFEA-C89DD459A5DA}"/>
-    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{70692CEF-78ED-4A2D-ACF5-A35A6B58655E}"/>
-    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{57C4FBB6-A92E-488A-92EB-59578036A88A}"/>
-    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{C4D8016B-A707-4F85-8987-AFAFB84EF298}"/>
-    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{293DB7B9-3DFF-433C-93A9-DA049B1CF77E}"/>
-    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{B7F3CB49-8D73-40DE-939B-C85E6FA3CE10}"/>
-    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{3CC20C99-2C93-4EC7-A657-2045ECB0DBCC}"/>
-    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{9FEA57C0-9399-4D4D-B7D2-EE479821B247}"/>
-    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{F277B3FE-6A81-44A9-BBBE-594C7E10BAF7}"/>
-    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{99C173A3-8147-4680-9B36-C4E804B560BE}"/>
-    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{275459FC-AEA7-4EB4-B0C8-DE677E893E47}"/>
-    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{125E7FBA-75FB-4EFE-8379-8B4D7C18B1FD}"/>
-    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{02762AB4-4B35-4E1F-8228-5A2B6907F0ED}"/>
-    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{21192263-6F93-4458-AB7C-2C41B24D1F51}"/>
-    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{FDD074FA-6CD5-4BB3-8462-2C6F9B604D6D}"/>
-    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{18015AB0-7875-4BF7-BC65-15998EF86ACB}"/>
-    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{900B0E52-8155-4838-893E-5BD6FBE5C860}"/>
-    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{1CAD854B-09AB-4EBD-81CB-6A75662E7E56}"/>
-    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{C9EB53B7-F8AE-490E-A03E-993A68A15D4C}"/>
-    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{7E55AE27-3E83-4CF9-8253-77F568087BE6}"/>
-    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{C9C8DA10-DC45-4211-A96E-80DDDDCB9439}"/>
-    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{11B210D0-855E-45EF-9FF5-D0BD6C3A48FC}"/>
-    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{490B6F03-4DC2-4865-AC88-3D12453768DD}"/>
-    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{DC6A6C14-8CA3-4BCC-96AC-8F1F6794515E}"/>
-    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{E3C9CDE2-7911-42E0-8BEE-B48546BAB575}"/>
-    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{08E189E4-1C01-41E0-80E1-697EEF8DC3F9}"/>
-    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{40C3D8FB-DA48-4B75-B9C2-E2B8B7477707}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{6CA89123-C8C6-4663-A5B1-9FEB9F6D73E4}"/>
-    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{2F11A377-4523-4A69-BF66-8186D31902A1}"/>
-    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{1F6BB93B-1816-4F17-9629-9FEC9DF1A167}"/>
-    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{CF1B9E94-6C93-4D38-B2B2-B4AC3AF22718}"/>
-    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{70AE736D-EBAD-4E85-8656-CBD5A5DEF8B5}"/>
-    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{C7073AAC-787F-49E9-8AF7-1A75FDDBC94E}"/>
-    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{3CA717DB-9F3E-4AF5-B09F-C63CD525EA9F}"/>
-    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{12AF662E-1763-49BE-B33E-3EDB2F75DB81}"/>
-    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{23041EA9-4BCD-4BE9-884A-F8A4EF6D4CE0}"/>
-    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{BE41C7CE-6D4C-4BE4-B0B9-4AA9186B2BEB}"/>
-    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{2858237B-CE56-4FCC-A9E7-32F04BCFB2D0}"/>
-    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{686717AC-31B1-482E-AEE6-8EFB199D4B54}"/>
-    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{F9D98A64-65FB-45E0-8DBD-FE301663AFD7}"/>
-    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{47B62886-8D42-4551-ABD3-BD57792E18B3}"/>
-    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{04DE8955-BDB5-434E-B070-E852BD2E5AEF}"/>
-    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{4C411850-E1BC-4C5B-A658-81AD8B065F17}"/>
-    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{0D69F557-0402-45E7-889B-FBCA0A57EC6C}"/>
-    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{4697794B-35E9-4EDE-8566-FD9944018FC9}"/>
-    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{12A343D9-DF9F-4407-BAB4-99930B2ECFBF}"/>
-    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{1AFFE813-1966-4E81-B97B-DA2DA9CF1D65}"/>
-    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{72EA8357-63C4-4773-91F3-865C8BB8BBCE}"/>
-    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{BC726F0B-D7BA-4DF4-9042-CB03212D47DD}"/>
-    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{44A98665-17B2-4545-BCB0-897F5EA182AB}"/>
-    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{81843F54-2F08-4DB6-8145-D822913C42C9}"/>
-    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{1EC04B7E-91B6-445E-8AE8-3A4CC6C28015}"/>
-    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{4CA94B10-41A0-4775-9A5E-7E2A6EF5582F}"/>
-    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{12585966-0F09-4045-9672-9906D51FA335}"/>
-    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{25BD4E51-0232-48FE-8AF1-3E0C71FF7EF0}"/>
-    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{D9D84557-B66C-446D-BDDE-BAB4F6A385B8}"/>
-    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{03E0EBFA-38F4-42AC-838F-E098A1811068}"/>
-    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{FE55EFBD-7099-4221-A7ED-06A049057E6C}"/>
-    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{B2144A6B-C20D-415A-A6CE-532FE7F0ED2C}"/>
-    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{C1FA2635-5C4B-4D5A-9D5C-F503FFBFF2D0}"/>
-    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{7469D590-F56E-462D-BBB5-9D732F988771}"/>
-    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{478BDA3A-5B17-4050-9035-A8D63D8C506D}"/>
-    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{FB5111A0-E838-4F46-A69F-282C6329392E}"/>
-    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{F54BD6DA-4729-4B23-B558-8DDB2A98E651}"/>
-    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{3758A706-F1A1-4A6D-98D3-41F7E0754372}"/>
-    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{94ADA259-F120-47E5-B48D-229A5D54D155}"/>
-    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{B5F05259-384E-432C-839D-BEBF4424D6A5}"/>
-    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{7D1060EF-4B34-4995-8115-94F28F2FEDF9}"/>
-    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{6618E98D-1727-4EFC-9E26-98C627C646D9}"/>
-    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{E51E89C0-DC85-4BA6-B06B-40C6A8057CFF}"/>
-    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{BBF70E11-604E-4168-BC01-750A3A8526E7}"/>
-    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{DDC6899F-2573-40BC-9E5F-F4CB3B0BD344}"/>
-    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{439C56DC-E64D-4514-B1FA-615A20718BF2}"/>
-    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{E7287DB5-E25F-4808-88C9-CA9EA885AADA}"/>
-    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{2C1F2860-952E-491A-BF01-C61E95F89B8B}"/>
-    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{7F1A7924-8454-45D7-B664-15F9E0BBC998}"/>
-    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{A26FDE9D-29B4-4BAB-A232-F307AD51879B}"/>
-    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{34CEB2C0-3A52-4A14-92EB-F2C6AD2C33F6}"/>
-    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{27700E61-3A15-48CD-898E-150A377882E5}"/>
-    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{2AE57E0E-92EA-4A31-B6A0-1DE5B9C941D2}"/>
-    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{944BA521-29A1-4063-974A-14B538F981DE}"/>
-    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{07AA365D-42D1-4C47-B7EF-F858DE815E5B}"/>
-    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{8F1881F5-1652-43E8-9042-A55439890964}"/>
-    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{4DF1A851-2B07-4B9B-A18F-10D4D50A5D73}"/>
-    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{C42B8024-5C2F-4517-A1F2-6138E4A3A266}"/>
-    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{BFF8AA93-AFCD-47B0-A841-5CB9B6AF7891}"/>
-    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{096E0E38-6976-4060-B67A-CA0E22EAFC26}"/>
-    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{60580C2E-5085-4470-9B45-4AF27E51C3B0}"/>
-    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{F05A7762-5160-4737-B880-1BE1A79B5961}"/>
-    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{27DBA3D9-29C2-495F-8163-F7D2BF3CFCA0}"/>
-    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{1CA86324-FD3C-40B2-9A61-F356802EFB2B}"/>
-    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{5C1B7B1B-B175-4DBE-807F-A4462854968D}"/>
-    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{DEC27BC4-5434-4AFE-93D3-A4402D8D7759}"/>
-    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{04924825-A94A-447D-96E4-031B5FF0504F}"/>
-    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{478F207C-20D3-4F4B-A08C-DAE3B6B529C4}"/>
-    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{2B2D9877-9557-4B12-9396-DF14CCC4DD58}"/>
-    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{19A2CBD3-2CA3-48F1-8F60-B6AC0EE60C11}"/>
-    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{9ADA1E1B-1978-4A8E-808C-2DB76A14B48D}"/>
-    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{A9A501C9-664E-47DF-850C-36A687E8D19B}"/>
-    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{A6D1B241-50F4-445A-A730-120FE415623B}"/>
-    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{A7562668-4717-46DC-8D23-FE31F8A8C302}"/>
-    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{32787952-AF3B-4FC8-B26D-27DF63D78438}"/>
-    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{28B74272-E223-4547-BE19-CBA0102D347B}"/>
-    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{FFD7A4C2-1132-4C29-BDF6-9B42402D348C}"/>
-    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{CF7AA2EF-8A09-48AA-B5A7-273601086615}"/>
-    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{82EDDB09-CC7E-4FA0-BC2D-FD29F47634E4}"/>
-    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{4DBDD9B3-4DC0-4C49-8995-C02E08A032BE}"/>
-    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{ECDCE062-CE7F-4CEE-A193-B7E937D035B9}"/>
-    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{CBC933BE-34E1-4506-B0B5-031BDAC53D1A}"/>
-    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{FF2F6AF9-EA17-4D6A-A284-3FF875AE567E}"/>
-    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{7606A263-ED32-4DA8-A33A-5CA14B44F733}"/>
-    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{A1255457-70A6-4A55-BB2A-C97E38F5D565}"/>
-    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{E3681523-AC26-4253-AD1D-A58D47DAF179}"/>
-    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{7D0C889F-46A3-4081-9CF7-572B71B58C45}"/>
-    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{A6F8E3E3-C7A8-4CFA-81E6-80C50750459A}"/>
-    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{12D67002-FED7-41EE-A476-C3FCCF95C5F2}"/>
-    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{D6705D1C-7463-42FF-B412-53BF5AAE2DD6}"/>
-    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{F011CC62-EEC7-4813-8EA9-1BF1E042F596}"/>
-    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{D9D3E851-2792-4861-AF35-AAFDB80FDB96}"/>
-    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{21D9C6AF-0424-4B6D-99C1-D4BB74368E7F}"/>
-    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{A7E5FA1C-F51D-4133-9311-BC4FAAF6C567}"/>
-    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{2A8A3E4D-B404-43FA-BC9F-F76F5BDB2B1F}"/>
-    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{A3987FD0-3DC2-4D31-B96E-FE4BB94691E5}"/>
-    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{A69B9C66-E89E-4E42-A06B-491FF0AC4515}"/>
-    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{8B811928-532D-4D48-82A2-A7B4AF2728E4}"/>
-    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{8A8DDA16-67CC-401E-853A-61D672502EA2}"/>
-    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{78A89724-4785-47E2-8655-F438C0EFF925}"/>
-    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{A5B4E085-1ADB-48D7-AB04-E4E9E13AF297}"/>
-    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{D4EC9CFC-A51E-465F-BD49-45297DC4964E}"/>
-    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{BA196D1A-A908-46FC-AF40-B3963E35FF5C}"/>
-    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{B7233543-5054-4B77-9EA8-F307F7C84438}"/>
-    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{CDF1F468-D221-46BA-83F5-CFB0DA4E0FD5}"/>
-    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{C1FFAD3A-1C56-43BD-B811-1EEB0B68D56F}"/>
-    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{8ABD8642-FDA1-492B-85D9-9C4119052163}"/>
-    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{2AEB00D6-82DB-48A4-87C4-FF794C7F4E03}"/>
-    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{B44611E8-6597-46CB-ADB7-752BE96EA5B5}"/>
-    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{3255FD6F-7825-4F6F-8153-2786118BBF4A}"/>
-    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{23CF815B-2449-4984-BD6F-A649F581F2FF}"/>
-    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{7CE553A2-4716-44EE-B116-690B3F21B758}"/>
-    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{E6C3AF01-060D-4869-9D42-72117C7E3159}"/>
-    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{1237DD09-F151-42DE-AFF7-E91355D867B6}"/>
-    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{3CA2E917-FDCC-4E02-94A4-540A95D6EB26}"/>
-    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{5EB998B2-B1BB-4D3C-AB53-C9BBE430ABBB}"/>
-    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{F86A8862-EB5C-4AF8-90C9-38C7E9398F07}"/>
-    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{A18FE846-877E-4817-9693-BC3A6FFD5B6D}"/>
-    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{D60E5709-7BE5-4E2A-9CA3-2C190AC7E0B6}"/>
-    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{0C42DD3D-9E47-440E-9D2D-C56C46E82C8A}"/>
-    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{8FFFB991-6DFA-40BA-8B8C-12A8C92A8254}"/>
-    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{9B9CFA47-5D1D-4848-B3D5-9950D40EA332}"/>
-    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{3ACE965A-9551-416F-8DB2-73AC013E064C}"/>
-    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{0BB9B3E5-B5CC-4601-997D-F3B4DCCEA712}"/>
-    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{BC202FEB-DF85-40AB-BBC8-6D44A60822DC}"/>
-    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{64E75BCF-1FDD-4F51-82CA-A98A35B54B78}"/>
-    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{5A35EB4B-5F8A-48FE-A451-0A5339E6F74C}"/>
-    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{0F820133-A41B-46C9-BCE5-9993146F0A33}"/>
-    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{7AD5A673-437B-443B-ADA6-C1A1EF68E181}"/>
-    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{4C09E369-123B-4574-B9A8-AF27BC31B793}"/>
-    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{06EC3B0E-E0D9-48F2-8023-1A2251FE5EF8}"/>
-    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{714BA9DC-2FD8-41D8-A256-DD26DE079321}"/>
-    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{4E6BEA0C-10A2-45B5-98AD-7699EDF4B8E5}"/>
-    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{E2B4417F-8380-45B7-A327-ED7E648E63C1}"/>
-    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{C642B823-4987-47EE-B2E9-B824EE3240EA}"/>
-    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{1AB61509-5E51-4ED9-91BC-5B4688AA2208}"/>
-    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{4EB3C5CF-26E1-49B8-90FD-193C0604EACC}"/>
-    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{480F8578-486A-400C-9B35-0A1399AC8010}"/>
-    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{39CFDC98-1409-433F-AD98-804F792D85B5}"/>
-    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{E1589BC1-ED76-435E-B1BB-21C44D0F8917}"/>
-    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{6B83A216-1832-47D6-A877-A4A940F742E2}"/>
-    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{D06DBCA3-6A5E-4F0B-A630-C27D4A157240}"/>
-    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{0AD80330-DB7A-4C55-A53B-E9CC8C53A46A}"/>
-    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{E38B68C4-4BB3-4796-B054-D539DC715ED5}"/>
-    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{FA71A184-3A69-4DAE-9848-5D5277C66052}"/>
-    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{D8E07BDB-8509-40C1-A768-3696B347E1A2}"/>
-    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{9975C54B-1978-4FEE-A240-480F22732376}"/>
-    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{CE32B67F-A4F6-4A79-A698-CA724FEF6BC7}"/>
-    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{C1065885-3775-4924-B32E-71540E14E4F0}"/>
-    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{B73AB7D3-6E05-4165-90C3-2A208782189C}"/>
-    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{FC48011B-872F-4E1B-AA1D-83310C6E6E13}"/>
-    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{F83DB681-D261-425B-84BF-86B81FA21B7B}"/>
-    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{B0BC0C1D-CEA1-49E8-87F2-6FE228366F4C}"/>
-    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{EA078A04-14A1-4A9E-BB59-B50699F4A5EE}"/>
-    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{0A9DCBE3-16B8-435A-8F1E-8DDF67D16E38}"/>
-    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{2C9EA3AE-337A-42CA-B702-2806FE8A3324}"/>
-    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{9C923AA1-BCF6-49A6-8807-BE67CBA79862}"/>
-    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{4B13D682-B098-4F4B-BFC5-596A6BBB1EA1}"/>
-    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{E2DFD4B1-275C-4176-A5BA-08A86A344C2D}"/>
-    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{1C5AE7CC-3D8D-4000-BF8E-4658FC1BF6C0}"/>
-    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{90AB284E-B0E1-4B32-B22A-2BFEEC28E80E}"/>
-    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{3E480A5F-ED65-42AB-93C3-B985365C7A14}"/>
-    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{B85FC8A7-31DC-43F7-8ADA-9F117C3647A5}"/>
-    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{2DA83086-8D29-4606-8E40-DA006C854032}"/>
-    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{D6BBBC5F-2481-4659-8AC7-342F38EF875A}"/>
-    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{0EF044F4-90D3-417C-BD96-5BC6768121B2}"/>
-    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{DED02D02-5BE2-4AB8-9FAB-A42FC7C76841}"/>
-    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{07D87658-D4F3-4C73-B840-9F99952F710B}"/>
-    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{4EA01B06-B305-4BB5-9C10-941D5560CBE4}"/>
-    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{057500BC-A8E0-4E32-A362-E7C67AA25980}"/>
-    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{89B71737-4C85-4F93-9F9C-93C1E03030F9}"/>
-    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{4EE26A8A-6854-42F5-A1AB-58FEBE9A6FA6}"/>
-    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{0BFE2223-65E5-446C-B53C-CD7C930F721D}"/>
-    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{85FBD4A4-A05B-4075-8ACB-55A292B4E370}"/>
-    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{57D0FDC9-0BF2-412F-AB0E-2554FBBE779E}"/>
-    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{0CE1557F-F2C0-422D-A94D-020F246D791D}"/>
-    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{7E295E41-BCFD-446C-8C0F-D88295FF6FE3}"/>
-    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{AF8219B3-BC18-46A1-85D8-D43593454770}"/>
-    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{B206BD3F-DB55-4179-92F3-F0F5F89A384E}"/>
-    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{F69A0EBB-38F3-4AB1-898C-6D0968E145D2}"/>
-    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{D81E92AD-DAF3-4D08-BCC9-BB4958CC101D}"/>
-    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{F3043AED-3EA4-4D12-B753-95F9B7455703}"/>
-    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{955B7A09-701B-4942-AF59-84875971A0F5}"/>
-    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{FE927F87-8811-4392-957A-D2F557D8425D}"/>
-    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{688F7334-922F-4E37-916D-A3B16014205A}"/>
-    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{8C76F9E8-1D18-47A6-A965-A1C0568F0409}"/>
-    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{E091E0D2-9E29-48E6-8C50-F2CFD8841AB5}"/>
-    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{6BC0259A-3DD7-4BC1-B020-1609EDD8EF87}"/>
-    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{B047E7CC-982E-4F96-B627-D761659B9384}"/>
-    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{BDC0FB9B-CACA-4059-8C89-E4ACD2141A0A}"/>
-    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{6B814CBA-CA65-4E81-8D19-971C7DD7EEBA}"/>
-    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{291CB43B-8877-468A-A91E-B91D2BAF3DC2}"/>
-    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{98ADC4EE-D5C0-40F8-B6D2-29ABA1507189}"/>
-    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{E5CBAF55-BADE-44AE-85DF-595A9ACDE186}"/>
-    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{6E0962C1-4B48-45E5-B0D7-F83CBC838715}"/>
-    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{97A4CFBE-D49C-4400-95D9-468F7EAF9731}"/>
-    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{1672AB97-B7E1-44C8-BB1A-B6B1A95A41CA}"/>
-    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{2EAEA243-CFA8-477E-9578-4699073E1871}"/>
-    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{66EF3882-8BA8-4E54-A2E4-3D440ECBC175}"/>
-    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{E590453C-F482-4F8D-BA78-DA264A698FAD}"/>
-    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{21F48C64-6B21-4CB0-8C7B-1752485E9FB0}"/>
-    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{223AE4CA-A202-4F59-A06D-1F9EC4400F66}"/>
-    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{26FFE85C-8D57-4F55-97CB-B1AE18A3740F}"/>
-    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{D4282466-5011-460B-BB9E-DF0A299A33FD}"/>
-    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{5953EBF0-18FC-4938-B785-A0CDA2424628}"/>
-    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{B2E867C1-A0D0-498B-8672-F3A271D0CDAD}"/>
-    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{72E30063-BD30-4F2B-97F2-294BEBB4A9D1}"/>
-    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{F7173FEA-D649-4B9C-95B1-2A31F41C55B1}"/>
-    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{9B1B5C15-4518-4747-BC4B-5F5A4AC60E41}"/>
-    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{296C744C-6E91-448E-A03C-5F05C497A019}"/>
-    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{6656630D-159C-43A4-8A30-0E5352811642}"/>
-    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{C2C767B5-6A91-4180-A72B-1625FCAD0CA0}"/>
-    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{119A5BD4-21B4-4C53-BF74-BDBEA9AEC1AB}"/>
-    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{EFA57F33-D4FE-4634-AA63-FE185162FCA8}"/>
-    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{75171705-F5B6-4B0B-8583-6173235D4D25}"/>
-    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{FC92D2F3-7F2C-4812-A56E-3CD891FE6AAB}"/>
-    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{F1B00700-7709-467D-8FD7-354B24141F72}"/>
-    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{97418F87-019F-489D-A6AB-FCACC0E58D54}"/>
-    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{4D384525-2DFB-4234-B942-B37C5E6319E7}"/>
-    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{A0011565-3F71-40F4-A1D1-424B451458F5}"/>
-    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{0317A3FF-09CB-4BC3-A31F-A651D497C2CB}"/>
-    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{8AC48587-E3F9-44BA-9EA5-43EF91C96CB7}"/>
-    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{7433C4AA-E65E-4AE0-9E05-B1DAB1FA3D68}"/>
-    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{35BB7AC4-9FA7-4900-B7A2-39A298844DBE}"/>
-    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{BFC21C75-961B-408B-9259-1449C829A313}"/>
-    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{52B9D160-D230-48DE-8999-0B1BD765DFC2}"/>
-    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{E4B64F11-0330-4D8B-BDCB-239E0A7472DB}"/>
-    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{3B9A4EEF-BBBD-47A1-97FF-D8F0389944E7}"/>
-    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{7110405C-510F-41B3-9990-F9CF69ED8218}"/>
-    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{70BB09E1-6671-4761-869D-528812A65B90}"/>
-    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{79620E42-2BB8-4AAE-9555-E28B277242E7}"/>
-    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{AAA6136D-31A0-49C1-AEE6-0BA47EA9874B}"/>
-    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{0F08FECE-0BB4-4648-8131-04E041494607}"/>
-    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{E9BFE642-E622-4A46-8831-C3FC9EBCF377}"/>
-    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{18FC112C-B063-4DF5-8E46-B1FCFBF58C11}"/>
-    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{CA62425F-8D73-467F-A69A-5DF36A059714}"/>
-    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{A92FD45E-35F0-426A-A916-FF6BA3EBAF58}"/>
-    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{AF59E558-ADC2-432A-92AA-FED84FB91834}"/>
-    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{9ABC1356-8CA7-4A56-A06C-04DA3EE19AC7}"/>
-    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{7C38BA93-2C9B-424F-B79D-51E736AC38B2}"/>
-    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{99E05172-D8BE-48F9-A276-767714008C97}"/>
-    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{EA96A598-FDA7-4210-9E67-1E2651093A55}"/>
-    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{8DB66287-38B3-4A12-BA5C-BD3215B4A1C2}"/>
-    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{62C3F883-1821-4F6E-937D-A2E546C8FFC7}"/>
-    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{0319B7F6-6A7B-4C3F-A699-AFF03984E82B}"/>
-    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{1F45F644-8389-4764-A7AE-6A8CC77F64BC}"/>
-    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{245C787C-49EA-47CE-AD73-A61832672F22}"/>
-    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{B7B7FBF9-96DA-4800-A5C3-43AD4C39B2B6}"/>
-    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{1E7D980A-10B6-4BFC-AAB0-8B4BB7F482FB}"/>
-    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{74A84635-214E-46DC-83C0-02CF359D0E43}"/>
-    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{FDAE85B8-800C-4454-A52A-053F75FA4179}"/>
-    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{C13EC8AD-9AA6-4994-AA7A-25064526D95B}"/>
-    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{F0BD1C14-3D2A-4F0E-A393-0FF58D0D1C10}"/>
-    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{85F0D3F7-E55E-4610-9E84-3FEA15F10DCE}"/>
-    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{CAB49B15-DE05-4886-BFB6-7E02FB3F032E}"/>
-    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{D4404E7D-6692-4320-A3E0-C0C3519FB335}"/>
-    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{D30F78AC-4132-4AE8-9E1C-F3BAEAEAE000}"/>
-    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{52B2EDEA-D35A-404F-B6C2-F3E86D15C3DC}"/>
-    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{0489156A-69B6-4BA9-BFFA-43201F63318C}"/>
-    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{FCCA01AB-D516-43BD-B24B-A395D4C09DFF}"/>
-    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{5B7A5521-61FD-4B5E-B079-C7ECAB5A24F8}"/>
-    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{0B36707C-E6C7-437A-A7D5-F967818FA030}"/>
-    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{0ADBFAF9-3743-4BC6-A7EF-DAF9E3C0E7BE}"/>
-    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{7AB71FC9-1375-492E-B1DA-7DDEDEDFD298}"/>
-    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{9C18E681-F905-4E7A-BACA-0B4F99908B0A}"/>
-    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{48F795CA-C0A8-46A6-B899-20CA2647AD8F}"/>
-    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{352E3A15-F3C4-4882-B031-FB1B401E5986}"/>
-    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{806869A3-D167-41A8-A392-3B24B128EF2B}"/>
-    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{84A2273B-A6E5-4B0D-B72B-D81D2E7979D1}"/>
-    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{F57E48A7-D873-4A77-B869-0BFD9033DF5F}"/>
-    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{3BEBAC2D-D02A-4A0D-A97C-AC748113D290}"/>
-    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{70122600-3A0F-48F5-873F-D7B3416BE735}"/>
-    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{EA9988A5-9E91-4D42-B4DC-23011D2FE641}"/>
-    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{BDF7A08D-1E0E-41D0-A6B3-F160C8DFA997}"/>
-    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{EDA7746A-9E39-45AC-AF79-D726E27C7881}"/>
-    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{33F1C9F7-FA6C-4F8B-B0DF-DD81B1F022B3}"/>
-    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{E2FCEE6A-E3D4-4D5E-9AAE-62DC371F6071}"/>
-    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{92AA383B-C6FD-443D-ADAF-3DFF9CFA1EF3}"/>
-    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{7A4522C1-B488-4799-9DF4-67991AD23A62}"/>
-    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{CEEB2429-1793-4EDA-801A-E5686A3A3C55}"/>
-    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{7AD41E70-7A51-42B6-9380-2E2BF365191B}"/>
-    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{9E741FB4-93D7-4B9C-A138-30DE232C4574}"/>
-    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{E23849CA-E205-4D20-86E9-3FA84C0E0FAA}"/>
-    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{D41DFA2D-B710-429F-95DD-4BF5E0702F22}"/>
-    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{EA450FEE-C442-4986-B609-61786CF987EC}"/>
-    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{E972AEB2-AEDE-4523-8061-817170880667}"/>
-    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{277B90A3-6E21-444F-A1BE-EDB50E3FEC1A}"/>
-    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{685B5B1A-EB97-490D-9B31-C0CFA3855CAA}"/>
-    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{B9837D0A-F816-4094-BA91-F8C223053BA2}"/>
-    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{535343F5-72CD-4F16-BDB0-6B9C549EDD63}"/>
-    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{85EDAEFB-5FDB-476C-8933-1931B4554496}"/>
-    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{0BC136E3-317A-4586-8137-AF3A52D2EB70}"/>
-    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{FCF0DF09-957C-4A96-89FE-24BDADDF3E1F}"/>
-    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{ACD44E04-6A6B-459F-BB80-A771867C4916}"/>
-    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{23F728A8-A5A9-40E3-93F8-E805B49A12C9}"/>
-    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{A28F56D2-C3ED-495D-8B68-0F744CD45A45}"/>
-    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{31196837-6659-4098-A8E1-85627D286142}"/>
-    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{3DA8EB30-3C6A-4954-9CF4-67FFF8D38035}"/>
-    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{943DF90B-6B2F-46F2-BE54-7FAF6C18A4B1}"/>
-    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{4FC19FB4-320D-4F3F-A811-453B9899D720}"/>
-    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{DDC841EE-C0FA-4980-9A8E-25306622331D}"/>
-    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{BFC792CF-E7E5-48D0-99E2-343E22FAB80C}"/>
-    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{F6B74E18-0764-4F7D-819C-1DC94337A5DC}"/>
-    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{EAECB7D8-3424-4BEC-9377-9EAA8F33AD4F}"/>
-    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{43A31073-D220-48A0-8189-79160B8EE051}"/>
-    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{C46D35E2-6B47-40DA-9779-6798621BEE3B}"/>
-    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{F3EBD67A-37BD-44C9-B840-49D5C46011E9}"/>
-    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{39D4A7C0-6F93-4316-A1BB-B3996719743F}"/>
-    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{BBE15010-5DCB-43B8-A7D3-E5BB8549C331}"/>
-    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{4C62BD72-D45C-4B14-BABF-C9339C81C066}"/>
-    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{D1E9ED8F-F83F-4FE2-B3F8-297EA58313CA}"/>
-    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{0779C52F-DBD2-4857-AB2E-FCB6DA6CA9E8}"/>
-    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{E2DFF156-8890-49E4-A8B0-21394C3EC6FC}"/>
-    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{22CBAF9F-D601-4489-9B04-11EDE7858A26}"/>
-    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{A88A001B-1B46-44AC-B02D-8BC2DD5634CE}"/>
-    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{551114BB-24C1-4FD6-A79E-AD20BB33CE15}"/>
-    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{88EFAD6F-FC4A-4A47-B8FD-07ECA8DB9778}"/>
-    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{0399FBB3-13AD-4486-8623-7AECAC6CCA70}"/>
-    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{5B5ECE7F-5738-42E8-8455-180524B17AB2}"/>
-    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{94ABB820-37BB-4333-9885-B6D6ED8328B6}"/>
-    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{42E929AA-4861-4F76-AFB7-B072239423B0}"/>
-    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{187DFB87-D784-4E89-8369-75A688659BE2}"/>
-    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{65191927-BDB0-4A2C-8680-04D0889B0BB8}"/>
-    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{823EB12A-5F4F-4B98-BF5B-5D883D0E7935}"/>
-    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{97F0AEF4-1885-48BF-9201-DE33E5247F76}"/>
-    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{A6273080-8C65-4DCB-9139-3F2F87FFF8F8}"/>
-    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{6B94AFE7-C111-4E5A-8EB8-BF223E81583D}"/>
-    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{C33BB8F6-966D-4D27-9C11-BAD9EF8E4874}"/>
-    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{230ADC0F-FA20-481E-8CCF-0B0E2927FE94}"/>
-    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{A12B8585-01BB-4623-993C-5FB15448E4A5}"/>
-    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{9501D82D-73CC-4468-B63F-9D68B5F48FA8}"/>
-    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{A33DC336-C01A-4009-BCE2-4C68F059B501}"/>
-    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{FA3BFFC0-3E8A-4461-99C3-424203C89743}"/>
-    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{87C428C6-FC49-4BF2-AB46-F8DBEB4118E2}"/>
-    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{F7A6BEF2-DEAF-41C7-9125-A8D91933267D}"/>
-    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{ACCB82A8-CDDB-4FF0-B24C-39B91E1D339F}"/>
-    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{33EE5E6D-001B-47FA-8321-FB548F5DE22E}"/>
-    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{673E33D2-17AA-45C3-8C53-7FEF125C82B9}"/>
-    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{574861DD-75A0-4699-84B0-08DEEF484A6D}"/>
-    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{FDAB81F1-7AE2-4F55-8B08-B39677E224F8}"/>
-    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{25C87BB1-7ADA-4666-8117-AE43224F42C0}"/>
-    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{D5FC2253-958C-4A0B-BF32-F591BE87A023}"/>
-    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{8A4BD246-D2CE-4083-B8A1-F3BBD9504EC1}"/>
-    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{581B044D-1F94-48A4-8C46-E8FFEE7D115F}"/>
-    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{E3089137-313D-4295-958C-8040BEBB1F7C}"/>
-    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{2170C333-4869-443D-A13F-1E1E923C8B47}"/>
-    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{1B103262-0E5A-4DE0-B286-F84958B9CABA}"/>
-    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{3C69B0EB-F531-43E4-A6FB-31965A8CC703}"/>
-    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{7EE36BCA-3E01-4C7A-9F01-BECB2CCDF45D}"/>
-    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{2EFDD92A-2AA1-4B89-A835-D0CB0C055218}"/>
-    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{2D1790D0-09DD-4677-865A-F203877B1090}"/>
-    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{C1785384-28CB-4005-93DF-EEBB20E6165E}"/>
-    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{E40690FE-79FA-4DE7-A875-EC688D655CE1}"/>
-    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{107A6236-6A6D-4A0C-8A5C-9AF95DD03EA7}"/>
-    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{381B2790-478B-4D7C-BFE3-E30FEF6EE46C}"/>
-    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{1C81D2D9-DBDE-460D-B22F-FF312779AE5B}"/>
-    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{B53552F9-A082-4D91-A9D9-468097E73DB8}"/>
-    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{4948C465-0376-4E41-875F-96176C67C898}"/>
-    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{004CC30E-5887-4566-BE3C-77E7A633961C}"/>
-    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{80573F9D-CFF0-41A3-8306-C7D050A8DFA4}"/>
-    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{0B4F2CDF-8587-4602-92C3-05AEA11AEEB3}"/>
-    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{5BE905C9-BB06-41E5-B957-6431F65FD323}"/>
-    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{EA3FA0D0-3DCB-4FD9-A5FD-0B7A85E5001E}"/>
-    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{8B150839-BC30-411E-818F-542768D04030}"/>
-    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{7E2DF5CD-4D94-4D79-9A95-AEF29E0F800B}"/>
-    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{DD723BE3-E9DD-487D-B5D0-23ECFEACC398}"/>
-    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{ADC6ED00-E4F9-41FB-83BA-5D56F7489A20}"/>
-    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{30F66D74-2F27-4317-A4DD-272E810FF763}"/>
-    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{7F04130A-5855-4D81-8270-C1FA5959F96E}"/>
-    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{172FC913-E4B2-477B-A759-82EE395A157E}"/>
-    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{2214DBE3-A556-4746-A80A-183AAD397CA0}"/>
-    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{442E1F4F-34AE-4EB7-BF37-E894552345E3}"/>
-    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{096DFEF5-9FF3-434A-AE47-FC2B5D7F5DF2}"/>
-    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{23EEE56C-C63D-41BB-89EE-D4EB9B9FC626}"/>
-    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{5D029458-C6EC-4E34-A464-1241D1FF44BD}"/>
-    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{0FDBBEC4-809A-468F-AEC6-CABE731017FA}"/>
-    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{91AEF8DB-6C70-4572-B0D2-567722EE47F7}"/>
-    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{D47A2B42-CCB1-4BB2-8FF6-F26803C132BE}"/>
-    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{075525A0-3B3C-4E3E-993E-1B8A515C76E8}"/>
-    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{5538B0D5-A85D-4406-8754-6C4A6831D2D2}"/>
-    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{D32C31CB-FB5C-4808-A340-BB1AEB6BD061}"/>
-    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{F4DFE4BA-3BA7-4057-9CE1-C93A92841C3B}"/>
-    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{EF0ECF1B-076D-452C-82B4-FAAC2345BB41}"/>
-    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{5C343CB7-8EB6-4A53-BFCE-0B350DD2E538}"/>
-    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{9F1BAADA-1177-42CF-B4F2-60F4BBAB4748}"/>
-    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{54FEA7DD-DA10-4248-859B-995A8928FB62}"/>
-    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{06011912-CC4F-42AB-9CF7-5F89D209675E}"/>
-    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{8A6C7319-3130-47B2-8E47-7EDD1FD1619E}"/>
-    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{7C1719A2-F5B5-4132-9AFF-C16DD8770415}"/>
-    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{58508B58-F472-4D43-87B3-21B99228BA98}"/>
-    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{F5E43C5F-88C9-4570-95CB-CBFCD00CDABE}"/>
-    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{F85E97A2-6B2A-417B-B0E5-2C38192C238C}"/>
-    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{D1BA79EA-D3A3-42B9-A888-4DB562A29A5E}"/>
-    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{87A76DBF-AF06-4F19-8452-91A1980C4AB9}"/>
-    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{4BBC5F9D-4EAB-45AC-8DB5-6D6634A8DCEC}"/>
-    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{75DF7A42-1126-46DF-8277-DE0B663F9C04}"/>
-    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{8C952D5F-C1CC-445F-99BA-79C8D63E9B59}"/>
-    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{B748FFC2-21C1-4CB6-8FC6-9F84542F6806}"/>
-    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{52A6C161-022B-416A-90E3-95BDF04846FF}"/>
-    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{A8B6AFF7-D08D-405C-BD68-C53802A4D3F6}"/>
-    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{AD927349-D35D-4BE8-B4E0-0BE6CFCAF2A5}"/>
-    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{38108639-FDCE-42C6-A65A-D5F31BB9AC19}"/>
-    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{5F633499-49B1-4D56-B95F-2BCEA44C857F}"/>
-    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{2BF85C1C-CE8D-4D09-BB23-B741F02A1478}"/>
-    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{CA66F850-9948-40D6-8436-309AB05F7D7C}"/>
-    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{211FCA0B-3B73-471A-AAA4-9E7251A21470}"/>
-    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{95014C38-31E8-424E-B8DE-7BD6E2326E19}"/>
-    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{2543FE5B-00BF-4A74-8249-41C9A2311325}"/>
-    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{312CB4E1-8C4A-448D-8A04-0CC9C5D0039A}"/>
-    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{931DFE9B-E7E6-416C-A42E-C77059FFF6C6}"/>
-    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{C6DB6FE3-7C75-4596-B1DE-8F95B29A4B37}"/>
-    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{BFC5B372-62A4-44E7-A7A5-89E03CA4AE49}"/>
-    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{ED2B8CB5-02D5-4EC4-B29C-03C94E2714A3}"/>
-    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{911BCF39-908B-4932-BDF6-5A33146B4788}"/>
-    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{9DCB96E3-B9EA-411B-AECE-456E9EB2154B}"/>
-    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{B0F93B41-3D8A-4F88-8805-9042E91A2F2A}"/>
-    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{BEC8811A-9C5C-44EF-8B64-1FFB99E0226D}"/>
-    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{88C28F6F-2B89-4245-AAA3-F627BEA2E851}"/>
-    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{5204C48C-86AD-4479-BEA2-283088FD8AD8}"/>
-    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{33B052B1-532B-41F4-9717-15AFB88BB5EB}"/>
-    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{FBC40021-AFEC-4DB3-ACAD-DB72C5DCF847}"/>
-    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{30770019-123D-43B6-A030-9941137D9927}"/>
-    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{F62CB21B-2334-4ACA-A6A2-5935FACF2ED5}"/>
-    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{C85A3A7D-1BC3-4025-A728-6F057905B04A}"/>
-    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{91AA869C-D777-4449-881C-5B0ABD8B0A2A}"/>
-    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{F70444C5-5155-4D1B-88EA-74C8CE49D216}"/>
-    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{ECAE748F-2F4A-446E-BB79-0A407FDD191C}"/>
-    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{7CE28ACE-9B7C-4D12-AE32-C7930F30A5C4}"/>
-    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{B8C7C9C1-F03B-4962-996A-122B644F062B}"/>
-    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{12FEDC41-DD15-4FD7-A19D-ACB967BB8F85}"/>
-    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{AE4ECB53-96D4-44EF-8A9C-690B488F501E}"/>
-    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{DCD5FD87-0055-40A7-AA64-DEE944633160}"/>
-    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{9C91BDF9-056E-480A-AEB1-21382CEFB431}"/>
-    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{EF591625-0283-4F3F-B790-C1814B9FEB5C}"/>
-    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{4F909526-A268-4617-A609-F337332EC7D8}"/>
-    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{DE3F0F9D-FFB0-4748-A02D-C0F0637E5A88}"/>
-    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{FE491598-F0C3-41DF-9908-4A6A4F4DCF3A}"/>
-    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{194DF245-ED1A-4377-8949-D9E8FE2CAD92}"/>
-    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{F813F25F-1537-40E4-83B9-6AF1BD51B4EA}"/>
-    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{E97BF132-13E1-463B-8DEE-3E711494CEE2}"/>
-    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{4923A6AC-D035-4B61-9686-CB94C04C9F2C}"/>
-    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{583170B2-7905-4B79-93FD-621D7F96CEB3}"/>
-    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{9731B73A-5F53-4FEE-AC3B-A4756196DE2B}"/>
-    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{563F69F6-1A34-4187-891F-C4DDC09237C7}"/>
-    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{D01CF549-68D7-4801-B63B-6B6A57587865}"/>
-    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{FF97D89E-4275-41D2-8ACB-025B736527A7}"/>
-    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{601AAEED-B404-42C1-9A51-3785117B121D}"/>
-    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{2FC3AA56-1D22-4BF8-8ED5-4EB317DA15E9}"/>
-    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{D10A210B-61C6-4841-9CB3-F74200AAC7C3}"/>
-    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{CC7F03E1-163B-4BAE-86A7-8C78C2B91700}"/>
-    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{EA633B60-C7A0-4302-A639-9662196BEE9A}"/>
-    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{56185330-4761-41CD-A93D-D0BFA7E51FA2}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{607C29CE-E9F4-4CCD-835E-5BE20AC7D9F3}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{871B9EEB-24C6-401A-88C0-CF2A9E206629}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{36F09244-E924-4C78-AA59-00A74B3E5FFF}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{DCD876EA-524D-4B68-B2A4-1A1CCAAC9096}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{5498BA67-039A-4889-8850-4BACDC8F1B73}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{726854FA-18E7-4147-9C53-2E45F8FA7495}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{367B6E8D-7429-4758-A8F1-AAD8FB2E612D}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{8EF5704C-54B7-4772-AC02-F159CC6B490E}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{88376681-0359-427F-9175-0EF1A31BFF93}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{8A71ECE2-2D95-4A3F-8321-E17E63F0732C}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{4C4D17BE-183A-4122-8B96-0BFF693BF704}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{72BFFB95-BEFF-4620-A08B-93DDE781C5E3}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{2A7EF8E0-F866-4832-A586-7A48BCB7B1D0}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{DB7DBA79-EAFE-4536-AE65-422E9FE6C3D7}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{A983A882-58DE-4DD7-9C1F-5D0A6ABA8EBD}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{57488062-D20F-4313-B56B-9CF730EF94A2}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{43B73458-0D38-4148-9674-846FA63B7F22}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{BD36FC53-F6CF-4905-AA3B-149D223E4F94}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{C26A6990-3D43-4AF8-8767-7CC0E39D3308}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{85D8CFC3-5042-4509-B500-76539B3ED081}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{A0672BE8-D916-41A0-8C12-20CB9D7E6EF2}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{20A99CC8-F07E-415D-933C-AFE6DF2DE488}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{6F086F1D-7FC6-4A17-BC45-EED89B7ADA34}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{3A07C26A-AE7F-4DEF-B457-40DA777CA5FC}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{757B3162-DA54-4CB9-B48C-916928073974}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{9B4C52A8-E587-44A0-8F32-FB5C5B1755AA}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{AA25B19D-9BB1-4196-95EF-935FA56FED97}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{95B73DA4-8E06-41EC-8006-6167F3CA16E6}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{AB88DF3E-DC94-447C-BEC4-EE91579E7DC3}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{26608C87-730F-4966-BC56-4304A656470A}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{BC2C06AB-91E8-4B80-95B0-980D25E535AD}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{D97ADC65-2922-4A58-A75F-B11B4C4F643E}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{30D81CE2-79DD-44D0-AA70-8A780736DD5E}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{93CBF7B8-2154-4FA4-8019-405349F79C4F}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{49980EF7-0659-4E0D-B609-336B30AA5824}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{2EE85581-E5D2-4F9C-9739-491FCDE15B33}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{DCF5A562-78AE-49B6-95F1-1DE7C5ABA207}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{95BA672E-F903-4982-9EFC-7DB54CD9081D}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{ECEAA6EE-D9F6-4C66-87C7-CDC24BFE981B}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{6A60724E-634B-4AD9-8242-71495D9FE323}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{2DA93540-14AA-4A6B-8248-13A6A2357EF8}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{EB34F336-AF56-4AD5-B0C9-2C972F6D14A5}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{61651658-67FA-449F-9E53-590FD8F2E4E1}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{90ADA6C3-B318-4965-8539-ED184D1DB8D8}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{324D25C2-E262-4683-ABF9-01157E9485C1}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{00117C73-1E2B-4647-A895-A40126B6192B}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{43173E90-A69B-4C31-9684-6DF960D0F639}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{4674D5C9-53EC-4C93-B8CB-5026538C7F54}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{C9DD63B1-7154-4B5C-AC9C-207A13373F98}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{D46FDA2C-F7DF-4804-BA77-B60CB4259641}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{3F4AEF15-F8D1-4D40-920F-881F9567586E}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{A1373178-F6F5-420F-AD22-056F2F5D5DF2}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{27084C35-F17E-40FD-B9BA-289A73EA32AC}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{96874A00-3B84-4659-B8A8-C515ADB64BA1}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{53F6D2E1-3333-46A9-AA87-7F86A329904B}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{DD50C04D-8547-4490-AB20-8B9A947278EF}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{9B94D61A-D961-45E8-B4B8-5080C292ECCF}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{B6F7E739-4C85-436A-979D-5F2728D07FFB}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{A3DEBA16-2E70-4C0E-9EF4-F0CEC99CC3F1}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{1936F794-9061-4CDB-B638-11B5618F7D81}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{5183FE9E-BB12-4B1A-AC2E-6E580C04A493}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{028982F4-15B2-44A7-9AA3-4AB7734FDA15}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{6323C26A-EB38-406D-BE04-F756E088B1BF}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{AC098FED-04C4-42BC-ABCB-D457164EE689}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{A8A5FE7D-34FA-42BF-9882-88949A1A9544}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{BDB17BC1-C57C-4700-B502-C95098A8FBBB}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{A4F4059A-EF7D-40BC-A30E-E25CC04AE258}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{7A1A2EC1-5A29-4328-B970-3C97D6BAA0C1}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{92B2BCB1-A8C0-42B8-A783-533092D8E503}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{8A337F14-B85A-44E4-BF0F-C3309A783439}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{2AFB338E-EAE8-4AD3-AA4F-99BC6435218A}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{99465418-ED04-4ECB-AF2E-02F689DE2D50}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{17641447-5A3C-438D-B080-2AB55229F0E4}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{8CF7BD64-C1E0-44D1-BE7B-0350E4DD2BF7}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{FCC617A6-BF7B-4FD0-B874-0AA99392EDEA}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{BFC32FEB-15D6-4504-8064-B1318A2F48F0}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{60D2C900-F251-4110-A98F-8468850AAC16}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{6C634DF9-AA35-429F-B4E6-FB4484435FA9}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{DBCD5E3B-5123-48FA-BD18-6A419B09EDDA}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{02127F0E-CBAE-4CC3-8C78-53C977A59A9E}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{AD5B3C16-1007-4340-8A94-50C8BB753D57}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{0C3241E3-CE7D-4987-AC9E-D9A57D07FD28}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{E3E50475-670F-4382-8460-414C655A29B9}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{43F5977E-351A-40C5-99B4-005A2B841C74}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{FBD900A6-EDA2-4B61-95B0-4E0C6C48D83B}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{ECDF43A0-046E-4FF1-982A-031EB35D7C9A}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{AEF8E254-9312-4309-BABC-531DA3EBD8DC}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{EBB48E2F-A06B-4C88-8031-D44E0C9E324B}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{9BD6C7A0-261B-4275-A644-F9EF164C8CCF}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{ADBE4DEE-1270-4E29-860A-A55C77480D3C}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{ED309B16-6795-45CE-A69F-CAE94BCC4B93}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{834DEBDC-EE20-45FB-A35B-2062AF4FA3C1}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{8F3CB043-BEF4-4650-BE44-C062122B54FD}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{8C5F1D32-41D8-4FDF-B72C-3013F921DEA7}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{2B073142-4FA5-48C2-978A-6FC456BD76BA}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{06C8367E-2076-4E90-9975-214E9A0064E6}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{3CB962D6-46A8-47BB-9AFD-BA5021E73A6C}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{D340C9F9-4E14-4C71-AFE4-7209E6C51FD0}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{34C1D6C4-CD0F-4D0B-8113-8DBEB7664815}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{FA0DB86D-4A4F-4A05-9580-7A7BFC94C295}"/>
+    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{33A168C9-4D00-4B14-9567-3DED0E11D241}"/>
+    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{03D5CB61-838E-4862-9C32-D416DA9392E5}"/>
+    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{559BAD0A-CEB7-496A-8C7D-9D0A9D520DD9}"/>
+    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{24FB2135-08B2-4D79-B2FD-6AB5DB770B88}"/>
+    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{584BECAF-FD15-453E-88EF-8DEEB3AEA2E7}"/>
+    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{6910D0BD-E79F-4F00-B46C-FFC7ED40DD84}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{B4347BEA-BE8F-461E-88D0-8BE7085A9738}"/>
+    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{1B52F2D6-B69E-47B6-B687-8DA9560054CE}"/>
+    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{92BDE90E-33DC-49BE-BBFE-1C26E998F62B}"/>
+    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{FA541893-4A7E-4957-B518-62F4E834DBB5}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{2F1F8F46-4ADF-44A1-8570-30FD0CB13802}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{A16810FC-67D5-44B2-B1F7-410ECCD4F76A}"/>
+    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{F9213C01-93FB-4927-B502-9C6086E7B8B1}"/>
+    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{39DEB097-2540-4A62-A12A-5B6DB658D509}"/>
+    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{16398A2A-FE94-4D54-A6E8-B3C08F84F8A3}"/>
+    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{7C6424F8-6B88-4E53-AF10-5E716B1C81A9}"/>
+    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{B1BF3172-B07C-4897-8996-8CB4A97FCED7}"/>
+    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{4A9F2EA5-891F-494D-90A6-E68372A0FC34}"/>
+    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{406B8481-1F7B-4EEA-A236-949A70DAACE7}"/>
+    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{ED2D0080-AA29-47CB-AF02-D0C9D56DCA92}"/>
+    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{7D1EACF2-333F-496F-AD1B-D9548E2EB25F}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{E79675FB-5088-4916-97F0-0FE8167A4998}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{643C4353-99A2-4F28-A918-B97F452B1554}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{8052DE3F-F2AF-4AD0-8984-FB24A6201B45}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{4D8F579C-2AE8-4CA2-8934-29864CC063ED}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{74DEB9A4-F292-4EE8-BF1E-49903144604E}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{E84D81C0-2C90-4D70-919F-842A1F7862AC}"/>
+    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{7AD9A020-6AFB-4264-AFCB-4A681E0E1CFE}"/>
+    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{FA806C79-728C-48D0-905B-02AE64256171}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{4EB71E5B-6273-402A-9643-E67F52C7AE5B}"/>
+    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{BCB7A418-645E-44B3-8A3B-778C1441CBDA}"/>
+    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{989ED701-0A3E-4B3E-9926-2F5A5FEA8DC3}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{75DBB2E8-4E9A-474E-9364-FD4B2B549389}"/>
+    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{3BD58C85-E48B-4BA1-AFDF-5D94A689B1CB}"/>
+    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{B4E96BAE-0AF4-46CB-AB48-B12E9C4892F7}"/>
+    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{9E7A05E1-32FC-464D-9A5C-A0B3270261C8}"/>
+    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{0A5135A0-E803-43D3-B034-3D01056E405D}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{D0F8944C-4C99-4E4E-85C3-79935B437D03}"/>
+    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{0D7D4586-BD6E-4A3B-A383-420AF2E62FCD}"/>
+    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{EA4501E9-31A2-4C39-ABBB-21755DAF7464}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{8B5B5809-8E77-47C9-9879-F7BA08525ED3}"/>
+    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{B3026CBA-F6DB-48E7-9D8A-D41B44DAE7A1}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{0EC5B124-06D8-4ECA-9C53-7C3C5634BD81}"/>
+    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{5DF6F338-E5B0-4E60-AE6E-E992CDB28587}"/>
+    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{F9DB9265-DA90-4B5E-8E62-1643E205D06E}"/>
+    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{FB7C1479-2D4B-4BCB-A4AB-0B8EE00AB315}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{4F0A0E12-8CD1-4BCD-8EF7-76070F638F84}"/>
+    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{C580AD03-78F7-4593-8606-067B65101DEA}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{443896B4-4692-436F-8FCB-ECEAD8CBBBDA}"/>
+    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{212DD8CE-9DF5-4F2C-A268-7C6FDCB90EAE}"/>
+    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{6F04A92C-B770-48D3-A7E8-A2C4D399FA21}"/>
+    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{86FF58E2-D5CF-4CB6-9EB5-66778CED2DD7}"/>
+    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{2573816F-BAF2-453D-9527-D6E43AE6F6E2}"/>
+    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{91BFE5BE-9BF8-4C7D-92EC-A32EFF6FC458}"/>
+    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{8B2DD693-D921-4FAB-84C7-530CDDDDBAF9}"/>
+    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{75FD391C-F363-464F-ACDB-85685F568914}"/>
+    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{F4AA5118-BDA1-4B8F-B867-36C535FCD69E}"/>
+    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{9502288B-E2F5-475B-A8C9-1B6523667E66}"/>
+    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{DB799140-05FA-44A0-8D14-36CDEB4EA012}"/>
+    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{011C0A03-9D7E-4FE2-9744-7C8CED886B77}"/>
+    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{927A5F8F-15FD-4734-82DD-4104B19D3C6D}"/>
+    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{8A00DC25-9438-4332-8CD7-A57F20F9C12F}"/>
+    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{8433D298-6AA6-4FF6-B7E5-499445A05945}"/>
+    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{F1DD17CB-FF2B-4D22-9A68-B42D25A18FF7}"/>
+    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{70BC8DD8-C4F5-4E9F-9BAF-54C7091A0424}"/>
+    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{E22D7541-4E56-43B9-8376-F28C86A9816E}"/>
+    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{595D21BC-47FF-478B-9BDF-3F49DD43A176}"/>
+    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{B4583BCD-2656-4C4F-AB0E-403AFA3AFD2B}"/>
+    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{9FD3C1DA-D67D-468D-A192-3154193B9A97}"/>
+    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{0E20E3DD-5DF1-46C8-BCD8-CF604AF6BFB0}"/>
+    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{9907C8F4-B39B-4FEC-91F8-0F1559E5632D}"/>
+    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{E614A78B-C79A-463A-A903-5F512E674D58}"/>
+    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{C61B979B-459E-46BF-A471-8F3EBF3D7121}"/>
+    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{AD4F949C-FA62-46D6-B5D9-55C5288BCEE7}"/>
+    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{C6845E13-1CC4-41C8-A0B0-BE1082B998BC}"/>
+    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{B314A602-3C93-4C1E-B0C9-5221F6B8DD07}"/>
+    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{A36EFBAE-AA69-454C-AD3E-B91E1A8F0819}"/>
+    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{BD37666E-4B3B-4A70-BB15-3E878CC6E317}"/>
+    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{BBCB7DA3-7E8A-4066-A9F8-059216439BF8}"/>
+    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{3B7EC163-DA9D-4823-AF84-2FFB86E20E45}"/>
+    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{E8019D7F-73FB-4EE4-8D5D-995152507ED0}"/>
+    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{F1FB5BBA-829B-4A5A-A973-00A60F0109E2}"/>
+    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{182F83F8-EF60-4219-A8E1-F224E4FA507A}"/>
+    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{90A2F766-0C09-4D6E-A4EC-ADCFF6F1D905}"/>
+    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{43335C38-DD36-4908-8CF8-DC0F3E4492FF}"/>
+    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{0B364548-FB26-4530-9E73-B7AE2BDF5263}"/>
+    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{9004049E-0F58-4BDF-A251-5E62B522FC32}"/>
+    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{220632DD-C6ED-4AC4-9731-26A7146BB355}"/>
+    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{F7BB31BD-217E-488E-B085-58D10B2479BB}"/>
+    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{91B279FD-BDDE-4264-968E-36537A8AF68B}"/>
+    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{3310B6CA-3310-4811-B5EB-2FA121840093}"/>
+    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{38280B30-8253-4F61-A4F2-5FAB29ECA067}"/>
+    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{1D24FDE6-2B80-437A-81F5-ED09EB4F176E}"/>
+    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{BAA7DC0C-51A3-4002-9423-7EEE7E665499}"/>
+    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{3A507B0E-A912-4292-8A76-DFD68CFFC7B7}"/>
+    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{24B358E7-23C3-4F29-8B9C-22E3F99BC126}"/>
+    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{B1A37CB6-EFA1-44E6-83E5-4A736518E282}"/>
+    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{454FCE36-36A6-4DEF-A8B8-6201959CD63A}"/>
+    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{93CC2747-9AEC-43D3-A954-B6A2E6697A00}"/>
+    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{4B322F6E-180B-48CF-A1C3-08D10338EEF7}"/>
+    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{D3BC4482-0C23-4E3B-AB46-604A2EB50228}"/>
+    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{5D021203-A0F3-4DFB-AC81-2214BB5D2530}"/>
+    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{974108C9-D37F-4A4C-9283-BF6C9ACEEFE3}"/>
+    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{2E0DB8D4-A830-4116-9B00-2C98CD62EA3C}"/>
+    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{410BC95C-8089-4342-8DD0-5F4BE65132BE}"/>
+    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{5D56B5C4-F9C0-403A-B362-21BB3E8E0405}"/>
+    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{0C0DA31A-67C9-487E-8E97-D8B061DE9F4B}"/>
+    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{CA53DC7A-9503-4425-9B71-3AED0C414924}"/>
+    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{BA2B50C5-375B-4F7B-93CF-702C97608792}"/>
+    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{9B95DEB1-552E-4514-BA3F-9E24FE88E6D7}"/>
+    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{58C341CD-D0BE-439B-96E6-D6FCD94218DB}"/>
+    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{DEFDF0DD-67D9-4635-B47A-9A23986A09F8}"/>
+    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{A13AC12C-FA8C-4D6B-9A89-1909389EAA5E}"/>
+    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{EE7D89AE-113C-4824-8DD5-70F21860F65E}"/>
+    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{2B0EF8C8-6FFF-4B82-BB4D-3B75396BDA30}"/>
+    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{C8CD039C-5314-47E1-88D9-B1D35103ACA5}"/>
+    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{9EA93E5B-E504-4DC0-8E78-8A09503C702B}"/>
+    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{33B60823-04DF-4C5E-A7DF-0D953B8A9CB3}"/>
+    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{CBB98267-6F23-4CB6-9FA2-6C3BCE9822E0}"/>
+    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{BAE0DE9E-7A97-409B-9D66-D8BE2C6F2389}"/>
+    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{A4BAF6C2-4B31-42C9-9898-45861FB1C5E0}"/>
+    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{10003DFC-7C69-4E2C-9902-5960BB0E09A6}"/>
+    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{C8AD304C-8F57-4AF6-BCA4-9086F3997813}"/>
+    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{B58A2255-6AD4-41F5-A861-FA393AF57FE9}"/>
+    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{8DCA1266-CF4C-4C09-8674-81D43D67C92D}"/>
+    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{4A6F7505-363D-42F4-AC4A-12F82EE60469}"/>
+    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{F3DADA8C-C77F-47DD-A5A6-E53EB16B7388}"/>
+    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{2B9BF3AF-5CAA-4C1D-8C86-8E29733E02C3}"/>
+    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{BB99D000-1BE3-4361-94AB-81256E4BF975}"/>
+    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{9CBCA594-E362-46FE-AA0F-6E2726BCBB4B}"/>
+    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{AD64145F-012A-4B04-B848-1510482EE9A1}"/>
+    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{E39F7CE7-4D07-4110-ABEF-DAE35307C19A}"/>
+    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{D8CFF5F9-9A9A-4CA5-BAD4-580EE62263C1}"/>
+    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{25E50A16-7E86-4671-B48C-EDDCE33CD2DB}"/>
+    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{148187A0-C70D-469A-8D2C-E56E907857D1}"/>
+    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{9390AB3D-D0F6-4A0F-8A0D-1E3C38EA6D41}"/>
+    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{AAA02738-CD0A-4ACA-8457-CBE3EFB9FA41}"/>
+    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{36B108E5-B972-46AA-AE1B-FEDA2C122947}"/>
+    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{1F1AA886-008B-4F67-9FFE-4D27E9DC30C4}"/>
+    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{D712740C-C273-4145-83D7-2D1E5A290453}"/>
+    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{6AD00DF7-D7EA-43E5-8A07-7C6A7754D786}"/>
+    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{4351D038-4A34-4FE3-8B4A-F3DAEB91083C}"/>
+    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{261EC49C-CE5D-4056-9927-2BF4A1BF6CFE}"/>
+    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{553285F8-1E72-4948-8FDE-E563721B87CB}"/>
+    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{269B5443-AE8D-479D-AFCF-2FB3E070B2F7}"/>
+    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{CDD21742-008C-4025-B23B-3D1128F86293}"/>
+    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{37C98EE0-4039-4566-9CBC-FE3FFC044180}"/>
+    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{CBB12B32-02C8-4663-A170-8BDD0F172349}"/>
+    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{60227C94-54D0-4827-84F4-E7DA85CC388B}"/>
+    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{574B3641-82B7-4C58-92E3-663A8F1BBC93}"/>
+    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{8BBCC4CA-19AC-4062-BA2F-9F27B308107A}"/>
+    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{E364404E-B7D2-4F19-A4C6-1A558F15408F}"/>
+    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{6B2B455A-F748-4FF8-9AC8-A80E43F124F4}"/>
+    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{008DCB75-F8B9-4F07-9F83-0E55FEA035CA}"/>
+    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{24582549-2163-4EFA-AAC4-85A14D90F98C}"/>
+    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{2349A5B9-279B-4277-9164-72F6765926AD}"/>
+    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{C966B172-ED0B-4FCA-89CD-4B49C84F550E}"/>
+    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{BC846F19-D3F1-4CC8-8492-083A0918C67B}"/>
+    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{6CBF768E-7A2F-4837-9B0D-9893ECAA6BBD}"/>
+    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{B31D0FE8-0A0B-4B4B-B2F8-5FD770EE5BE2}"/>
+    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{B739EE22-3498-4A24-B73F-592BB81A81FC}"/>
+    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{D45788F9-370F-4F5E-AF55-8A5403D560B8}"/>
+    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{7F114330-7278-44C0-9C65-6B5102CB03B5}"/>
+    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{4B980AA7-1BF5-4F74-88AA-25351DD5AB9C}"/>
+    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{2C819BC8-83EE-48C3-B4DF-7E962F9127AF}"/>
+    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{70D12C7E-6A75-4793-96F6-6133834C7539}"/>
+    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{918E1CBE-5D64-4016-AF0C-4165530A7C50}"/>
+    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{07C962B3-4D44-4976-884C-B74D53DB173A}"/>
+    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{1CDF140A-D6DB-4309-A72D-0E2875488C19}"/>
+    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{CD4D4D5A-0F79-4D26-819D-A13DEA9E4726}"/>
+    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{53B23B46-CAD9-4BA0-B131-C856A916A2E4}"/>
+    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{84AB11CC-B684-444D-B265-4FC12BE8C43E}"/>
+    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{1F361570-4E22-4C94-AB8A-216167203CFD}"/>
+    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{F6D6A0AA-69F4-4883-BB10-A1BDA289CC3B}"/>
+    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{E99E0C15-FC1C-459F-81A1-01C156AAE1BD}"/>
+    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{3D34879F-DF7E-4556-8A7C-993519EF82FD}"/>
+    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{C4FBFD5C-6F95-4532-83D2-7758DC6FC924}"/>
+    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{DB0FDFAC-66B3-4762-9A3C-F30AD0F21C32}"/>
+    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{E02C9AE6-D9D3-433C-90A9-C5ED34747D20}"/>
+    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{328F2367-F272-4B88-AFEF-D64664C10196}"/>
+    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{AB02AE2D-BEF9-4C72-AD41-C1555777873A}"/>
+    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{5F1FF03F-1933-4410-92BA-5782A3EE5F0D}"/>
+    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{64529711-8017-4DD8-9074-F31597E33139}"/>
+    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{5EBFEE3C-497F-44D4-89D2-80F7A7737E90}"/>
+    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{DF5C359F-E0D0-48E5-9DE5-6E74B2C568A2}"/>
+    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{D079FCC7-57B1-4AA0-8826-4FBD10134D50}"/>
+    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{F32329F1-D4B8-4EAD-A842-FE60C5AC446B}"/>
+    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{119E811E-27DD-4A8C-A972-D3BEBF5A0125}"/>
+    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{F0DEFF4F-002A-40AE-8899-F0C390C1FA7A}"/>
+    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{6F8113BE-64AA-40F5-9435-B302439A2524}"/>
+    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{132AAAE2-E26F-4A2E-A9E3-DB158E86807F}"/>
+    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{33DD63B0-97F8-4772-8D0E-281F86188FDA}"/>
+    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{14DFEE7D-05A6-40DB-A70C-48954177FF19}"/>
+    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{D0196A15-55BE-4109-B4B2-89C0D7CF2356}"/>
+    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{D2191E4F-1A11-4753-B3C2-A58E54EEC533}"/>
+    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{C4C23B66-4F1C-4602-A619-ED1BF4706CD9}"/>
+    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{7DEDD017-393F-406C-8FD1-39DF6133C5DB}"/>
+    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{883C8358-EC99-42C6-B580-B432CB65F615}"/>
+    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{155F21E8-56B2-4D9D-80C8-CC2F65839043}"/>
+    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{821852D8-2DA3-462A-BABF-662E3D3620C0}"/>
+    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{04449726-20FF-46AB-995A-B7D36B3BBB10}"/>
+    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{B5907017-B69B-44C9-873D-3A51F6925A27}"/>
+    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{23637A3C-D59F-46B5-81DC-BEA60D8457E8}"/>
+    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{CAA657A0-F672-4334-BE91-535C7F18C23B}"/>
+    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{BD258D34-15E0-4EAA-881E-FE00642547AA}"/>
+    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{D3E2EEF5-ACB7-425F-8D6E-3A4C1BEA8405}"/>
+    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{6323256C-DDA2-41B4-A9C2-C8778A21829C}"/>
+    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{8C6C9B15-ED78-4ED7-93FC-DC05FB2B5C7B}"/>
+    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{64B84355-0E37-48E1-9D03-55EFD8FE8B11}"/>
+    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{329FB948-8628-4DED-9609-EA6F912FC830}"/>
+    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{275DB4D9-643A-439D-B04B-9DBDEEFB4A98}"/>
+    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{D21CD718-984A-4361-BA33-9E931604C0E7}"/>
+    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{76ACF451-D40A-4DF2-82BB-CF42515F868A}"/>
+    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{19394227-A3C5-4267-B4C0-DDEBC00A31CA}"/>
+    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{F868940B-482A-4FAC-A186-BFA3418F2FBB}"/>
+    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{391199B2-1A64-4E26-A576-2167E1E33249}"/>
+    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{CB495B95-5E99-450C-A9E8-AD19BDAD19C2}"/>
+    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{0663F925-73C6-4D48-92BF-24BE17686382}"/>
+    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{1ED23733-D17E-4B2E-B3F0-565B42D781CF}"/>
+    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{A888D93F-4982-4DCE-9E05-39D48FCA3738}"/>
+    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{44037546-6411-4326-B3FA-F689E521B34F}"/>
+    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{FD6866F2-1135-4976-B421-AD2B8760AA52}"/>
+    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{4ED6E649-4D2F-4C21-9F57-6F012E49B475}"/>
+    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{0E078AD1-76FB-4B70-A697-BC541B21DEDB}"/>
+    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{E02FA272-5AAF-4C7B-B9B1-39134F4B11C5}"/>
+    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{C4B15CE6-8581-4FFC-8D0B-06665CABBC1E}"/>
+    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{85ED709E-0020-4A52-9783-807E904D20A5}"/>
+    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{1E56D71B-5AFF-4168-9AEC-9C9B47023FF7}"/>
+    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{3525940A-F842-42E8-9399-534406FF323F}"/>
+    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{F7DBE883-4656-4C37-AE0A-0061C1991A22}"/>
+    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{B6A14DDA-DF30-4B53-98EA-4C988BC396F8}"/>
+    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{2211A63F-1AC6-4335-AD24-72432A747822}"/>
+    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{8B837E8E-08EB-4C28-8A93-2B7612529DD3}"/>
+    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{7D47FADA-F89E-4AA9-931E-C441272809CD}"/>
+    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{EABC8328-DE41-435B-AB2C-EC86D9399EF3}"/>
+    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{6BA40A6B-93A6-4FFF-8ACF-7269F21F8F85}"/>
+    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{58AE4FA0-3DFF-4F2B-B505-07F3014EEA10}"/>
+    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{4A47EAC6-2E2B-4F2B-B1E9-31753EA05AFF}"/>
+    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{046014FD-7BB9-488C-B0E8-D726EDBE2116}"/>
+    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{D9759C50-E062-49D3-BFEB-2FF76C696214}"/>
+    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{56D0291C-851D-48C2-B815-3F6ABD4F09EB}"/>
+    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{5122B93F-6E38-47CB-9075-245D703BF923}"/>
+    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{0F594181-40D0-4E82-A900-850231FAB6DA}"/>
+    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{8D81E0A6-FDE8-406F-9F1D-E4059FFE2DD5}"/>
+    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{EF0BCDCB-7E2F-4C51-9B08-430C366C091A}"/>
+    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{8595B0D5-86EE-4108-8593-812E78065B79}"/>
+    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{1A85C3D9-1B24-4B7B-A54A-248A0DBDC51E}"/>
+    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{8748E4DB-3E89-40DB-9391-CBDD2509F05E}"/>
+    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{8FF14805-56F8-4DCC-B90A-FAADD4EC1407}"/>
+    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{C2A66417-1608-40A2-B382-B115ED41F2F8}"/>
+    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{4099FF37-2201-4D3C-B071-8B14ED69FE17}"/>
+    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{0FF7F67D-4642-40C5-A523-BBFC177C9008}"/>
+    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{8C25E0B8-7040-4E19-A536-9F5305DBCD14}"/>
+    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{63B5763F-5C15-4DB1-A223-DB15229E488E}"/>
+    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{D86002A0-F348-4F80-98A6-8FE32907EC2C}"/>
+    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{4EEC9EF5-B5E2-427F-B2E5-620FB08AD058}"/>
+    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{B7436E6F-DC1A-4A7F-946C-BD1080B744F6}"/>
+    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{9E4B05FC-D29B-48F1-8859-5738C14BDB42}"/>
+    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{54605508-50F9-4BC8-884C-53E0AB6016D1}"/>
+    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{03D61244-405D-4D0B-9154-D097AAD8B087}"/>
+    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{15F14318-00A7-4A03-9118-413394B5167C}"/>
+    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{99EB364E-ADA6-49DD-B914-781F74C5F57F}"/>
+    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{8C90ADB3-E9DF-48B2-B1B1-97F80F02A75B}"/>
+    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{054B8448-C877-44F8-A9A2-0A815DCC482E}"/>
+    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{6EBEB177-926D-46C1-9C9F-EB3291EE3AEA}"/>
+    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{BFC58DF1-6689-4630-BC08-A078CE56E124}"/>
+    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{AC7C1185-E5BC-4D93-8EF9-1F2925E48C48}"/>
+    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{5567119A-E077-4A4E-9AEC-997BD5568C28}"/>
+    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{E8ECACF5-4911-43EA-9DE1-E96FC245B72B}"/>
+    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{B3E88EB4-3D94-4512-9B04-9A0F0BD7C58A}"/>
+    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{CAD2E47D-F89E-47F6-B0AB-FDDA5A839D79}"/>
+    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{F489DECA-0D29-4AFC-8CE3-51C3BF7688EC}"/>
+    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{8D019035-C91C-457A-9625-573D5938CE26}"/>
+    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{94094934-251B-414C-BEF3-8E8D07A4E7FF}"/>
+    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{49604E2D-FAC0-47A3-871E-A49924D2CE05}"/>
+    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{1B63F4D6-CE64-4184-987A-7FC2AD65618E}"/>
+    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{E4189F91-1232-4FC1-9992-436E254DF83C}"/>
+    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{13EEFEFE-24DD-41B7-A0DE-783628A296D1}"/>
+    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{87873AC9-B061-4A4F-978C-0D58A1CFEB9D}"/>
+    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{B67B787D-8540-4EBE-A1A5-1CCFD4DE6465}"/>
+    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{FEEA914E-9EE4-4130-A01C-679E6339A023}"/>
+    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{7A52A957-4265-435F-9427-CE8EF33DF9C8}"/>
+    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{19B52048-2017-459C-AFFF-203025F38152}"/>
+    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{27A7FED8-6D4D-4099-8978-B92D5CCA6113}"/>
+    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{4A3B163A-FC8D-4C5D-B88B-DE0B7315DCD4}"/>
+    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{32E75DEB-6D8C-426D-BDFB-25851CF07FA2}"/>
+    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{ADFAA959-322E-4A99-B9EA-9E04A08A4F3C}"/>
+    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{4650FA9C-D7AE-44C6-9044-D3AE19305219}"/>
+    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{92197B6C-675D-4E04-A3F5-339C48405434}"/>
+    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{31DE1BAC-B5C4-40F1-9F56-A471401DD914}"/>
+    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{A0151880-F279-4002-B8D8-1E6910CCD8AF}"/>
+    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{AEE474F9-E589-4F30-B4BC-BE179B73FD29}"/>
+    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{483086EF-9726-403C-8211-F4BBC26682D4}"/>
+    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{B059BA46-5C43-47F6-A447-84CFA8EDE279}"/>
+    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{211940E0-E170-497E-BDB7-D7B781EC1EE3}"/>
+    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{45E00C45-2ECA-4E7C-A2B5-55D4C579825C}"/>
+    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{4E69BC43-D1D4-40C6-A6A4-931BBC63B542}"/>
+    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{1CC32C7E-CAFC-4E87-B831-8E28762A1824}"/>
+    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{BA285618-B686-4458-8324-EF153A867556}"/>
+    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{BBC3B632-2817-4F7E-9DE6-F1852B5520B0}"/>
+    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{4A424D2C-5725-4D55-8B54-6D9104EFA5C0}"/>
+    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{2A7675B7-6A4D-471F-AB97-31B4361B0D90}"/>
+    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{BDF446E2-714D-426E-990A-D64F9F24BB69}"/>
+    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{A57A55B0-9AAA-4B01-BAE4-7739F937D1D7}"/>
+    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{99C460D2-5954-4AAD-AE69-150DC823028D}"/>
+    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{B6ED3F31-31D7-4786-9361-8B1D0822CB2F}"/>
+    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{51A1E1EF-4975-48D6-9D76-0FADA00689F2}"/>
+    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{32B02B76-1A58-4137-8D2D-2E65225ABF9A}"/>
+    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{1D8E2B7A-F42B-40F5-A8B7-6FEAC1F11D5A}"/>
+    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{0586A4E6-86D4-455D-B35C-8C6A58A2BC67}"/>
+    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{B422320C-F521-4353-8348-83F9715BD263}"/>
+    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{6F2A8428-ED73-43F7-8042-EAF93CF6A325}"/>
+    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{041535B3-A21B-4FCC-ABDC-1FA57D56647F}"/>
+    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{62CB530E-D662-47B8-BE27-6B287551D8FB}"/>
+    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{DF2A61C5-D2B0-479C-8380-AF6571942BE9}"/>
+    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{C11767BB-D458-4578-91DA-B50E6B700D05}"/>
+    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{01ED1D66-91D3-4F49-9E59-FB54073BFABD}"/>
+    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{079B4C0A-C23A-492E-86E0-D207C628C8DE}"/>
+    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{41B64D02-996F-41F8-AA09-E2E4D13AF105}"/>
+    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{9D1BAAA7-13A0-44A4-B2B7-44EDB703492E}"/>
+    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{8AF2FF6F-C75B-4FC2-9104-B52931166A58}"/>
+    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{B0AB422E-2FEF-40B4-BFDF-DBADC522E233}"/>
+    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{E51A449F-5BC1-4E2E-83EA-F18CAF317960}"/>
+    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{D586E7AB-7E26-4F3C-9D60-542EC34F5F44}"/>
+    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{93A818AD-D529-451B-9AAF-531F6E061787}"/>
+    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{E04CB442-4E85-4427-AB5B-E74859C6EAA3}"/>
+    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{EC8A9FB3-2675-497B-92E6-FE5B360C4708}"/>
+    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{8C25D63B-B533-4457-90CB-0975145FD1EA}"/>
+    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{27AC27B0-135B-4C4B-AF9B-0814E0CB01D3}"/>
+    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{A6819083-67D0-486B-9F2A-41C0133BFA37}"/>
+    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{1B9800D6-8A1B-4903-990A-98272447B4C9}"/>
+    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{B703BAE0-055E-471A-BEC6-29274F7CFE2D}"/>
+    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{62B14E72-09D5-43A7-820E-73C7F8CC7790}"/>
+    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{C01CC112-5955-4708-8EB8-CA8D7F2F6703}"/>
+    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{0853358F-E56D-43F4-A657-4964DB6F42D7}"/>
+    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{722DB8B6-D8FA-4CDF-AD0C-4C3E832875E0}"/>
+    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{0F54D6A1-C863-4771-B712-51AFEBF6A95E}"/>
+    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{3D9695AB-278F-4376-9503-6964B14CFE0C}"/>
+    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{A19FBCAB-4D84-4A95-9B55-68BA8633C048}"/>
+    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{3EA67024-5F22-4E2C-8B29-F38C3ECE3279}"/>
+    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{E3BC5D11-A192-4F40-8928-2855362F4637}"/>
+    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{60DF38F6-1DF0-4D80-A049-75A28768EACB}"/>
+    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{3E82FA37-A151-411A-935A-8103CA4D0A50}"/>
+    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{86911393-A92D-44FA-AF27-920577EDF750}"/>
+    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{B143C701-4EBD-4079-9E1A-BAD67895F08B}"/>
+    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{52521F40-0571-4593-B97A-1E9F3DF5B718}"/>
+    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{E0535565-C87F-4E4E-9B44-CFFE792D6426}"/>
+    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{32E16D32-8251-4B5C-8BDF-8DD35D680BA1}"/>
+    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{D4AEEB79-05C4-4717-ADF8-1180315FDC00}"/>
+    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{CA4895A2-C346-4883-9F61-ECF972F7678A}"/>
+    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{212D4507-0898-4223-BD9C-C9AA61A8D9DA}"/>
+    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{620D70A2-FA18-4D94-ADAE-938901AF3FD0}"/>
+    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{3B254FA7-3BA0-45D8-9D56-62158AC2CA5F}"/>
+    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{27D22CC3-43E3-485A-B406-C911E2F3D627}"/>
+    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{1AD8F92C-4D67-4EA5-B434-A0B1CA9E9C11}"/>
+    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{7D3CBC9E-2594-4FEB-A369-1B07C2B57263}"/>
+    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{25C0F388-F21C-49F0-AFA8-3340A7BDB20F}"/>
+    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{875015BD-B5DE-4C05-A3E5-DF5AE61554A0}"/>
+    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{A908D1D1-35EA-4B5B-A284-7955BA675231}"/>
+    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{65FB2F20-B02F-4301-90B3-26D208E18C89}"/>
+    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{C3C9CF29-8583-4AEC-A76B-D442B2AEA855}"/>
+    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{4253EA51-02F1-4B3F-83DA-F149A8F28673}"/>
+    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{ECBA6FA9-E362-49D4-9F7D-1C2BCA13263A}"/>
+    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{9F920F2E-C549-43F1-BB34-C071F23EBEED}"/>
+    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{F57400A0-822C-4330-AB97-736B70276AAB}"/>
+    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{FB59C51D-2007-45AF-BEC9-FF84581C9B0A}"/>
+    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{2487BA6F-BDA2-476A-8F72-EEC5861C25A1}"/>
+    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{88DE7510-EE79-4883-9B57-A60608E3846D}"/>
+    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{F1530C07-55AE-48D1-81A4-76E8E3861F69}"/>
+    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{6A37FCCE-AA41-4460-8E11-DD57C4982273}"/>
+    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{5492A185-58DE-485D-85A2-19E5D0A381C0}"/>
+    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{A7DDACC1-0CF3-48E8-B5D9-FDCA8AD0AC2B}"/>
+    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{5DB199C3-AB14-402E-B732-B79CB0DA0B2C}"/>
+    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{3246CB4B-A154-4924-AECC-A408F024929C}"/>
+    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{42069288-6D6B-43CF-AA3D-9446FCC12D62}"/>
+    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{5B56A2A4-2C13-4B45-87CA-35841632BBAB}"/>
+    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{FE7CF59B-B561-4BE7-AD85-F53C3A2D9820}"/>
+    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{021E8F6D-DEF7-452B-9890-134097EF60FF}"/>
+    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{12D5F2A7-ABFD-4232-9A24-4A17645425E4}"/>
+    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{BBB6944E-2239-4A3F-9299-6CD2F123FBC9}"/>
+    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{A5903583-760D-48CB-A171-1F4A6839A66C}"/>
+    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{52DA4E98-4AA9-4316-9BD6-F1CF57E0B67D}"/>
+    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{80C7E91D-AC64-4E0F-B008-48CB010C04FD}"/>
+    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{2C2F6E98-F958-4B30-BEB5-D4210D17B22A}"/>
+    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{B61A32A3-FBB1-4593-9A11-5227561F56CB}"/>
+    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{624EA99F-A210-43F0-B615-BEE7A1C32F4D}"/>
+    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{E7044937-4A69-4E2D-9DB8-3D7EAF971716}"/>
+    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{ADFE69C3-A5CA-475E-8004-3EF9925202CB}"/>
+    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{D8FEDB20-9A03-4E31-A3E9-C00D68B79A27}"/>
+    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{CBBB545F-A043-4CE8-9F31-1BBC74EA8CAB}"/>
+    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{28F90954-561B-4408-A3EF-800D3B5857E5}"/>
+    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{585921D1-C708-493A-AAEE-49A351F361F6}"/>
+    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{6179EBA9-3EDE-4FE3-BB2F-A00021183E0C}"/>
+    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{8C55BBBC-545F-449F-9673-7112B49FF864}"/>
+    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{D29249C4-FDA0-4F70-BDD0-6EE37C489D7F}"/>
+    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{47BFCC3D-8A6B-4F42-AE56-9369D9E8F836}"/>
+    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{E274D884-8759-49F6-9440-1AD310A927EE}"/>
+    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{AC61E306-7C16-42EC-AF12-DE699B54BFB8}"/>
+    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{ECB1DA03-8AE5-4F6D-ADDA-C10307C4F47E}"/>
+    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{387658DE-4F40-41B0-80D6-F754568D1791}"/>
+    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{E84C7C2C-8C55-41D3-95E0-AC1F83B852DF}"/>
+    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{639AB87F-D9D2-4637-8C9E-A069DBBD695B}"/>
+    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{5C305875-A943-4F19-9405-7718EB662061}"/>
+    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{5DD7ECEF-FB97-4C9F-AF50-7A1323EC276F}"/>
+    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{9333043C-4156-48C1-B297-82D374068180}"/>
+    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{7278E213-D8C3-451A-B51B-6A4FA7BDCD4C}"/>
+    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{4CABE99C-F341-4879-B8CE-5A5FFC98E469}"/>
+    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{912440B8-5E53-4946-96E0-3D87704974A1}"/>
+    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{573AEDF3-B3FC-42B1-B049-F08BA43A50AD}"/>
+    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{CE4CDA45-81B1-4A64-9C6B-62C197C382BF}"/>
+    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{227A07F6-97DA-4E9D-B30E-37EE120987C9}"/>
+    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{ED92D904-F5F8-404C-B105-DEE0663E3E26}"/>
+    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{818909A9-7CD4-4015-91CD-7628B39F49A5}"/>
+    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{B04550D4-D286-4DA9-8454-96CB91A36FCD}"/>
+    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{C4F6D189-D929-4180-8B15-4DFEB4CAB320}"/>
+    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{FCCBA214-A734-467E-8CBE-60E32B80B4B8}"/>
+    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{931AC6DC-57BD-4B20-9711-AA9DB48D87E9}"/>
+    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{83A26C77-DF09-4672-A790-54676A72DFDC}"/>
+    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{DB6695FB-A835-4544-ACCF-A936F13A8648}"/>
+    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{674B0365-09D3-4981-B9EE-E3DD52CF564D}"/>
+    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{3D3D6B16-83A8-4C8B-A8DF-3A4E50E99619}"/>
+    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{737F54D5-8686-4B3B-BD83-14C06900E651}"/>
+    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{5BFBF27B-6298-4889-BC7B-22C23751E24F}"/>
+    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{D6D1AE55-D0C7-4E1A-ADDE-521F434D9214}"/>
+    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{C63F0A97-AADD-4310-A1F0-282AA8BEC7D7}"/>
+    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{FA56886B-87AE-43D2-AB4A-CB8460BB7451}"/>
+    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{924F7CD9-2ECA-4B49-A711-FC66C8C1965E}"/>
+    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{C1F40298-92C2-4933-B455-9D6A22EE77DF}"/>
+    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{1E75D653-FD1F-4D37-AB6E-CFD5FE79769E}"/>
+    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{E9747E9A-0A84-49DA-92F0-4F5A5E674D63}"/>
+    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{1AB9A3E2-94C2-4783-8A33-787AA3126A2D}"/>
+    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{FD28EDFF-7CEB-4248-9CD8-AAD2D294DFB1}"/>
+    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{D152A766-C52A-4519-87E2-02B4DDC108D5}"/>
+    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{FA4B2816-3D2E-44F8-ACDE-E75E6BF30963}"/>
+    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{7C775A24-5BEF-4AA7-B13F-D1E818B3FFBB}"/>
+    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{2188B3B2-DA8C-499A-ACEB-F870B18D9A08}"/>
+    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{EA3437F0-E44D-4711-860B-2899D81258AE}"/>
+    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{CF44F98D-956B-46F2-B6BC-41B22B293C69}"/>
+    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{ABDC83D6-CB87-44DF-B6A8-7E1E853D6E0C}"/>
+    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{3CB4E8AE-2528-4064-83A4-8405CA3749A8}"/>
+    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{E02DF7D0-CC9B-40F9-9921-406A5B5BEA45}"/>
+    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{C74536F0-02C5-47F2-B8F4-0640FE1EF957}"/>
+    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{BA36770A-2113-44EF-B1E3-2B04D92DD72C}"/>
+    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{3B7F2884-C1A9-41CE-9586-D02C6EDABE24}"/>
+    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{90CB44D1-2C10-4234-9323-84A2DB665A49}"/>
+    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{D3828AE2-705C-4B35-85F7-5011AA72A44A}"/>
+    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{6EBAF0AA-2447-4045-AF44-02325238BED2}"/>
+    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{F640494C-A14B-499B-93AD-3ACBA113D9A6}"/>
+    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{501428FA-056E-424C-9540-B951DC7690CC}"/>
+    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{B02846E2-950E-40EF-A81A-538C0AD6C996}"/>
+    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{448EB6BE-A235-41E1-8D8F-D3FD7027C41E}"/>
+    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{BF6AE9CA-33C2-4100-9FED-3136914D80B8}"/>
+    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{5B1A3410-695E-410E-BAF4-C9BB71209F5C}"/>
+    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{6DAC62BB-ACB9-4598-8396-EEDA6447E044}"/>
+    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{64476EEA-1B1B-4CEE-9A08-7A5D932CC12A}"/>
+    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{278DB2B4-0414-4E4A-B1FF-E09AA1B65E99}"/>
+    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{D9147CCE-1BAA-4263-856E-794BFC7E0894}"/>
+    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{9C4BC943-2BC9-41EB-BB1A-9F243A007BAE}"/>
+    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{2555129C-D282-41C2-99FD-0491FF40EC0C}"/>
+    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{25F71BC6-3F59-40E7-A654-82917A5A0F54}"/>
+    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{A8FDE8F8-7DEB-456E-A6D0-9BFBB99427EC}"/>
+    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{B189A43A-06C7-49D1-8E62-DE1203820E0C}"/>
+    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{1EC6DA7B-3EE5-43CE-9BE9-C7673E483E85}"/>
+    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{78B636EA-C053-4AF0-9DEE-92A8CB9C1C99}"/>
+    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{7269390A-4223-4A20-B055-A2A10217E398}"/>
+    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{18584C2C-984A-46D6-B04B-48443C56519B}"/>
+    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{FA8DD4FF-D882-4024-82AB-368DEDC54909}"/>
+    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{9E3B2EC8-8427-41FD-969E-D842ECC47682}"/>
+    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{A79B3EC8-85DB-4312-9DD1-5084EB1C54F1}"/>
+    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{F9C7EFF4-E190-4632-AED8-294E1E9180B3}"/>
+    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{4A092EB7-D42B-4F12-9261-E0833E4153C9}"/>
+    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{30017B99-6991-4983-B7C4-AEED98BF3F41}"/>
+    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{EDEA093C-9022-4D60-94F8-E91C759B5503}"/>
+    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{CF0337CE-F729-4F54-AE1B-504557A50737}"/>
+    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{B188AFDE-776F-4AEE-9168-4BB4D77C80F4}"/>
+    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{971D08DF-93CD-4428-9C88-4745A7CD857B}"/>
+    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{8D3D7F40-975D-47E9-B3BF-F8C00FA6CCE3}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>

<commit_message>
Organização do fluxo em cada arquivo
</commit_message>
<xml_diff>
--- a/src/data/uploads/Project Room (Jira).xlsx
+++ b/src/data/uploads/Project Room (Jira).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/paulo_vieira_d_silva_accenture_com/Documents/Desktop/Automação_v3/src/data/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35D7498F-00B4-4AFF-A755-8A9E1A83145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4562BDD-B630-4156-87DA-FC07F9C2F6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D86CF08D-308C-4181-A076-5BE61EE2D276}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1437ABEB-B5A6-45DF-AB5E-011A69CEC4B7}"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -10620,7 +10620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DD4AC3-1407-4A9D-B827-6B3E926823BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E8A357-6941-4DEB-87E8-D529A7C60D0A}">
   <dimension ref="A1:AR578"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -66555,583 +66555,583 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{607C29CE-E9F4-4CCD-835E-5BE20AC7D9F3}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{871B9EEB-24C6-401A-88C0-CF2A9E206629}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{36F09244-E924-4C78-AA59-00A74B3E5FFF}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{DCD876EA-524D-4B68-B2A4-1A1CCAAC9096}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{5498BA67-039A-4889-8850-4BACDC8F1B73}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{726854FA-18E7-4147-9C53-2E45F8FA7495}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{367B6E8D-7429-4758-A8F1-AAD8FB2E612D}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{8EF5704C-54B7-4772-AC02-F159CC6B490E}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{88376681-0359-427F-9175-0EF1A31BFF93}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{8A71ECE2-2D95-4A3F-8321-E17E63F0732C}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{4C4D17BE-183A-4122-8B96-0BFF693BF704}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{72BFFB95-BEFF-4620-A08B-93DDE781C5E3}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{2A7EF8E0-F866-4832-A586-7A48BCB7B1D0}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{DB7DBA79-EAFE-4536-AE65-422E9FE6C3D7}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{A983A882-58DE-4DD7-9C1F-5D0A6ABA8EBD}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{57488062-D20F-4313-B56B-9CF730EF94A2}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{43B73458-0D38-4148-9674-846FA63B7F22}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{BD36FC53-F6CF-4905-AA3B-149D223E4F94}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{C26A6990-3D43-4AF8-8767-7CC0E39D3308}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{85D8CFC3-5042-4509-B500-76539B3ED081}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{A0672BE8-D916-41A0-8C12-20CB9D7E6EF2}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{20A99CC8-F07E-415D-933C-AFE6DF2DE488}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{6F086F1D-7FC6-4A17-BC45-EED89B7ADA34}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{3A07C26A-AE7F-4DEF-B457-40DA777CA5FC}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{757B3162-DA54-4CB9-B48C-916928073974}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{9B4C52A8-E587-44A0-8F32-FB5C5B1755AA}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{AA25B19D-9BB1-4196-95EF-935FA56FED97}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{95B73DA4-8E06-41EC-8006-6167F3CA16E6}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{AB88DF3E-DC94-447C-BEC4-EE91579E7DC3}"/>
-    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{26608C87-730F-4966-BC56-4304A656470A}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{BC2C06AB-91E8-4B80-95B0-980D25E535AD}"/>
-    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{D97ADC65-2922-4A58-A75F-B11B4C4F643E}"/>
-    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{30D81CE2-79DD-44D0-AA70-8A780736DD5E}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{93CBF7B8-2154-4FA4-8019-405349F79C4F}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{49980EF7-0659-4E0D-B609-336B30AA5824}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{2EE85581-E5D2-4F9C-9739-491FCDE15B33}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{DCF5A562-78AE-49B6-95F1-1DE7C5ABA207}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{95BA672E-F903-4982-9EFC-7DB54CD9081D}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{ECEAA6EE-D9F6-4C66-87C7-CDC24BFE981B}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{6A60724E-634B-4AD9-8242-71495D9FE323}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{2DA93540-14AA-4A6B-8248-13A6A2357EF8}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{EB34F336-AF56-4AD5-B0C9-2C972F6D14A5}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{61651658-67FA-449F-9E53-590FD8F2E4E1}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{90ADA6C3-B318-4965-8539-ED184D1DB8D8}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{324D25C2-E262-4683-ABF9-01157E9485C1}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{00117C73-1E2B-4647-A895-A40126B6192B}"/>
-    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{43173E90-A69B-4C31-9684-6DF960D0F639}"/>
-    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{4674D5C9-53EC-4C93-B8CB-5026538C7F54}"/>
-    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{C9DD63B1-7154-4B5C-AC9C-207A13373F98}"/>
-    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{D46FDA2C-F7DF-4804-BA77-B60CB4259641}"/>
-    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{3F4AEF15-F8D1-4D40-920F-881F9567586E}"/>
-    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{A1373178-F6F5-420F-AD22-056F2F5D5DF2}"/>
-    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{27084C35-F17E-40FD-B9BA-289A73EA32AC}"/>
-    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{96874A00-3B84-4659-B8A8-C515ADB64BA1}"/>
-    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{53F6D2E1-3333-46A9-AA87-7F86A329904B}"/>
-    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{DD50C04D-8547-4490-AB20-8B9A947278EF}"/>
-    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{9B94D61A-D961-45E8-B4B8-5080C292ECCF}"/>
-    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{B6F7E739-4C85-436A-979D-5F2728D07FFB}"/>
-    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{A3DEBA16-2E70-4C0E-9EF4-F0CEC99CC3F1}"/>
-    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{1936F794-9061-4CDB-B638-11B5618F7D81}"/>
-    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{5183FE9E-BB12-4B1A-AC2E-6E580C04A493}"/>
-    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{028982F4-15B2-44A7-9AA3-4AB7734FDA15}"/>
-    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{6323C26A-EB38-406D-BE04-F756E088B1BF}"/>
-    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{AC098FED-04C4-42BC-ABCB-D457164EE689}"/>
-    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{A8A5FE7D-34FA-42BF-9882-88949A1A9544}"/>
-    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{BDB17BC1-C57C-4700-B502-C95098A8FBBB}"/>
-    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{A4F4059A-EF7D-40BC-A30E-E25CC04AE258}"/>
-    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{7A1A2EC1-5A29-4328-B970-3C97D6BAA0C1}"/>
-    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{92B2BCB1-A8C0-42B8-A783-533092D8E503}"/>
-    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{8A337F14-B85A-44E4-BF0F-C3309A783439}"/>
-    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{2AFB338E-EAE8-4AD3-AA4F-99BC6435218A}"/>
-    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{99465418-ED04-4ECB-AF2E-02F689DE2D50}"/>
-    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{17641447-5A3C-438D-B080-2AB55229F0E4}"/>
-    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{8CF7BD64-C1E0-44D1-BE7B-0350E4DD2BF7}"/>
-    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{FCC617A6-BF7B-4FD0-B874-0AA99392EDEA}"/>
-    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{BFC32FEB-15D6-4504-8064-B1318A2F48F0}"/>
-    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{60D2C900-F251-4110-A98F-8468850AAC16}"/>
-    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{6C634DF9-AA35-429F-B4E6-FB4484435FA9}"/>
-    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{DBCD5E3B-5123-48FA-BD18-6A419B09EDDA}"/>
-    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{02127F0E-CBAE-4CC3-8C78-53C977A59A9E}"/>
-    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{AD5B3C16-1007-4340-8A94-50C8BB753D57}"/>
-    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{0C3241E3-CE7D-4987-AC9E-D9A57D07FD28}"/>
-    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{E3E50475-670F-4382-8460-414C655A29B9}"/>
-    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{43F5977E-351A-40C5-99B4-005A2B841C74}"/>
-    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{FBD900A6-EDA2-4B61-95B0-4E0C6C48D83B}"/>
-    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{ECDF43A0-046E-4FF1-982A-031EB35D7C9A}"/>
-    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{AEF8E254-9312-4309-BABC-531DA3EBD8DC}"/>
-    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{EBB48E2F-A06B-4C88-8031-D44E0C9E324B}"/>
-    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{9BD6C7A0-261B-4275-A644-F9EF164C8CCF}"/>
-    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{ADBE4DEE-1270-4E29-860A-A55C77480D3C}"/>
-    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{ED309B16-6795-45CE-A69F-CAE94BCC4B93}"/>
-    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{834DEBDC-EE20-45FB-A35B-2062AF4FA3C1}"/>
-    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{8F3CB043-BEF4-4650-BE44-C062122B54FD}"/>
-    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{8C5F1D32-41D8-4FDF-B72C-3013F921DEA7}"/>
-    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{2B073142-4FA5-48C2-978A-6FC456BD76BA}"/>
-    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{06C8367E-2076-4E90-9975-214E9A0064E6}"/>
-    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{3CB962D6-46A8-47BB-9AFD-BA5021E73A6C}"/>
-    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{D340C9F9-4E14-4C71-AFE4-7209E6C51FD0}"/>
-    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{34C1D6C4-CD0F-4D0B-8113-8DBEB7664815}"/>
-    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{FA0DB86D-4A4F-4A05-9580-7A7BFC94C295}"/>
-    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{33A168C9-4D00-4B14-9567-3DED0E11D241}"/>
-    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{03D5CB61-838E-4862-9C32-D416DA9392E5}"/>
-    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{559BAD0A-CEB7-496A-8C7D-9D0A9D520DD9}"/>
-    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{24FB2135-08B2-4D79-B2FD-6AB5DB770B88}"/>
-    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{584BECAF-FD15-453E-88EF-8DEEB3AEA2E7}"/>
-    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{6910D0BD-E79F-4F00-B46C-FFC7ED40DD84}"/>
-    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{B4347BEA-BE8F-461E-88D0-8BE7085A9738}"/>
-    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{1B52F2D6-B69E-47B6-B687-8DA9560054CE}"/>
-    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{92BDE90E-33DC-49BE-BBFE-1C26E998F62B}"/>
-    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{FA541893-4A7E-4957-B518-62F4E834DBB5}"/>
-    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{2F1F8F46-4ADF-44A1-8570-30FD0CB13802}"/>
-    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{A16810FC-67D5-44B2-B1F7-410ECCD4F76A}"/>
-    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{F9213C01-93FB-4927-B502-9C6086E7B8B1}"/>
-    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{39DEB097-2540-4A62-A12A-5B6DB658D509}"/>
-    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{16398A2A-FE94-4D54-A6E8-B3C08F84F8A3}"/>
-    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{7C6424F8-6B88-4E53-AF10-5E716B1C81A9}"/>
-    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{B1BF3172-B07C-4897-8996-8CB4A97FCED7}"/>
-    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{4A9F2EA5-891F-494D-90A6-E68372A0FC34}"/>
-    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{406B8481-1F7B-4EEA-A236-949A70DAACE7}"/>
-    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{ED2D0080-AA29-47CB-AF02-D0C9D56DCA92}"/>
-    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{7D1EACF2-333F-496F-AD1B-D9548E2EB25F}"/>
-    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{E79675FB-5088-4916-97F0-0FE8167A4998}"/>
-    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{643C4353-99A2-4F28-A918-B97F452B1554}"/>
-    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{8052DE3F-F2AF-4AD0-8984-FB24A6201B45}"/>
-    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{4D8F579C-2AE8-4CA2-8934-29864CC063ED}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{74DEB9A4-F292-4EE8-BF1E-49903144604E}"/>
-    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{E84D81C0-2C90-4D70-919F-842A1F7862AC}"/>
-    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{7AD9A020-6AFB-4264-AFCB-4A681E0E1CFE}"/>
-    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{FA806C79-728C-48D0-905B-02AE64256171}"/>
-    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{4EB71E5B-6273-402A-9643-E67F52C7AE5B}"/>
-    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{BCB7A418-645E-44B3-8A3B-778C1441CBDA}"/>
-    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{989ED701-0A3E-4B3E-9926-2F5A5FEA8DC3}"/>
-    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{75DBB2E8-4E9A-474E-9364-FD4B2B549389}"/>
-    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{3BD58C85-E48B-4BA1-AFDF-5D94A689B1CB}"/>
-    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{B4E96BAE-0AF4-46CB-AB48-B12E9C4892F7}"/>
-    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{9E7A05E1-32FC-464D-9A5C-A0B3270261C8}"/>
-    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{0A5135A0-E803-43D3-B034-3D01056E405D}"/>
-    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{D0F8944C-4C99-4E4E-85C3-79935B437D03}"/>
-    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{0D7D4586-BD6E-4A3B-A383-420AF2E62FCD}"/>
-    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{EA4501E9-31A2-4C39-ABBB-21755DAF7464}"/>
-    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{8B5B5809-8E77-47C9-9879-F7BA08525ED3}"/>
-    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{B3026CBA-F6DB-48E7-9D8A-D41B44DAE7A1}"/>
-    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{0EC5B124-06D8-4ECA-9C53-7C3C5634BD81}"/>
-    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{5DF6F338-E5B0-4E60-AE6E-E992CDB28587}"/>
-    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{F9DB9265-DA90-4B5E-8E62-1643E205D06E}"/>
-    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{FB7C1479-2D4B-4BCB-A4AB-0B8EE00AB315}"/>
-    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{4F0A0E12-8CD1-4BCD-8EF7-76070F638F84}"/>
-    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{C580AD03-78F7-4593-8606-067B65101DEA}"/>
-    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{443896B4-4692-436F-8FCB-ECEAD8CBBBDA}"/>
-    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{212DD8CE-9DF5-4F2C-A268-7C6FDCB90EAE}"/>
-    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{6F04A92C-B770-48D3-A7E8-A2C4D399FA21}"/>
-    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{86FF58E2-D5CF-4CB6-9EB5-66778CED2DD7}"/>
-    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{2573816F-BAF2-453D-9527-D6E43AE6F6E2}"/>
-    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{91BFE5BE-9BF8-4C7D-92EC-A32EFF6FC458}"/>
-    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{8B2DD693-D921-4FAB-84C7-530CDDDDBAF9}"/>
-    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{75FD391C-F363-464F-ACDB-85685F568914}"/>
-    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{F4AA5118-BDA1-4B8F-B867-36C535FCD69E}"/>
-    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{9502288B-E2F5-475B-A8C9-1B6523667E66}"/>
-    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{DB799140-05FA-44A0-8D14-36CDEB4EA012}"/>
-    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{011C0A03-9D7E-4FE2-9744-7C8CED886B77}"/>
-    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{927A5F8F-15FD-4734-82DD-4104B19D3C6D}"/>
-    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{8A00DC25-9438-4332-8CD7-A57F20F9C12F}"/>
-    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{8433D298-6AA6-4FF6-B7E5-499445A05945}"/>
-    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{F1DD17CB-FF2B-4D22-9A68-B42D25A18FF7}"/>
-    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{70BC8DD8-C4F5-4E9F-9BAF-54C7091A0424}"/>
-    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{E22D7541-4E56-43B9-8376-F28C86A9816E}"/>
-    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{595D21BC-47FF-478B-9BDF-3F49DD43A176}"/>
-    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{B4583BCD-2656-4C4F-AB0E-403AFA3AFD2B}"/>
-    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{9FD3C1DA-D67D-468D-A192-3154193B9A97}"/>
-    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{0E20E3DD-5DF1-46C8-BCD8-CF604AF6BFB0}"/>
-    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{9907C8F4-B39B-4FEC-91F8-0F1559E5632D}"/>
-    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{E614A78B-C79A-463A-A903-5F512E674D58}"/>
-    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{C61B979B-459E-46BF-A471-8F3EBF3D7121}"/>
-    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{AD4F949C-FA62-46D6-B5D9-55C5288BCEE7}"/>
-    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{C6845E13-1CC4-41C8-A0B0-BE1082B998BC}"/>
-    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{B314A602-3C93-4C1E-B0C9-5221F6B8DD07}"/>
-    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{A36EFBAE-AA69-454C-AD3E-B91E1A8F0819}"/>
-    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{BD37666E-4B3B-4A70-BB15-3E878CC6E317}"/>
-    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{BBCB7DA3-7E8A-4066-A9F8-059216439BF8}"/>
-    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{3B7EC163-DA9D-4823-AF84-2FFB86E20E45}"/>
-    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{E8019D7F-73FB-4EE4-8D5D-995152507ED0}"/>
-    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{F1FB5BBA-829B-4A5A-A973-00A60F0109E2}"/>
-    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{182F83F8-EF60-4219-A8E1-F224E4FA507A}"/>
-    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{90A2F766-0C09-4D6E-A4EC-ADCFF6F1D905}"/>
-    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{43335C38-DD36-4908-8CF8-DC0F3E4492FF}"/>
-    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{0B364548-FB26-4530-9E73-B7AE2BDF5263}"/>
-    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{9004049E-0F58-4BDF-A251-5E62B522FC32}"/>
-    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{220632DD-C6ED-4AC4-9731-26A7146BB355}"/>
-    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{F7BB31BD-217E-488E-B085-58D10B2479BB}"/>
-    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{91B279FD-BDDE-4264-968E-36537A8AF68B}"/>
-    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{3310B6CA-3310-4811-B5EB-2FA121840093}"/>
-    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{38280B30-8253-4F61-A4F2-5FAB29ECA067}"/>
-    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{1D24FDE6-2B80-437A-81F5-ED09EB4F176E}"/>
-    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{BAA7DC0C-51A3-4002-9423-7EEE7E665499}"/>
-    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{3A507B0E-A912-4292-8A76-DFD68CFFC7B7}"/>
-    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{24B358E7-23C3-4F29-8B9C-22E3F99BC126}"/>
-    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{B1A37CB6-EFA1-44E6-83E5-4A736518E282}"/>
-    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{454FCE36-36A6-4DEF-A8B8-6201959CD63A}"/>
-    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{93CC2747-9AEC-43D3-A954-B6A2E6697A00}"/>
-    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{4B322F6E-180B-48CF-A1C3-08D10338EEF7}"/>
-    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{D3BC4482-0C23-4E3B-AB46-604A2EB50228}"/>
-    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{5D021203-A0F3-4DFB-AC81-2214BB5D2530}"/>
-    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{974108C9-D37F-4A4C-9283-BF6C9ACEEFE3}"/>
-    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{2E0DB8D4-A830-4116-9B00-2C98CD62EA3C}"/>
-    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{410BC95C-8089-4342-8DD0-5F4BE65132BE}"/>
-    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{5D56B5C4-F9C0-403A-B362-21BB3E8E0405}"/>
-    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{0C0DA31A-67C9-487E-8E97-D8B061DE9F4B}"/>
-    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{CA53DC7A-9503-4425-9B71-3AED0C414924}"/>
-    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{BA2B50C5-375B-4F7B-93CF-702C97608792}"/>
-    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{9B95DEB1-552E-4514-BA3F-9E24FE88E6D7}"/>
-    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{58C341CD-D0BE-439B-96E6-D6FCD94218DB}"/>
-    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{DEFDF0DD-67D9-4635-B47A-9A23986A09F8}"/>
-    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{A13AC12C-FA8C-4D6B-9A89-1909389EAA5E}"/>
-    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{EE7D89AE-113C-4824-8DD5-70F21860F65E}"/>
-    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{2B0EF8C8-6FFF-4B82-BB4D-3B75396BDA30}"/>
-    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{C8CD039C-5314-47E1-88D9-B1D35103ACA5}"/>
-    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{9EA93E5B-E504-4DC0-8E78-8A09503C702B}"/>
-    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{33B60823-04DF-4C5E-A7DF-0D953B8A9CB3}"/>
-    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{CBB98267-6F23-4CB6-9FA2-6C3BCE9822E0}"/>
-    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{BAE0DE9E-7A97-409B-9D66-D8BE2C6F2389}"/>
-    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{A4BAF6C2-4B31-42C9-9898-45861FB1C5E0}"/>
-    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{10003DFC-7C69-4E2C-9902-5960BB0E09A6}"/>
-    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{C8AD304C-8F57-4AF6-BCA4-9086F3997813}"/>
-    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{B58A2255-6AD4-41F5-A861-FA393AF57FE9}"/>
-    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{8DCA1266-CF4C-4C09-8674-81D43D67C92D}"/>
-    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{4A6F7505-363D-42F4-AC4A-12F82EE60469}"/>
-    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{F3DADA8C-C77F-47DD-A5A6-E53EB16B7388}"/>
-    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{2B9BF3AF-5CAA-4C1D-8C86-8E29733E02C3}"/>
-    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{BB99D000-1BE3-4361-94AB-81256E4BF975}"/>
-    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{9CBCA594-E362-46FE-AA0F-6E2726BCBB4B}"/>
-    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{AD64145F-012A-4B04-B848-1510482EE9A1}"/>
-    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{E39F7CE7-4D07-4110-ABEF-DAE35307C19A}"/>
-    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{D8CFF5F9-9A9A-4CA5-BAD4-580EE62263C1}"/>
-    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{25E50A16-7E86-4671-B48C-EDDCE33CD2DB}"/>
-    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{148187A0-C70D-469A-8D2C-E56E907857D1}"/>
-    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{9390AB3D-D0F6-4A0F-8A0D-1E3C38EA6D41}"/>
-    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{AAA02738-CD0A-4ACA-8457-CBE3EFB9FA41}"/>
-    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{36B108E5-B972-46AA-AE1B-FEDA2C122947}"/>
-    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{1F1AA886-008B-4F67-9FFE-4D27E9DC30C4}"/>
-    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{D712740C-C273-4145-83D7-2D1E5A290453}"/>
-    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{6AD00DF7-D7EA-43E5-8A07-7C6A7754D786}"/>
-    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{4351D038-4A34-4FE3-8B4A-F3DAEB91083C}"/>
-    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{261EC49C-CE5D-4056-9927-2BF4A1BF6CFE}"/>
-    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{553285F8-1E72-4948-8FDE-E563721B87CB}"/>
-    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{269B5443-AE8D-479D-AFCF-2FB3E070B2F7}"/>
-    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{CDD21742-008C-4025-B23B-3D1128F86293}"/>
-    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{37C98EE0-4039-4566-9CBC-FE3FFC044180}"/>
-    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{CBB12B32-02C8-4663-A170-8BDD0F172349}"/>
-    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{60227C94-54D0-4827-84F4-E7DA85CC388B}"/>
-    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{574B3641-82B7-4C58-92E3-663A8F1BBC93}"/>
-    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{8BBCC4CA-19AC-4062-BA2F-9F27B308107A}"/>
-    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{E364404E-B7D2-4F19-A4C6-1A558F15408F}"/>
-    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{6B2B455A-F748-4FF8-9AC8-A80E43F124F4}"/>
-    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{008DCB75-F8B9-4F07-9F83-0E55FEA035CA}"/>
-    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{24582549-2163-4EFA-AAC4-85A14D90F98C}"/>
-    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{2349A5B9-279B-4277-9164-72F6765926AD}"/>
-    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{C966B172-ED0B-4FCA-89CD-4B49C84F550E}"/>
-    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{BC846F19-D3F1-4CC8-8492-083A0918C67B}"/>
-    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{6CBF768E-7A2F-4837-9B0D-9893ECAA6BBD}"/>
-    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{B31D0FE8-0A0B-4B4B-B2F8-5FD770EE5BE2}"/>
-    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{B739EE22-3498-4A24-B73F-592BB81A81FC}"/>
-    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{D45788F9-370F-4F5E-AF55-8A5403D560B8}"/>
-    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{7F114330-7278-44C0-9C65-6B5102CB03B5}"/>
-    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{4B980AA7-1BF5-4F74-88AA-25351DD5AB9C}"/>
-    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{2C819BC8-83EE-48C3-B4DF-7E962F9127AF}"/>
-    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{70D12C7E-6A75-4793-96F6-6133834C7539}"/>
-    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{918E1CBE-5D64-4016-AF0C-4165530A7C50}"/>
-    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{07C962B3-4D44-4976-884C-B74D53DB173A}"/>
-    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{1CDF140A-D6DB-4309-A72D-0E2875488C19}"/>
-    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{CD4D4D5A-0F79-4D26-819D-A13DEA9E4726}"/>
-    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{53B23B46-CAD9-4BA0-B131-C856A916A2E4}"/>
-    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{84AB11CC-B684-444D-B265-4FC12BE8C43E}"/>
-    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{1F361570-4E22-4C94-AB8A-216167203CFD}"/>
-    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{F6D6A0AA-69F4-4883-BB10-A1BDA289CC3B}"/>
-    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{E99E0C15-FC1C-459F-81A1-01C156AAE1BD}"/>
-    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{3D34879F-DF7E-4556-8A7C-993519EF82FD}"/>
-    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{C4FBFD5C-6F95-4532-83D2-7758DC6FC924}"/>
-    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{DB0FDFAC-66B3-4762-9A3C-F30AD0F21C32}"/>
-    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{E02C9AE6-D9D3-433C-90A9-C5ED34747D20}"/>
-    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{328F2367-F272-4B88-AFEF-D64664C10196}"/>
-    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{AB02AE2D-BEF9-4C72-AD41-C1555777873A}"/>
-    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{5F1FF03F-1933-4410-92BA-5782A3EE5F0D}"/>
-    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{64529711-8017-4DD8-9074-F31597E33139}"/>
-    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{5EBFEE3C-497F-44D4-89D2-80F7A7737E90}"/>
-    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{DF5C359F-E0D0-48E5-9DE5-6E74B2C568A2}"/>
-    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{D079FCC7-57B1-4AA0-8826-4FBD10134D50}"/>
-    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{F32329F1-D4B8-4EAD-A842-FE60C5AC446B}"/>
-    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{119E811E-27DD-4A8C-A972-D3BEBF5A0125}"/>
-    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{F0DEFF4F-002A-40AE-8899-F0C390C1FA7A}"/>
-    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{6F8113BE-64AA-40F5-9435-B302439A2524}"/>
-    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{132AAAE2-E26F-4A2E-A9E3-DB158E86807F}"/>
-    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{33DD63B0-97F8-4772-8D0E-281F86188FDA}"/>
-    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{14DFEE7D-05A6-40DB-A70C-48954177FF19}"/>
-    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{D0196A15-55BE-4109-B4B2-89C0D7CF2356}"/>
-    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{D2191E4F-1A11-4753-B3C2-A58E54EEC533}"/>
-    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{C4C23B66-4F1C-4602-A619-ED1BF4706CD9}"/>
-    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{7DEDD017-393F-406C-8FD1-39DF6133C5DB}"/>
-    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{883C8358-EC99-42C6-B580-B432CB65F615}"/>
-    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{155F21E8-56B2-4D9D-80C8-CC2F65839043}"/>
-    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{821852D8-2DA3-462A-BABF-662E3D3620C0}"/>
-    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{04449726-20FF-46AB-995A-B7D36B3BBB10}"/>
-    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{B5907017-B69B-44C9-873D-3A51F6925A27}"/>
-    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{23637A3C-D59F-46B5-81DC-BEA60D8457E8}"/>
-    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{CAA657A0-F672-4334-BE91-535C7F18C23B}"/>
-    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{BD258D34-15E0-4EAA-881E-FE00642547AA}"/>
-    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{D3E2EEF5-ACB7-425F-8D6E-3A4C1BEA8405}"/>
-    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{6323256C-DDA2-41B4-A9C2-C8778A21829C}"/>
-    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{8C6C9B15-ED78-4ED7-93FC-DC05FB2B5C7B}"/>
-    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{64B84355-0E37-48E1-9D03-55EFD8FE8B11}"/>
-    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{329FB948-8628-4DED-9609-EA6F912FC830}"/>
-    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{275DB4D9-643A-439D-B04B-9DBDEEFB4A98}"/>
-    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{D21CD718-984A-4361-BA33-9E931604C0E7}"/>
-    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{76ACF451-D40A-4DF2-82BB-CF42515F868A}"/>
-    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{19394227-A3C5-4267-B4C0-DDEBC00A31CA}"/>
-    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{F868940B-482A-4FAC-A186-BFA3418F2FBB}"/>
-    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{391199B2-1A64-4E26-A576-2167E1E33249}"/>
-    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{CB495B95-5E99-450C-A9E8-AD19BDAD19C2}"/>
-    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{0663F925-73C6-4D48-92BF-24BE17686382}"/>
-    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{1ED23733-D17E-4B2E-B3F0-565B42D781CF}"/>
-    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{A888D93F-4982-4DCE-9E05-39D48FCA3738}"/>
-    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{44037546-6411-4326-B3FA-F689E521B34F}"/>
-    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{FD6866F2-1135-4976-B421-AD2B8760AA52}"/>
-    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{4ED6E649-4D2F-4C21-9F57-6F012E49B475}"/>
-    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{0E078AD1-76FB-4B70-A697-BC541B21DEDB}"/>
-    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{E02FA272-5AAF-4C7B-B9B1-39134F4B11C5}"/>
-    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{C4B15CE6-8581-4FFC-8D0B-06665CABBC1E}"/>
-    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{85ED709E-0020-4A52-9783-807E904D20A5}"/>
-    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{1E56D71B-5AFF-4168-9AEC-9C9B47023FF7}"/>
-    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{3525940A-F842-42E8-9399-534406FF323F}"/>
-    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{F7DBE883-4656-4C37-AE0A-0061C1991A22}"/>
-    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{B6A14DDA-DF30-4B53-98EA-4C988BC396F8}"/>
-    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{2211A63F-1AC6-4335-AD24-72432A747822}"/>
-    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{8B837E8E-08EB-4C28-8A93-2B7612529DD3}"/>
-    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{7D47FADA-F89E-4AA9-931E-C441272809CD}"/>
-    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{EABC8328-DE41-435B-AB2C-EC86D9399EF3}"/>
-    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{6BA40A6B-93A6-4FFF-8ACF-7269F21F8F85}"/>
-    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{58AE4FA0-3DFF-4F2B-B505-07F3014EEA10}"/>
-    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{4A47EAC6-2E2B-4F2B-B1E9-31753EA05AFF}"/>
-    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{046014FD-7BB9-488C-B0E8-D726EDBE2116}"/>
-    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{D9759C50-E062-49D3-BFEB-2FF76C696214}"/>
-    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{56D0291C-851D-48C2-B815-3F6ABD4F09EB}"/>
-    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{5122B93F-6E38-47CB-9075-245D703BF923}"/>
-    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{0F594181-40D0-4E82-A900-850231FAB6DA}"/>
-    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{8D81E0A6-FDE8-406F-9F1D-E4059FFE2DD5}"/>
-    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{EF0BCDCB-7E2F-4C51-9B08-430C366C091A}"/>
-    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{8595B0D5-86EE-4108-8593-812E78065B79}"/>
-    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{1A85C3D9-1B24-4B7B-A54A-248A0DBDC51E}"/>
-    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{8748E4DB-3E89-40DB-9391-CBDD2509F05E}"/>
-    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{8FF14805-56F8-4DCC-B90A-FAADD4EC1407}"/>
-    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{C2A66417-1608-40A2-B382-B115ED41F2F8}"/>
-    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{4099FF37-2201-4D3C-B071-8B14ED69FE17}"/>
-    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{0FF7F67D-4642-40C5-A523-BBFC177C9008}"/>
-    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{8C25E0B8-7040-4E19-A536-9F5305DBCD14}"/>
-    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{63B5763F-5C15-4DB1-A223-DB15229E488E}"/>
-    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{D86002A0-F348-4F80-98A6-8FE32907EC2C}"/>
-    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{4EEC9EF5-B5E2-427F-B2E5-620FB08AD058}"/>
-    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{B7436E6F-DC1A-4A7F-946C-BD1080B744F6}"/>
-    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{9E4B05FC-D29B-48F1-8859-5738C14BDB42}"/>
-    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{54605508-50F9-4BC8-884C-53E0AB6016D1}"/>
-    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{03D61244-405D-4D0B-9154-D097AAD8B087}"/>
-    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{15F14318-00A7-4A03-9118-413394B5167C}"/>
-    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{99EB364E-ADA6-49DD-B914-781F74C5F57F}"/>
-    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{8C90ADB3-E9DF-48B2-B1B1-97F80F02A75B}"/>
-    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{054B8448-C877-44F8-A9A2-0A815DCC482E}"/>
-    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{6EBEB177-926D-46C1-9C9F-EB3291EE3AEA}"/>
-    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{BFC58DF1-6689-4630-BC08-A078CE56E124}"/>
-    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{AC7C1185-E5BC-4D93-8EF9-1F2925E48C48}"/>
-    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{5567119A-E077-4A4E-9AEC-997BD5568C28}"/>
-    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{E8ECACF5-4911-43EA-9DE1-E96FC245B72B}"/>
-    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{B3E88EB4-3D94-4512-9B04-9A0F0BD7C58A}"/>
-    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{CAD2E47D-F89E-47F6-B0AB-FDDA5A839D79}"/>
-    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{F489DECA-0D29-4AFC-8CE3-51C3BF7688EC}"/>
-    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{8D019035-C91C-457A-9625-573D5938CE26}"/>
-    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{94094934-251B-414C-BEF3-8E8D07A4E7FF}"/>
-    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{49604E2D-FAC0-47A3-871E-A49924D2CE05}"/>
-    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{1B63F4D6-CE64-4184-987A-7FC2AD65618E}"/>
-    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{E4189F91-1232-4FC1-9992-436E254DF83C}"/>
-    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{13EEFEFE-24DD-41B7-A0DE-783628A296D1}"/>
-    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{87873AC9-B061-4A4F-978C-0D58A1CFEB9D}"/>
-    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{B67B787D-8540-4EBE-A1A5-1CCFD4DE6465}"/>
-    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{FEEA914E-9EE4-4130-A01C-679E6339A023}"/>
-    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{7A52A957-4265-435F-9427-CE8EF33DF9C8}"/>
-    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{19B52048-2017-459C-AFFF-203025F38152}"/>
-    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{27A7FED8-6D4D-4099-8978-B92D5CCA6113}"/>
-    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{4A3B163A-FC8D-4C5D-B88B-DE0B7315DCD4}"/>
-    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{32E75DEB-6D8C-426D-BDFB-25851CF07FA2}"/>
-    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{ADFAA959-322E-4A99-B9EA-9E04A08A4F3C}"/>
-    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{4650FA9C-D7AE-44C6-9044-D3AE19305219}"/>
-    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{92197B6C-675D-4E04-A3F5-339C48405434}"/>
-    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{31DE1BAC-B5C4-40F1-9F56-A471401DD914}"/>
-    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{A0151880-F279-4002-B8D8-1E6910CCD8AF}"/>
-    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{AEE474F9-E589-4F30-B4BC-BE179B73FD29}"/>
-    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{483086EF-9726-403C-8211-F4BBC26682D4}"/>
-    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{B059BA46-5C43-47F6-A447-84CFA8EDE279}"/>
-    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{211940E0-E170-497E-BDB7-D7B781EC1EE3}"/>
-    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{45E00C45-2ECA-4E7C-A2B5-55D4C579825C}"/>
-    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{4E69BC43-D1D4-40C6-A6A4-931BBC63B542}"/>
-    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{1CC32C7E-CAFC-4E87-B831-8E28762A1824}"/>
-    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{BA285618-B686-4458-8324-EF153A867556}"/>
-    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{BBC3B632-2817-4F7E-9DE6-F1852B5520B0}"/>
-    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{4A424D2C-5725-4D55-8B54-6D9104EFA5C0}"/>
-    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{2A7675B7-6A4D-471F-AB97-31B4361B0D90}"/>
-    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{BDF446E2-714D-426E-990A-D64F9F24BB69}"/>
-    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{A57A55B0-9AAA-4B01-BAE4-7739F937D1D7}"/>
-    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{99C460D2-5954-4AAD-AE69-150DC823028D}"/>
-    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{B6ED3F31-31D7-4786-9361-8B1D0822CB2F}"/>
-    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{51A1E1EF-4975-48D6-9D76-0FADA00689F2}"/>
-    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{32B02B76-1A58-4137-8D2D-2E65225ABF9A}"/>
-    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{1D8E2B7A-F42B-40F5-A8B7-6FEAC1F11D5A}"/>
-    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{0586A4E6-86D4-455D-B35C-8C6A58A2BC67}"/>
-    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{B422320C-F521-4353-8348-83F9715BD263}"/>
-    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{6F2A8428-ED73-43F7-8042-EAF93CF6A325}"/>
-    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{041535B3-A21B-4FCC-ABDC-1FA57D56647F}"/>
-    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{62CB530E-D662-47B8-BE27-6B287551D8FB}"/>
-    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{DF2A61C5-D2B0-479C-8380-AF6571942BE9}"/>
-    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{C11767BB-D458-4578-91DA-B50E6B700D05}"/>
-    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{01ED1D66-91D3-4F49-9E59-FB54073BFABD}"/>
-    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{079B4C0A-C23A-492E-86E0-D207C628C8DE}"/>
-    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{41B64D02-996F-41F8-AA09-E2E4D13AF105}"/>
-    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{9D1BAAA7-13A0-44A4-B2B7-44EDB703492E}"/>
-    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{8AF2FF6F-C75B-4FC2-9104-B52931166A58}"/>
-    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{B0AB422E-2FEF-40B4-BFDF-DBADC522E233}"/>
-    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{E51A449F-5BC1-4E2E-83EA-F18CAF317960}"/>
-    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{D586E7AB-7E26-4F3C-9D60-542EC34F5F44}"/>
-    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{93A818AD-D529-451B-9AAF-531F6E061787}"/>
-    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{E04CB442-4E85-4427-AB5B-E74859C6EAA3}"/>
-    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{EC8A9FB3-2675-497B-92E6-FE5B360C4708}"/>
-    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{8C25D63B-B533-4457-90CB-0975145FD1EA}"/>
-    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{27AC27B0-135B-4C4B-AF9B-0814E0CB01D3}"/>
-    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{A6819083-67D0-486B-9F2A-41C0133BFA37}"/>
-    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{1B9800D6-8A1B-4903-990A-98272447B4C9}"/>
-    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{B703BAE0-055E-471A-BEC6-29274F7CFE2D}"/>
-    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{62B14E72-09D5-43A7-820E-73C7F8CC7790}"/>
-    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{C01CC112-5955-4708-8EB8-CA8D7F2F6703}"/>
-    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{0853358F-E56D-43F4-A657-4964DB6F42D7}"/>
-    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{722DB8B6-D8FA-4CDF-AD0C-4C3E832875E0}"/>
-    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{0F54D6A1-C863-4771-B712-51AFEBF6A95E}"/>
-    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{3D9695AB-278F-4376-9503-6964B14CFE0C}"/>
-    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{A19FBCAB-4D84-4A95-9B55-68BA8633C048}"/>
-    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{3EA67024-5F22-4E2C-8B29-F38C3ECE3279}"/>
-    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{E3BC5D11-A192-4F40-8928-2855362F4637}"/>
-    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{60DF38F6-1DF0-4D80-A049-75A28768EACB}"/>
-    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{3E82FA37-A151-411A-935A-8103CA4D0A50}"/>
-    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{86911393-A92D-44FA-AF27-920577EDF750}"/>
-    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{B143C701-4EBD-4079-9E1A-BAD67895F08B}"/>
-    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{52521F40-0571-4593-B97A-1E9F3DF5B718}"/>
-    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{E0535565-C87F-4E4E-9B44-CFFE792D6426}"/>
-    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{32E16D32-8251-4B5C-8BDF-8DD35D680BA1}"/>
-    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{D4AEEB79-05C4-4717-ADF8-1180315FDC00}"/>
-    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{CA4895A2-C346-4883-9F61-ECF972F7678A}"/>
-    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{212D4507-0898-4223-BD9C-C9AA61A8D9DA}"/>
-    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{620D70A2-FA18-4D94-ADAE-938901AF3FD0}"/>
-    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{3B254FA7-3BA0-45D8-9D56-62158AC2CA5F}"/>
-    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{27D22CC3-43E3-485A-B406-C911E2F3D627}"/>
-    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{1AD8F92C-4D67-4EA5-B434-A0B1CA9E9C11}"/>
-    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{7D3CBC9E-2594-4FEB-A369-1B07C2B57263}"/>
-    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{25C0F388-F21C-49F0-AFA8-3340A7BDB20F}"/>
-    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{875015BD-B5DE-4C05-A3E5-DF5AE61554A0}"/>
-    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{A908D1D1-35EA-4B5B-A284-7955BA675231}"/>
-    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{65FB2F20-B02F-4301-90B3-26D208E18C89}"/>
-    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{C3C9CF29-8583-4AEC-A76B-D442B2AEA855}"/>
-    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{4253EA51-02F1-4B3F-83DA-F149A8F28673}"/>
-    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{ECBA6FA9-E362-49D4-9F7D-1C2BCA13263A}"/>
-    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{9F920F2E-C549-43F1-BB34-C071F23EBEED}"/>
-    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{F57400A0-822C-4330-AB97-736B70276AAB}"/>
-    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{FB59C51D-2007-45AF-BEC9-FF84581C9B0A}"/>
-    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{2487BA6F-BDA2-476A-8F72-EEC5861C25A1}"/>
-    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{88DE7510-EE79-4883-9B57-A60608E3846D}"/>
-    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{F1530C07-55AE-48D1-81A4-76E8E3861F69}"/>
-    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{6A37FCCE-AA41-4460-8E11-DD57C4982273}"/>
-    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{5492A185-58DE-485D-85A2-19E5D0A381C0}"/>
-    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{A7DDACC1-0CF3-48E8-B5D9-FDCA8AD0AC2B}"/>
-    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{5DB199C3-AB14-402E-B732-B79CB0DA0B2C}"/>
-    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{3246CB4B-A154-4924-AECC-A408F024929C}"/>
-    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{42069288-6D6B-43CF-AA3D-9446FCC12D62}"/>
-    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{5B56A2A4-2C13-4B45-87CA-35841632BBAB}"/>
-    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{FE7CF59B-B561-4BE7-AD85-F53C3A2D9820}"/>
-    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{021E8F6D-DEF7-452B-9890-134097EF60FF}"/>
-    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{12D5F2A7-ABFD-4232-9A24-4A17645425E4}"/>
-    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{BBB6944E-2239-4A3F-9299-6CD2F123FBC9}"/>
-    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{A5903583-760D-48CB-A171-1F4A6839A66C}"/>
-    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{52DA4E98-4AA9-4316-9BD6-F1CF57E0B67D}"/>
-    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{80C7E91D-AC64-4E0F-B008-48CB010C04FD}"/>
-    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{2C2F6E98-F958-4B30-BEB5-D4210D17B22A}"/>
-    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{B61A32A3-FBB1-4593-9A11-5227561F56CB}"/>
-    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{624EA99F-A210-43F0-B615-BEE7A1C32F4D}"/>
-    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{E7044937-4A69-4E2D-9DB8-3D7EAF971716}"/>
-    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{ADFE69C3-A5CA-475E-8004-3EF9925202CB}"/>
-    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{D8FEDB20-9A03-4E31-A3E9-C00D68B79A27}"/>
-    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{CBBB545F-A043-4CE8-9F31-1BBC74EA8CAB}"/>
-    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{28F90954-561B-4408-A3EF-800D3B5857E5}"/>
-    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{585921D1-C708-493A-AAEE-49A351F361F6}"/>
-    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{6179EBA9-3EDE-4FE3-BB2F-A00021183E0C}"/>
-    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{8C55BBBC-545F-449F-9673-7112B49FF864}"/>
-    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{D29249C4-FDA0-4F70-BDD0-6EE37C489D7F}"/>
-    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{47BFCC3D-8A6B-4F42-AE56-9369D9E8F836}"/>
-    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{E274D884-8759-49F6-9440-1AD310A927EE}"/>
-    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{AC61E306-7C16-42EC-AF12-DE699B54BFB8}"/>
-    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{ECB1DA03-8AE5-4F6D-ADDA-C10307C4F47E}"/>
-    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{387658DE-4F40-41B0-80D6-F754568D1791}"/>
-    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{E84C7C2C-8C55-41D3-95E0-AC1F83B852DF}"/>
-    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{639AB87F-D9D2-4637-8C9E-A069DBBD695B}"/>
-    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{5C305875-A943-4F19-9405-7718EB662061}"/>
-    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{5DD7ECEF-FB97-4C9F-AF50-7A1323EC276F}"/>
-    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{9333043C-4156-48C1-B297-82D374068180}"/>
-    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{7278E213-D8C3-451A-B51B-6A4FA7BDCD4C}"/>
-    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{4CABE99C-F341-4879-B8CE-5A5FFC98E469}"/>
-    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{912440B8-5E53-4946-96E0-3D87704974A1}"/>
-    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{573AEDF3-B3FC-42B1-B049-F08BA43A50AD}"/>
-    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{CE4CDA45-81B1-4A64-9C6B-62C197C382BF}"/>
-    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{227A07F6-97DA-4E9D-B30E-37EE120987C9}"/>
-    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{ED92D904-F5F8-404C-B105-DEE0663E3E26}"/>
-    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{818909A9-7CD4-4015-91CD-7628B39F49A5}"/>
-    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{B04550D4-D286-4DA9-8454-96CB91A36FCD}"/>
-    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{C4F6D189-D929-4180-8B15-4DFEB4CAB320}"/>
-    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{FCCBA214-A734-467E-8CBE-60E32B80B4B8}"/>
-    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{931AC6DC-57BD-4B20-9711-AA9DB48D87E9}"/>
-    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{83A26C77-DF09-4672-A790-54676A72DFDC}"/>
-    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{DB6695FB-A835-4544-ACCF-A936F13A8648}"/>
-    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{674B0365-09D3-4981-B9EE-E3DD52CF564D}"/>
-    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{3D3D6B16-83A8-4C8B-A8DF-3A4E50E99619}"/>
-    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{737F54D5-8686-4B3B-BD83-14C06900E651}"/>
-    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{5BFBF27B-6298-4889-BC7B-22C23751E24F}"/>
-    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{D6D1AE55-D0C7-4E1A-ADDE-521F434D9214}"/>
-    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{C63F0A97-AADD-4310-A1F0-282AA8BEC7D7}"/>
-    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{FA56886B-87AE-43D2-AB4A-CB8460BB7451}"/>
-    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{924F7CD9-2ECA-4B49-A711-FC66C8C1965E}"/>
-    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{C1F40298-92C2-4933-B455-9D6A22EE77DF}"/>
-    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{1E75D653-FD1F-4D37-AB6E-CFD5FE79769E}"/>
-    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{E9747E9A-0A84-49DA-92F0-4F5A5E674D63}"/>
-    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{1AB9A3E2-94C2-4783-8A33-787AA3126A2D}"/>
-    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{FD28EDFF-7CEB-4248-9CD8-AAD2D294DFB1}"/>
-    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{D152A766-C52A-4519-87E2-02B4DDC108D5}"/>
-    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{FA4B2816-3D2E-44F8-ACDE-E75E6BF30963}"/>
-    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{7C775A24-5BEF-4AA7-B13F-D1E818B3FFBB}"/>
-    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{2188B3B2-DA8C-499A-ACEB-F870B18D9A08}"/>
-    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{EA3437F0-E44D-4711-860B-2899D81258AE}"/>
-    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{CF44F98D-956B-46F2-B6BC-41B22B293C69}"/>
-    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{ABDC83D6-CB87-44DF-B6A8-7E1E853D6E0C}"/>
-    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{3CB4E8AE-2528-4064-83A4-8405CA3749A8}"/>
-    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{E02DF7D0-CC9B-40F9-9921-406A5B5BEA45}"/>
-    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{C74536F0-02C5-47F2-B8F4-0640FE1EF957}"/>
-    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{BA36770A-2113-44EF-B1E3-2B04D92DD72C}"/>
-    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{3B7F2884-C1A9-41CE-9586-D02C6EDABE24}"/>
-    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{90CB44D1-2C10-4234-9323-84A2DB665A49}"/>
-    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{D3828AE2-705C-4B35-85F7-5011AA72A44A}"/>
-    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{6EBAF0AA-2447-4045-AF44-02325238BED2}"/>
-    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{F640494C-A14B-499B-93AD-3ACBA113D9A6}"/>
-    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{501428FA-056E-424C-9540-B951DC7690CC}"/>
-    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{B02846E2-950E-40EF-A81A-538C0AD6C996}"/>
-    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{448EB6BE-A235-41E1-8D8F-D3FD7027C41E}"/>
-    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{BF6AE9CA-33C2-4100-9FED-3136914D80B8}"/>
-    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{5B1A3410-695E-410E-BAF4-C9BB71209F5C}"/>
-    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{6DAC62BB-ACB9-4598-8396-EEDA6447E044}"/>
-    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{64476EEA-1B1B-4CEE-9A08-7A5D932CC12A}"/>
-    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{278DB2B4-0414-4E4A-B1FF-E09AA1B65E99}"/>
-    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{D9147CCE-1BAA-4263-856E-794BFC7E0894}"/>
-    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{9C4BC943-2BC9-41EB-BB1A-9F243A007BAE}"/>
-    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{2555129C-D282-41C2-99FD-0491FF40EC0C}"/>
-    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{25F71BC6-3F59-40E7-A654-82917A5A0F54}"/>
-    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{A8FDE8F8-7DEB-456E-A6D0-9BFBB99427EC}"/>
-    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{B189A43A-06C7-49D1-8E62-DE1203820E0C}"/>
-    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{1EC6DA7B-3EE5-43CE-9BE9-C7673E483E85}"/>
-    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{78B636EA-C053-4AF0-9DEE-92A8CB9C1C99}"/>
-    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{7269390A-4223-4A20-B055-A2A10217E398}"/>
-    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{18584C2C-984A-46D6-B04B-48443C56519B}"/>
-    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{FA8DD4FF-D882-4024-82AB-368DEDC54909}"/>
-    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{9E3B2EC8-8427-41FD-969E-D842ECC47682}"/>
-    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{A79B3EC8-85DB-4312-9DD1-5084EB1C54F1}"/>
-    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{F9C7EFF4-E190-4632-AED8-294E1E9180B3}"/>
-    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{4A092EB7-D42B-4F12-9261-E0833E4153C9}"/>
-    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{30017B99-6991-4983-B7C4-AEED98BF3F41}"/>
-    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{EDEA093C-9022-4D60-94F8-E91C759B5503}"/>
-    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{CF0337CE-F729-4F54-AE1B-504557A50737}"/>
-    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{B188AFDE-776F-4AEE-9168-4BB4D77C80F4}"/>
-    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{971D08DF-93CD-4428-9C88-4745A7CD857B}"/>
-    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{8D3D7F40-975D-47E9-B3BF-F8C00FA6CCE3}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{E5D88052-626F-475A-B40A-D9A6CB83CAF3}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{7634EB03-6E25-443B-992E-429DBB50D9DA}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{D4E21ED2-33F5-41FC-AB79-F2B28440606D}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{5F0B833C-83F8-4DEB-BC9E-AF1706B1F9FC}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{7B3A5B76-AC5A-4D13-A89A-AE53A6E8F296}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{51A8B915-BDD4-4464-8EBF-24F4F18D7328}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{CAE42CCE-540A-419D-901D-C046F35CE2D8}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{B72ACC82-E8A6-412E-A233-48606FC85B05}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{32788DAD-9B09-4AAB-999F-6B569B224191}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{7C570ADB-E6B1-4D4E-9202-A9C2D5C10256}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{DD4408A1-5F62-4A8B-BF22-E898D8B6AF5D}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{A4614502-2210-4DF0-8CA3-DE1E522FB1CE}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{72E4573B-82F0-4DF9-A76D-CD015518DFFC}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{5015CC24-FA82-4EB9-9AB9-E1FDB7EADA65}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{83953ACC-1B12-4010-BA81-782FFCB76018}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{8E5348E6-ECBD-48AF-9A4A-B0F1089E3019}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{78EAA804-9B8B-4F62-9E89-2FD22624617F}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{7537866A-8BBD-41C2-9C20-BABFD0CB63AB}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{CE4FE6E6-CB80-4CDF-A56C-6B47DED1C084}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{8B3F7672-A7E4-4558-BB85-31C2CEA91302}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{8069D816-C887-451C-A730-3DB3A1DC4FC4}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{5D0FDA74-1CF3-4AB6-9576-186EA61C2A16}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{4186FCBD-455F-4EEA-9F82-D96DB2F52A6F}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{C4A887AE-5310-4118-9402-71C6F4C9247F}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{37BE768D-A4A0-4179-900C-D6619099DB5D}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{E969E587-9C9A-4C53-9BEA-E0DB72669D9A}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{2FC1934A-95EC-43A7-86C7-74C25AD6E5AE}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{AE9C5207-7B1A-4A57-8EA1-5553DCE6D9EB}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{92315DC2-C228-4207-B706-BADBFC1FE953}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{01645D5C-5AA4-446A-B209-53AA644931EC}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{CC02C372-507D-4D63-A3DB-2D02BEF9F65A}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{8A3C3AB2-2C72-4A03-AF9C-29E7D35CC8C7}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{609763B0-D83F-4EAE-A10A-A66D22F373D1}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{C5DA7C2A-B1B5-4BB7-B796-6CE58095325E}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{0FCD9F32-8952-4912-88E3-9594A949CB17}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{D17EEA62-B5A5-4425-A02A-3B575EACAE88}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{E21FBCF0-A7F4-4AC2-A917-F4DC7FFD25E1}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{E3CB7CC3-1D79-41BC-97A2-6EDA5C4A9C31}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{D5398DD3-DB14-40C2-A2E4-2140CFE6FB6B}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{551E2C4C-4BE5-46AC-B242-33A1C522CB60}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{654BFCE9-DDE5-4986-9EAC-11DF25851EA7}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{1646D4C2-2EDA-4187-A06D-2EFEF6156E0C}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{72A6BEFB-B641-426E-AE20-845FC3FD2080}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{807BB098-6B46-4307-A6C4-A87DFC378777}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{E65F3C7E-986B-4F03-863A-7A2AEBC147DF}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{6231B508-3E78-4A54-BA01-6E46CA537840}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{6CE35B20-74B3-40FF-8307-536BFC813744}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{DE7C5AD7-93BB-451F-A4FA-BF78D53C4CFF}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{3AF98F5B-A4E3-4176-8426-6B66957643E8}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{BFB6276C-2C54-40DB-8D27-0C67A02AA0C6}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{A27C6EAB-CC57-4F32-ACFD-BEEA61C72AF6}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{545B9564-6C30-4791-9192-E87528B57F45}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{ABD03237-BB83-4548-9935-9921C602AB25}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{AF45FD1A-DDDA-4308-8536-68CBCD21FCEC}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{5480969A-0021-42E2-8FB8-09AE7A730B4D}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{52294B2F-B975-40D4-92C9-51E173CB9EFE}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{A58D5B19-148E-48F1-B90B-B8BA3C0AA430}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{C521E528-AF0E-43FE-BE02-748EA3633581}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{F0815592-9F99-46AF-B4F8-3D539623575C}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{148ADBA3-1CE4-4FC5-8748-FFF9B422C0BF}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{F3D95F34-2F9E-477C-AB34-214586D93C09}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{A3D572F5-F196-4B6D-BDD6-366A34CEB5A0}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{80705FB1-A500-47DB-A2BF-432DCD7AD313}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{8AE15189-D215-4BAC-B449-EE725F0BF6B9}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{0A536BEE-779E-4840-9E41-ADFFD981B6DE}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{09E621AA-FC53-4599-8807-BEBA9B6FF2C2}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{565BA570-A04A-42C4-B8E1-ECED9387E9E5}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{563C7169-39DD-46D5-9EDD-D479848F4C22}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{E78AD24E-4455-426A-A884-FFD155546678}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{1C770956-200A-4BD9-812D-8FE3DB6B6DEA}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{CB34EB82-FE35-4C83-8191-51059CF0D33A}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{586A9ECC-D187-4467-B673-5748B181943E}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{3CF0FD36-CA13-4B3D-8173-DCE5D14C2E82}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{471C76C4-D4C7-4C56-AE9C-FF653685805E}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{0FA28DFA-4B94-47EA-8B2D-47836D0D2FAD}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{18D8D2F6-B26B-4452-9D46-7EA02922318F}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{B8F77DE1-000C-4C9E-AF65-A62268EB7A1E}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{B115DC02-5018-4236-B0AD-E7F26E66E6CB}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{3B91D8ED-746B-461A-9076-B03431463A65}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{C6CC0496-176E-42BA-B796-DF2E89F651BC}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{6E85CCBE-A1E6-497F-B390-BB0A620401D9}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{AE18D034-C168-4B94-B91A-976B9992EA6C}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{78784FCE-051C-4F4D-85D3-6A777D0BC953}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{C6815F4E-6A15-4D17-82F4-853303C493F9}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{E6FB4545-45FC-43DA-BE6B-7A3F77280B5B}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{12DB6E36-FB2B-432E-BE73-861F65C57413}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{A35E61CE-3759-4608-8609-1EA38CF94EE5}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{BBACB7BA-030F-4723-88C5-47B83DAAC7B9}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{90E94B08-7DA1-43A7-BA9E-315AC592CA7D}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{0F28A204-D854-4C82-B8FE-C580BDC59B1E}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{3F19A407-61F6-438F-A4E8-C88BF10FB8DD}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{00305898-C94C-4427-8408-FFBA213B10DB}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{CBE2A796-D0B2-4769-8BD1-DD6073165F9C}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{5C637B91-E8A7-41A8-A740-24693254761A}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{ED855A86-1343-465B-8118-DD48826AB82A}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{C6A1A048-6BA2-403B-8169-4C69A2C9D9AC}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{869D8311-4E61-4116-8750-4A602B275245}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{6F3344DC-E181-4A77-A0F2-D6F19E17BFEE}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{C8A4D9E6-FC59-40F1-BFA9-45B9D0A7408B}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{C52148AC-0DC1-4C3E-8EB4-8A931882ED6D}"/>
+    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{2F1BA042-2780-4837-97A7-645758E67DAB}"/>
+    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{C1CC9A9E-8990-411A-84F3-980AAB761864}"/>
+    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{36F7DA17-81F6-41E2-89E2-745BDD0C6EDA}"/>
+    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{EBDBE84D-6C7C-43AF-B464-DCA7294996D0}"/>
+    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{887C8280-5594-415E-AB35-9B4BE2BF9E1A}"/>
+    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{BF8B2FFC-9DAA-47AC-BCDC-3D7448747AE1}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{587855BF-F99F-482A-913C-C4A794725D28}"/>
+    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{99823CC9-3836-448F-B2B1-D7D3C0C8695B}"/>
+    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{2AE26AB7-89CB-46EE-B51B-2BCB0D39A1A7}"/>
+    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{58F2A1AB-7393-4168-B032-D4B503D85F4F}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{BF6544CA-4469-4959-9400-2A4E18B3AD22}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{59D2D733-A0B2-4A91-AD18-13FAD45D2C3C}"/>
+    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{55347B97-A32C-4A80-9833-593D4331E825}"/>
+    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{2D49D0DE-E15D-49B7-9C3C-422789E5F44D}"/>
+    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{A3E89A1A-2438-49AE-BAEA-822AAF9909B2}"/>
+    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{73C2C81A-F189-49DA-97D2-F5076433112D}"/>
+    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{CE54E5B7-134D-4672-962C-A15DFC513432}"/>
+    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{C8E4B5D4-7B7C-4150-AF5F-66946ACBCF23}"/>
+    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{344B9F16-1A33-4DF5-B259-57341ED5BB06}"/>
+    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{B7011F9D-1BEE-4E9F-BA29-5805FE889775}"/>
+    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{538ACA58-DFDE-42C8-BDC0-84EB6D937A6E}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{D352C2BE-13C6-421D-ABD1-30753E0CC3F0}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{E06B079A-D929-4E09-92FE-0A1810AD79DC}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{F17E74E4-94BE-4BC4-880B-7E220ED8546B}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{384CA16D-F889-4813-AF23-8D050133B4A7}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{E0F505CF-B5FE-4152-A846-5DD59540536A}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{8632E226-FE98-41F8-91B4-F5ACBEE7A6DB}"/>
+    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{31397CED-613A-4C86-AB1E-2227675E1581}"/>
+    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{B5C23577-E034-460B-A0F6-ED2EF5659D36}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{B0127436-0C93-45DC-AF7B-0E2B8A581E99}"/>
+    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{FE1B8E3C-256C-4E71-A9E7-C2C89766819A}"/>
+    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{B6C05E15-D85E-4F9D-BF59-63BD12DA03DF}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{D395B66A-5F8C-4843-B889-F6D72A68E998}"/>
+    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{158E6259-7666-4877-835A-30CB5BEB2843}"/>
+    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{A0152879-EA8F-4851-B5AD-48AF4C6ADA02}"/>
+    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{E9437613-3DD4-4B98-845A-9D5DF2F0AF7D}"/>
+    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{7FE43CBF-BF89-4FDE-B4BC-D5B354BCC25F}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{A055C0E5-4118-492B-B0FB-CC2DD16F0061}"/>
+    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{5CC6D72A-A604-4426-8FFE-ECDEA2C4F806}"/>
+    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{7DC9D807-1AA0-47C0-BA00-93DB99681558}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{62B99182-CCDE-41FB-A847-C492158DD7B5}"/>
+    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{55EBCDC0-2404-41B5-AE2C-0E95380CDF8A}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{362803DB-5138-4DBC-BB08-A4723CCDDD5F}"/>
+    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{1290319F-5844-43BD-8DC2-82273F4D22C2}"/>
+    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{35C38185-67D3-4819-9F93-3A9D47832189}"/>
+    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{82C168A5-89C4-4F93-9AC9-19A331DE70A1}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{FA056A89-97BC-4120-A97E-BD1DE9313796}"/>
+    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{10BEE488-838D-4F8D-B8C8-D4ACC5A5167A}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{D0501352-C2C9-4C34-B6F3-5E9791A518C7}"/>
+    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{9D1B98C5-C4EB-486E-AE8B-21CC968B8AFD}"/>
+    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{751FB3D3-456B-44B7-B41B-827842E4A80A}"/>
+    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{65861D40-7333-41A3-8CBC-3446B6B7DC22}"/>
+    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{A2C5F943-6160-412E-A6AC-57F5D6419AF4}"/>
+    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{C114F23F-02CF-418D-8422-6ED3D97E8E2F}"/>
+    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{80E86D0C-0D59-485C-BF29-05E6C51299D3}"/>
+    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{ED06B5F7-221B-4D1F-BEF2-241448E03F03}"/>
+    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{4C1417F7-1256-4D60-80FC-511B9D34DF1C}"/>
+    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{3142F96A-70B8-4655-B939-67573D407261}"/>
+    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{CD1192E9-10FD-4993-9271-2D4DA9D7FE8C}"/>
+    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{2A6C1EE5-0F43-4F30-B9F4-1D546540D3EE}"/>
+    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{C8723DC2-607B-4B3E-8767-BE870CC0895C}"/>
+    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{759C267B-260B-4FBC-855B-69BBF073558E}"/>
+    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{577C0669-7F9D-47A9-9CCA-CBB3F3CCDC2C}"/>
+    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{9CC591F3-1DD4-46E9-9F81-92384F9A7FBB}"/>
+    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{0898C2F2-02F2-48FB-96C5-0B00932F0679}"/>
+    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{98DEBB39-D916-407F-B720-9AB2106BD192}"/>
+    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{D58F3827-DED1-41C8-9EB9-211DA3903BE4}"/>
+    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{2405893D-500B-44EA-BC7A-8FA4F6DA85C7}"/>
+    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{AE70CF03-8D51-44F4-BCB7-6E5098871878}"/>
+    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{B8D89257-D74D-49DF-91FF-C532BCF607D3}"/>
+    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{C14088DA-69E3-474A-93B6-9A3410E9F6CC}"/>
+    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{A2C0D00B-50FB-42DB-A102-9D0C443BD8F0}"/>
+    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{5013E428-FC68-450D-9952-3E3E87345FCF}"/>
+    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{F9A1D36F-93D8-4340-B274-E3CFE2AA5D28}"/>
+    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{104CF332-8F1D-4658-BD6F-19BCB62DFF7C}"/>
+    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{9E76CFCD-6EBD-4E86-BE18-CD62023A4E81}"/>
+    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{A4BCD58E-A0E2-4042-A468-7C16E92E8516}"/>
+    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{7EF64DA1-94FB-4FE1-8E5C-D4B936F50D72}"/>
+    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{B9FA9858-0716-4499-8BF0-7816A6BFCC2D}"/>
+    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{13B8A0D0-AB4B-48F6-98D0-117AC8FFCA2A}"/>
+    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{4A7E2876-D606-49F8-AA8A-D60080C1DB50}"/>
+    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{2FBAA2D7-9AC0-4BE1-B529-5928669F18B1}"/>
+    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{89D8BDA2-5FA5-43FB-BBEE-260DD6CDD868}"/>
+    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{62B99530-45BF-4F6A-BE8A-19D3AC0D94B2}"/>
+    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{38CF4162-C888-46CA-B8B9-266AF4EA8855}"/>
+    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{9219F6BF-6DD1-4A0A-9AA8-B73681DE0777}"/>
+    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{5A8E8DC8-FFDF-438E-8B98-38B02AC7D0F4}"/>
+    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{F1EB2E11-56BF-4358-A6E2-762B58993199}"/>
+    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{9B18C20C-2740-434E-8D06-37D374E1583D}"/>
+    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{11FA1B21-A2C9-4684-9D34-FBB657953380}"/>
+    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{31AD8E94-03D2-4061-B3B5-DAC4ACA9C5C3}"/>
+    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{FF141023-853D-424A-97E8-C0D9C4EEE9FC}"/>
+    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{0FCBF4C7-930F-4CFF-8866-9E2549777C09}"/>
+    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{151B554C-295E-436C-B122-5A7280ED1768}"/>
+    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{2F42BF34-BB01-4792-AFE5-1255F003D954}"/>
+    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{7FF43F7B-7F14-473A-AFFD-6155A011E8E6}"/>
+    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{2B6A81A6-A128-4E4C-8BEA-9392B9F9EF93}"/>
+    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{040CB7BD-CFF4-4C68-84B6-E1FC2B2850BF}"/>
+    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{92B35488-E659-4AF4-87FE-05D791D86455}"/>
+    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{794FF9AD-5890-4D88-9B9B-2A61AF558962}"/>
+    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{85F1D661-916D-4786-BEFF-2F6198D741BA}"/>
+    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{4541B899-63D4-470C-890A-8B1D8CFA6279}"/>
+    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{048B435A-6E74-41BA-B488-ACFDFBE56350}"/>
+    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{3F1D1F05-036C-4F50-8EBD-A11433198F85}"/>
+    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{5FFD0B5B-16E2-4870-85A6-F180AF998311}"/>
+    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{4F164C87-1C14-4D2C-8C8B-C74178C4D46B}"/>
+    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{FEF44001-68A5-4B93-A467-CAD0B8F6B72E}"/>
+    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{601737F8-1BC5-4269-B769-AF4B42E687D4}"/>
+    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{17D06F31-6F5A-4506-9E5B-91124EF795CF}"/>
+    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{88B80F85-07EB-4672-8E5B-030D6C7B2774}"/>
+    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{A893927A-6B28-4F61-9EDE-A8D91D43C638}"/>
+    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{D3FEE920-EDF0-4DAD-89C1-5047AACB7803}"/>
+    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{34E57D4F-E3D4-4D78-9CA2-37992DDECFD7}"/>
+    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{5D05E3CF-3672-4831-9430-3F25749724DB}"/>
+    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{B342E33C-11F8-41D3-A2A9-C59D4CA88721}"/>
+    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{F5A51FAB-111F-417E-A63C-F1F85756296D}"/>
+    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{CB1990FC-6588-49AF-B896-AD7EE97DC825}"/>
+    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{1124BB8B-EAAC-4603-BD5A-DF185AFBE88F}"/>
+    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{1F7FB546-B949-4F9F-91F1-407CC6B34C7C}"/>
+    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{FA74C281-3908-465F-8EF9-1092C9F45AEE}"/>
+    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{57626ADD-8550-4CC6-815C-A477A9752BBC}"/>
+    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{7F3E3830-D57F-422F-B6C0-C2229155E344}"/>
+    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{E5DE09AE-9137-4BC9-B6C1-8576071D14F0}"/>
+    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{A95DCB8B-1441-4073-A881-A3F341F6B368}"/>
+    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{1B8AD0AE-DE68-477D-B643-88E9D2D44B42}"/>
+    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{74B9C3BD-A23B-4A11-94C4-B82FACDFB081}"/>
+    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{BF1B084A-EE3E-4DD2-ADA5-1D1817EBAC15}"/>
+    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{3D380157-B7B6-4EF4-8985-8C486C25EA56}"/>
+    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{D0AD5BFF-06F0-4976-A9A2-169C0B56B6C2}"/>
+    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{F1C2D1E2-2603-4B56-BB14-A249FB817B54}"/>
+    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{7E1F4432-7A75-4C66-BC63-4364A8D49AF4}"/>
+    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{BBE1F54F-1B3B-43C3-B5FB-38DE7203C48D}"/>
+    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{65C065D7-FCB2-4F7C-B554-55665C6E728A}"/>
+    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{2CF7C558-21D3-4972-BD1A-F1D5B69E5393}"/>
+    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{C2AEFAD9-A2FB-46EF-A27A-E1B24FFA7251}"/>
+    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{4EB0B443-2556-4709-92C0-A1D558A34641}"/>
+    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{70E2C25C-FEA6-4FB5-94C6-4A4C1B74B6B8}"/>
+    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{5DC8A45C-32A9-4E5C-B10F-3328A8B027FB}"/>
+    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{71BA0820-86F2-462D-AA62-1CF956EC22A0}"/>
+    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{A277B784-8294-49B8-BC49-6FAE770B7058}"/>
+    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{FCEFD61E-B8A8-4DEC-92FD-A4C30F443504}"/>
+    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{8429EC86-0451-4759-9809-358F7840EAF1}"/>
+    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{C657093D-0F58-497F-A6C6-FA27FA6008B4}"/>
+    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{29A50218-7B5C-42A3-8355-245F9D5EFF40}"/>
+    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{E88E0FAC-B0B2-4C4A-B19F-0809EB4E1C18}"/>
+    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{62035E8D-37AC-4239-ADE4-FD341141816F}"/>
+    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{0C69C193-963F-47DC-9BE7-3B42CC60B36A}"/>
+    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{60136DFD-F1FF-4E6E-8200-3E7FF33099E9}"/>
+    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{5D0DCD16-1988-49EE-AEEB-156F9864FF42}"/>
+    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{7BE3B17C-534B-433C-BBDC-553FD451CF57}"/>
+    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{295CB2B6-B3C4-47D8-8D03-54D8697F84BB}"/>
+    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{7623FCD5-CEC4-4055-9055-87621C5DF07C}"/>
+    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{698022BB-82FD-4710-A33B-8673A44A3D9E}"/>
+    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{EAA7DF6D-DAE1-42AA-A8B1-C42C94A5FF46}"/>
+    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{90FD54A1-564D-484F-BE29-868F1333940C}"/>
+    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{8A596E39-5886-4234-9135-C99150DB4CF7}"/>
+    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{8C99A142-DC7E-4ACF-8C5F-CA9053561512}"/>
+    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{33CF3B72-C980-432C-A0C6-903840799CC6}"/>
+    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{2A48EAA8-E665-4980-8F9E-D6243B69FD65}"/>
+    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{6043FD95-01AF-46B7-9D57-FF78B996CC21}"/>
+    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{6C0443D3-C39D-4E61-BFFD-224F0D82A2F5}"/>
+    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{CC97842B-F8EB-4B38-9D12-756D57DE5BF6}"/>
+    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{CA9339CF-B6A8-4832-BD9B-906FCC0E5AC6}"/>
+    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{BC02E316-BF33-474D-BD22-3BBBA6CF69EA}"/>
+    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{FE4DA010-49DC-4B18-B620-1C327CB8DD5F}"/>
+    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{6BC88C68-7A38-415E-BA34-C345C1E98844}"/>
+    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{575B87DB-D10B-4391-B330-89F937A10437}"/>
+    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{D2B3B0FD-87EA-41E3-B458-5FD60C6FE965}"/>
+    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{88637DDD-F25E-4DB6-A176-60FA8CB9A8A2}"/>
+    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{4ACE3FAD-8279-46CE-AD74-C711D53F2BCE}"/>
+    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{D4C2A5CD-AA25-48B6-8ACE-4A739DACE3C6}"/>
+    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{C04925EB-1974-485F-8854-9547AEEDE086}"/>
+    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{CF3F32EC-2CA7-419D-8A88-04EAE7BB208C}"/>
+    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{797179F1-1955-49AC-AAC9-A7FEA991EDB5}"/>
+    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{A4F46CDD-8370-4D32-B977-782DC7B574DF}"/>
+    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{C773810B-57CF-4DE6-8351-A221E910E9BE}"/>
+    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{FBC14FA2-B061-4A41-A3FC-EA7F2CD40DAE}"/>
+    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{F10690D5-71FB-4369-A13A-F0A7B9F788AD}"/>
+    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{5DF3168C-0F5C-4A74-884C-0C49DE6272F4}"/>
+    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{43327C6D-FC7B-48BF-8937-F3A949060BC9}"/>
+    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{C73D3459-96D1-4242-96A4-122EC7D94A71}"/>
+    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{A61EA0C7-8531-4BCB-9D39-4097B07A732C}"/>
+    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{C88E85EA-25CD-4D8D-A8A8-1976A4727CF1}"/>
+    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{E2421B27-C617-4506-A125-61D46540F671}"/>
+    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{3FA90833-C8BD-4F35-9473-6B049ECAAE05}"/>
+    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{3D66AD3B-F1B0-4C8E-8CDA-CF81CDE7BA93}"/>
+    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{036554E2-AF96-47D3-AF82-3E0130C32EEE}"/>
+    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{DF132149-5C6B-4B15-9977-43CE7572FB12}"/>
+    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{4F3A809F-88E8-413F-8707-1CE646850F75}"/>
+    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{564B4501-3837-4271-B911-A2517454BAF5}"/>
+    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{C3498DC4-D4DD-4ABF-A6C1-4FFB4879426E}"/>
+    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{48C15595-2D09-4811-8D20-DF728E81D78A}"/>
+    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{B2830596-3EA2-416C-A196-931F448EEA82}"/>
+    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{657C6136-204A-4085-8EE4-4990FD547D43}"/>
+    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{A36B4BCB-C51C-49D1-8717-267BE9E16ABB}"/>
+    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{0A5086A9-F166-4399-82CC-7CFF352C6CF2}"/>
+    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{184D36D2-A956-43FB-9465-7786FEB70E1E}"/>
+    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{28EABBE5-91F7-44D9-BE00-8E0D131D44D1}"/>
+    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{9E3B7B35-9404-4113-99B9-04149326ABC8}"/>
+    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{64C3200F-CA29-4461-9305-C4B05FDEDCBC}"/>
+    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{DD675132-D7A0-49EA-92EB-71ED119DD7E0}"/>
+    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{A530F427-68D4-4DB1-9C55-D00235DCF0A8}"/>
+    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{37D07D07-88D6-4C4A-8EC0-ACD2149BE115}"/>
+    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{F6472E59-DB46-45F4-97C5-47D512C6BB56}"/>
+    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{5FDDC544-44FA-449C-A94D-00CDE51B1E3F}"/>
+    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{0EC2007D-CC82-4008-B5D1-E89ABB98E8DD}"/>
+    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{E1C89FD7-24CB-408C-A70F-63763CE7BE4E}"/>
+    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{2D2C436E-4B84-4FE4-8346-4F89FB375080}"/>
+    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{B01EF244-DF41-4880-8E7D-01E2275046DD}"/>
+    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{937F73DC-FD98-4A0B-BD88-968B9830DF98}"/>
+    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{4AEFD37C-E0AD-4E72-AE26-B445656F57BE}"/>
+    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{DAB0FF1E-FE0D-4D4E-8344-CBD5C99336C5}"/>
+    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{760B19C9-7F25-4A9F-AE91-005FDB899593}"/>
+    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{469A439F-83B0-4870-9B71-58A7AB0827AF}"/>
+    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{3863B75D-0ECD-4633-B595-73389626101F}"/>
+    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{94F43D6D-6EFC-4503-9FB9-0AF42E4B8DD6}"/>
+    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{84EEE0A2-020A-43D2-9DA7-323879DB6CDC}"/>
+    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{F6AA23AC-336A-4158-991F-1933145B4BEC}"/>
+    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{C4A745F7-FEFB-4E6D-8018-EDFBDF2AB02C}"/>
+    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{E2952F06-19A2-46F3-8D49-F368A5B5EFB2}"/>
+    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{56E1A122-FC42-4EBC-9B41-24F3CE277743}"/>
+    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{FB5287D6-008C-4D66-B737-A3286112680D}"/>
+    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{FBA80C5E-B4F9-4E9D-9C23-110DF033046C}"/>
+    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{B222BA59-BBD8-4DA3-B441-D8FC13B8A905}"/>
+    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{44983526-445E-409E-98F7-0ED5470DB49E}"/>
+    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{5B299A75-E889-4EF8-959F-43EF90B37071}"/>
+    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{332A0327-988C-46AB-9ACD-F054A4DACA9D}"/>
+    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{48AA9F49-1251-4BC9-A7FB-C4D64F8F4B3E}"/>
+    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{C3A611B0-99A2-417F-B589-F30FE78A1558}"/>
+    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{A36EBBC7-71A4-455C-858D-1E1945EC7E93}"/>
+    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{63DD9593-C0EF-4E68-8B6D-A4EB3150BE76}"/>
+    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{F3AFAC39-A99B-4C94-BED9-A8A7D2C6AF74}"/>
+    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{C6162EB4-BD46-4CD8-BBBA-AA43943E6537}"/>
+    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{9FE31B47-62BF-4A5E-9EAA-B74C6C52808A}"/>
+    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{E53D3B84-67E0-40BC-9CC2-5F37B796A06F}"/>
+    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{EA940CB0-656B-4E24-8DF7-2AB7D5280BC1}"/>
+    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{FD59E745-CFA6-4DFE-B52F-22CD9F6CF725}"/>
+    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{952C42A7-1F5B-447F-BE14-E2C47A361775}"/>
+    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{94163A8D-3571-4815-B7FE-5CC807CA7315}"/>
+    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{ECFA6289-E039-4E35-9A18-7D132B53513C}"/>
+    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{F9E0E1E1-0799-4981-8E07-55AC82E173B9}"/>
+    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{C7A67AE1-7D25-4B80-944F-DD32624C232B}"/>
+    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{B8835C12-8A1D-4A0C-BFE4-A44536A7133D}"/>
+    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{A5B6A47B-AFA3-4701-B302-922244DF881A}"/>
+    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{74A50165-F28A-48BB-BBD7-774070D75F95}"/>
+    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{8643EE84-937E-4503-A54E-5C90DE8A3B3E}"/>
+    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{2C878C0D-C703-4938-B10E-026735AB535A}"/>
+    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{D22979EB-2E93-4254-BF3A-92502884196F}"/>
+    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{B9719964-43B5-4EA6-A1C5-25DEE02D737D}"/>
+    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{E30AC724-D67C-41DD-91DC-2EFD6471C854}"/>
+    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{8D5B5F79-A487-4D37-87B3-8D8294BEC42F}"/>
+    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{15F55F21-E915-4499-AC16-80108DC0C685}"/>
+    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{77B59923-5D8E-4BB3-91D3-998235CFA485}"/>
+    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{BF8D41E1-D356-440A-A877-0A1A8B589D25}"/>
+    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{644648A3-E70F-46F3-8099-4FA017978F82}"/>
+    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{60D4DAD8-2A5B-4BC7-B522-F3B274C2B0E9}"/>
+    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{5C4A28F7-CFF4-4067-928D-DF2CEDD5AF1A}"/>
+    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{D18C8E85-1115-4DB7-A3FB-CD3FB8D928ED}"/>
+    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{2A9D18D0-AFD5-4624-AF52-FD5E33CF6200}"/>
+    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{2A79B856-89F8-4EAE-8A81-D617A853314B}"/>
+    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{F8B3B6E5-6139-455A-A643-8FAB40067AAA}"/>
+    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{3699D8C6-3AEA-4093-8BE0-B22E51C0BD48}"/>
+    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{35C52E9D-128A-4250-90A5-8E7D0091CCCD}"/>
+    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{04457381-B1B3-4E34-A3F6-2B3118AF6B61}"/>
+    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{46368B88-72F8-4E5E-A3FF-4EBE3C38B411}"/>
+    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{74847BBF-52DB-453B-BEB4-9320A8A62FDE}"/>
+    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{DD94160A-5AA0-4223-87D5-3D6582D17065}"/>
+    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{088DE059-230A-4497-8C10-C356A4E3C0BE}"/>
+    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{D0A6967C-3637-4C73-89B4-F30D63A81CF9}"/>
+    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{833CF146-7206-476E-9335-4B4E57C95378}"/>
+    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{F37B3E3D-6ABB-4C68-A6F4-A6FB633A91E9}"/>
+    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{D985823E-D474-49CF-9AD6-9CB8654388F5}"/>
+    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{AA5A7DE5-3032-4D67-883A-8BE43C847DFB}"/>
+    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{B1F78705-CDC0-41E2-BF0A-331A3DDDFE03}"/>
+    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{6FF835BD-7764-4446-80F3-041C0116B30E}"/>
+    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{11671E1E-1C52-482A-A88A-5112A851DAF1}"/>
+    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{D0FD16B5-0291-42FA-8FBE-765BEF131680}"/>
+    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{9FAC35BD-DB0B-4A8C-9DB8-2DFCB9F4CB69}"/>
+    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{797E569F-EFD8-46C0-8E04-85A4A50A7CA1}"/>
+    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{7A5C8C51-1445-432E-B56D-E7165446B490}"/>
+    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{3AFF4169-2222-4F95-97FA-E95001DABC1E}"/>
+    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{039A6187-D091-481B-8335-3DA3AC252BD6}"/>
+    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{57721AD3-E352-49A5-B0E6-8648BA809A48}"/>
+    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{B0CBC9F3-F1E7-45C8-80E1-F428F7A310ED}"/>
+    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{339DC8DE-1FCD-4F1F-88F2-6EDD785CC057}"/>
+    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{F95E3010-E433-496B-9FC3-852FF8CBE0F9}"/>
+    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{C4458D47-7AE8-487A-AA4E-CFC6C86925F9}"/>
+    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{A30994F3-4464-4FE7-B83E-8E3E59C6DE89}"/>
+    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{8A702EB3-E1AE-47FB-B230-308C4ED52096}"/>
+    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{74BED2FC-F520-4E6E-8A58-46EA818F48D2}"/>
+    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{34C9D3C3-4601-4D0F-A074-5A1D128CE4C5}"/>
+    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{A717A725-0E21-49F5-8F7C-A5DEC22F4C59}"/>
+    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{F0EE0AE6-5A10-4C1E-A4B1-3349014998C0}"/>
+    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{745EBCB5-4D07-41E3-B85E-34FBE29E9F55}"/>
+    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{EC57AE99-F8EE-4C20-928F-F3EB99ED1926}"/>
+    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{CFA851A3-0C38-478A-9DC6-025269199692}"/>
+    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{8C06E1DD-9661-4865-B61C-406AC658CBB7}"/>
+    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{33D78E5C-869F-43F0-A2E7-09F248D39559}"/>
+    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{74CABB5F-6D02-4EB7-83B1-2712A08871DE}"/>
+    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{444E201C-A3C3-4EEE-A8C1-5BAE983FCEC3}"/>
+    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{1E3FC478-8C86-4494-B2E0-F3D915977240}"/>
+    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{6101F952-5303-4C49-96DB-688EE6EA7349}"/>
+    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{E14BAD02-BA16-4EDB-BDAE-A08F07C3C56A}"/>
+    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{09437A5E-7153-44F8-A8BF-63BCB3918479}"/>
+    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{101E32C1-49B0-4552-AD7B-8FF52A552A87}"/>
+    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{9C1F9349-851D-4B40-AC46-B2E11E52C0E9}"/>
+    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{F3B95B19-05FE-4C85-B62F-B670F23460A5}"/>
+    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{E40E86C1-1BA5-47AF-A1F9-D5FBB77A2A08}"/>
+    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{900A2D01-CC53-445C-A846-7086FC577468}"/>
+    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{57826B27-9EBB-437D-BEC7-9737FDAD6E6F}"/>
+    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{05E9F03A-192A-467E-B1BD-0ECDB23753C0}"/>
+    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{69A76B69-A94A-4BE0-94B6-407A3061B36A}"/>
+    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{15031982-6CDD-4A66-A6BC-7C1D3BC12BAA}"/>
+    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{6036BE64-699C-4A06-B504-CE14914F22FB}"/>
+    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{83D7FDC5-B25F-420C-B895-9947F2E5844C}"/>
+    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{2AFBB254-FBCE-4233-B08F-4EC2E2860637}"/>
+    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{B4CF8408-B335-45A9-BF6A-B4A462F1C061}"/>
+    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{E6211595-092D-4874-92A2-4C7CBC2EB69D}"/>
+    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{11CBB1A6-891A-4374-9B03-1CAF62BA5A97}"/>
+    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{82AA4C78-069B-474C-83C2-8C9B8F50B0AC}"/>
+    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{3F603674-972C-4C2F-B9DF-2293DA1D6FB5}"/>
+    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{91771828-778A-40BA-AFFB-10ACC0B294D2}"/>
+    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{3C7BC8FC-B428-4DD5-9262-18521CACBA5E}"/>
+    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{F86A066F-9E45-4517-9153-7428F53A94B9}"/>
+    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{B511E96E-924B-4F1E-9B91-CB7CE23F6C8B}"/>
+    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{D29F9CD1-837E-48C4-9D8A-6F1A57A78F76}"/>
+    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{282680CB-A496-4BC5-A850-31A4335D9BDF}"/>
+    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{E3A3D49D-610E-41AA-9B20-E093D8A0D18F}"/>
+    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{BA817FEB-C0A5-4D3B-9F5F-63EEC07E8F9A}"/>
+    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{C43C1AB7-E82A-47B2-8155-58B63C1404DA}"/>
+    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{173E3F4E-8944-4A72-AD2F-2E0DD4451CF0}"/>
+    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{4D6FB0C2-E417-4AFB-988F-8ED811657392}"/>
+    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{140593FA-F7FB-4212-948A-38DA2187B1D2}"/>
+    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{CF9814F4-91E1-4C90-AFBE-FFFBD0EA69EC}"/>
+    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{236CFA28-6549-44BC-9483-DC514770BD12}"/>
+    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{BB5F8C24-7C41-47E7-8182-49BBEBA9E403}"/>
+    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{AD34F542-9B39-40E7-B826-1853F84A0389}"/>
+    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{2E8BC7D8-0A2A-461F-BF17-AA4E6EA44DA1}"/>
+    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{09E4B4B3-51A2-41ED-92F7-133A0F805088}"/>
+    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{FFCFBB9E-279C-4713-98B5-324124A60787}"/>
+    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{663874A9-4CA8-420A-9BD2-619DE3E953D8}"/>
+    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{2CB3838B-7921-4AA9-A78C-1B12DDFAAB59}"/>
+    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{83730E34-489F-44E6-A21C-6D42EADEB231}"/>
+    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{C8E30ECE-45B4-4E41-843A-8ED821D90AC5}"/>
+    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{1B4F91B6-377B-4B94-9E6D-266E725B14EC}"/>
+    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{9F406FF3-3904-4D60-AC7B-0E49A099B265}"/>
+    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{8AF1E31C-473A-4975-BE75-C17CFCA05DD1}"/>
+    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{CD5B6900-89ED-42FB-B953-32D25BB96BF3}"/>
+    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{7EFC7064-FF7C-4438-93A8-16362FCA1F86}"/>
+    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{53840CE7-AD6C-4F8E-8A40-1DD1A1B73B5C}"/>
+    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{18001D1F-1959-4FE0-A5E5-E8BBBEE4C36A}"/>
+    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{56A236BD-47D7-4BAA-BA8E-4D5326A5CBD7}"/>
+    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{663EDB01-A68B-4AF0-90FA-D0E7B9B24236}"/>
+    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{453ECCE3-C310-442C-A224-42015421531A}"/>
+    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{71C30768-5727-4889-B839-C608A184C7BC}"/>
+    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{7E1A9C96-65A8-4648-B827-28EDC1ED8DEC}"/>
+    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{28872254-080F-457C-84B7-F10E0918D148}"/>
+    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{7A78F034-88C6-419F-8AE9-DA9463A8A781}"/>
+    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{0A607850-C50B-4935-AEDD-82280CB651F3}"/>
+    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{EB8F3D78-158E-4593-A576-5F245E9F9F29}"/>
+    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{001DD59C-DA2B-4B57-BA40-DC2E8BC31A05}"/>
+    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{68E8336E-989A-427E-9B09-AFF243EA32AA}"/>
+    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{8C53B17D-8C7B-4B40-B41C-89CC9CCE6C27}"/>
+    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{7D6FB443-F3A2-40AB-931A-C0D072C8C3E7}"/>
+    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{5E5F91BB-0F08-4764-806A-0E364F9175EE}"/>
+    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{24540104-37B5-47DC-90CB-DFFB0667D3D5}"/>
+    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{93E7215A-7E4E-465A-ADD7-EBF6AE816484}"/>
+    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{F76B012C-CBB3-4D30-A4F4-7B23AFD1D7DE}"/>
+    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{7D3B280B-BD8B-4064-9DF4-8B2417285913}"/>
+    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{9D90D241-8952-47DC-ADC0-20B5D151EE15}"/>
+    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{3A9E35D6-8C76-4161-942C-F4E47120C7BB}"/>
+    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{D2246ACD-B767-46C1-B95A-0DA4D9A36562}"/>
+    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{A95C9E38-EC0C-4C98-805D-CD843699DD0E}"/>
+    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{34049A2A-5A46-4708-B5AF-9EEDE0198805}"/>
+    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{06B114AE-A7BA-4C12-A160-9896139E3A7F}"/>
+    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{F92EB04D-18A6-408C-857A-A2C45F49F05B}"/>
+    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{AC54BE52-565A-48BD-B984-A402F841746E}"/>
+    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{3F9F289E-8372-4F41-9523-D12602515E9E}"/>
+    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{C7E209AA-6185-409F-95BE-2DF5B5AA61AE}"/>
+    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{DD19F2BF-9B77-4A71-863F-134088E6AD6E}"/>
+    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{FBBDF71A-B751-4EBC-9DB5-B1E0C8871431}"/>
+    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{24238FB6-7F46-4B84-89EE-E78F2BA1D1E4}"/>
+    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{FCC451B8-F835-49E1-8815-35A21D501697}"/>
+    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{C91C43DB-AE3C-4D29-8B63-55079D9D5939}"/>
+    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{2FE0BED9-C357-4BBE-A95C-D0311AF543BF}"/>
+    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{D5502ACE-CCBF-460F-87F9-94B254E42C4D}"/>
+    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{A2BF3915-4AB3-4566-ADA1-C1BB0CDAE289}"/>
+    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{189013FD-31AA-4CA1-BF7D-1042B1F86AA3}"/>
+    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{6B12A282-04AC-4020-8665-D5337D4315F1}"/>
+    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{4DAF0C1D-A2B7-4F03-BE77-808D64F1EDEE}"/>
+    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{39CCBD56-163B-45A6-BF4B-201E75F2E092}"/>
+    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{9BEA5CBC-AEC3-4716-9E7A-7FE574C951AF}"/>
+    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{528A89B7-ABB0-4440-BEF4-440C624105D5}"/>
+    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{A950D9E2-B238-480B-853E-E4D435AF42F9}"/>
+    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{3ECE6489-C878-45A9-ADC7-6529EFAAE333}"/>
+    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{602E9D6C-6553-4DC2-87AD-385413FF64BC}"/>
+    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{A7B89C44-3864-4DFE-87B7-5870E11193AD}"/>
+    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{CA6DC3E5-9C67-4137-9E9E-236F9DC13801}"/>
+    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{108E5805-B54E-4D98-B521-B8E0F23EC1C8}"/>
+    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{E6A94E55-2943-46BF-9E1F-5273D68766C5}"/>
+    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{6E38A382-8B9D-453B-ADBB-9C3B1FFCC628}"/>
+    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{F645CDFE-583C-4FD1-8189-C5503D599B63}"/>
+    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{A2311519-87CB-4F8B-A173-B80ACBFB2BF5}"/>
+    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{0160E74F-01F8-40AC-82F3-7A153068DD8D}"/>
+    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{95A153FA-37C0-474D-AF1D-C1949729A478}"/>
+    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{6B4B554F-E483-42AC-99F5-73780F266591}"/>
+    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{63525E4C-2FA3-4F9F-A0C2-16CA2AE5365A}"/>
+    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{AF777522-7EE4-4A2A-BEC7-4541A13AD375}"/>
+    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{F2425208-E9F5-48D7-AD02-7BE5A1EC462C}"/>
+    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{38F0113E-7B3B-442F-AA1E-255EB81ECDFE}"/>
+    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{CFCD6A70-C177-471C-9ACA-51F8F71EE393}"/>
+    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{5157CD80-E991-4182-8D7F-05214401F5D4}"/>
+    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{39BFE576-CC4A-4237-B2F8-15932A4BA62C}"/>
+    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{9A732C93-56A5-47AD-BD02-9A1E52B0C1D9}"/>
+    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{FF5ACF91-EDD0-498D-A94D-B37A31A15B7D}"/>
+    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{EDB8DE1E-DB83-40CD-A53E-7E87C924CAB5}"/>
+    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{BF0D28F6-6B41-419C-819F-324EFDE70F6B}"/>
+    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{781F9850-60B7-4E87-AF05-00E5679C870A}"/>
+    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{EDE3CC86-5CEB-4A7A-BD1D-4A24D4446833}"/>
+    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{C1E8C6B0-B221-466E-BD5E-EC218DB46AD2}"/>
+    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{AD5CD903-F2D1-4B95-8818-2F18F3CE56A2}"/>
+    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{43A5DB40-F73F-4CE1-8C68-718CD7E76654}"/>
+    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{2CEADB3E-9F4D-4A5A-A320-7BC7CC90713E}"/>
+    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{81D9E68C-5134-4B9D-AC22-5AACF94E5892}"/>
+    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{8E52B9BB-BA21-4915-A2E1-A5A18EEFC9C7}"/>
+    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{3FA3C283-9EA1-47B2-AD4A-B5E516C1905F}"/>
+    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{A4142024-E933-4FF9-9731-5E73A589FE24}"/>
+    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{4E7DE45E-12C6-4465-8129-AFFCAD3EDF53}"/>
+    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{FC1E564C-8F03-43AA-B8B2-39808B76CFA5}"/>
+    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{B4A78DD4-7698-4CCB-8C68-19864A3B56EB}"/>
+    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{4D08C1D7-E63E-4406-9366-8BBF407EFD29}"/>
+    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{79B19802-F84E-4C24-839B-12F482A980D3}"/>
+    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{4AC0714F-D732-4F8C-8FEB-5070C1EE0784}"/>
+    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{0F52DD2B-CE8B-4887-B9E7-4C6C3D4FDB70}"/>
+    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{454660CF-4BE8-4F91-BB7C-7993231BCB84}"/>
+    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{9FA56135-4EC7-476F-9EA9-6C73064B6AD2}"/>
+    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{840955E5-5030-4346-9C50-3BA0160F0BCD}"/>
+    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{AABE3DEC-0031-4107-A75F-7D750FD5658E}"/>
+    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{B18B90BF-F5B8-4A72-B64F-AC5F9855AD37}"/>
+    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{66A0A730-CBE7-4806-B747-FA11364C0DF7}"/>
+    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{4566BB35-4F92-497D-B325-07C635D93CFF}"/>
+    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{09A48C86-6748-4A1B-832F-C9D31CFC91E6}"/>
+    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{6EC4E450-791E-4389-9897-78041B486289}"/>
+    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{AACE02A4-7368-4A25-9E80-E07DD2443C54}"/>
+    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{BE86B91F-2F41-4532-896F-10F9A22B9D3B}"/>
+    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{4124D9F0-AA3C-4F40-BEF5-3DCAE8819281}"/>
+    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{316DF98D-4C96-4335-A1C8-D9123BDB102B}"/>
+    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{9E63C537-0119-4E2D-A50C-A9867152765C}"/>
+    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{C59793C9-96A5-4CD8-AA34-FF84F5C2CC94}"/>
+    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{E0142E53-CEC6-4B40-AC89-56933FCFB4BB}"/>
+    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{875F1F04-F0B8-4D84-9110-D6603EF9E72C}"/>
+    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{7238C701-CDBF-4C90-AF13-FB62A526241A}"/>
+    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{009C0E0F-DD55-409E-A826-EBDBC11D4FD2}"/>
+    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{7601288E-3E6C-4B57-87BC-D6698C70BF22}"/>
+    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{F0A4BE7E-61B5-466C-A74D-F8A183040323}"/>
+    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{F37A2971-52AC-44E7-9791-2E7E2C7CFA51}"/>
+    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{6EB9A689-2BE0-4C50-BADE-8440CE26F7CF}"/>
+    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{77C0F5B5-32B5-49D2-88A1-898B45F89321}"/>
+    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{7A37B585-B49F-49D0-8EE6-E16D45FE71E3}"/>
+    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{E8DA6E25-F419-435D-ADB3-D6C8A8EEF00F}"/>
+    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{E46391D6-3FAC-43F5-A557-CDB334AC56ED}"/>
+    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{263B1E5A-FE7A-4012-B977-F47F101FB34F}"/>
+    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{201255BB-B8DD-44C4-8CD5-8B742C8E4CAD}"/>
+    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{40DAB385-51F8-4D3A-89ED-ED7D4E9A195B}"/>
+    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{1B377359-D889-49D4-910E-103317368ED1}"/>
+    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{10AEAD31-40AD-4BFD-B166-74543885C069}"/>
+    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{35C44212-BE05-46EF-B218-65DC1F37851C}"/>
+    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{DFC3A22F-FD38-4E2E-A560-8F1BEAEBA9C5}"/>
+    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{3ABBDD13-7699-482C-A711-E9EEA6EA9724}"/>
+    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{B3444AC0-454E-484A-8B3B-C88205AE61F2}"/>
+    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{29C8DC47-D2EC-4AEA-9B17-1A4DB394240B}"/>
+    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{1FA0675A-EDFB-4531-9DF4-C5B17A814539}"/>
+    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{D2CC77D9-9F0F-4611-8448-428048F6DD71}"/>
+    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{735C1DDC-56E9-4226-A39C-63A828BE25F3}"/>
+    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{9B407359-EFAF-4E5F-B9FA-E7DA21BE8719}"/>
+    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{CD6077F8-5670-4E5D-8018-F22B8D8B2D12}"/>
+    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{FFC566AE-5947-47E4-B7E9-D4D8A6C45BF1}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>

<commit_message>
Reorganização do mapeamento e ajuste na fn processar_arquivo_xlsx
</commit_message>
<xml_diff>
--- a/src/data/uploads/Project Room (Jira).xlsx
+++ b/src/data/uploads/Project Room (Jira).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/paulo_vieira_d_silva_accenture_com/Documents/Desktop/Automação_v3/src/data/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BED651C-71F6-4BB4-93B2-FF25E875FC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{299B5564-187D-4A44-9E34-727D34BB76C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{42D54320-9212-40D4-AF32-F5168D11473A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F86A383-3699-40A4-8BE4-07CDFD4D95EB}"/>
   </bookViews>
   <sheets>
     <sheet name="general_report" sheetId="2" r:id="rId1"/>
@@ -10620,7 +10620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB8EDEF-10D2-4D77-B049-577CDD18516B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54A52F2E-3353-412B-B072-36570D4E60CF}">
   <dimension ref="A1:AR578"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -66555,583 +66555,583 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{964643AB-1B7E-420B-93ED-4955A44BBDC6}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{3DF2B890-A4C7-4DD0-8CE8-699890A28E3D}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{12692B96-E471-4EDD-B26F-404DC87539B4}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{98CF668B-EC14-42AE-8530-4F30161E9F97}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{810699AC-6D13-4464-956F-40924C959E90}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{F4750573-FB68-4544-B158-1DBFC29D18BB}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{257F4E01-BE06-41EA-ADBC-6A9C49B1076E}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{423A91A3-2150-4D10-9654-F7B64EF35741}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{AF752B9C-2857-45B6-9D98-18FA544C9A9A}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{1E80679C-77FC-484D-BDEB-72A0BBABE8CC}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{45151FD7-C631-4A84-9E9E-64392B4DC884}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{08827021-17B5-4652-8C66-54B234160F8F}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{7ADC403F-1849-431E-BC6A-0F93A90065B6}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{F06CE729-D5A6-4CFE-BA5D-7B07DCA4183B}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{C17773BA-9937-4BC7-825F-CB4D4BC4F698}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{E89C1453-9DCC-40A6-9D34-14993740E8E1}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{5004BD90-6012-4FE0-B545-8DEBAD015A70}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{885ADFFC-85E0-4F79-8019-100E2B210176}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{E6556AC6-88B5-4914-920B-A0F37911E87B}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{3832504D-3722-47AB-8212-02E33AFACD03}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{2251E47E-B1FD-4A40-B178-344CE9332C02}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{06AD0C5D-EAED-449E-885D-984AB85535F7}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{19473D0A-18C3-448F-AFC2-337D0E23B48E}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{A55F6DED-BFD9-4451-825F-CB01CF9CBEC5}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{8ED660FE-1A0B-463E-AB64-C4072E620032}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{9A07B660-C6AA-40E5-AF14-CBDC48265955}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{92F2DE06-0447-4DFF-A2A1-19632E0701BB}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{0F694B14-0FD3-4F09-BB56-890CE7AE099B}"/>
-    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{69E6A97D-F596-4D3F-9A20-4FE971C61A2F}"/>
-    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{A83207F0-B6B3-4DA8-93B4-BC8B103AB3B6}"/>
-    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{9C2EF6A3-5C54-4AB5-B44C-4F0594E82998}"/>
-    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{A7C11260-B0B1-470F-A8EF-6BEAA5527727}"/>
-    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{D31C73CD-0496-476F-B835-EA51DB05C970}"/>
-    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{EC8F109E-A95E-47D7-9CF7-3FD907A7B6BE}"/>
-    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{04296969-042A-4322-993F-B3DA0164F0B4}"/>
-    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{B22C11A6-7E51-4397-8AD2-B432C2DD566A}"/>
-    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{0916D9F0-91DB-4D18-A2F4-0BF5EC365C48}"/>
-    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{2B0D2C2A-C6C4-451C-8F35-7D6CDAC65203}"/>
-    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{AEF8C49B-D741-4D9B-ACA8-CE3069697973}"/>
-    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{027EF08C-4803-4F9A-A64B-066E3AF99847}"/>
-    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{ED32A1AA-0448-4CAF-8F6D-4977B7546DEA}"/>
-    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{BD0AD01F-E290-4953-9808-3290131EB13F}"/>
-    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{DA6A874E-ACEC-4424-A564-074C81521BC4}"/>
-    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{E277B268-7460-4E75-9005-9770F90E026F}"/>
-    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{A8DEBD82-EA4E-45D5-8376-0A846B6D2D93}"/>
-    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{1EB77ED9-8A11-4DA9-A074-BCEA03183812}"/>
-    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{29287ABD-3A06-42E2-964F-449C6C65B1ED}"/>
-    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{45E1F77B-18A5-4CD5-9770-AC191E37A4B9}"/>
-    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{3BE11D19-2072-4E14-A906-A11BF9DF3629}"/>
-    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{4095F2F9-68F6-4DBD-A40B-38A262D6D165}"/>
-    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{88E64637-3A83-4794-993E-1908F6BB0A1C}"/>
-    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{FFB369D3-B05E-46DA-B0E9-6859C49240E1}"/>
-    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{39BB9FD5-5217-4723-AE18-D29637B860B8}"/>
-    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{FE8BB845-FE48-43E9-B3C1-88CD061699DF}"/>
-    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{8A537231-3C72-45E2-950E-F768E78B689A}"/>
-    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{A24C7836-EEDE-48C8-B454-C029C4FCC99B}"/>
-    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{03D7D093-6D81-4B92-82A5-48B01C633EF3}"/>
-    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{BB790EDD-FD87-4D3E-BDA8-C0ACA242C529}"/>
-    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{A5BA1325-5493-467B-B048-F28F96FD996F}"/>
-    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{CEEFC114-3271-45C1-A7E2-E88FA96EC780}"/>
-    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{301E3B82-7F06-4747-92ED-84721948B060}"/>
-    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{C2AA8D6A-88B1-413D-8D2E-8AA0B04FAF11}"/>
-    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{A3B99878-9E44-4612-90DB-827BEDE4DFF3}"/>
-    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{EC72FA0C-2CCA-41F5-A65D-F9AC09B89B08}"/>
-    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{D0931C5B-AF63-4941-B429-5707FD8F4027}"/>
-    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{C2BABFF3-0AE0-4178-8F28-D97E4FD03594}"/>
-    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{65C41C8E-FD31-427E-AEA8-7B80CFB1C866}"/>
-    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{C9E1394C-2A04-427C-A221-A5CED81F8C27}"/>
-    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{61596100-13FD-4BE5-B627-9958FC9FCF98}"/>
-    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{FCA362C6-B39C-448E-9B89-466A2542330C}"/>
-    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{DE37F0AE-6291-4E8C-90FA-1A329373A72D}"/>
-    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{488741B9-1E08-4FA4-903D-01990E920C9A}"/>
-    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{6BEA9D24-7AC5-45A6-B0FA-F2AA7BD7D05F}"/>
-    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{4F34534C-5921-4701-9BFC-DD1A36891D18}"/>
-    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{B9D06EE5-70CC-4433-A182-737D42554251}"/>
-    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{B82C4BCB-8A76-4C0F-990F-4FF25E50195F}"/>
-    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{A69BC286-E37A-484D-9849-DA5075298523}"/>
-    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{0C27E583-DEB4-4D58-B5F1-BDE50C2E4300}"/>
-    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{A85317C8-D16E-4B40-A57C-D67DFE698C63}"/>
-    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{9C1E9703-0C0F-4E07-86FB-6D65FC3B93C6}"/>
-    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{B5E3D3E4-22E9-47FE-A049-B306A7917136}"/>
-    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{DF2D7940-4561-4DA3-A8D0-CFF3AC37B4D9}"/>
-    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{F6007FE6-F1F9-41B2-BA6D-5AD5D2E35F7E}"/>
-    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{1F65CB80-01F3-4847-B6F1-005B733427A1}"/>
-    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{953C8D8C-C553-4F4D-806D-89917838EF3A}"/>
-    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{30061B2F-0E83-41F2-8905-9A0D094098D7}"/>
-    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{192F216B-B35F-4982-BB1B-695758C715FF}"/>
-    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{663FEEE4-AE54-4289-B236-DE16C115B8CA}"/>
-    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{5F0923A1-EC1F-4B3A-9E8C-22FC8AB187C7}"/>
-    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{33A15260-01A9-4629-AE2F-60E568E6D8C0}"/>
-    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{F1146180-205B-45FF-B0FA-8F2EA87A88FC}"/>
-    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{28AFEAA6-7738-4ECA-B836-B5296E3A3C07}"/>
-    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{FCF97132-F868-4BD6-A0D8-DDED3A273EA7}"/>
-    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{2C8A9B33-8BCB-45CB-8DF8-AE5AD2B60BB8}"/>
-    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{61592542-DBAF-4EE2-8FFB-AD48402234E4}"/>
-    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{BE33C761-8175-4BF2-8EE0-4726141456B6}"/>
-    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{B5C6171B-DAF6-47CF-B222-7F5F3279D70E}"/>
-    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{37DED0A6-8FEA-4FE6-9BDE-7E3062F2EB6E}"/>
-    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{857C528A-83A9-457B-A4BB-FFFDEBAF6E33}"/>
-    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{61671816-D84F-4257-9E04-DC6FAB2AD850}"/>
-    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{89B1704C-8F71-4A6C-A722-727EC9F208E7}"/>
-    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{664BEC39-5936-47FA-B012-0550F7439AE5}"/>
-    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{E1DA38C3-DDFB-40BB-81CC-507C54861F1E}"/>
-    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{DA224FD4-E4D3-48D1-B8B2-D7C9B6CF9F11}"/>
-    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{7770BABD-D2FB-4685-AE01-B979F28CEA0C}"/>
-    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{1E59A938-9165-4FB6-B661-F36F7E7A6E3F}"/>
-    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{020C48A9-852C-478B-8DEF-1833F8B3B9A4}"/>
-    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{FC27ECF9-CE3A-40AE-8A5C-2F63BB20513B}"/>
-    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{48D82FD0-A734-4D42-BA83-62F10D904CC4}"/>
-    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{5FD90C13-9EED-46A6-857F-4A7373C24B94}"/>
-    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{E5385DF2-2A78-4BB1-8805-C68957C7FA03}"/>
-    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{C58BD3A4-B7FB-49D9-BDC4-547ED4DC4AFF}"/>
-    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{4B96E329-0504-44FF-9C6B-9B21AFE43FD6}"/>
-    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{17FC97B2-030D-45C9-977E-F1394D34A56F}"/>
-    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{A2D1A69C-FDF0-4E04-92FA-E878463E74DD}"/>
-    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{50B407A9-7E38-478D-B740-E1E447924BCE}"/>
-    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{A35385D8-06F4-479F-91E4-429CE32CFB79}"/>
-    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{DB745693-8B57-4BA4-9701-2C05E5399572}"/>
-    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{FA8CFC8C-C3B9-4960-B23B-72009308C1F6}"/>
-    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{58F6831F-459E-41D7-B0F8-82017E424FD9}"/>
-    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{5E3C948F-4F81-4AE5-8BA3-22D4DD137CE8}"/>
-    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{1AC83455-181D-48E2-8B91-F0472CAA7CEC}"/>
-    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{B18FF758-C2E9-4BF1-9907-42404F529998}"/>
-    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{F2048E4C-A3F5-4EB0-9191-D11290353D0A}"/>
-    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{AC5818A5-0758-417C-936D-266CB5275464}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{5FE34769-517C-4387-884D-5A2B7C273499}"/>
-    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{1934829A-BB61-4632-B3E3-5D3595AD3A62}"/>
-    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{D2A3211D-B85B-460E-885B-DC99303A45CE}"/>
-    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{C8A1D828-5C6C-4FB9-8B79-276116590FC9}"/>
-    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{59BE0F33-88B0-4AB6-8BF2-81654D950E33}"/>
-    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{3CABB914-E445-435E-A60A-EBBDDEDC06E0}"/>
-    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{030804B4-9B28-4AF4-B1A5-BB1E1C9052C3}"/>
-    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{478E91E5-8955-4D27-9131-46A82DB37FFF}"/>
-    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{F52ABF13-8482-446B-AF10-4754FCA43FC2}"/>
-    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{81AA5E1E-98CC-4930-BC9B-01DECC6BD1BF}"/>
-    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{58F2A401-AE2F-4DF8-BDE5-FFE883585814}"/>
-    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{7450672C-648D-448A-9846-826B594B439F}"/>
-    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{E31F8431-0D0F-49B2-A495-6F97CAE511E8}"/>
-    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{00D2646F-BB25-44AF-97CE-C92F705830CB}"/>
-    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{65CABFA1-8839-43F7-9FBA-5BD9C09DF396}"/>
-    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{AC36FE7D-411C-43F9-A044-0292D0CB0A76}"/>
-    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{AD22DD14-8D24-41CF-B9EC-4805052B0A12}"/>
-    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{8CE0747A-51C9-4128-BA9C-E955DFE9D60B}"/>
-    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{00062002-B693-40F4-B270-EA55D5F8644C}"/>
-    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{2118450F-F97C-4F79-9F7C-5D8310779DD8}"/>
-    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{00053DE5-619B-4D95-BFBB-70038CD4E0B7}"/>
-    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{AE435CD4-6404-42A5-A738-C22950D74800}"/>
-    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{2920ADE0-EA6A-454E-A015-800F7CBDC744}"/>
-    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{EF78B3AD-665B-4966-9D07-F03CDE294F14}"/>
-    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{0ABA0723-EBCE-46B1-BE0C-1DCF639EA8A2}"/>
-    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{E5A32ADD-08F6-4B38-9200-C054B0F9FC89}"/>
-    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{89AD9649-2D17-4637-B053-71D702A83CCC}"/>
-    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{41A68358-B198-4F6D-B89E-C6F665E59148}"/>
-    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{D5D32F1C-9031-44ED-90F9-1BF460385DDF}"/>
-    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{AE75E35C-DBFE-401E-970B-D4503048F18A}"/>
-    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{FD8C5F3E-1C9E-4D0A-B455-33AB06E459EE}"/>
-    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{6C1B8697-2791-4792-8790-BA0F7A9DE567}"/>
-    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{86772883-9DF6-438F-8D51-98ED13CE9398}"/>
-    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{9E00F9B1-AC9F-4F79-B0B6-3A99E7A4EFD0}"/>
-    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{2B604280-7FA0-460F-86E4-C03C8A07195A}"/>
-    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{40058F9C-8FDD-4EC3-A90D-660F6DE7B4A0}"/>
-    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{F9C3A0CF-63B3-455E-AFDC-3F1E5883352D}"/>
-    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{C2669817-1ABC-4E9C-B51F-422EEDC254F7}"/>
-    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{65983AF9-6CB3-4B19-B8F7-0C6A5CF57ED5}"/>
-    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{02B613D1-D456-4EC8-ACFC-39F68AEABF92}"/>
-    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{506E138D-CAC4-4301-AF9D-331063527AFF}"/>
-    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{2036AB21-E602-498D-9A39-E8415D19ECC8}"/>
-    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{C80789C6-6CB6-4472-AF31-B9B54AE09FB6}"/>
-    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{9E858282-7450-4D76-BE12-1772A5BF4BAB}"/>
-    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{F18CCAA2-3017-435C-B8DC-7795E29289FD}"/>
-    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{FF7585E1-812A-4F35-9011-A0B108BB15B0}"/>
-    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{2EEE2DEA-9D32-4D35-B4A0-2A8E848C929B}"/>
-    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{B474162F-7ECA-4E83-BFE6-02EDA146F23D}"/>
-    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{0D8C62F9-7242-4176-8C91-9928381E16D9}"/>
-    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{B658EA5F-A822-4BD5-8A50-8E9E4DFC5215}"/>
-    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{6073A0E9-2B12-42F7-8675-E144579EA8FB}"/>
-    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{0AF5F626-1D35-4BDE-8D7F-8400509FC5B9}"/>
-    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{EF027DB0-93E4-40BF-8326-FB06233636C3}"/>
-    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{DD717DF4-252E-4EEA-9942-1D1416D5C037}"/>
-    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{DA0B2223-AC35-47EB-9012-9991EE7DDBDE}"/>
-    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{61643BD2-6CEC-4F69-9B2A-2E1B9807EA10}"/>
-    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{B6003021-91F7-4A00-B88B-27EC57C44A41}"/>
-    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{71974EC5-DDBB-4760-80A9-C9E28A45FE1E}"/>
-    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{A4418A48-893B-4D06-A388-DBF83574FE21}"/>
-    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{FCC98CF2-C9FD-4E5A-9DE7-99FC2AA035A5}"/>
-    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{8F1467F3-BD86-46E0-B759-CE1FCD162096}"/>
-    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{0D567F21-01DB-4AD9-A1A0-2414B76D9E1D}"/>
-    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{BE7386AD-65C7-44AC-9AEB-6D564B3C6CBC}"/>
-    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{1BBEF30B-561B-4948-85AC-03957B5536E5}"/>
-    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{F00DFD6F-FA94-443D-9F21-7D659FB9EA4E}"/>
-    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{FA12B98A-4AF3-4912-9918-826A98B8A12C}"/>
-    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{94965354-30C3-4E2B-A807-F9AB254C0CC2}"/>
-    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{0399197D-EC76-4C8D-8BCA-0FAD3FE33B96}"/>
-    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{C78177E4-8A7E-4F31-9DB0-3816F2464D86}"/>
-    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{74AB797A-E60C-40DC-B0C4-C5B64EB4BC7F}"/>
-    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{CA403379-0EE9-43C1-A908-8FFF7D81AC3B}"/>
-    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{9CDD47C2-E406-4580-854E-8802920D29CC}"/>
-    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{D1B4E38C-8450-4498-A3B7-DDEDFF6CEFB7}"/>
-    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{2E8387E1-D2A6-4D5A-877F-207E98E0E8D3}"/>
-    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{D1E464E3-446E-4DA9-9F70-BF7B5CE8B1D5}"/>
-    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{3D8C1CA9-214B-4D50-867C-299856952E51}"/>
-    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{A854211C-13A1-4127-A774-1E2751D6A653}"/>
-    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{C6F77181-D588-48D5-94B5-5EB8F028A5ED}"/>
-    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{7EF37ABA-959D-4D8B-B0D1-AEC9BC05AAFA}"/>
-    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{C83C4BBA-501D-48FB-A151-D45E8CF4F5D5}"/>
-    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{58588983-0CFA-458D-A5A9-FA20CBAD7150}"/>
-    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{1008C174-0F9C-47F2-ACF1-7099684057FE}"/>
-    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{04B33121-AAEF-45BA-A091-E4D8EB0A4D51}"/>
-    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{876E2244-4446-4B51-B634-24A4498B26CC}"/>
-    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{242B1DE5-5441-4FBE-81DC-8BE84C07C2E8}"/>
-    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{70A7C840-5319-4EC9-8481-8FD552BB161B}"/>
-    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{BACD2709-620A-4DB9-BF40-004C18BDC557}"/>
-    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{F0C0AA46-044A-409F-8707-6356129945F5}"/>
-    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{90CD1C4F-AB10-462D-BD11-03477D6CDC59}"/>
-    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{2D4A735F-E2FD-4A69-B7F7-3DFAA5B5E725}"/>
-    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{52859482-70C8-49BB-8D64-BD2FB6C95B87}"/>
-    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{88AFCDD7-CCA1-4A99-B058-A951850E343C}"/>
-    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{CE04715D-5273-478B-A676-82C9A979DB32}"/>
-    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{2E33205E-880C-4E02-8829-D3B77C9735A8}"/>
-    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{961CA5D7-B67C-48A9-854D-84B6C4D61C1A}"/>
-    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{6463D77B-5E41-465F-A88E-B0262C18BADC}"/>
-    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{7BF2A645-CC62-4925-B536-E8BD051E140D}"/>
-    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{84370F4F-94BD-4F88-9624-41AC8EC0B4CC}"/>
-    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{4167DAF4-E895-4F67-A0F5-0309C2015950}"/>
-    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{7D04D2C4-DFE4-424B-884E-C4DB807DC822}"/>
-    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{E1B481F7-8B61-406A-AE1E-3A94D1CDE4A2}"/>
-    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{81D73250-3037-41F4-B957-FC714560738E}"/>
-    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{A424196D-9A5B-4B4B-8AA3-EB228315CAFA}"/>
-    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{7193499F-7D1B-4ECA-BC9C-84015E2935D3}"/>
-    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{BA87F613-AB66-4FC2-B754-582C0034CAC9}"/>
-    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{69F39102-EE4F-47E6-AD56-674F76784549}"/>
-    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{700788D8-B09A-4888-8345-7F8C159182F3}"/>
-    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{0C8EFEF3-A56F-4B63-8416-1543811D7DA7}"/>
-    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{938BB2B7-4D29-41E4-B987-F190FE60E107}"/>
-    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{DDE848F1-0A85-4261-B665-D41732C6C7D4}"/>
-    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{B0324654-DD6B-4CA2-94C1-E230721E0686}"/>
-    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{9AE13312-5500-417A-88BB-EDA199D0923A}"/>
-    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{77ECADC0-24B8-4D7B-B458-3C7E9BF6170B}"/>
-    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{165245DC-6611-439D-9ADE-F8EB7208EEC5}"/>
-    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{E9E223DC-73B0-4640-9B5E-46C9C096648A}"/>
-    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{E97312B6-FD3D-42C0-A70E-E4FBE0B69220}"/>
-    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{093DD83C-9742-41C0-8A71-13C97DD91E6C}"/>
-    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{A6029C47-A972-4FE4-8616-BEFF7A21F275}"/>
-    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{F0C7241D-D26B-4170-9E75-06EF550AA8B9}"/>
-    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{A74B4A24-47D0-41CD-B506-FEE2205B0B91}"/>
-    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{BB22F0F7-9DB0-48C7-838E-638647646A0E}"/>
-    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{F69C2869-4021-4A1C-BCCA-9ECC03B9F86A}"/>
-    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{951D30EF-07A9-40ED-964D-66412081FA5F}"/>
-    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{F136C310-5D5E-4A89-BDAA-403C9EB9FA59}"/>
-    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{457253E1-7567-4DB5-8F2A-24993C9C5BBF}"/>
-    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{A518C0CA-30B4-4EA7-970B-C1BBB7D5F4C8}"/>
-    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{C30D0808-9A74-499F-ACE8-D6F5E5A44552}"/>
-    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{16B70248-C951-4E10-9BE3-25365CB8F913}"/>
-    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{D49B910D-1838-4CA9-9A87-82EA4DE004E2}"/>
-    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{44BA2076-029A-4244-AF73-52FF2A985AED}"/>
-    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{1E038EE7-A7FC-4A77-BD1F-4D6916EB3C8D}"/>
-    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{7B03E22B-9292-478D-A157-1BD92FD8B8DD}"/>
-    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{9DF71CD9-5525-4866-996B-71C25FE07FF9}"/>
-    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{2F4CF871-333B-4038-9BF6-C485371344AF}"/>
-    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{5F8793D0-ADB6-41C6-8402-B135C5E3BFA5}"/>
-    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{72871D48-9167-4F74-9A61-9221CB33A90F}"/>
-    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{8DF56FAC-4EA8-4F3D-83B9-399CD5B5CE2A}"/>
-    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{259A7B48-F8CA-4F7C-B287-D60F6CFE00B7}"/>
-    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{8345C3DB-17EF-41F0-90D6-78FAECAB339C}"/>
-    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{6723EBF9-90BF-4934-AD4B-9C6D8C5553CA}"/>
-    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{366F4F9D-20C7-427F-8113-C902EB26B218}"/>
-    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{986BA17D-17EC-4882-92B5-F884E3A56BFA}"/>
-    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{F3B445F4-D2EE-4833-BE7A-EDF9FD1721E8}"/>
-    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{CCFDC39E-C134-4A16-AFE0-8FD9603E5F30}"/>
-    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{71F5A98A-D803-438E-9FC7-928CE1BC12E8}"/>
-    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{AACB935C-A246-4CE2-9EC7-D830DC9447EF}"/>
-    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{C343E1A1-D97A-46B1-B65F-10BF8E734FC2}"/>
-    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{A461CD14-5814-49BB-9FC0-1AEF02F505D7}"/>
-    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{B30F1FEB-3873-4996-A585-1C511EEDA659}"/>
-    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{538FC730-0108-4BA5-A887-EF5C79CC18C7}"/>
-    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{614C58D0-20D7-4996-B5BF-B4AA3F92BB42}"/>
-    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{DC49CE7B-41E1-41C7-9EC5-0C798E31B617}"/>
-    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{9F6B8194-F4E8-4D58-BC23-E3A3B3C59586}"/>
-    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{B21BF9D3-992E-4FCC-8D57-3F65B86B4D96}"/>
-    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{190805EE-0F58-4B18-BBD3-7B2075A34801}"/>
-    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{53EC7323-83E6-4246-BA97-215EF143CC54}"/>
-    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{92DB3BFD-4CCF-44F6-82F4-2F92E5EE30C6}"/>
-    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{DD26C00E-0D3A-4EC4-B1E5-F5647797D31E}"/>
-    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{EC8E4562-944B-44A2-BD82-A966A680E746}"/>
-    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{7CC90AD3-72BA-460D-8D11-14BD33C7E09A}"/>
-    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{FB355CBE-3473-45C8-9E80-75B80D5CDB5A}"/>
-    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{A44CDA47-B495-4A7C-A58D-A2466B26E9C5}"/>
-    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{5C635F8E-63BC-4C8A-A88E-39EDB7DE99EC}"/>
-    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{F5249AEA-37FB-476E-BEBA-1C06E890E36D}"/>
-    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{99C4AC23-CA96-4D75-BD6A-3934C8BD1886}"/>
-    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{AB888771-0A95-4267-81DC-66CDD8B770A1}"/>
-    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{EF424ABD-189B-4EF2-A6BE-6A25A3AE0193}"/>
-    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{5BBD5E18-2A3E-48A5-8358-B72A66CA8DEA}"/>
-    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{9515043E-D17D-4AF2-B488-40E1664F8B24}"/>
-    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{4810C118-B0F0-43AF-A3E3-94DD04A951DE}"/>
-    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{5C34D9EB-5BAD-4606-B7F1-6C3025A0AB50}"/>
-    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{7CA93A57-315D-4802-8307-050556C461F4}"/>
-    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{E3FA66EB-725B-4F4A-A21E-3BED444EF7E6}"/>
-    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{D96BDD9B-CB89-4D91-AB07-8F294C1AA38C}"/>
-    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{DCE965FD-7249-48F5-812D-DF2BE8D42519}"/>
-    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{2C52E850-CF9A-4C60-9626-EAAB4866EA5E}"/>
-    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{51D40859-A5A7-4544-8EE8-9B7B340460AC}"/>
-    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{67E7FFAC-681C-4A55-84FD-ABD0BC09A129}"/>
-    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{973B6473-461D-4254-8C67-242959DA16FB}"/>
-    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{E91D48B5-C328-4FE7-A796-D82FDB66D6E8}"/>
-    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{863499C3-91EA-45F0-8DC7-C732625A27DE}"/>
-    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{F6A39B55-527B-48A0-80EB-E77030B7FC12}"/>
-    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{3E9BE9EC-3CE9-4110-AF2F-D488CA27791C}"/>
-    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{8A51DF8F-232A-4C85-9D19-C948B9E926AD}"/>
-    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{38C29F49-D499-42CC-A02F-F63AF3292E34}"/>
-    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{18B7F6C2-0413-4513-B431-0AA0C5675C62}"/>
-    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{57BD9F4A-3E6C-4404-9C99-9B06EF4865A3}"/>
-    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{BF0851E9-929B-48B9-A148-DE49970E229F}"/>
-    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{4372E4F0-49DF-4576-AA41-8B5DC628EFCD}"/>
-    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{4A17CF8F-4962-4300-8BB4-4F12C442BE7B}"/>
-    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{D590B6FD-8343-4FB0-9A63-9D90BB8000DF}"/>
-    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{887439F4-99D4-4716-9709-3EDCB7B1265B}"/>
-    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{2E9F3A53-21B6-4013-9522-0D4DB8B6874D}"/>
-    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{C5302C29-E0B1-47BA-B55A-D5A69376D7FE}"/>
-    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{3CB58FA5-E63B-43B2-B2B0-D58888D50059}"/>
-    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{7F7D6C04-EB4C-4551-B89C-ED12FEEE5904}"/>
-    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{0B4F897A-D8B9-47DD-9B1F-197572145599}"/>
-    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{84E524F9-DB8E-4675-8CCD-788CDDFBA93A}"/>
-    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{CDC470F5-CE13-4313-AFA9-A5FBE9678850}"/>
-    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{A98EA498-237F-4D24-A377-8B4CC4DFE085}"/>
-    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{2832CAD1-BAEB-4223-83FE-693FE055D64C}"/>
-    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{C7265D6C-CA38-4A3E-A641-B90F32B1587D}"/>
-    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{39DCF9F1-BD70-4387-A978-CAEA8A53AF1D}"/>
-    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{5BDB0AB1-8436-4048-B54B-138E861CE4E7}"/>
-    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{7E162C34-4899-4BA1-8583-E982A534E3ED}"/>
-    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{6AC4F201-474F-408C-8F08-46DDDDA97B63}"/>
-    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{BAB6F758-0000-4D3B-AB3D-D429ED0078A5}"/>
-    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{34EF45DD-F610-4943-A9A1-3A1EA0FA2C84}"/>
-    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{31F7055F-DC31-4B82-8013-ED7F29A77A74}"/>
-    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{03EC2B83-C5EB-4D4F-A4F0-D37EE694CDDD}"/>
-    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{566C8A98-DAE0-42D4-AB05-D40A4E479F64}"/>
-    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{AF16CF11-4024-4AC4-B567-CCCCD1EF6532}"/>
-    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{14582C2B-7E46-4AB5-ABA2-AB561B2DCBB1}"/>
-    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{A9CD7A53-B2A9-42E1-954F-93B401C8C754}"/>
-    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{9DFBF768-4F91-4E88-9F17-EDD852583A48}"/>
-    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{289CE8F3-53F9-4F07-A569-E40C39D103BF}"/>
-    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{CD125EA6-D32D-433D-9708-2DFD1F430CE5}"/>
-    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{6EE89862-0574-40E2-BC6A-11FF8ABB3B73}"/>
-    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{0840E614-2AAE-4193-8B3A-207F4CF4FEB7}"/>
-    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{2A949099-3B23-4013-A5E6-9B844F7DCE02}"/>
-    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{4A11FC1F-17A0-42A8-AADC-E85F0A96DAD4}"/>
-    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{501565D0-6842-4302-93BD-3603A50A0D4C}"/>
-    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{32060861-89BA-4FB4-9D7D-F2DB8C362813}"/>
-    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{70F6917A-8BB5-4908-8B37-AC041641A6D6}"/>
-    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{CFCC0F7B-DFDA-43F9-9E9F-3B41FD0BBDAD}"/>
-    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{AB9E5521-820E-4FC2-AD8E-6AC51D2DA853}"/>
-    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{B26FA1BC-E55E-4EEE-AC04-35073EC42303}"/>
-    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{325DD945-F08A-4A3C-9805-98B9C2FCFD07}"/>
-    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{7507B4C4-DB8E-4943-868F-6159F02C5841}"/>
-    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{C7673769-9C11-4254-8A01-909164F2ACE8}"/>
-    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{CB0D3229-3859-4999-A137-E3F44FC3D96A}"/>
-    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{BC255852-E6F9-4C50-9961-B8C650637CB2}"/>
-    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{86E22D43-8DEA-4E78-9895-C979133C7F0F}"/>
-    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{08810A03-C0D5-4D0F-8E7D-58596B8FADC1}"/>
-    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{2B7F7FEF-4D10-4EFF-BEDD-F8B6EC33D7EA}"/>
-    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{AF88A63F-6E8E-4245-9A1A-01B60F3C7B62}"/>
-    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{758786C3-65DB-44AE-AA13-D94554020A27}"/>
-    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{CDD87DF2-EA32-4F67-AFEA-031383EBA032}"/>
-    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{9771E94D-ACC6-408F-B83F-04984F8B51E4}"/>
-    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{92354BA7-DFED-49AC-92B5-75B247E01B2C}"/>
-    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{9F1A2C1D-15FF-4CF9-9CC0-ECAD0F89675D}"/>
-    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{83F8C9FE-2CC8-47E0-A0F1-5E6C9778FF26}"/>
-    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{F8AAC8D5-7390-4B97-9614-62D2A4A45FCF}"/>
-    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{9FEA6DBA-DC7B-497E-86BF-F26AA8DBE1DA}"/>
-    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{ABFAFD1E-714E-4132-81C8-AF5165E9C67D}"/>
-    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{5B5DF6FE-5858-461F-95E5-B65F3037F72F}"/>
-    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{228C4CA5-27C1-405D-A95D-AF07F826BA07}"/>
-    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{E9A99AF2-6828-4230-9EAB-B79D5A9901E6}"/>
-    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{8C44445B-7728-443D-8D20-6A967CAA7901}"/>
-    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{77F50377-2080-453F-8909-A0796BB7F7CD}"/>
-    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{11C13D14-F7BB-423B-8500-DC392E2A4F48}"/>
-    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{6CD23C2B-C5A5-43A1-BA59-D8A1CF793B6D}"/>
-    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{9C30D7E6-624D-4BC8-A8CE-28C947BE5E85}"/>
-    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{E45273CE-88A7-43F3-B157-B2DFC6DCA516}"/>
-    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{84EE4D89-7351-43AC-8BC1-1E3A4BA07860}"/>
-    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{850DD61B-AD9A-45A7-B728-96BB22EEC920}"/>
-    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{E2AF02EE-9C7B-4C8E-842B-D3C28D17D709}"/>
-    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{5C2568BA-02E4-4829-868A-1E07CEFCB435}"/>
-    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{7B931B1B-AA13-4392-BD6E-34E618646185}"/>
-    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{A219FDC5-5BEB-4578-939D-8EC0BB2D198F}"/>
-    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{DA9B268A-72D2-45A9-AE14-BE9ED707FDC4}"/>
-    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{11200D5A-659D-419A-9C92-A7C9F89A4608}"/>
-    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{8291FD87-3510-4776-9A44-D018632AC370}"/>
-    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{AEB32323-485C-445E-B51B-1A927994AA20}"/>
-    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{2C388AC3-B6CD-4A2F-AE8F-61C85DE47418}"/>
-    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{F4961FC0-5D70-433E-A0F4-601F53BBDA80}"/>
-    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{E99E48C0-D3D4-411D-AD98-B9E1D82A5578}"/>
-    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{A0E2DD29-9FE0-401C-9336-0960711CDA58}"/>
-    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{5CEBF9BE-BE00-48DF-A83C-BE28AECB9599}"/>
-    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{D63FD0A0-40B8-4962-8DD1-1EE6A05C1B47}"/>
-    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{181EAD31-02BB-4C15-AB00-747511916FD8}"/>
-    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{216D1252-779E-4126-8DCF-A4060563BCCE}"/>
-    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{CF184D68-66C3-4182-9C2E-C4745C51A3F6}"/>
-    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{06F9AA7E-23F4-4CF6-AD48-A780DFE0D5E5}"/>
-    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{DFFCF772-49BA-478A-B361-19AD647D1ED4}"/>
-    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{04DAB830-801F-4C10-A656-73B81C9F77D1}"/>
-    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{50D79095-2C9B-4142-AFFC-43A8657127CE}"/>
-    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{E2BC94FA-2470-4C35-AE92-3538DB1DA14D}"/>
-    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{18370386-5E4D-4B19-9E42-00F04A1000F3}"/>
-    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{5772ACF4-AF57-4F99-BA0C-B7B93E14C166}"/>
-    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{4E24A1A4-3AD3-484B-BCF3-F184484FE516}"/>
-    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{7216690F-4ECA-4A22-9A00-60570B0972F0}"/>
-    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{8BC37A89-072D-4C20-94EE-3C5768725B9F}"/>
-    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{3BA91C5E-BACD-421A-B565-0D2677BAEAC5}"/>
-    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{5CD52FAB-C8DE-4418-A5D3-6835AD3B3522}"/>
-    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{27D90575-D60A-4F20-9F9A-60D8076A6A32}"/>
-    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{1E25E5FE-6D2E-4438-A83E-5588A98C07AB}"/>
-    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{89615029-DEF8-48F0-9398-B7FE4B25C202}"/>
-    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{9D4D3C14-96E0-49F1-BBD3-28FAA66DC8C4}"/>
-    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{A29CEE03-1127-4D36-83BD-B5E794F5E92A}"/>
-    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{4AC2E664-680A-4343-BF45-16900FC33AEF}"/>
-    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{99D86400-AADA-4916-AE61-21728165D235}"/>
-    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{62344EF4-D5C7-4DE0-8763-E030A8C6F528}"/>
-    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{8BA161D8-EEAF-4386-A2CF-8E226D3C9521}"/>
-    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{3F0F6654-2BA9-46E0-811D-1D99B2F2DBA5}"/>
-    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{F23D1CA1-8339-4228-B128-EA787DA4B99D}"/>
-    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{2BBF070F-2F4D-498E-AC9F-3A6AA945E8B6}"/>
-    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{BEB59619-7C33-438A-80B7-06E30A293C67}"/>
-    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{1CCC6661-B258-40EC-9061-1274FC78170A}"/>
-    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{36D20346-E6E7-470D-9C4F-E54A6EB9D4AE}"/>
-    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{655906F9-435A-4257-BC71-BD70DA4D8256}"/>
-    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{7545E3A0-94DD-4A88-89F1-9036BBCCA08B}"/>
-    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{FDBE6727-83FE-473F-A872-A2C26E03FAB5}"/>
-    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{0F15B34E-C48D-4EB0-8441-55A8DE9302A5}"/>
-    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{8E482853-6BB2-49D0-ABFC-2C546D73BA99}"/>
-    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{91A2249B-048D-43CE-914B-9F858B557121}"/>
-    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{CC843349-82A4-4528-AFCD-33982E4757F5}"/>
-    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{76E3B674-778E-4C50-A8C2-9C267C070307}"/>
-    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{0C6818E8-9D10-44F4-A79D-DF2EB553D28F}"/>
-    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{5D156D64-0BC2-4414-A952-3D6455B1C40D}"/>
-    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{E3E690C5-A03B-415A-9800-D821D1A01E10}"/>
-    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{57BFCD1D-DEA7-4FD0-893A-B0B65403D013}"/>
-    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{343EDCDF-5C3F-452F-8A17-8D696215A8AF}"/>
-    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{2F41587C-76B5-42A6-B6C4-D9B3EFAC2BCB}"/>
-    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{5103E9A1-DC20-4ADC-999C-66A86F60EEB6}"/>
-    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{FAAEE51F-37F2-40A0-B70F-1384FFFEFD5E}"/>
-    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{6D87E3FB-648E-45FD-8C81-4A933F67D566}"/>
-    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{32F52385-C20C-4CD6-9C53-B1B805F7A282}"/>
-    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{4BD58D66-5404-4F3F-B422-C4033F3D69B4}"/>
-    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{DFF8821C-FBC4-4403-8EB3-4C0DFEA064E9}"/>
-    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{ECB6CD48-6B71-4FFC-B5CE-B574286B23A5}"/>
-    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{69969006-5E1E-4E87-9602-F0B20109D5FF}"/>
-    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{61AE5756-9AA6-44D0-9ACF-34582DD75836}"/>
-    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{7BA961FC-09C1-4736-B300-1717081D84A0}"/>
-    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{8A850EB5-6783-4D45-9A46-3C9FE2584EFE}"/>
-    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{BB22BC74-39FB-4D36-82C5-11A8A9BD18C4}"/>
-    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{E866F62C-A8FB-4D9A-9792-63A012950931}"/>
-    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{4ED374A0-E7DD-4FDC-BDB3-190E4DDF6FD2}"/>
-    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{7AE72A8C-4DA5-4079-BC4B-BE3C424E6435}"/>
-    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{AB26CF15-75B1-4E1A-826B-BD52BA685A11}"/>
-    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{3ED868F9-63EC-45CE-AE1A-FA6135FCE5D8}"/>
-    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{EE893CCF-3452-4FD2-9B4A-7C525A128D8B}"/>
-    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{D5B4E9EE-6698-4A86-8281-350818DA721E}"/>
-    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{CFB1870E-3C50-4F90-A16E-E765408CC3C7}"/>
-    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{A7F03B59-6CA6-4A6C-86DE-1C816DABEE53}"/>
-    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{725AD3D1-5E35-410E-B30A-30750DA2664F}"/>
-    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{BC8091F0-118B-4DE8-875A-876F67DA03DC}"/>
-    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{3A5F62C1-AF41-4980-9FFB-44FBC739985B}"/>
-    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{20CF04C3-B26C-4B41-BA90-F9136C3BB337}"/>
-    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{099A58D8-B891-4144-B2A8-5A717DB61B90}"/>
-    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{756B43E7-1384-41F5-96AF-73FEEF05E48F}"/>
-    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{B4E08CDB-907D-46DA-A698-D9682D601717}"/>
-    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{526B1AC9-5F0F-4072-9D82-B2E1A281B380}"/>
-    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{74FFCAC3-C12C-4B42-9A63-46AFD4AF36DF}"/>
-    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{C178746A-833F-4EC1-A1B5-62457DD03C9A}"/>
-    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{92536712-1BEA-42FA-BD47-C23CB745D5DB}"/>
-    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{E2D67988-D7C0-43B7-87BB-D2F5779B76C0}"/>
-    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{F09FF61E-7D4D-4E69-86EF-FAF2A8C17191}"/>
-    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{D30867DF-6B15-42ED-806D-AD3DAC4F20FC}"/>
-    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{A04E9D76-1D03-4D6B-A361-DB0443308148}"/>
-    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{387A66D5-BFBA-4D92-8641-D5E5FA90B8F0}"/>
-    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{675960EC-F8E9-47D2-909B-E2AF6AFF0170}"/>
-    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{F40DA545-D5A7-4620-87B8-8355EE294641}"/>
-    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{F0416487-1D86-4764-A42B-616AFD96D41F}"/>
-    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{1FF31742-E23A-4CB2-8FCF-F36FE5CB2763}"/>
-    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{DF6D9FF8-F55D-4343-974E-5F20E457B5E7}"/>
-    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{9831FD97-B2BB-4A53-8090-6F3CB4D83EC4}"/>
-    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{C02AA55E-7F9A-416E-8871-F4A735FB062E}"/>
-    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{32520C2D-3768-4863-9F98-89DBDB214E06}"/>
-    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{02F0A0D7-C24F-4351-8E5D-26C291267AEE}"/>
-    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{BC3CA6CD-F59B-490F-B7D3-302588FC8510}"/>
-    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{D4066896-6C74-484B-B4BB-9DEC2C8FF46C}"/>
-    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{B68B3480-EA05-4C70-88A1-0071B5E64DBA}"/>
-    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{C810B6F8-4BA7-44BA-9D46-A60D4D86F569}"/>
-    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{E455A03B-E9DA-4237-85B9-D1E39597BED3}"/>
-    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{786DEE77-1362-435A-870E-0368C14C9FA4}"/>
-    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{787B4BEC-7C7F-4FE0-92CD-C94DC60790A1}"/>
-    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{D3049F8E-0FDE-4FEC-81B6-56FCD806094C}"/>
-    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{84863B8A-9278-4EE5-9A24-955A912C02A0}"/>
-    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{30437BB6-850E-4586-B50B-547A0FDB2B7E}"/>
-    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{E13207CD-CC83-488F-B63F-A8E44B2997B3}"/>
-    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{2F8E7BD7-6311-4B27-8DAE-9EE7ACC0DA9E}"/>
-    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{ADD16A57-5379-4E26-8CF2-5A127D5C22F0}"/>
-    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{D81C7907-9239-4B0F-90CF-4D2F26141DB3}"/>
-    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{BCE54B2D-E842-4C40-9118-6F63FA336306}"/>
-    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{014448D9-FF8C-462F-9953-FED524491046}"/>
-    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{481A3025-DB20-42C9-87F5-34C66F5E1E65}"/>
-    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{5E6C1C76-F6BD-4013-AF00-94E52F318611}"/>
-    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{161C8541-27E9-4E93-BAA3-69258885AFCA}"/>
-    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{4C8A1C4D-6A4D-4541-8DB1-7B32E6B54667}"/>
-    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{DD2EB574-D849-4E25-8F3B-A144DD6F1022}"/>
-    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{311954D0-A3AA-4FB9-B2EC-C337473B0704}"/>
-    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{49027ADB-82FB-4368-AAAA-F30C7D268A75}"/>
-    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{84633A66-DC31-4292-AC29-8D39C03CEE85}"/>
-    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{D6043F05-478A-41D3-8007-8676FF44ED65}"/>
-    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{3DA2B6F3-31D5-4F35-B3FF-F3E59C72430A}"/>
-    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{21E53F1B-7BED-4155-B7BB-43CE82C5A3CB}"/>
-    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{2EB45A7F-1EF8-4C91-8B7E-6135E39BBAC8}"/>
-    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{D43E5ECF-AD4F-43AF-B1FB-B1B38CB21A5F}"/>
-    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{F837AB37-14F8-4F21-879E-629486F7BFE8}"/>
-    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{BE38F19F-C94A-4E16-B4FA-1DDD3436A70B}"/>
-    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{2E992A19-4DA6-4A9B-BF35-06950CDD602B}"/>
-    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{CA88ACC9-F93B-4661-B319-C233334B75D6}"/>
-    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{9C8D15D2-5D06-412B-B46F-1C732A0BC73C}"/>
-    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{0707279E-5650-4918-8073-9F5B6B19F2DB}"/>
-    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{97695C19-BE29-46C5-9A75-E80EA81C9807}"/>
-    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{7AC70990-D0F3-4130-9FB0-4A21835E54CC}"/>
-    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{60BD12D8-3294-4381-8D49-0E0ACDD72455}"/>
-    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{B2033988-7405-49B3-960A-51317F7DCF56}"/>
-    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{E13ECD98-3EC4-4752-92F4-25223BA94DB3}"/>
-    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{5C14CFB8-1C75-4105-9D6A-4AB58D4D709C}"/>
-    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{77B6685A-1A4B-4FA2-B06F-72C6F6B41CD1}"/>
-    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{A3600611-58B0-4A72-BE59-8B03EC9AFA4D}"/>
-    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{336505F0-C702-4E1D-A718-A3D43886367E}"/>
-    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{5E060666-A0CD-46A0-8644-99A7194A2A61}"/>
-    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{41714F12-416E-4E92-AA8D-0F85A5AA440A}"/>
-    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{B380332E-D1EE-43BF-83A3-97ABF2CFDC2D}"/>
-    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{D5B854DA-2710-41D7-AB58-40F596C930FC}"/>
-    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{8682A1DC-3872-45AB-9903-545AEE348AB5}"/>
-    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{E0132E52-62C3-4487-8458-446C27CF82FE}"/>
-    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{CBB31172-5651-41CA-BED6-21E551E496B9}"/>
-    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{E055FE6B-682D-4830-81FB-2ABA6BC01AB2}"/>
-    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{D6287E0F-A36D-45A6-916E-0570812775A2}"/>
-    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{8FA1036D-6019-4547-BE68-722718597F49}"/>
-    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{04144B09-8D8E-49E5-A34F-DFBC43876363}"/>
-    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{13E4518F-36BA-46EA-ACD7-B1DE342616D0}"/>
-    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{563AE535-213E-4A95-A85B-33C1227F4847}"/>
-    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{3E96A4ED-DBAA-47DF-A71F-3C7545C7B336}"/>
-    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{29709376-06E3-471E-A1D6-A50904E3CCCA}"/>
-    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{332758C1-9F6B-4035-9B8E-3390EA1DC0D0}"/>
-    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{97A7156D-2355-4533-A443-59CC0B286C9F}"/>
-    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{F9618F25-EC96-459D-A796-29C1640500E0}"/>
-    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{6FC8390B-9304-49BB-8AF7-DB6F46759272}"/>
-    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{64204F9B-A0DA-4B10-B0EB-CAE7A25651CE}"/>
-    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{DC888779-130D-4A3A-914C-864394BDE05B}"/>
-    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{47C1410F-E356-4EB4-AB72-F3B73CB29F0C}"/>
-    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{2CEB6EB7-5BBC-4359-ACFC-8C53BAEB391F}"/>
-    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{776145AD-5E39-4979-AC55-B69289DF101D}"/>
-    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{8D3ECEFA-0D2D-4F58-BA54-7112C49903C4}"/>
-    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{E343D7A1-9EF0-44D1-A2FF-2AECBE270D3E}"/>
-    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{1EEA349D-5C38-45E8-AB30-6FD176839490}"/>
-    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{2A1717FB-2D10-4720-8CE5-3DB0FCB2841F}"/>
-    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{7ABD20A0-068F-45F2-B322-1CB7F243D398}"/>
-    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{CC230E1C-30F5-4B58-9F1D-2DD528CE7FDE}"/>
-    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{6A513C51-EAA9-4E62-A14C-81D036B5F198}"/>
-    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{97B44F40-35F5-44A2-9E88-8221E9CC3369}"/>
-    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{4DA4D3DC-4C1A-400A-A40E-4B3E38CF471C}"/>
-    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{5BBD76E5-84C3-46DC-9388-7FEDCA8798FC}"/>
-    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{A8CA4D82-83DD-4A07-B678-D31EB3205F4F}"/>
-    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{A6F8553C-C592-40ED-9877-C2C57B626B04}"/>
-    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{FC684D79-24E1-4855-BFDF-E7DEC3FA4764}"/>
-    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{5135D4F9-DEB5-41E6-9212-CCBBE5759AC0}"/>
-    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{DFCA70A6-E077-487E-AAF4-F84E18E13813}"/>
-    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{40E1117C-E95C-4DF0-B6BF-FD93099587CF}"/>
-    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{351FBAB0-9F39-4084-A70D-3D8E3927B0E6}"/>
-    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{C4977360-F1B9-4478-A8CF-5841F2782C70}"/>
-    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{0AB01C61-7DFE-4677-B0CE-33894D991007}"/>
-    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{21730A8C-1CC5-456E-8D57-AECEAD7270D7}"/>
-    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{FE18B3E3-3840-4578-A8E0-3AF65F2FC1E5}"/>
-    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{57C6F425-A47F-4DF0-8127-68A982BD4FEE}"/>
-    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{9ED7F747-7F99-4738-BE36-32569A0C3E64}"/>
-    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{91B170FE-890E-4243-A366-2A083D288326}"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://jira.sky.com.br/browse/SKYIT-78463" xr:uid="{5EB596DF-77BE-4852-B0B9-A4C18F74EA77}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://jira.sky.com.br/browse/SKYIT-78566" xr:uid="{836611FC-72AE-4FC1-9FD6-05E1A6BFD996}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://jira.sky.com.br/browse/SKYIT-79251" xr:uid="{910DC217-7E9C-4CEE-80CA-2A6B6562AFD8}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://jira.sky.com.br/browse/SKYIT-80687" xr:uid="{37341884-6BB2-456A-B66C-652D793E09E0}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://jira.sky.com.br/browse/SKYIT-85419" xr:uid="{CCA78CBC-A68C-4E65-AFF2-F690002EBFB3}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://jira.sky.com.br/browse/SKYIT-86522" xr:uid="{8C69491F-06FA-4E48-BAB5-B32C9755206C}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://jira.sky.com.br/browse/SKYIT-86525" xr:uid="{34D93BDE-D38A-461F-A658-2902CC80A853}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://jira.sky.com.br/browse/SKYIT-87511" xr:uid="{575C6A3A-8F20-4C19-B351-9B447E89361A}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://jira.sky.com.br/browse/SKYIT-87594" xr:uid="{437A3DCE-AB1E-46E2-92B0-BEF14CC11C51}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://jira.sky.com.br/browse/SKYIT-87621" xr:uid="{6BD93F0F-28E1-48A3-8B03-33DAFC7FADB9}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://jira.sky.com.br/browse/SKYIT-87677" xr:uid="{A41C1435-4945-41F5-BC22-EDBA33D47C64}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://jira.sky.com.br/browse/SKYIT-87808" xr:uid="{CF98CEDA-D1FB-4335-8EBF-7998F6BB7182}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://jira.sky.com.br/browse/SKYIT-89585" xr:uid="{FEC504FA-5E1D-49B2-9ADE-C2322133F922}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://jira.sky.com.br/browse/SKYIT-94232" xr:uid="{D05E02B0-AF67-4932-B220-DA719B07BBC5}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://jira.sky.com.br/browse/SKYIT-97685" xr:uid="{35FDE0E0-6A3B-4B4A-A11E-6B5909639556}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://jira.sky.com.br/browse/SKYIT-98726" xr:uid="{8E7B7159-A43A-4C6F-B2B8-2264E6BAB9AC}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://jira.sky.com.br/browse/SKYIT-99208" xr:uid="{8A49A077-02EE-449B-9BF7-2D0B8698F489}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://jira.sky.com.br/browse/SKYIT-101994" xr:uid="{7522092E-5728-43E4-A421-9BBDDBF7E832}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://jira.sky.com.br/browse/SKYIT-104164" xr:uid="{FF5ED003-3137-4A75-9195-9F0C595CD1D9}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://jira.sky.com.br/browse/SKYIT-104631" xr:uid="{94350200-47B6-4E7F-A398-8F8AA30DAB06}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://jira.sky.com.br/browse/SKYIT-104872" xr:uid="{5E2D32D2-F91C-4748-A296-76CEA8B10B2F}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://jira.sky.com.br/browse/SKYIT-107918" xr:uid="{1C52F4BF-AAD0-4A7E-A8BC-44032D6E47A4}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://jira.sky.com.br/browse/SKYIT-108838" xr:uid="{1B2ED329-3062-4EEE-A11E-0B3E04094112}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://jira.sky.com.br/browse/SKYIT-108852" xr:uid="{FD76F1AE-E3A8-488B-9E21-D07BB2C4F17C}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://jira.sky.com.br/browse/SKYIT-109397" xr:uid="{C47CDA90-ABF3-4A2A-81A9-021EE2FE24A7}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://jira.sky.com.br/browse/SKYIT-110370" xr:uid="{9DED8105-16D4-46E5-AE7F-CC27097FCF5B}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://jira.sky.com.br/browse/SKYIT-110636" xr:uid="{75287CF4-9882-46D4-9AB6-87FB50F3AEC9}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://jira.sky.com.br/browse/SKYIT-115993" xr:uid="{A2817644-22AB-4146-BC5C-34D359A6EC8F}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://jira.sky.com.br/browse/SKYIT-116767" xr:uid="{FF63C0BA-8EA7-4227-9BFE-B562E00E05AA}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://jira.sky.com.br/browse/SKYIT-116797" xr:uid="{A1259B11-B078-4E8F-87B9-EB308E27E8AB}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://jira.sky.com.br/browse/SKYIT-116828" xr:uid="{020A33F9-F6DF-41F8-A393-5242AB4B0098}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://jira.sky.com.br/browse/SKYIT-117292" xr:uid="{3431E36B-527D-4D64-A356-BACF4637700A}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://jira.sky.com.br/browse/SKYIT-119830" xr:uid="{192F383A-2D10-4889-9A38-D3CC560F0B81}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://jira.sky.com.br/browse/SKYIT-120613" xr:uid="{CFF08315-E2AD-4118-A182-14575EA7E6EC}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://jira.sky.com.br/browse/SKYIT-125174" xr:uid="{96EC06FD-046F-48EA-A6E6-13F7EC733179}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://jira.sky.com.br/browse/SKYIT-126567" xr:uid="{3548BDF0-B5CE-473D-9DAE-304713EA263D}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://jira.sky.com.br/browse/SKYIT-126590" xr:uid="{B8764930-A19D-497F-885E-B5A1662E3361}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://jira.sky.com.br/browse/SKYIT-126701" xr:uid="{F8EED70E-8E6E-421D-9A59-4DF0250AE56B}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://jira.sky.com.br/browse/SKYIT-127874" xr:uid="{41E0079A-BE69-42D7-81C9-C649499AD341}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://jira.sky.com.br/browse/SKYIT-128875" xr:uid="{6973A606-B84C-4D59-B413-7456BFC01508}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://jira.sky.com.br/browse/SKYIT-129159" xr:uid="{14D75411-3390-4BF6-B022-43D02E6A87F4}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://jira.sky.com.br/browse/SKYIT-129303" xr:uid="{EF85BF8A-EB3E-42B6-ACC1-7AC49DBFCCCE}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://jira.sky.com.br/browse/SKYIT-131024" xr:uid="{C9A67775-8C8D-415B-9605-0DE8C4EC7ED0}"/>
+    <hyperlink ref="A45" r:id="rId44" display="https://jira.sky.com.br/browse/SKYIT-133777" xr:uid="{B019D4B5-0708-4DAC-A7A1-8BB0B8979EE6}"/>
+    <hyperlink ref="A46" r:id="rId45" display="https://jira.sky.com.br/browse/SKYIT-133970" xr:uid="{B45A34A5-88DD-4D9C-9FD5-A3D7EDFB19E9}"/>
+    <hyperlink ref="A47" r:id="rId46" display="https://jira.sky.com.br/browse/SKYIT-134048" xr:uid="{CE99B523-2C5D-4F1D-9BB3-6532E849BAAD}"/>
+    <hyperlink ref="A48" r:id="rId47" display="https://jira.sky.com.br/browse/SKYIT-134280" xr:uid="{E000796A-1EE7-4B52-AB9E-F36F62B8B408}"/>
+    <hyperlink ref="A49" r:id="rId48" display="https://jira.sky.com.br/browse/SKYIT-134300" xr:uid="{3682BA36-B532-4AD6-B9C7-BF7477F41802}"/>
+    <hyperlink ref="A50" r:id="rId49" display="https://jira.sky.com.br/browse/SKYIT-134310" xr:uid="{CED9C88D-7231-4CCC-B89D-9ECA21F7944F}"/>
+    <hyperlink ref="A51" r:id="rId50" display="https://jira.sky.com.br/browse/SKYIT-134442" xr:uid="{D7A1BB54-211E-4E6A-A984-614C80E4850B}"/>
+    <hyperlink ref="A52" r:id="rId51" display="https://jira.sky.com.br/browse/SKYIT-135338" xr:uid="{81EC5677-FCE7-4B3D-A2A8-DE540A79913A}"/>
+    <hyperlink ref="A53" r:id="rId52" display="https://jira.sky.com.br/browse/SKYIT-135387" xr:uid="{D665C16E-97BF-4C36-A0C0-5E6023D27491}"/>
+    <hyperlink ref="A54" r:id="rId53" display="https://jira.sky.com.br/browse/SKYIT-135470" xr:uid="{4B581157-1B34-4230-8FD3-8350A8CE9C1C}"/>
+    <hyperlink ref="A55" r:id="rId54" display="https://jira.sky.com.br/browse/SKYIT-135760" xr:uid="{7AA167E6-8115-4429-8E90-B60743CE4169}"/>
+    <hyperlink ref="A56" r:id="rId55" display="https://jira.sky.com.br/browse/SKYIT-136182" xr:uid="{C1D879EF-877D-464B-A731-169038F8F6A0}"/>
+    <hyperlink ref="A57" r:id="rId56" display="https://jira.sky.com.br/browse/SKYIT-136487" xr:uid="{4050FB2A-18FF-4C3C-A71F-AD657FF8DC4B}"/>
+    <hyperlink ref="A58" r:id="rId57" display="https://jira.sky.com.br/browse/SKYIT-136614" xr:uid="{E981A632-F4A2-4F2C-B6E7-00D1349A6C68}"/>
+    <hyperlink ref="A59" r:id="rId58" display="https://jira.sky.com.br/browse/SKYIT-136857" xr:uid="{C77F922A-6F97-4F48-A8A2-321A619D1171}"/>
+    <hyperlink ref="A60" r:id="rId59" display="https://jira.sky.com.br/browse/SKYIT-137800" xr:uid="{80EA2255-04C9-4DF9-8BC0-0663C961F46E}"/>
+    <hyperlink ref="A61" r:id="rId60" display="https://jira.sky.com.br/browse/SKYIT-140058" xr:uid="{ABBB269E-3130-43A1-A8D0-D2E39C97D015}"/>
+    <hyperlink ref="A62" r:id="rId61" display="https://jira.sky.com.br/browse/SKYIT-141135" xr:uid="{D5CDD762-21C0-4401-BE57-ADD5257EDD78}"/>
+    <hyperlink ref="A63" r:id="rId62" display="https://jira.sky.com.br/browse/SKYIT-141255" xr:uid="{248CB911-078F-4DE7-9CBE-51079B621A45}"/>
+    <hyperlink ref="A64" r:id="rId63" display="https://jira.sky.com.br/browse/SKYIT-143191" xr:uid="{82E0D1E5-7F84-4C47-BC9D-13A0874C6328}"/>
+    <hyperlink ref="A65" r:id="rId64" display="https://jira.sky.com.br/browse/SKYIT-145064" xr:uid="{4854FFED-1D6E-4FDB-A911-7CD9AEE42107}"/>
+    <hyperlink ref="A66" r:id="rId65" display="https://jira.sky.com.br/browse/SKYIT-145566" xr:uid="{25CD8A2E-BBD9-4110-929D-62FE91BB994A}"/>
+    <hyperlink ref="A67" r:id="rId66" display="https://jira.sky.com.br/browse/SKYIT-149434" xr:uid="{61745344-593E-4618-9BA4-6839A55E3816}"/>
+    <hyperlink ref="A68" r:id="rId67" display="https://jira.sky.com.br/browse/SKYIT-152489" xr:uid="{81AFE6F0-CE10-44FC-B620-D15BE297D169}"/>
+    <hyperlink ref="A69" r:id="rId68" display="https://jira.sky.com.br/browse/SKYIT-154187" xr:uid="{ECFC8FDE-6BAC-4507-9E64-F17E6DB5CAD4}"/>
+    <hyperlink ref="A70" r:id="rId69" display="https://jira.sky.com.br/browse/SKYIT-156586" xr:uid="{F09107F5-6152-414A-9925-61F6BD1CC779}"/>
+    <hyperlink ref="A71" r:id="rId70" display="https://jira.sky.com.br/browse/SKYIT-158631" xr:uid="{88B0DF04-C082-4806-BCF6-761786CE8BB0}"/>
+    <hyperlink ref="A72" r:id="rId71" display="https://jira.sky.com.br/browse/SKYIT-158696" xr:uid="{86222CA8-A37F-4230-BB3D-C4000A89809E}"/>
+    <hyperlink ref="A73" r:id="rId72" display="https://jira.sky.com.br/browse/SKYIT-160504" xr:uid="{22CED32E-FC0A-4D12-8562-ECED489B0AD4}"/>
+    <hyperlink ref="A74" r:id="rId73" display="https://jira.sky.com.br/browse/SKYIT-160597" xr:uid="{5ECE8E09-5CAA-451C-87FB-4797B26DF13D}"/>
+    <hyperlink ref="A75" r:id="rId74" display="https://jira.sky.com.br/browse/SKYIT-160791" xr:uid="{4BDE374C-4B65-4528-9A62-D695BD9BC419}"/>
+    <hyperlink ref="A76" r:id="rId75" display="https://jira.sky.com.br/browse/SKYIT-162330" xr:uid="{F55A18E8-813C-4E27-8ADC-CBE730767914}"/>
+    <hyperlink ref="A77" r:id="rId76" display="https://jira.sky.com.br/browse/SKYIT-163195" xr:uid="{D13B21C1-5948-45BF-8AA8-AD3A56F49134}"/>
+    <hyperlink ref="A78" r:id="rId77" display="https://jira.sky.com.br/browse/SKYIT-168821" xr:uid="{775FEC3E-1F44-40D9-8B9E-FA4ABB2AEE9E}"/>
+    <hyperlink ref="A79" r:id="rId78" display="https://jira.sky.com.br/browse/SKYIT-170163" xr:uid="{37CC6D2A-4489-436D-8309-DD7BA713DEF5}"/>
+    <hyperlink ref="A80" r:id="rId79" display="https://jira.sky.com.br/browse/SKYIT-170300" xr:uid="{9590C168-9151-493E-900D-50DB4D20067E}"/>
+    <hyperlink ref="A81" r:id="rId80" display="https://jira.sky.com.br/browse/SKYIT-170479" xr:uid="{24CDEA26-DB5B-4C0B-BC14-C89643034E22}"/>
+    <hyperlink ref="A82" r:id="rId81" display="https://jira.sky.com.br/browse/SKYIT-170735" xr:uid="{DAAD9301-5989-4395-8858-22958687A733}"/>
+    <hyperlink ref="A83" r:id="rId82" display="https://jira.sky.com.br/browse/SKYIT-171043" xr:uid="{176D0E42-4D8D-4306-9B84-667C42F1BEEE}"/>
+    <hyperlink ref="A84" r:id="rId83" display="https://jira.sky.com.br/browse/SKYIT-171455" xr:uid="{96B8E9EB-FAEF-44A8-A7CB-FA310E9C89D1}"/>
+    <hyperlink ref="A85" r:id="rId84" display="https://jira.sky.com.br/browse/SKYIT-172326" xr:uid="{73290F05-0A20-4533-9015-F401A79D3939}"/>
+    <hyperlink ref="A86" r:id="rId85" display="https://jira.sky.com.br/browse/SKYIT-172490" xr:uid="{73CD8D4B-ECE7-4BCD-9505-79AE0A410C00}"/>
+    <hyperlink ref="A87" r:id="rId86" display="https://jira.sky.com.br/browse/SKYIT-172831" xr:uid="{0165F7D3-7CA3-4A5E-8C7A-69E990817951}"/>
+    <hyperlink ref="A88" r:id="rId87" display="https://jira.sky.com.br/browse/SKYIT-173047" xr:uid="{01C64E6D-EB70-4BD6-9D1B-FD3AC2C44E0F}"/>
+    <hyperlink ref="A89" r:id="rId88" display="https://jira.sky.com.br/browse/SKYIT-175300" xr:uid="{73A7890B-9B3E-40EC-967E-FE40E76DA007}"/>
+    <hyperlink ref="A90" r:id="rId89" display="https://jira.sky.com.br/browse/SKYIT-175335" xr:uid="{92B0760A-C117-4A22-BEB3-9533892AD1DB}"/>
+    <hyperlink ref="A91" r:id="rId90" display="https://jira.sky.com.br/browse/SKYIT-176055" xr:uid="{2ED14ABD-16B0-4B68-8EFE-C49128A35E00}"/>
+    <hyperlink ref="A92" r:id="rId91" display="https://jira.sky.com.br/browse/SKYIT-177334" xr:uid="{9C261723-E5B8-4B49-A02D-25498740114F}"/>
+    <hyperlink ref="A93" r:id="rId92" display="https://jira.sky.com.br/browse/SKYIT-177927" xr:uid="{01E956CA-A728-4105-8487-A34FDDEABA35}"/>
+    <hyperlink ref="A94" r:id="rId93" display="https://jira.sky.com.br/browse/SKYIT-177962" xr:uid="{3A6F9F2C-BD3A-401A-A2DD-A2103BF68448}"/>
+    <hyperlink ref="A95" r:id="rId94" display="https://jira.sky.com.br/browse/SKYIT-178171" xr:uid="{6843A358-5A56-4E2B-96D6-E39746A1CDED}"/>
+    <hyperlink ref="A96" r:id="rId95" display="https://jira.sky.com.br/browse/SKYIT-180652" xr:uid="{A3C120DE-1E66-45AA-98CC-ECEDD1ECB0F0}"/>
+    <hyperlink ref="A97" r:id="rId96" display="https://jira.sky.com.br/browse/SKYIT-180994" xr:uid="{8AEF8259-8313-420A-A419-FE353B13CBD9}"/>
+    <hyperlink ref="A98" r:id="rId97" display="https://jira.sky.com.br/browse/SKYIT-182062" xr:uid="{B90E7A1A-5EAD-4AD8-8BDA-40CA57F7B4C5}"/>
+    <hyperlink ref="A99" r:id="rId98" display="https://jira.sky.com.br/browse/SKYIT-182696" xr:uid="{C97BB59A-6C0B-4648-98F7-4E36B72FF7C2}"/>
+    <hyperlink ref="A100" r:id="rId99" display="https://jira.sky.com.br/browse/SKYIT-183422" xr:uid="{A999D663-4D3F-4ACC-B739-D811594A63E5}"/>
+    <hyperlink ref="A101" r:id="rId100" display="https://jira.sky.com.br/browse/SKYIT-183591" xr:uid="{0ED5FE79-D343-4485-8CF6-6ED5039EE7A2}"/>
+    <hyperlink ref="A102" r:id="rId101" display="https://jira.sky.com.br/browse/SKYIT-183638" xr:uid="{3CF7E56F-F0EE-47D9-8898-20CB6111945C}"/>
+    <hyperlink ref="A103" r:id="rId102" display="https://jira.sky.com.br/browse/SKYIT-184454" xr:uid="{47D893D4-75CF-4A50-9D82-3DD866165B18}"/>
+    <hyperlink ref="A104" r:id="rId103" display="https://jira.sky.com.br/browse/SKYIT-185945" xr:uid="{55595BFD-92E1-4B53-A80E-A062E407C564}"/>
+    <hyperlink ref="A105" r:id="rId104" display="https://jira.sky.com.br/browse/SKYIT-186242" xr:uid="{B7759BAA-E4DD-4978-829D-D8A1F43FE7F7}"/>
+    <hyperlink ref="A106" r:id="rId105" display="https://jira.sky.com.br/browse/SKYIT-187024" xr:uid="{961D751F-DE23-4E63-9C7E-A096E8F10C6F}"/>
+    <hyperlink ref="A107" r:id="rId106" display="https://jira.sky.com.br/browse/SKYIT-188337" xr:uid="{23350624-09F5-4CB4-8819-92AD6B0D7382}"/>
+    <hyperlink ref="A108" r:id="rId107" display="https://jira.sky.com.br/browse/SKYIT-188921" xr:uid="{D1EBA601-F398-4600-8AFB-CCF4C45780E6}"/>
+    <hyperlink ref="A109" r:id="rId108" display="https://jira.sky.com.br/browse/SKYIT-190046" xr:uid="{30F4CD1F-EEFD-4D47-8EE8-BCA2EB241BB4}"/>
+    <hyperlink ref="A110" r:id="rId109" display="https://jira.sky.com.br/browse/SKYIT-190969" xr:uid="{8412FC6C-E852-4D54-BDCE-D5592839A711}"/>
+    <hyperlink ref="A111" r:id="rId110" display="https://jira.sky.com.br/browse/SKYIT-191640" xr:uid="{2F8F6466-9AB8-4DD2-BACF-E67AE7D9CD80}"/>
+    <hyperlink ref="A112" r:id="rId111" display="https://jira.sky.com.br/browse/SKYIT-191650" xr:uid="{14B27612-D7C2-4AF5-9CD0-CB2746C008E8}"/>
+    <hyperlink ref="A113" r:id="rId112" display="https://jira.sky.com.br/browse/SKYIT-191796" xr:uid="{0D9FC054-618C-44CA-9216-EE6622879E7E}"/>
+    <hyperlink ref="A114" r:id="rId113" display="https://jira.sky.com.br/browse/SKYIT-191840" xr:uid="{9FA8B19F-D47D-4CC7-9CC8-67784533E909}"/>
+    <hyperlink ref="A115" r:id="rId114" display="https://jira.sky.com.br/browse/SKYIT-191906" xr:uid="{8FB1FE31-F92F-4CA4-9908-EB3BA6D095A0}"/>
+    <hyperlink ref="A116" r:id="rId115" display="https://jira.sky.com.br/browse/SKYIT-192384" xr:uid="{F0AC10D7-3A3C-4276-BEFC-19C1241BB237}"/>
+    <hyperlink ref="A117" r:id="rId116" display="https://jira.sky.com.br/browse/SKYIT-192445" xr:uid="{F01166EF-922A-4513-B53C-3C2B334008D5}"/>
+    <hyperlink ref="A118" r:id="rId117" display="https://jira.sky.com.br/browse/SKYIT-192947" xr:uid="{AD158D2C-2C3F-4979-9A91-2BD8962B72F2}"/>
+    <hyperlink ref="A119" r:id="rId118" display="https://jira.sky.com.br/browse/SKYIT-193104" xr:uid="{F4770BEA-854B-496D-B99F-9AA0FCF5650F}"/>
+    <hyperlink ref="A120" r:id="rId119" display="https://jira.sky.com.br/browse/SKYIT-193636" xr:uid="{84B273C1-DF1B-4490-95DB-094BAA44ED3D}"/>
+    <hyperlink ref="A121" r:id="rId120" display="https://jira.sky.com.br/browse/SKYIT-195943" xr:uid="{EC5DDFB8-2AF6-44D3-AB5D-A2B1710114AF}"/>
+    <hyperlink ref="A122" r:id="rId121" display="https://jira.sky.com.br/browse/SKYIT-197176" xr:uid="{49454476-58EA-401D-B071-59A97B3CAAB1}"/>
+    <hyperlink ref="A123" r:id="rId122" display="https://jira.sky.com.br/browse/SKYIT-198454" xr:uid="{5EE0551A-7D45-47CC-B7F7-25657B9FCD44}"/>
+    <hyperlink ref="A124" r:id="rId123" display="https://jira.sky.com.br/browse/SKYIT-199628" xr:uid="{51225DAB-FC93-46D3-9AE1-BCF1EDFE19F2}"/>
+    <hyperlink ref="A125" r:id="rId124" display="https://jira.sky.com.br/browse/SKYIT-199819" xr:uid="{E358BED3-4BBE-4422-B184-DD3E0B99E47D}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://jira.sky.com.br/browse/SKYIT-200412" xr:uid="{4FCB7C71-102C-42B8-9FCE-ECCC189ECA51}"/>
+    <hyperlink ref="A127" r:id="rId126" display="https://jira.sky.com.br/browse/SKYIT-200417" xr:uid="{8952D51C-A3CC-4769-9342-BA2810594F84}"/>
+    <hyperlink ref="A128" r:id="rId127" display="https://jira.sky.com.br/browse/SKYIT-201141" xr:uid="{24058B85-1647-490B-A437-3487028F5BA9}"/>
+    <hyperlink ref="A129" r:id="rId128" display="https://jira.sky.com.br/browse/SKYIT-201156" xr:uid="{D06FD4C7-9C4A-4D3D-9DCB-BECC6AD3CB8C}"/>
+    <hyperlink ref="A130" r:id="rId129" display="https://jira.sky.com.br/browse/SKYIT-201159" xr:uid="{42EBA229-DB7E-40D6-BE29-DA37956E1E38}"/>
+    <hyperlink ref="A131" r:id="rId130" display="https://jira.sky.com.br/browse/SKYIT-203819" xr:uid="{005EEB00-5560-40B4-96AF-31F6232F405A}"/>
+    <hyperlink ref="A132" r:id="rId131" display="https://jira.sky.com.br/browse/SKYIT-204845" xr:uid="{2C0E2E34-BE1F-46A2-B609-6C3F34D1E96C}"/>
+    <hyperlink ref="A133" r:id="rId132" display="https://jira.sky.com.br/browse/SKYIT-204911" xr:uid="{851ACE4D-6BA5-4AFA-8866-753EC474AE90}"/>
+    <hyperlink ref="A134" r:id="rId133" display="https://jira.sky.com.br/browse/SKYIT-205817" xr:uid="{89471E9D-C458-4A8D-9A3E-8932290DD44A}"/>
+    <hyperlink ref="A135" r:id="rId134" display="https://jira.sky.com.br/browse/SKYIT-207866" xr:uid="{554FC56A-6DC7-42D4-AB05-818F4B444B44}"/>
+    <hyperlink ref="A136" r:id="rId135" display="https://jira.sky.com.br/browse/SKYIT-208220" xr:uid="{49688392-E2B1-49EC-9939-74732ADB7513}"/>
+    <hyperlink ref="A137" r:id="rId136" display="https://jira.sky.com.br/browse/SKYIT-211339" xr:uid="{56370030-7874-4F64-BDCF-0AD3FBC8EEA4}"/>
+    <hyperlink ref="A138" r:id="rId137" display="https://jira.sky.com.br/browse/SKYIT-213193" xr:uid="{FBDE76E6-052B-407E-B0E0-C8661B9E1CFE}"/>
+    <hyperlink ref="A139" r:id="rId138" display="https://jira.sky.com.br/browse/SKYIT-214570" xr:uid="{C9865B37-EB93-4BF8-AF40-F028C20010A3}"/>
+    <hyperlink ref="A140" r:id="rId139" display="https://jira.sky.com.br/browse/SKYIT-217459" xr:uid="{DADCA68B-55AB-4074-BE8B-381EC2827BEA}"/>
+    <hyperlink ref="A141" r:id="rId140" display="https://jira.sky.com.br/browse/SKYIT-217685" xr:uid="{A8E3D0C3-6216-4813-B9E8-36C96D4A9A1E}"/>
+    <hyperlink ref="A142" r:id="rId141" display="https://jira.sky.com.br/browse/SKYIT-218753" xr:uid="{925A5362-1BB5-4A7F-BFE6-16BF43C2BA06}"/>
+    <hyperlink ref="A143" r:id="rId142" display="https://jira.sky.com.br/browse/SKYIT-219029" xr:uid="{5601D56F-E6D5-4938-918D-5BB6C51E9368}"/>
+    <hyperlink ref="A144" r:id="rId143" display="https://jira.sky.com.br/browse/SKYIT-221558" xr:uid="{14C44642-E15C-416C-83C7-7E11102AF7D7}"/>
+    <hyperlink ref="A145" r:id="rId144" display="https://jira.sky.com.br/browse/SKYIT-222064" xr:uid="{4C64E584-6B2E-491F-BFE6-C5266F1E0205}"/>
+    <hyperlink ref="A146" r:id="rId145" display="https://jira.sky.com.br/browse/SKYIT-222361" xr:uid="{65F4B88C-2046-4D0C-A573-F40F2621AA55}"/>
+    <hyperlink ref="A147" r:id="rId146" display="https://jira.sky.com.br/browse/SKYIT-222907" xr:uid="{CD2FD96E-769F-495F-B7BF-11FCED7E8A03}"/>
+    <hyperlink ref="A148" r:id="rId147" display="https://jira.sky.com.br/browse/SKYIT-222977" xr:uid="{FCCB714A-6E16-4CF0-8C64-644EFA3B15DB}"/>
+    <hyperlink ref="A149" r:id="rId148" display="https://jira.sky.com.br/browse/SKYIT-223289" xr:uid="{417D8F12-FDF7-4C80-BFCE-797361BAF53B}"/>
+    <hyperlink ref="A150" r:id="rId149" display="https://jira.sky.com.br/browse/SKYIT-226115" xr:uid="{24C2127A-F3EF-4462-A02E-DDB419BCDA76}"/>
+    <hyperlink ref="A151" r:id="rId150" display="https://jira.sky.com.br/browse/SKYIT-228050" xr:uid="{4A3FA93D-4F32-4420-BA43-5823AEE78B25}"/>
+    <hyperlink ref="A152" r:id="rId151" display="https://jira.sky.com.br/browse/SKYIT-228238" xr:uid="{C00066A7-293C-4A63-B766-7E6E6EB37689}"/>
+    <hyperlink ref="A153" r:id="rId152" display="https://jira.sky.com.br/browse/SKYIT-228514" xr:uid="{4CB96D6D-9209-4777-AC43-A47DD6CF1C45}"/>
+    <hyperlink ref="A154" r:id="rId153" display="https://jira.sky.com.br/browse/SKYIT-229545" xr:uid="{6E8B0CB4-D857-409D-84E3-6C09E0D7E3B4}"/>
+    <hyperlink ref="A155" r:id="rId154" display="https://jira.sky.com.br/browse/SKYIT-231046" xr:uid="{C6F48166-BBB1-455E-A221-9B44722E62FD}"/>
+    <hyperlink ref="A156" r:id="rId155" display="https://jira.sky.com.br/browse/SKYIT-231286" xr:uid="{9B26938E-7653-46AF-B2A1-F99827AC7C9C}"/>
+    <hyperlink ref="A157" r:id="rId156" display="https://jira.sky.com.br/browse/SKYIT-231773" xr:uid="{8933BE78-DA19-4004-A02F-83D9F061AF4A}"/>
+    <hyperlink ref="A158" r:id="rId157" display="https://jira.sky.com.br/browse/SKYIT-232592" xr:uid="{2D6BFE02-E962-4DE2-8DE0-7D6EA80C2EC2}"/>
+    <hyperlink ref="A159" r:id="rId158" display="https://jira.sky.com.br/browse/SKYIT-232863" xr:uid="{C0842B00-AEA0-412C-8BF2-76DDCCADB943}"/>
+    <hyperlink ref="A160" r:id="rId159" display="https://jira.sky.com.br/browse/SKYIT-233519" xr:uid="{8D8248CB-52BC-4CDC-BD6B-C49876FA37D1}"/>
+    <hyperlink ref="A161" r:id="rId160" display="https://jira.sky.com.br/browse/SKYIT-233568" xr:uid="{8761065B-B500-4187-9B0D-181F8D13B48A}"/>
+    <hyperlink ref="A162" r:id="rId161" display="https://jira.sky.com.br/browse/SKYIT-234789" xr:uid="{F4E644DF-2B7B-49E9-9114-D485331141AC}"/>
+    <hyperlink ref="A163" r:id="rId162" display="https://jira.sky.com.br/browse/SKYIT-235153" xr:uid="{090CC489-4973-4E50-9D66-B9D7E8EDB727}"/>
+    <hyperlink ref="A164" r:id="rId163" display="https://jira.sky.com.br/browse/SKYIT-236217" xr:uid="{AF0FC6FC-75AC-46DC-8625-8B461226CDAA}"/>
+    <hyperlink ref="A165" r:id="rId164" display="https://jira.sky.com.br/browse/SKYIT-237228" xr:uid="{4801CDCF-CDCD-49E6-B500-EEE25CAA3DBF}"/>
+    <hyperlink ref="A166" r:id="rId165" display="https://jira.sky.com.br/browse/SKYIT-237462" xr:uid="{3168D208-AD38-4025-A5D9-450EFDDC8FF3}"/>
+    <hyperlink ref="A167" r:id="rId166" display="https://jira.sky.com.br/browse/SKYIT-238522" xr:uid="{CA9CAAE3-19E4-4B1E-8CBE-DCBF6E6FA799}"/>
+    <hyperlink ref="A168" r:id="rId167" display="https://jira.sky.com.br/browse/SKYIT-239586" xr:uid="{A893E939-C85B-4CA3-BBBF-F826EA63346A}"/>
+    <hyperlink ref="A169" r:id="rId168" display="https://jira.sky.com.br/browse/SKYIT-240143" xr:uid="{675D3006-A1F6-4EF5-8DDB-BE077486E1C9}"/>
+    <hyperlink ref="A170" r:id="rId169" display="https://jira.sky.com.br/browse/SKYIT-240280" xr:uid="{726C5EB8-F82F-47EE-806A-C0C006D4BF78}"/>
+    <hyperlink ref="A171" r:id="rId170" display="https://jira.sky.com.br/browse/SKYIT-243078" xr:uid="{DDB72220-D797-4EBD-A265-D2EDAFB78F53}"/>
+    <hyperlink ref="A172" r:id="rId171" display="https://jira.sky.com.br/browse/SKYIT-243212" xr:uid="{8C82E82B-4E4D-4070-85A1-BC27A3BDB206}"/>
+    <hyperlink ref="A173" r:id="rId172" display="https://jira.sky.com.br/browse/SKYIT-243213" xr:uid="{4267FBBF-6A5A-4AEB-ADA0-E0D6760B38B2}"/>
+    <hyperlink ref="A174" r:id="rId173" display="https://jira.sky.com.br/browse/SKYIT-243679" xr:uid="{3B16BC52-9111-42D1-9E59-3296781292D6}"/>
+    <hyperlink ref="A175" r:id="rId174" display="https://jira.sky.com.br/browse/SKYIT-244659" xr:uid="{A09D9656-5386-4FA0-9D3F-9E514C805985}"/>
+    <hyperlink ref="A176" r:id="rId175" display="https://jira.sky.com.br/browse/SKYIT-244672" xr:uid="{882AD0EA-0861-4DAC-BFC1-014E33045202}"/>
+    <hyperlink ref="A177" r:id="rId176" display="https://jira.sky.com.br/browse/SKYIT-245128" xr:uid="{9273C77D-6019-4348-8515-D663C7AC0C50}"/>
+    <hyperlink ref="A178" r:id="rId177" display="https://jira.sky.com.br/browse/SKYIT-246054" xr:uid="{5CDC3D10-7669-4C70-AFDA-F226556C583E}"/>
+    <hyperlink ref="A179" r:id="rId178" display="https://jira.sky.com.br/browse/SKYIT-246432" xr:uid="{F8EBD364-40EB-45CE-B713-A6538EED9D14}"/>
+    <hyperlink ref="A180" r:id="rId179" display="https://jira.sky.com.br/browse/SKYIT-247849" xr:uid="{19CBF54F-2E1E-4624-BD53-285A4D11FCF6}"/>
+    <hyperlink ref="A181" r:id="rId180" display="https://jira.sky.com.br/browse/SKYIT-247931" xr:uid="{195D4D78-5130-4BF8-8626-AAF850633D63}"/>
+    <hyperlink ref="A182" r:id="rId181" display="https://jira.sky.com.br/browse/SKYIT-248041" xr:uid="{CAB7D56D-F545-4467-B9D8-3BB84676D466}"/>
+    <hyperlink ref="A183" r:id="rId182" display="https://jira.sky.com.br/browse/SKYIT-248223" xr:uid="{F2C5D31F-A142-408B-9FB3-9DC91BF759B2}"/>
+    <hyperlink ref="A184" r:id="rId183" display="https://jira.sky.com.br/browse/SKYIT-249152" xr:uid="{4FE1ADE7-6908-44A6-98D0-6DA8E9F12BE8}"/>
+    <hyperlink ref="A185" r:id="rId184" display="https://jira.sky.com.br/browse/SKYIT-251390" xr:uid="{096A8CBF-9528-4D15-8E37-A549CFD0DD26}"/>
+    <hyperlink ref="A186" r:id="rId185" display="https://jira.sky.com.br/browse/SKYIT-251815" xr:uid="{F6BA9BE9-25DD-4CF3-9141-9FAF2234CD3E}"/>
+    <hyperlink ref="A187" r:id="rId186" display="https://jira.sky.com.br/browse/SKYIT-252539" xr:uid="{688CC42A-6F6C-4D9B-A850-6F0B80823CAD}"/>
+    <hyperlink ref="A188" r:id="rId187" display="https://jira.sky.com.br/browse/SKYIT-253577" xr:uid="{C7E8964C-1211-4E46-BF26-F1880A526767}"/>
+    <hyperlink ref="A189" r:id="rId188" display="https://jira.sky.com.br/browse/SKYIT-256295" xr:uid="{7B872032-32B0-41F0-B128-76B4F03A26BC}"/>
+    <hyperlink ref="A190" r:id="rId189" display="https://jira.sky.com.br/browse/SKYIT-256977" xr:uid="{A65CD09C-2A34-4AA9-8748-912F131B354B}"/>
+    <hyperlink ref="A191" r:id="rId190" display="https://jira.sky.com.br/browse/SKYIT-257565" xr:uid="{B0F572C4-9ED2-4241-A3CD-4BC7FEA06B18}"/>
+    <hyperlink ref="A192" r:id="rId191" display="https://jira.sky.com.br/browse/SKYIT-257976" xr:uid="{3332E562-A244-4E99-A150-BF08A4896399}"/>
+    <hyperlink ref="A193" r:id="rId192" display="https://jira.sky.com.br/browse/SKYIT-260687" xr:uid="{D7BAEA8D-27F7-49C4-B3C7-EA00A0CB94DB}"/>
+    <hyperlink ref="A194" r:id="rId193" display="https://jira.sky.com.br/browse/SKYIT-261563" xr:uid="{4A6019D1-6E59-47F8-A9FA-D66F9A61994F}"/>
+    <hyperlink ref="A195" r:id="rId194" display="https://jira.sky.com.br/browse/SKYIT-262619" xr:uid="{D8360E1F-0F1F-408D-8EE3-562FF3890691}"/>
+    <hyperlink ref="A196" r:id="rId195" display="https://jira.sky.com.br/browse/SKYIT-263001" xr:uid="{B33778FC-E243-4768-943E-9F2E0D8EBCF7}"/>
+    <hyperlink ref="A197" r:id="rId196" display="https://jira.sky.com.br/browse/SKYIT-267374" xr:uid="{AFDE8E53-7D77-400B-83F8-13A263142D74}"/>
+    <hyperlink ref="A198" r:id="rId197" display="https://jira.sky.com.br/browse/SKYIT-267444" xr:uid="{7797EAF9-C3C6-4C98-9222-52AEB0532679}"/>
+    <hyperlink ref="A199" r:id="rId198" display="https://jira.sky.com.br/browse/SKYIT-267739" xr:uid="{DC95B184-5D1E-405A-A6C0-1067E089C892}"/>
+    <hyperlink ref="A200" r:id="rId199" display="https://jira.sky.com.br/browse/SKYIT-269645" xr:uid="{D9C3B418-1F82-4CEA-B88C-7FC9115BF188}"/>
+    <hyperlink ref="A201" r:id="rId200" display="https://jira.sky.com.br/browse/SKYIT-269846" xr:uid="{82E3C664-007F-48A6-90C6-25A90027835A}"/>
+    <hyperlink ref="A202" r:id="rId201" display="https://jira.sky.com.br/browse/SKYIT-270028" xr:uid="{32F64859-210F-45BA-9972-9DD118F95409}"/>
+    <hyperlink ref="A203" r:id="rId202" display="https://jira.sky.com.br/browse/SKYIT-271408" xr:uid="{2497A894-582D-423A-A8F0-B80CE9E55A28}"/>
+    <hyperlink ref="A204" r:id="rId203" display="https://jira.sky.com.br/browse/SKYIT-272579" xr:uid="{0DD92D9C-6988-4F0A-B96C-CFC4BA70AD41}"/>
+    <hyperlink ref="A205" r:id="rId204" display="https://jira.sky.com.br/browse/SKYIT-274237" xr:uid="{9DD1167B-FF94-4639-B5A2-4EEE768EA81B}"/>
+    <hyperlink ref="A206" r:id="rId205" display="https://jira.sky.com.br/browse/SKYIT-275371" xr:uid="{028C3184-40F6-43F8-AD21-411C99174CFE}"/>
+    <hyperlink ref="A207" r:id="rId206" display="https://jira.sky.com.br/browse/SKYIT-275381" xr:uid="{362270BC-033E-482D-8E68-7FB40C0FD315}"/>
+    <hyperlink ref="A208" r:id="rId207" display="https://jira.sky.com.br/browse/SKYIT-276092" xr:uid="{38525037-3E8D-4FCC-890F-65ABE0E9BDD1}"/>
+    <hyperlink ref="A209" r:id="rId208" display="https://jira.sky.com.br/browse/SKYIT-276151" xr:uid="{B574325D-D370-485E-8220-8DE87014052C}"/>
+    <hyperlink ref="A210" r:id="rId209" display="https://jira.sky.com.br/browse/SKYIT-280140" xr:uid="{D42C48EC-3EFB-4A86-BEAA-B7EABB11CD37}"/>
+    <hyperlink ref="A211" r:id="rId210" display="https://jira.sky.com.br/browse/SKYIT-280179" xr:uid="{335FB7E5-3093-469F-AC43-06F202EA9791}"/>
+    <hyperlink ref="A212" r:id="rId211" display="https://jira.sky.com.br/browse/SKYIT-280297" xr:uid="{811965FD-086F-4315-AF8C-450C1E5E7E98}"/>
+    <hyperlink ref="A213" r:id="rId212" display="https://jira.sky.com.br/browse/SKYIT-280321" xr:uid="{C83764BE-7EF7-402E-928D-85A21A2D8788}"/>
+    <hyperlink ref="A214" r:id="rId213" display="https://jira.sky.com.br/browse/SKYIT-280331" xr:uid="{C9145274-B7C3-4A93-9D5F-ECF8538770F6}"/>
+    <hyperlink ref="A215" r:id="rId214" display="https://jira.sky.com.br/browse/SKYIT-280366" xr:uid="{392B7C29-706E-4C80-B7F4-AF8F22EFD561}"/>
+    <hyperlink ref="A216" r:id="rId215" display="https://jira.sky.com.br/browse/SKYIT-280453" xr:uid="{8F132B02-EEBA-4231-A46A-345EE3EB2831}"/>
+    <hyperlink ref="A217" r:id="rId216" display="https://jira.sky.com.br/browse/SKYIT-280503" xr:uid="{8BA03CFA-3770-43B7-9385-37B576FB39A4}"/>
+    <hyperlink ref="A218" r:id="rId217" display="https://jira.sky.com.br/browse/SKYIT-282079" xr:uid="{6E9F845B-4644-4829-83A2-1E5B1F0D4115}"/>
+    <hyperlink ref="A219" r:id="rId218" display="https://jira.sky.com.br/browse/SKYIT-284505" xr:uid="{243E1DEF-125E-4A17-9D14-8F0E3001A9DA}"/>
+    <hyperlink ref="A220" r:id="rId219" display="https://jira.sky.com.br/browse/SKYIT-286540" xr:uid="{2E5C241D-95B0-4470-B2C9-EF432204609B}"/>
+    <hyperlink ref="A221" r:id="rId220" display="https://jira.sky.com.br/browse/SKYIT-287482" xr:uid="{24A1EB12-D547-429A-A7FB-B008C1C2D4E3}"/>
+    <hyperlink ref="A222" r:id="rId221" display="https://jira.sky.com.br/browse/SKYIT-289888" xr:uid="{8AF9B7F0-37CD-4F83-AB45-80BE8F8B58C2}"/>
+    <hyperlink ref="A223" r:id="rId222" display="https://jira.sky.com.br/browse/SKYIT-292433" xr:uid="{7892DFE2-C2A1-4FAF-96EA-3F8C0B8B4274}"/>
+    <hyperlink ref="A224" r:id="rId223" display="https://jira.sky.com.br/browse/SKYIT-292643" xr:uid="{DDC1EB07-51A6-4DFE-B797-9999BBB3591D}"/>
+    <hyperlink ref="A225" r:id="rId224" display="https://jira.sky.com.br/browse/SKYIT-292648" xr:uid="{FFE4728A-1111-49EA-8D75-7343B72500C8}"/>
+    <hyperlink ref="A226" r:id="rId225" display="https://jira.sky.com.br/browse/SKYIT-295097" xr:uid="{F5AC82BE-0A9E-4344-BA46-88AD64B70678}"/>
+    <hyperlink ref="A227" r:id="rId226" display="https://jira.sky.com.br/browse/SKYIT-295236" xr:uid="{6CE10A27-8C67-470D-A417-AE5D6ACF3676}"/>
+    <hyperlink ref="A228" r:id="rId227" display="https://jira.sky.com.br/browse/SKYIT-295772" xr:uid="{B80E8FAE-83BC-4FBB-8AF8-A9B41E7BB72D}"/>
+    <hyperlink ref="A229" r:id="rId228" display="https://jira.sky.com.br/browse/SKYIT-297358" xr:uid="{77E371E0-F7CD-44EB-AB62-7656A26D8373}"/>
+    <hyperlink ref="A230" r:id="rId229" display="https://jira.sky.com.br/browse/SKYIT-297482" xr:uid="{47022C84-20C7-44EF-A0BE-E2DC6D975F65}"/>
+    <hyperlink ref="A231" r:id="rId230" display="https://jira.sky.com.br/browse/SKYIT-297483" xr:uid="{A2F013A3-C0C7-40D8-B649-6B8132E7CF80}"/>
+    <hyperlink ref="A232" r:id="rId231" display="https://jira.sky.com.br/browse/SKYIT-297773" xr:uid="{349BE79B-43B9-44F1-8DB6-8A0BBED03CC2}"/>
+    <hyperlink ref="A233" r:id="rId232" display="https://jira.sky.com.br/browse/SKYIT-297960" xr:uid="{D8674996-C86E-4FBC-87E4-9BEE57441F00}"/>
+    <hyperlink ref="A234" r:id="rId233" display="https://jira.sky.com.br/browse/SKYIT-301564" xr:uid="{AC684379-1089-4FEA-B16F-EE8850956D75}"/>
+    <hyperlink ref="A235" r:id="rId234" display="https://jira.sky.com.br/browse/SKYIT-301617" xr:uid="{DA923D55-3E1E-4DB8-AB41-C3E0BB283EEF}"/>
+    <hyperlink ref="A236" r:id="rId235" display="https://jira.sky.com.br/browse/SKYIT-302934" xr:uid="{11AE13C8-EA8E-4CB1-B965-EF116321D1F5}"/>
+    <hyperlink ref="A237" r:id="rId236" display="https://jira.sky.com.br/browse/SKYIT-303426" xr:uid="{A2A126B4-312B-4FA9-BD08-6429DFD2A870}"/>
+    <hyperlink ref="A238" r:id="rId237" display="https://jira.sky.com.br/browse/SKYIT-305332" xr:uid="{0B736A09-B52E-4504-A2A1-4907D80DF187}"/>
+    <hyperlink ref="A239" r:id="rId238" display="https://jira.sky.com.br/browse/SKYIT-305393" xr:uid="{13CF8570-AB0D-4E13-B896-90324E3BC0AA}"/>
+    <hyperlink ref="A240" r:id="rId239" display="https://jira.sky.com.br/browse/SKYIT-306354" xr:uid="{98984FA4-577C-4FA8-BCD0-004DDA282F37}"/>
+    <hyperlink ref="A241" r:id="rId240" display="https://jira.sky.com.br/browse/SKYIT-306909" xr:uid="{F88A5C2F-EA81-40F1-BD96-3BD76D840C0A}"/>
+    <hyperlink ref="A242" r:id="rId241" display="https://jira.sky.com.br/browse/SKYIT-307373" xr:uid="{6D280B00-EA4B-475A-AC61-9C02329AA0E8}"/>
+    <hyperlink ref="A243" r:id="rId242" display="https://jira.sky.com.br/browse/SKYIT-307374" xr:uid="{87354852-5F2D-4409-89BB-ED22EA052EB4}"/>
+    <hyperlink ref="A244" r:id="rId243" display="https://jira.sky.com.br/browse/SKYIT-307375" xr:uid="{4237FE1A-9A1A-45DC-AC86-53C9422B946D}"/>
+    <hyperlink ref="A245" r:id="rId244" display="https://jira.sky.com.br/browse/SKYIT-307531" xr:uid="{7404D076-6512-4E6A-B51B-F1EC80AE3990}"/>
+    <hyperlink ref="A246" r:id="rId245" display="https://jira.sky.com.br/browse/SKYIT-307973" xr:uid="{D7A99FB8-9B31-4CF3-8E24-0E2CDBD06CA9}"/>
+    <hyperlink ref="A247" r:id="rId246" display="https://jira.sky.com.br/browse/SKYIT-308336" xr:uid="{955C1392-6F01-40C4-9294-474EB165F3C2}"/>
+    <hyperlink ref="A248" r:id="rId247" display="https://jira.sky.com.br/browse/SKYIT-308349" xr:uid="{5934D214-02F2-4251-B29C-F3971C8F2305}"/>
+    <hyperlink ref="A249" r:id="rId248" display="https://jira.sky.com.br/browse/SKYIT-308953" xr:uid="{69249837-AF3A-4C0B-8447-86401CD05945}"/>
+    <hyperlink ref="A250" r:id="rId249" display="https://jira.sky.com.br/browse/SKYIT-310033" xr:uid="{EC2CABD7-BDE3-4044-A62F-B567DD850F78}"/>
+    <hyperlink ref="A251" r:id="rId250" display="https://jira.sky.com.br/browse/SKYIT-311883" xr:uid="{30ED2E1F-22DA-4342-9148-23B7EE817D16}"/>
+    <hyperlink ref="A252" r:id="rId251" display="https://jira.sky.com.br/browse/SKYIT-314217" xr:uid="{BEBE93C1-DA8D-49C7-8582-774C4F96BFDA}"/>
+    <hyperlink ref="A253" r:id="rId252" display="https://jira.sky.com.br/browse/SKYIT-315098" xr:uid="{3F74DDFD-A73A-412A-8AE7-CFA4C8FCB9C5}"/>
+    <hyperlink ref="A254" r:id="rId253" display="https://jira.sky.com.br/browse/SKYIT-316007" xr:uid="{87834BB2-E3B9-4938-9380-0D88D52DD8BB}"/>
+    <hyperlink ref="A255" r:id="rId254" display="https://jira.sky.com.br/browse/SKYIT-316154" xr:uid="{642ECBA3-84B2-4001-9AA0-777666603CC0}"/>
+    <hyperlink ref="A256" r:id="rId255" display="https://jira.sky.com.br/browse/SKYIT-316315" xr:uid="{C6EAF102-38E0-4E01-87F1-047DE4D2F8AF}"/>
+    <hyperlink ref="A257" r:id="rId256" display="https://jira.sky.com.br/browse/SKYIT-317481" xr:uid="{65E65A0B-284C-4BFC-9252-3ACC82FE9510}"/>
+    <hyperlink ref="A258" r:id="rId257" display="https://jira.sky.com.br/browse/SKYIT-317723" xr:uid="{A45B5B92-822F-4DC7-BB15-95C79FB708F1}"/>
+    <hyperlink ref="A259" r:id="rId258" display="https://jira.sky.com.br/browse/SKYIT-319239" xr:uid="{28F1086F-3C60-4BE5-A52A-A6300BD6101E}"/>
+    <hyperlink ref="A260" r:id="rId259" display="https://jira.sky.com.br/browse/SKYIT-319886" xr:uid="{A22F77F6-5BE1-447C-AB67-CDF2970A1A67}"/>
+    <hyperlink ref="A261" r:id="rId260" display="https://jira.sky.com.br/browse/SKYIT-320098" xr:uid="{73B86804-F9CE-4A3E-82F4-9B741609DA9B}"/>
+    <hyperlink ref="A262" r:id="rId261" display="https://jira.sky.com.br/browse/SKYIT-320315" xr:uid="{D7D9959A-A464-4F8A-BBE4-773007DFF153}"/>
+    <hyperlink ref="A263" r:id="rId262" display="https://jira.sky.com.br/browse/SKYIT-321323" xr:uid="{C95015B7-27A4-4D27-9EC2-9120927D7DCF}"/>
+    <hyperlink ref="A264" r:id="rId263" display="https://jira.sky.com.br/browse/SKYIT-322701" xr:uid="{C7CA4FD1-2C52-4280-A4E8-46BF484AA620}"/>
+    <hyperlink ref="A265" r:id="rId264" display="https://jira.sky.com.br/browse/SKYIT-323457" xr:uid="{665FB63D-86E4-4F8E-9701-425E3207ECA0}"/>
+    <hyperlink ref="A266" r:id="rId265" display="https://jira.sky.com.br/browse/SKYIT-323472" xr:uid="{C133BA9B-FAB3-4D38-8DE2-5566BEAB59A9}"/>
+    <hyperlink ref="A267" r:id="rId266" display="https://jira.sky.com.br/browse/SKYIT-323675" xr:uid="{1F004787-14AD-43C2-995F-DC6F1384BA8F}"/>
+    <hyperlink ref="A268" r:id="rId267" display="https://jira.sky.com.br/browse/SKYIT-323808" xr:uid="{ED11A50A-2C72-4234-B9C9-432A1625A77D}"/>
+    <hyperlink ref="A269" r:id="rId268" display="https://jira.sky.com.br/browse/SKYIT-334778" xr:uid="{4766545A-5D54-4F77-A313-6E59E3003C8C}"/>
+    <hyperlink ref="A270" r:id="rId269" display="https://jira.sky.com.br/browse/SKYIT-335215" xr:uid="{23F274CF-D0D2-43E5-B6AF-7CF3A5AA3CCD}"/>
+    <hyperlink ref="A271" r:id="rId270" display="https://jira.sky.com.br/browse/SKYIT-335960" xr:uid="{C19FADE4-EEB1-4525-97C7-BF3DECE01E8B}"/>
+    <hyperlink ref="A272" r:id="rId271" display="https://jira.sky.com.br/browse/SKYIT-337021" xr:uid="{E9B2B94A-AE71-4ECC-975C-C0D73FB7DE9B}"/>
+    <hyperlink ref="A273" r:id="rId272" display="https://jira.sky.com.br/browse/SKYIT-338155" xr:uid="{CB4C0E5B-F1D1-48EE-AAFF-DB301EFBCA10}"/>
+    <hyperlink ref="A274" r:id="rId273" display="https://jira.sky.com.br/browse/SKYIT-338254" xr:uid="{D7857E44-830F-4956-A6BD-0303351709CB}"/>
+    <hyperlink ref="A275" r:id="rId274" display="https://jira.sky.com.br/browse/SKYIT-338403" xr:uid="{817508A9-BFEA-4C88-9893-3DEBDFB54D22}"/>
+    <hyperlink ref="A276" r:id="rId275" display="https://jira.sky.com.br/browse/SKYIT-340186" xr:uid="{0ECDCBA8-893C-42AF-ADFE-F4431DE288BB}"/>
+    <hyperlink ref="A277" r:id="rId276" display="https://jira.sky.com.br/browse/SKYIT-340227" xr:uid="{83F45146-5713-4455-9E00-C9BA2C378B11}"/>
+    <hyperlink ref="A278" r:id="rId277" display="https://jira.sky.com.br/browse/SKYIT-340695" xr:uid="{A9F280C3-FC3A-41AF-9D99-D999EA8D7775}"/>
+    <hyperlink ref="A279" r:id="rId278" display="https://jira.sky.com.br/browse/SKYIT-341304" xr:uid="{E413B92A-630D-4F44-9108-417D8630A230}"/>
+    <hyperlink ref="A280" r:id="rId279" display="https://jira.sky.com.br/browse/SKYIT-341348" xr:uid="{3652198C-A7C3-43F2-8D8E-806295494C6E}"/>
+    <hyperlink ref="A281" r:id="rId280" display="https://jira.sky.com.br/browse/SKYIT-341382" xr:uid="{B94A7567-AE39-46E9-9839-AB266A9C12F8}"/>
+    <hyperlink ref="A282" r:id="rId281" display="https://jira.sky.com.br/browse/SKYIT-342624" xr:uid="{933BB182-D146-45D0-909D-D50D953FC2A9}"/>
+    <hyperlink ref="A283" r:id="rId282" display="https://jira.sky.com.br/browse/SKYIT-345587" xr:uid="{7F3646B6-18D3-46BD-92DB-B9B1BF0DFF69}"/>
+    <hyperlink ref="A284" r:id="rId283" display="https://jira.sky.com.br/browse/SKYIT-345898" xr:uid="{3F0B1FA1-2B3F-4A65-A9C9-F2CC6EA15FE6}"/>
+    <hyperlink ref="A285" r:id="rId284" display="https://jira.sky.com.br/browse/SKYIT-349707" xr:uid="{2ECFD4CF-58C2-41B8-8747-11D66C5441E2}"/>
+    <hyperlink ref="A286" r:id="rId285" display="https://jira.sky.com.br/browse/SKYIT-350617" xr:uid="{CDA67E23-2C7C-429B-AC9E-72BA7A93FB23}"/>
+    <hyperlink ref="A287" r:id="rId286" display="https://jira.sky.com.br/browse/SKYIT-350901" xr:uid="{076CAB7B-BC5D-484F-9FD4-C5E8D7A77DC9}"/>
+    <hyperlink ref="A288" r:id="rId287" display="https://jira.sky.com.br/browse/SKYIT-352161" xr:uid="{F2B71ACF-9448-4D88-9E13-D10504F53301}"/>
+    <hyperlink ref="A289" r:id="rId288" display="https://jira.sky.com.br/browse/SKYIT-355414" xr:uid="{C6BB0AB6-014F-40E7-969D-414102AF88E5}"/>
+    <hyperlink ref="A290" r:id="rId289" display="https://jira.sky.com.br/browse/SKYIT-355549" xr:uid="{5D82049A-1D9A-45FD-8CB7-5A974416381C}"/>
+    <hyperlink ref="A291" r:id="rId290" display="https://jira.sky.com.br/browse/SKYIT-355619" xr:uid="{C104E86F-1BED-4540-84DB-6730ACBA0514}"/>
+    <hyperlink ref="A292" r:id="rId291" display="https://jira.sky.com.br/browse/SKYIT-355857" xr:uid="{F1395045-56DE-498A-AE86-278253A6E38A}"/>
+    <hyperlink ref="A293" r:id="rId292" display="https://jira.sky.com.br/browse/SKYIT-357991" xr:uid="{195A6942-BDBF-4CC4-8F61-30D0CC7E8A0A}"/>
+    <hyperlink ref="A294" r:id="rId293" display="https://jira.sky.com.br/browse/SKYIT-359005" xr:uid="{A93B53AE-984A-4491-BE00-1D4761283975}"/>
+    <hyperlink ref="A295" r:id="rId294" display="https://jira.sky.com.br/browse/SKYIT-359092" xr:uid="{4FEA8BF5-7BFD-45E7-8034-FAAE4CB7B6C6}"/>
+    <hyperlink ref="A296" r:id="rId295" display="https://jira.sky.com.br/browse/SKYIT-359590" xr:uid="{E51F689F-81A3-4365-80ED-7B7A81F35AE1}"/>
+    <hyperlink ref="A297" r:id="rId296" display="https://jira.sky.com.br/browse/SKYIT-359607" xr:uid="{51469FF1-4626-4542-85B8-6AF289657434}"/>
+    <hyperlink ref="A298" r:id="rId297" display="https://jira.sky.com.br/browse/SKYIT-361547" xr:uid="{A8B6C813-837A-418B-9478-50FD6203EA55}"/>
+    <hyperlink ref="A299" r:id="rId298" display="https://jira.sky.com.br/browse/SKYIT-362468" xr:uid="{F9BB5160-3745-414E-A697-EC0E8C2D5186}"/>
+    <hyperlink ref="A300" r:id="rId299" display="https://jira.sky.com.br/browse/SKYIT-362484" xr:uid="{16E47C78-B2E1-4D1F-9466-11E865BC0015}"/>
+    <hyperlink ref="A301" r:id="rId300" display="https://jira.sky.com.br/browse/SKYIT-362614" xr:uid="{17A92EB2-CAB8-4389-B55B-D3B255DA499B}"/>
+    <hyperlink ref="A302" r:id="rId301" display="https://jira.sky.com.br/browse/SKYIT-363073" xr:uid="{7D7D263C-9BCE-4ECB-9849-1DADFADAD1CE}"/>
+    <hyperlink ref="A303" r:id="rId302" display="https://jira.sky.com.br/browse/SKYIT-363937" xr:uid="{F9CA7BC7-9A9A-4C40-AF27-1B8800BCC785}"/>
+    <hyperlink ref="A304" r:id="rId303" display="https://jira.sky.com.br/browse/SKYIT-364597" xr:uid="{04678AEE-571F-4A73-906E-EBF00C27364F}"/>
+    <hyperlink ref="A305" r:id="rId304" display="https://jira.sky.com.br/browse/SKYIT-364982" xr:uid="{0E8A84B7-BBAF-450E-9F3E-0028F65155DB}"/>
+    <hyperlink ref="A306" r:id="rId305" display="https://jira.sky.com.br/browse/SKYIT-365180" xr:uid="{41F4FCA1-164B-49E1-BF53-A5C6462479CA}"/>
+    <hyperlink ref="A307" r:id="rId306" display="https://jira.sky.com.br/browse/SKYIT-366050" xr:uid="{85F6A3C6-812A-4F97-BD4B-E5EF8E3BCE65}"/>
+    <hyperlink ref="A308" r:id="rId307" display="https://jira.sky.com.br/browse/SKYIT-366521" xr:uid="{8709947B-1301-4F5A-A918-8BF187B7F583}"/>
+    <hyperlink ref="A309" r:id="rId308" display="https://jira.sky.com.br/browse/SKYIT-367114" xr:uid="{2AACB349-7806-4C53-A839-6E5EF5844202}"/>
+    <hyperlink ref="A310" r:id="rId309" display="https://jira.sky.com.br/browse/SKYIT-367298" xr:uid="{AEF78581-9289-444E-AD58-4BB28378D54E}"/>
+    <hyperlink ref="A311" r:id="rId310" display="https://jira.sky.com.br/browse/SKYIT-368247" xr:uid="{2E4C3AA5-49D7-4D99-A289-9493031A7BBA}"/>
+    <hyperlink ref="A312" r:id="rId311" display="https://jira.sky.com.br/browse/SKYIT-368376" xr:uid="{2A08F790-9BF5-40BB-8C34-EBDBC7E2297A}"/>
+    <hyperlink ref="A313" r:id="rId312" display="https://jira.sky.com.br/browse/SKYIT-369770" xr:uid="{BA3AEDBD-0CAB-4DEA-BF0C-363BF1ADDEB2}"/>
+    <hyperlink ref="A314" r:id="rId313" display="https://jira.sky.com.br/browse/SKYIT-370540" xr:uid="{A7B1EC47-113C-43B3-97C9-B6E04CFC9CA0}"/>
+    <hyperlink ref="A315" r:id="rId314" display="https://jira.sky.com.br/browse/SKYIT-370567" xr:uid="{638049B1-3B7A-4497-A893-B2731BBE82BB}"/>
+    <hyperlink ref="A316" r:id="rId315" display="https://jira.sky.com.br/browse/SKYIT-371818" xr:uid="{D9C3773C-3F84-41F1-8212-0F8E88593199}"/>
+    <hyperlink ref="A317" r:id="rId316" display="https://jira.sky.com.br/browse/SKYIT-372460" xr:uid="{BE763E7E-7411-46BA-BA52-BFA06F4FD55E}"/>
+    <hyperlink ref="A318" r:id="rId317" display="https://jira.sky.com.br/browse/SKYIT-372486" xr:uid="{0F94C7EB-83CF-49BB-BFAA-395264A863BF}"/>
+    <hyperlink ref="A319" r:id="rId318" display="https://jira.sky.com.br/browse/SKYIT-373309" xr:uid="{E799161C-A82E-4048-87CA-501759F440FD}"/>
+    <hyperlink ref="A320" r:id="rId319" display="https://jira.sky.com.br/browse/SKYIT-373352" xr:uid="{157E40D9-6D50-48AE-8C88-B811E59360F6}"/>
+    <hyperlink ref="A321" r:id="rId320" display="https://jira.sky.com.br/browse/SKYIT-373478" xr:uid="{42EBD62C-7FC4-4250-8355-504BBB388FC8}"/>
+    <hyperlink ref="A322" r:id="rId321" display="https://jira.sky.com.br/browse/SKYIT-373504" xr:uid="{39834BCD-C39D-4E38-BEEF-285F1F14F7DD}"/>
+    <hyperlink ref="A323" r:id="rId322" display="https://jira.sky.com.br/browse/SKYIT-374027" xr:uid="{466FF58C-0CBD-4910-99C7-9FFA1A969D64}"/>
+    <hyperlink ref="A324" r:id="rId323" display="https://jira.sky.com.br/browse/SKYIT-374457" xr:uid="{C30D7EC1-6AB6-4228-BBC0-977A04BC01F3}"/>
+    <hyperlink ref="A325" r:id="rId324" display="https://jira.sky.com.br/browse/SKYIT-378023" xr:uid="{FB70313D-512E-4CE0-8A65-1729E9557F80}"/>
+    <hyperlink ref="A326" r:id="rId325" display="https://jira.sky.com.br/browse/SKYIT-378041" xr:uid="{A0AC544B-53C0-438F-B6B1-4177275539EE}"/>
+    <hyperlink ref="A327" r:id="rId326" display="https://jira.sky.com.br/browse/SKYIT-379653" xr:uid="{82416D96-63EB-404E-A2B1-01ED41402A9A}"/>
+    <hyperlink ref="A328" r:id="rId327" display="https://jira.sky.com.br/browse/SKYIT-379883" xr:uid="{BE0CA254-A2C9-4114-B321-312A88D8094B}"/>
+    <hyperlink ref="A329" r:id="rId328" display="https://jira.sky.com.br/browse/SKYIT-379947" xr:uid="{CB79BA45-7991-4383-B235-84C26F5820B9}"/>
+    <hyperlink ref="A330" r:id="rId329" display="https://jira.sky.com.br/browse/SKYIT-380572" xr:uid="{E6B72E33-4B8C-48E5-A946-35D1FDB32520}"/>
+    <hyperlink ref="A331" r:id="rId330" display="https://jira.sky.com.br/browse/SKYIT-380879" xr:uid="{2DDB4EBC-31D6-4F85-8FBD-86D205671A14}"/>
+    <hyperlink ref="A332" r:id="rId331" display="https://jira.sky.com.br/browse/SKYIT-381375" xr:uid="{1E1E45F4-14E6-4B50-BE04-3DA86514938F}"/>
+    <hyperlink ref="A333" r:id="rId332" display="https://jira.sky.com.br/browse/SKYIT-381775" xr:uid="{960299E3-6B9B-4E29-8D0A-C8E5C072720E}"/>
+    <hyperlink ref="A334" r:id="rId333" display="https://jira.sky.com.br/browse/SKYIT-381939" xr:uid="{914E3E82-1523-42D5-AE56-5F3CF61DEE20}"/>
+    <hyperlink ref="A335" r:id="rId334" display="https://jira.sky.com.br/browse/SKYIT-382017" xr:uid="{5B1DD324-07B5-451B-9CE4-B9BE868BA04B}"/>
+    <hyperlink ref="A336" r:id="rId335" display="https://jira.sky.com.br/browse/SKYIT-382124" xr:uid="{C055504A-8A72-4B5D-8134-9D0D67D12538}"/>
+    <hyperlink ref="A337" r:id="rId336" display="https://jira.sky.com.br/browse/SKYIT-382145" xr:uid="{2F26FB90-78E7-44A5-BE38-DA8797DD4B96}"/>
+    <hyperlink ref="A338" r:id="rId337" display="https://jira.sky.com.br/browse/SKYIT-382467" xr:uid="{724D4CB5-5C21-4DA4-8E46-9C11BACB2E54}"/>
+    <hyperlink ref="A339" r:id="rId338" display="https://jira.sky.com.br/browse/SKYIT-382746" xr:uid="{0B0C616F-8E31-4C35-A3D8-2C541241A051}"/>
+    <hyperlink ref="A340" r:id="rId339" display="https://jira.sky.com.br/browse/SKYIT-384459" xr:uid="{A2E3698B-E90F-4465-A379-03A7872B9EFB}"/>
+    <hyperlink ref="A341" r:id="rId340" display="https://jira.sky.com.br/browse/SKYIT-384714" xr:uid="{DEC6BE75-B730-43A9-8F4C-3A5D93E4A569}"/>
+    <hyperlink ref="A342" r:id="rId341" display="https://jira.sky.com.br/browse/SKYIT-384868" xr:uid="{110C65FA-4BA1-4B2D-B84E-65118062B7BD}"/>
+    <hyperlink ref="A343" r:id="rId342" display="https://jira.sky.com.br/browse/SKYIT-384934" xr:uid="{F4FE378D-8183-4E13-ADB9-6CF4AFB8CEE5}"/>
+    <hyperlink ref="A344" r:id="rId343" display="https://jira.sky.com.br/browse/SKYIT-385491" xr:uid="{38298691-8B83-4E45-A46C-0DDDFF139341}"/>
+    <hyperlink ref="A345" r:id="rId344" display="https://jira.sky.com.br/browse/SKYIT-385644" xr:uid="{E34A9AC9-DE8F-4114-A6A6-288032D50DA4}"/>
+    <hyperlink ref="A346" r:id="rId345" display="https://jira.sky.com.br/browse/SKYIT-385815" xr:uid="{23CF02A7-CA37-45A7-8F8E-9499FDAE8F79}"/>
+    <hyperlink ref="A347" r:id="rId346" display="https://jira.sky.com.br/browse/SKYIT-386262" xr:uid="{F5EDAF1B-57A2-4491-A788-9C472154C5FB}"/>
+    <hyperlink ref="A348" r:id="rId347" display="https://jira.sky.com.br/browse/SKYIT-387104" xr:uid="{D635B796-BE9A-4359-A8D3-0BDBD0178FC9}"/>
+    <hyperlink ref="A349" r:id="rId348" display="https://jira.sky.com.br/browse/SKYIT-387298" xr:uid="{BE78862B-61AC-43DD-B7C4-CF12DAD800AC}"/>
+    <hyperlink ref="A350" r:id="rId349" display="https://jira.sky.com.br/browse/SKYIT-387310" xr:uid="{25D51B05-DCA5-4049-9829-07B26F24EFC9}"/>
+    <hyperlink ref="A351" r:id="rId350" display="https://jira.sky.com.br/browse/SKYIT-387592" xr:uid="{1667A6BD-B3B3-4F84-B06E-622FD71CDDE2}"/>
+    <hyperlink ref="A352" r:id="rId351" display="https://jira.sky.com.br/browse/SKYIT-387679" xr:uid="{0D374EDC-F387-4FE8-956D-E408F14DECD1}"/>
+    <hyperlink ref="A353" r:id="rId352" display="https://jira.sky.com.br/browse/SKYIT-387774" xr:uid="{D4F5ACFE-16DF-49B9-A640-A5E23BE481F7}"/>
+    <hyperlink ref="A354" r:id="rId353" display="https://jira.sky.com.br/browse/SKYIT-388256" xr:uid="{07098E79-0757-445B-9D35-69F97DCA51A1}"/>
+    <hyperlink ref="A355" r:id="rId354" display="https://jira.sky.com.br/browse/SKYIT-389092" xr:uid="{F9424003-D97D-49BF-B383-7C6EE624AA89}"/>
+    <hyperlink ref="A356" r:id="rId355" display="https://jira.sky.com.br/browse/SKYIT-389093" xr:uid="{F4973DB6-65E2-44CB-AF9D-80B9C8552063}"/>
+    <hyperlink ref="A357" r:id="rId356" display="https://jira.sky.com.br/browse/SKYIT-389697" xr:uid="{9AD763A4-BEDF-4428-ACB4-8433B4D5B8BA}"/>
+    <hyperlink ref="A358" r:id="rId357" display="https://jira.sky.com.br/browse/SKYIT-390323" xr:uid="{F2EE8174-E30F-4E0E-A872-4C40A4D2FC18}"/>
+    <hyperlink ref="A359" r:id="rId358" display="https://jira.sky.com.br/browse/SKYIT-392173" xr:uid="{543B90AE-1C58-468E-AAAE-30C6552FD874}"/>
+    <hyperlink ref="A360" r:id="rId359" display="https://jira.sky.com.br/browse/SKYIT-393391" xr:uid="{9ADB2FD6-765F-4CD3-A359-E91532C4729C}"/>
+    <hyperlink ref="A361" r:id="rId360" display="https://jira.sky.com.br/browse/SKYIT-395352" xr:uid="{84D831E8-F0CC-47FD-BBFD-CE30B67ACA1A}"/>
+    <hyperlink ref="A362" r:id="rId361" display="https://jira.sky.com.br/browse/SKYIT-396638" xr:uid="{B166E044-76C5-4452-A612-1A467A0E5090}"/>
+    <hyperlink ref="A363" r:id="rId362" display="https://jira.sky.com.br/browse/SKYIT-399743" xr:uid="{A152E6FB-EFE3-400B-8157-3033E4993F1A}"/>
+    <hyperlink ref="A364" r:id="rId363" display="https://jira.sky.com.br/browse/SKYIT-403708" xr:uid="{77DF9BC1-8C1E-4504-AE24-C332577A1D6B}"/>
+    <hyperlink ref="A365" r:id="rId364" display="https://jira.sky.com.br/browse/SKYIT-403759" xr:uid="{8BEA18DB-7191-411E-A51F-A1F51510F5B8}"/>
+    <hyperlink ref="A366" r:id="rId365" display="https://jira.sky.com.br/browse/SKYIT-405600" xr:uid="{AF7002ED-5E27-4C76-96A6-3532855DC131}"/>
+    <hyperlink ref="A367" r:id="rId366" display="https://jira.sky.com.br/browse/SKYIT-406252" xr:uid="{797FFC5E-83AF-4AD0-90AB-42D70D778E58}"/>
+    <hyperlink ref="A368" r:id="rId367" display="https://jira.sky.com.br/browse/SKYIT-407734" xr:uid="{F66CBF90-A032-433D-B85A-9A077524CDF7}"/>
+    <hyperlink ref="A369" r:id="rId368" display="https://jira.sky.com.br/browse/SKYIT-408288" xr:uid="{2421BDD8-7E79-4848-A3D7-0722D7A8AD28}"/>
+    <hyperlink ref="A370" r:id="rId369" display="https://jira.sky.com.br/browse/SKYIT-409426" xr:uid="{70BB17A3-317A-425E-BABE-F4073A730952}"/>
+    <hyperlink ref="A371" r:id="rId370" display="https://jira.sky.com.br/browse/SKYIT-411064" xr:uid="{C3E659C1-5BA9-48E5-A174-87B24B1A4850}"/>
+    <hyperlink ref="A372" r:id="rId371" display="https://jira.sky.com.br/browse/SKYIT-411108" xr:uid="{C643CE30-B939-4DA2-A2EA-F8AED7DC6787}"/>
+    <hyperlink ref="A373" r:id="rId372" display="https://jira.sky.com.br/browse/SKYIT-411526" xr:uid="{F3F52148-694A-4D8F-938C-63DD3C780681}"/>
+    <hyperlink ref="A374" r:id="rId373" display="https://jira.sky.com.br/browse/SKYIT-411528" xr:uid="{907584B0-C071-4C55-A660-CAF3D388679D}"/>
+    <hyperlink ref="A375" r:id="rId374" display="https://jira.sky.com.br/browse/SKYIT-415131" xr:uid="{8794CFA9-AF9D-4371-A827-C7BE35324D74}"/>
+    <hyperlink ref="A376" r:id="rId375" display="https://jira.sky.com.br/browse/SKYIT-419008" xr:uid="{763ECF72-F375-4999-B385-84B20CBB29E1}"/>
+    <hyperlink ref="A377" r:id="rId376" display="https://jira.sky.com.br/browse/SKYIT-419832" xr:uid="{03B72E39-F69F-493E-B7CE-DEF20229EF0E}"/>
+    <hyperlink ref="A378" r:id="rId377" display="https://jira.sky.com.br/browse/SKYIT-423849" xr:uid="{8C89E32E-4586-4DA1-934C-8B813552C54D}"/>
+    <hyperlink ref="A379" r:id="rId378" display="https://jira.sky.com.br/browse/SKYIT-425046" xr:uid="{E8D8C78D-A798-4CF0-B987-BB05DB319158}"/>
+    <hyperlink ref="A380" r:id="rId379" display="https://jira.sky.com.br/browse/SKYIT-426728" xr:uid="{BF81163E-1640-45F3-ADA5-54C31E523BA0}"/>
+    <hyperlink ref="A381" r:id="rId380" display="https://jira.sky.com.br/browse/SKYIT-426871" xr:uid="{34741A95-DE7C-4B2B-95AB-125A3F1CBFD6}"/>
+    <hyperlink ref="A382" r:id="rId381" display="https://jira.sky.com.br/browse/SKYIT-426995" xr:uid="{59B29EC6-DBCF-4C6F-A984-1956D6204B2A}"/>
+    <hyperlink ref="A383" r:id="rId382" display="https://jira.sky.com.br/browse/SKYIT-427501" xr:uid="{3F9BAF56-C851-49B7-B396-76FADEF16EC5}"/>
+    <hyperlink ref="A384" r:id="rId383" display="https://jira.sky.com.br/browse/SKYIT-429084" xr:uid="{5775EF08-32FB-407C-B598-EBFBBF22EFE1}"/>
+    <hyperlink ref="A385" r:id="rId384" display="https://jira.sky.com.br/browse/SKYIT-432647" xr:uid="{D6527EBD-F740-49F8-AD09-3932CC42E791}"/>
+    <hyperlink ref="A386" r:id="rId385" display="https://jira.sky.com.br/browse/SKYIT-432944" xr:uid="{BECB41FE-8740-4639-9D97-E4D6211026EE}"/>
+    <hyperlink ref="A387" r:id="rId386" display="https://jira.sky.com.br/browse/SKYIT-436893" xr:uid="{A448297E-8F77-4C0B-9D02-0142B2D9D8B3}"/>
+    <hyperlink ref="A388" r:id="rId387" display="https://jira.sky.com.br/browse/SKYIT-437556" xr:uid="{7D1D942C-F768-49ED-912A-224E71DA18B3}"/>
+    <hyperlink ref="A389" r:id="rId388" display="https://jira.sky.com.br/browse/SKYIT-440908" xr:uid="{BD6E0235-1209-445C-8258-8104099D967A}"/>
+    <hyperlink ref="A390" r:id="rId389" display="https://jira.sky.com.br/browse/SKYIT-440910" xr:uid="{95B38565-923E-4CF1-83C4-730601828E16}"/>
+    <hyperlink ref="A391" r:id="rId390" display="https://jira.sky.com.br/browse/SKYIT-441269" xr:uid="{38BB22D7-0F6F-4D60-801C-01E4DC308A63}"/>
+    <hyperlink ref="A392" r:id="rId391" display="https://jira.sky.com.br/browse/SKYIT-453085" xr:uid="{CEC16D54-F247-43F7-B5C2-A71252AB41F6}"/>
+    <hyperlink ref="A393" r:id="rId392" display="https://jira.sky.com.br/browse/SKYIT-453104" xr:uid="{DA7C2779-C20C-473D-8341-9A5CC5D5C17F}"/>
+    <hyperlink ref="A394" r:id="rId393" display="https://jira.sky.com.br/browse/SKYIT-453354" xr:uid="{EFB9D191-002B-4DDE-A926-782E38DEDECC}"/>
+    <hyperlink ref="A395" r:id="rId394" display="https://jira.sky.com.br/browse/SKYIT-453529" xr:uid="{87B99DD6-E4C7-4E28-97B7-B3C06F910CD9}"/>
+    <hyperlink ref="A396" r:id="rId395" display="https://jira.sky.com.br/browse/SKYIT-453706" xr:uid="{DA61EF5E-50B0-458A-9FCF-D914AA46CD49}"/>
+    <hyperlink ref="A397" r:id="rId396" display="https://jira.sky.com.br/browse/SKYIT-453738" xr:uid="{F669C62B-E7A0-4238-BBC6-C29363C3F6CF}"/>
+    <hyperlink ref="A398" r:id="rId397" display="https://jira.sky.com.br/browse/SKYIT-454540" xr:uid="{E51B7517-1086-414C-BF59-0F29BE3BD04E}"/>
+    <hyperlink ref="A399" r:id="rId398" display="https://jira.sky.com.br/browse/SKYIT-456985" xr:uid="{52A52091-038B-4321-AC86-6FB6DE1C7A52}"/>
+    <hyperlink ref="A400" r:id="rId399" display="https://jira.sky.com.br/browse/SKYIT-466380" xr:uid="{ABA2F6C1-4644-4310-80BF-C53D1BF93D21}"/>
+    <hyperlink ref="A401" r:id="rId400" display="https://jira.sky.com.br/browse/SKYIT-468498" xr:uid="{F643ED9E-F2AD-45AB-892C-492D6DEBECC9}"/>
+    <hyperlink ref="A402" r:id="rId401" display="https://jira.sky.com.br/browse/SKYIT-470025" xr:uid="{C19E388D-9DFB-44CB-8FE8-903AC79187DA}"/>
+    <hyperlink ref="A403" r:id="rId402" display="https://jira.sky.com.br/browse/SKYIT-473024" xr:uid="{8755DCA0-C5B7-4DBE-8DFE-3890B7FD3BB9}"/>
+    <hyperlink ref="A404" r:id="rId403" display="https://jira.sky.com.br/browse/SKYIT-477282" xr:uid="{CEA1E5BD-CE01-4997-A315-12316E5E7623}"/>
+    <hyperlink ref="A405" r:id="rId404" display="https://jira.sky.com.br/browse/SKYIT-477468" xr:uid="{EDEE2276-4EA1-4F58-8501-ACAFDB17F815}"/>
+    <hyperlink ref="A406" r:id="rId405" display="https://jira.sky.com.br/browse/SKYIT-478373" xr:uid="{1BE79090-09AD-4E25-AA9D-A82B04F67799}"/>
+    <hyperlink ref="A407" r:id="rId406" display="https://jira.sky.com.br/browse/SKYIT-479002" xr:uid="{1EAB329A-9AC6-4F38-8A24-45CE5A6DFC35}"/>
+    <hyperlink ref="A408" r:id="rId407" display="https://jira.sky.com.br/browse/SKYIT-479323" xr:uid="{ABC249A6-B9EC-4CD4-89E0-43F09B42949C}"/>
+    <hyperlink ref="A409" r:id="rId408" display="https://jira.sky.com.br/browse/SKYIT-484432" xr:uid="{6906F51F-D8F9-4FD6-B6C1-1974AD767B0D}"/>
+    <hyperlink ref="A410" r:id="rId409" display="https://jira.sky.com.br/browse/SKYIT-486392" xr:uid="{5D21A13B-3348-42C8-B2A7-EE5E64C52195}"/>
+    <hyperlink ref="A411" r:id="rId410" display="https://jira.sky.com.br/browse/SKYIT-487929" xr:uid="{1D7DB21C-D5BD-470E-9843-ADA95F2B4C68}"/>
+    <hyperlink ref="A412" r:id="rId411" display="https://jira.sky.com.br/browse/SKYIT-493834" xr:uid="{90057B46-F4CB-4B76-96F7-A09DE688FE45}"/>
+    <hyperlink ref="A413" r:id="rId412" display="https://jira.sky.com.br/browse/SKYIT-494607" xr:uid="{C591187E-83F6-430C-BFD0-7179D7EB77CB}"/>
+    <hyperlink ref="A414" r:id="rId413" display="https://jira.sky.com.br/browse/SKYIT-496105" xr:uid="{7697B09C-B6C4-4B15-94F6-F7B2AC3DE0CD}"/>
+    <hyperlink ref="A415" r:id="rId414" display="https://jira.sky.com.br/browse/SKYIT-498247" xr:uid="{6B442AF4-7DA3-487A-8A65-A411B41A13AA}"/>
+    <hyperlink ref="A416" r:id="rId415" display="https://jira.sky.com.br/browse/SKYIT-503448" xr:uid="{7E5B1EE9-0136-44EC-A621-06A4EB420CA6}"/>
+    <hyperlink ref="A417" r:id="rId416" display="https://jira.sky.com.br/browse/SKYIT-503452" xr:uid="{6B908380-FD5C-4A9E-8453-9650EE00E27F}"/>
+    <hyperlink ref="A418" r:id="rId417" display="https://jira.sky.com.br/browse/SKYIT-503453" xr:uid="{C2E5C2E0-E497-42F6-9F20-017260C27BE8}"/>
+    <hyperlink ref="A419" r:id="rId418" display="https://jira.sky.com.br/browse/SKYIT-504402" xr:uid="{20A17EC8-E5BF-4BED-BDFC-0E48D7BCA4B0}"/>
+    <hyperlink ref="A420" r:id="rId419" display="https://jira.sky.com.br/browse/SKYIT-504678" xr:uid="{5B59C3F0-2DE4-492E-A458-A53951ACA3F9}"/>
+    <hyperlink ref="A421" r:id="rId420" display="https://jira.sky.com.br/browse/SKYIT-505420" xr:uid="{D198B861-5328-4BB9-8671-1569C403334C}"/>
+    <hyperlink ref="A422" r:id="rId421" display="https://jira.sky.com.br/browse/SKYIT-507109" xr:uid="{E95C409A-A770-4F00-AB1A-8344218E2FDA}"/>
+    <hyperlink ref="A423" r:id="rId422" display="https://jira.sky.com.br/browse/SKYIT-507183" xr:uid="{77E891E0-59B7-49C5-A6BB-6891142749A7}"/>
+    <hyperlink ref="A424" r:id="rId423" display="https://jira.sky.com.br/browse/SKYIT-508156" xr:uid="{90EDEDAE-23D6-4BDD-99FA-B288C04DD0CB}"/>
+    <hyperlink ref="A425" r:id="rId424" display="https://jira.sky.com.br/browse/SKYIT-508637" xr:uid="{2E64F1A0-0831-4A8C-AC47-275AEBE4DB85}"/>
+    <hyperlink ref="A426" r:id="rId425" display="https://jira.sky.com.br/browse/SKYIT-509161" xr:uid="{E969F569-A130-42BF-9FFF-3BE6FB8BC709}"/>
+    <hyperlink ref="A427" r:id="rId426" display="https://jira.sky.com.br/browse/SKYIT-509207" xr:uid="{B81D36A8-43D8-412E-9E23-31859D5B7F11}"/>
+    <hyperlink ref="A428" r:id="rId427" display="https://jira.sky.com.br/browse/SKYIT-509212" xr:uid="{DFB370DD-1E9A-499C-A9E0-5F954C108495}"/>
+    <hyperlink ref="A429" r:id="rId428" display="https://jira.sky.com.br/browse/SKYIT-510889" xr:uid="{7DDF5356-081D-4B7B-BF9F-8B8A14E0FFEF}"/>
+    <hyperlink ref="A430" r:id="rId429" display="https://jira.sky.com.br/browse/SKYIT-514830" xr:uid="{ED8AE776-5F24-4646-B8DA-11BB4D710AB1}"/>
+    <hyperlink ref="A431" r:id="rId430" display="https://jira.sky.com.br/browse/SKYIT-524933" xr:uid="{9A27EBF2-F48A-40BD-9393-AC65FDEB7D01}"/>
+    <hyperlink ref="A432" r:id="rId431" display="https://jira.sky.com.br/browse/SKYIT-530334" xr:uid="{83E80621-4C66-45D9-A0A4-27F13BFA4EDC}"/>
+    <hyperlink ref="A433" r:id="rId432" display="https://jira.sky.com.br/browse/SKYIT-531695" xr:uid="{7C1A3D14-EF4B-4FAA-944E-3AB1560676B9}"/>
+    <hyperlink ref="A434" r:id="rId433" display="https://jira.sky.com.br/browse/SKYIT-533091" xr:uid="{0FAAE540-0F13-4AF5-B660-ED863D5F944F}"/>
+    <hyperlink ref="A435" r:id="rId434" display="https://jira.sky.com.br/browse/SKYIT-533147" xr:uid="{CFDA2D60-4AF4-46E7-B42F-F6896ECF4ECB}"/>
+    <hyperlink ref="A436" r:id="rId435" display="https://jira.sky.com.br/browse/SKYIT-533446" xr:uid="{78C89872-AA76-42C4-B0CB-AAB212FB3173}"/>
+    <hyperlink ref="A437" r:id="rId436" display="https://jira.sky.com.br/browse/SKYIT-537684" xr:uid="{B8C305FA-66BB-45A6-BAE4-14F5384BF140}"/>
+    <hyperlink ref="A438" r:id="rId437" display="https://jira.sky.com.br/browse/SKYIT-541189" xr:uid="{0D052878-2F51-4BD4-AB9C-A5D8203791E0}"/>
+    <hyperlink ref="A439" r:id="rId438" display="https://jira.sky.com.br/browse/SKYIT-543600" xr:uid="{B9E25EA9-E052-4406-8EB6-4A19A69874C2}"/>
+    <hyperlink ref="A440" r:id="rId439" display="https://jira.sky.com.br/browse/SKYIT-544411" xr:uid="{5CF26F6F-AE6C-42C7-A159-3AB02977E7C0}"/>
+    <hyperlink ref="A441" r:id="rId440" display="https://jira.sky.com.br/browse/SKYIT-545486" xr:uid="{C3E8D4E9-C8EE-4C2D-B237-1B92887BE2B8}"/>
+    <hyperlink ref="A442" r:id="rId441" display="https://jira.sky.com.br/browse/SKYIT-545949" xr:uid="{BA283457-C4B5-47E5-939E-04F8FEB2846E}"/>
+    <hyperlink ref="A443" r:id="rId442" display="https://jira.sky.com.br/browse/SKYIT-547406" xr:uid="{E05CF201-85F0-4AE4-8DF6-F7C94784076E}"/>
+    <hyperlink ref="A444" r:id="rId443" display="https://jira.sky.com.br/browse/SKYIT-548024" xr:uid="{EF968434-1F6C-498F-9356-EE9B72A54BB7}"/>
+    <hyperlink ref="A445" r:id="rId444" display="https://jira.sky.com.br/browse/SKYIT-550104" xr:uid="{D2D6F9F7-6B4A-4D56-A1FC-63AE09988C2F}"/>
+    <hyperlink ref="A446" r:id="rId445" display="https://jira.sky.com.br/browse/SKYIT-557173" xr:uid="{69E1173F-08F8-4AEC-BE89-5DB9E6207725}"/>
+    <hyperlink ref="A447" r:id="rId446" display="https://jira.sky.com.br/browse/SKYIT-566609" xr:uid="{6AEFE6A8-0A20-4286-9565-4B42C5E5E368}"/>
+    <hyperlink ref="A448" r:id="rId447" display="https://jira.sky.com.br/browse/SKYIT-566942" xr:uid="{A966D05C-7E26-4DF6-8DB5-FF44262470C6}"/>
+    <hyperlink ref="A449" r:id="rId448" display="https://jira.sky.com.br/browse/SKYIT-567074" xr:uid="{9AB5718B-E1FA-470A-AE46-A4D94843A842}"/>
+    <hyperlink ref="A450" r:id="rId449" display="https://jira.sky.com.br/browse/SKYIT-567779" xr:uid="{72809509-C893-4BB5-A54D-F120FDF3E49A}"/>
+    <hyperlink ref="A451" r:id="rId450" display="https://jira.sky.com.br/browse/SKYIT-568592" xr:uid="{6C29DBC8-D1B1-46AB-A545-083E1679776D}"/>
+    <hyperlink ref="A452" r:id="rId451" display="https://jira.sky.com.br/browse/SKYIT-570590" xr:uid="{29F75F94-A7B7-46C9-B526-E8D9675C175C}"/>
+    <hyperlink ref="A453" r:id="rId452" display="https://jira.sky.com.br/browse/SKYIT-575434" xr:uid="{AACB246C-4D90-4896-9620-C9B6ABCCBEEE}"/>
+    <hyperlink ref="A454" r:id="rId453" display="https://jira.sky.com.br/browse/SKYIT-575651" xr:uid="{34C69C68-3D2A-4026-9A22-AF937C5F606F}"/>
+    <hyperlink ref="A455" r:id="rId454" display="https://jira.sky.com.br/browse/SKYIT-578611" xr:uid="{FF08F1EB-9DFC-4BC0-876C-D035E4BF4BE1}"/>
+    <hyperlink ref="A456" r:id="rId455" display="https://jira.sky.com.br/browse/SKYIT-585529" xr:uid="{5F0D38E6-8FCA-4282-9227-6BECF6529204}"/>
+    <hyperlink ref="A457" r:id="rId456" display="https://jira.sky.com.br/browse/SKYIT-585537" xr:uid="{F37B74D8-3B94-4495-BF3F-FCF2D0826ACA}"/>
+    <hyperlink ref="A458" r:id="rId457" display="https://jira.sky.com.br/browse/SKYIT-586610" xr:uid="{2D9B7F85-254F-4CDF-B36E-B89F8654DE7B}"/>
+    <hyperlink ref="A459" r:id="rId458" display="https://jira.sky.com.br/browse/SKYIT-590891" xr:uid="{A5735019-06BB-42C2-9ADE-EC256EFC2B92}"/>
+    <hyperlink ref="A460" r:id="rId459" display="https://jira.sky.com.br/browse/SKYIT-593473" xr:uid="{320BAC23-B152-470D-8B90-5A6DFF07A61A}"/>
+    <hyperlink ref="A461" r:id="rId460" display="https://jira.sky.com.br/browse/SKYIT-593567" xr:uid="{2D9805F8-D5C4-4D63-9F12-06838E30A082}"/>
+    <hyperlink ref="A462" r:id="rId461" display="https://jira.sky.com.br/browse/SKYIT-595081" xr:uid="{BA5E40B7-25E7-4AC4-B694-D36D1769D805}"/>
+    <hyperlink ref="A463" r:id="rId462" display="https://jira.sky.com.br/browse/SKYIT-595111" xr:uid="{ED61F16C-1BA2-487B-B47F-58583C80D3E5}"/>
+    <hyperlink ref="A464" r:id="rId463" display="https://jira.sky.com.br/browse/SKYIT-595735" xr:uid="{39C5DACC-5DE9-46C5-9EB6-CA8AC45F0790}"/>
+    <hyperlink ref="A465" r:id="rId464" display="https://jira.sky.com.br/browse/SKYIT-596222" xr:uid="{81457EBE-BEBF-4A92-A459-923FA16A707C}"/>
+    <hyperlink ref="A466" r:id="rId465" display="https://jira.sky.com.br/browse/SKYIT-597656" xr:uid="{DBDE9E06-0C18-4D97-B17C-6B1FC9B54AE8}"/>
+    <hyperlink ref="A467" r:id="rId466" display="https://jira.sky.com.br/browse/SKYIT-598443" xr:uid="{40622B4A-9DAD-4221-9C53-033BEA536E60}"/>
+    <hyperlink ref="A468" r:id="rId467" display="https://jira.sky.com.br/browse/SKYIT-598821" xr:uid="{3103065D-FD37-45D5-AEDE-CEAD318A1CAB}"/>
+    <hyperlink ref="A469" r:id="rId468" display="https://jira.sky.com.br/browse/SKYIT-599095" xr:uid="{F0580376-A048-4B1F-B7E9-033CC5B8B038}"/>
+    <hyperlink ref="A470" r:id="rId469" display="https://jira.sky.com.br/browse/SKYIT-599337" xr:uid="{E76F553A-C845-4641-A485-9CDDEB1E85F6}"/>
+    <hyperlink ref="A471" r:id="rId470" display="https://jira.sky.com.br/browse/SKYIT-599951" xr:uid="{559A9DF7-C4EC-44F0-BD2B-C42A953AF9FA}"/>
+    <hyperlink ref="A472" r:id="rId471" display="https://jira.sky.com.br/browse/SKYIT-600388" xr:uid="{7823F546-A4B0-4625-A8DD-836CBD6A4BAE}"/>
+    <hyperlink ref="A473" r:id="rId472" display="https://jira.sky.com.br/browse/SKYIT-601272" xr:uid="{F73EE843-FFCE-473C-BB6C-E9642C3D44DD}"/>
+    <hyperlink ref="A474" r:id="rId473" display="https://jira.sky.com.br/browse/SKYIT-602692" xr:uid="{F5754390-7032-4A1B-8DAE-3D127337279A}"/>
+    <hyperlink ref="A475" r:id="rId474" display="https://jira.sky.com.br/browse/SKYIT-603061" xr:uid="{E77EEFA4-9501-4FC0-A11F-BBF74A911692}"/>
+    <hyperlink ref="A476" r:id="rId475" display="https://jira.sky.com.br/browse/SKYIT-604275" xr:uid="{CE57DDAB-DEF2-4E21-918D-731EAFB801ED}"/>
+    <hyperlink ref="A477" r:id="rId476" display="https://jira.sky.com.br/browse/SKYIT-604803" xr:uid="{A6D3D988-91DE-4CBC-A5D0-89228EA0A1D4}"/>
+    <hyperlink ref="A478" r:id="rId477" display="https://jira.sky.com.br/browse/SKYIT-612020" xr:uid="{E154D2E8-5066-4174-8937-09B02309CB1D}"/>
+    <hyperlink ref="A479" r:id="rId478" display="https://jira.sky.com.br/browse/SKYIT-617188" xr:uid="{BD8B8121-D16B-4F33-95C4-B56693EC34F8}"/>
+    <hyperlink ref="A480" r:id="rId479" display="https://jira.sky.com.br/browse/SKYIT-617413" xr:uid="{C6C1C297-AC3C-4262-9957-7353193A6EF4}"/>
+    <hyperlink ref="A481" r:id="rId480" display="https://jira.sky.com.br/browse/SKYIT-620455" xr:uid="{2BC0E6B2-7AD3-4876-9A01-E98EFD0CFE42}"/>
+    <hyperlink ref="A482" r:id="rId481" display="https://jira.sky.com.br/browse/SKYIT-625254" xr:uid="{895A5A53-7A95-438A-B3EC-F89DF18257D4}"/>
+    <hyperlink ref="A483" r:id="rId482" display="https://jira.sky.com.br/browse/SKYIT-626444" xr:uid="{0D2C2238-7BAC-416A-B3ED-BB843D4367A8}"/>
+    <hyperlink ref="A484" r:id="rId483" display="https://jira.sky.com.br/browse/SKYIT-629943" xr:uid="{9CA34510-3AB7-4C6F-A458-C346BCF88D63}"/>
+    <hyperlink ref="A485" r:id="rId484" display="https://jira.sky.com.br/browse/SKYIT-630004" xr:uid="{41B82E0C-FC30-456A-ACEA-F585EA5F94FE}"/>
+    <hyperlink ref="A486" r:id="rId485" display="https://jira.sky.com.br/browse/SKYIT-633672" xr:uid="{AE0F3DC6-C4D5-4D50-93DE-8E6299A809D2}"/>
+    <hyperlink ref="A487" r:id="rId486" display="https://jira.sky.com.br/browse/SKYIT-633858" xr:uid="{2E51DB78-1BA4-41E6-816C-0403381BBC96}"/>
+    <hyperlink ref="A488" r:id="rId487" display="https://jira.sky.com.br/browse/SKYIT-633924" xr:uid="{ADEA596A-CC00-4D0C-BB68-636C3460AADE}"/>
+    <hyperlink ref="A489" r:id="rId488" display="https://jira.sky.com.br/browse/SKYIT-634063" xr:uid="{15D3614C-BB5F-4BE6-A782-2363A0099340}"/>
+    <hyperlink ref="A490" r:id="rId489" display="https://jira.sky.com.br/browse/SKYIT-634419" xr:uid="{31DD48EB-3854-4B69-AF43-F844B6484EB5}"/>
+    <hyperlink ref="A491" r:id="rId490" display="https://jira.sky.com.br/browse/SKYIT-642926" xr:uid="{C97BEB92-6490-467A-AB4E-763034417A44}"/>
+    <hyperlink ref="A492" r:id="rId491" display="https://jira.sky.com.br/browse/SKYIT-648428" xr:uid="{D894BA5F-5EBF-4469-A77F-92C842FB6D46}"/>
+    <hyperlink ref="A493" r:id="rId492" display="https://jira.sky.com.br/browse/SKYIT-656600" xr:uid="{731C2F3A-74B4-47C8-8988-504D6B9C12AE}"/>
+    <hyperlink ref="A494" r:id="rId493" display="https://jira.sky.com.br/browse/SKYIT-657803" xr:uid="{A5F694AD-B536-4078-A9EC-84CDFD623CF5}"/>
+    <hyperlink ref="A495" r:id="rId494" display="https://jira.sky.com.br/browse/SKYIT-660240" xr:uid="{C7354A9A-79D4-4F60-8EE8-91A249B1912D}"/>
+    <hyperlink ref="A496" r:id="rId495" display="https://jira.sky.com.br/browse/SKYIT-661347" xr:uid="{7EAB7014-5C28-4F27-A18E-97136FEE10DF}"/>
+    <hyperlink ref="A497" r:id="rId496" display="https://jira.sky.com.br/browse/SKYIT-665363" xr:uid="{C919F279-24E9-426A-B550-B69A4B05AED8}"/>
+    <hyperlink ref="A498" r:id="rId497" display="https://jira.sky.com.br/browse/SKYIT-666881" xr:uid="{79F27965-D717-401D-87EB-ED3871C25AE4}"/>
+    <hyperlink ref="A499" r:id="rId498" display="https://jira.sky.com.br/browse/SKYIT-667171" xr:uid="{7125B769-B9D1-4233-AF83-8094778E8638}"/>
+    <hyperlink ref="A500" r:id="rId499" display="https://jira.sky.com.br/browse/SKYIT-672515" xr:uid="{58E9678A-E701-407F-BE87-EBFA8F36E60E}"/>
+    <hyperlink ref="A501" r:id="rId500" display="https://jira.sky.com.br/browse/SKYIT-672544" xr:uid="{5C7404E6-1B13-4BBC-B9A9-E77E1354E7E3}"/>
+    <hyperlink ref="A502" r:id="rId501" display="https://jira.sky.com.br/browse/SKYIT-682844" xr:uid="{49BFCC0C-7A7E-4CDE-BD72-551174955377}"/>
+    <hyperlink ref="A503" r:id="rId502" display="https://jira.sky.com.br/browse/SKYIT-687421" xr:uid="{C1DA5718-45E7-4438-90D7-9BB11E30A8B6}"/>
+    <hyperlink ref="A504" r:id="rId503" display="https://jira.sky.com.br/browse/SKYIT-693677" xr:uid="{B4A9D767-FA81-4618-BE68-7E7949D69B8A}"/>
+    <hyperlink ref="A505" r:id="rId504" display="https://jira.sky.com.br/browse/SKYIT-702210" xr:uid="{F34678F3-BF9C-46A4-954C-F9CE4EFDC1AD}"/>
+    <hyperlink ref="A506" r:id="rId505" display="https://jira.sky.com.br/browse/SKYIT-702931" xr:uid="{35B2144C-8C9D-4EA8-ABE0-B0B584A8C06D}"/>
+    <hyperlink ref="A507" r:id="rId506" display="https://jira.sky.com.br/browse/SKYIT-705723" xr:uid="{C9CD6139-B30D-490E-B9A9-79EA2D37FC7F}"/>
+    <hyperlink ref="A508" r:id="rId507" display="https://jira.sky.com.br/browse/SKYIT-706467" xr:uid="{808A689F-ACB3-415C-BA76-AE6F9322DF32}"/>
+    <hyperlink ref="A509" r:id="rId508" display="https://jira.sky.com.br/browse/SKYIT-706670" xr:uid="{8FBD0CCD-7699-4307-8C7C-0847C77555FF}"/>
+    <hyperlink ref="A510" r:id="rId509" display="https://jira.sky.com.br/browse/SKYIT-707395" xr:uid="{98F7F3E1-9972-4FA2-9DBA-79C9D607D5CE}"/>
+    <hyperlink ref="A511" r:id="rId510" display="https://jira.sky.com.br/browse/SKYIT-708880" xr:uid="{5F50BCA7-EE01-4E50-B21C-BBF389AF1DA7}"/>
+    <hyperlink ref="A512" r:id="rId511" display="https://jira.sky.com.br/browse/SKYIT-709652" xr:uid="{B2CD35EB-BD53-46D3-B8F0-785B014651CA}"/>
+    <hyperlink ref="A513" r:id="rId512" display="https://jira.sky.com.br/browse/SKYIT-712168" xr:uid="{E7B45FE7-6DFA-413D-A235-FBB1F00B98EE}"/>
+    <hyperlink ref="A514" r:id="rId513" display="https://jira.sky.com.br/browse/SKYIT-716674" xr:uid="{C4A943C5-48A7-4622-A797-D0D0CFBFFBBB}"/>
+    <hyperlink ref="A515" r:id="rId514" display="https://jira.sky.com.br/browse/SKYIT-716779" xr:uid="{DA18F3C4-17F2-49E4-A63E-93D4289DA636}"/>
+    <hyperlink ref="A516" r:id="rId515" display="https://jira.sky.com.br/browse/SKYIT-718638" xr:uid="{D37DB2F3-DEF5-40F1-BD1E-60E901A595BB}"/>
+    <hyperlink ref="A517" r:id="rId516" display="https://jira.sky.com.br/browse/SKYIT-719355" xr:uid="{2CE9F464-0CE3-40BF-A168-6D2061015E99}"/>
+    <hyperlink ref="A518" r:id="rId517" display="https://jira.sky.com.br/browse/SKYIT-725543" xr:uid="{A2771D7A-7AC4-401C-BA0B-9D155F09A610}"/>
+    <hyperlink ref="A519" r:id="rId518" display="https://jira.sky.com.br/browse/SKYIT-743117" xr:uid="{EBE81F80-489D-4BE3-9C85-F98080E9CC0F}"/>
+    <hyperlink ref="A520" r:id="rId519" display="https://jira.sky.com.br/browse/SKYIT-746911" xr:uid="{BCE7ACEF-1A09-47C9-9839-AABB9ECD38BC}"/>
+    <hyperlink ref="A521" r:id="rId520" display="https://jira.sky.com.br/browse/SKYIT-752289" xr:uid="{5AD88721-C52D-4ED5-9A0C-E14C95DFDC3D}"/>
+    <hyperlink ref="A522" r:id="rId521" display="https://jira.sky.com.br/browse/SKYIT-765439" xr:uid="{F881E3DB-5EC0-4F21-9E1F-6E88A28A0E11}"/>
+    <hyperlink ref="A523" r:id="rId522" display="https://jira.sky.com.br/browse/SKYIT-767411" xr:uid="{E86DB7D4-9FF5-439E-B54B-4CF0301D59B0}"/>
+    <hyperlink ref="A524" r:id="rId523" display="https://jira.sky.com.br/browse/SKYIT-775485" xr:uid="{C0B89293-83F5-4E8B-B9D5-CE8C5EEB9A54}"/>
+    <hyperlink ref="A525" r:id="rId524" display="https://jira.sky.com.br/browse/SKYIT-777202" xr:uid="{AB2AA2E1-F487-4EE1-8800-F33A7861F364}"/>
+    <hyperlink ref="A526" r:id="rId525" display="https://jira.sky.com.br/browse/SKYIT-782946" xr:uid="{A6F8AEAE-E1B4-461A-B4B2-0ED6A8AD51F0}"/>
+    <hyperlink ref="A527" r:id="rId526" display="https://jira.sky.com.br/browse/SKYIT-785655" xr:uid="{938897A4-867F-4B9C-A771-22C0597C5D7B}"/>
+    <hyperlink ref="A528" r:id="rId527" display="https://jira.sky.com.br/browse/SKYIT-788247" xr:uid="{EB4CDA5A-43A2-4F3D-AF2E-632AB5EE4C61}"/>
+    <hyperlink ref="A529" r:id="rId528" display="https://jira.sky.com.br/browse/SKYIT-788890" xr:uid="{542BBE4F-9C01-42C5-93CB-00DCEE8907B9}"/>
+    <hyperlink ref="A530" r:id="rId529" display="https://jira.sky.com.br/browse/SKYIT-789894" xr:uid="{6E1ECDA1-4A11-4534-9FE0-A0BA638AED89}"/>
+    <hyperlink ref="A531" r:id="rId530" display="https://jira.sky.com.br/browse/SKYIT-790290" xr:uid="{2075BA0B-D6E5-41B4-B479-6D0F3D6D78F8}"/>
+    <hyperlink ref="A532" r:id="rId531" display="https://jira.sky.com.br/browse/SKYIT-791151" xr:uid="{7465A866-50A8-4AAA-ACC5-9DF6DF16B20B}"/>
+    <hyperlink ref="A533" r:id="rId532" display="https://jira.sky.com.br/browse/SKYIT-800332" xr:uid="{F225A319-A5E2-4CFC-A5C5-99D7B5C9DB84}"/>
+    <hyperlink ref="A534" r:id="rId533" display="https://jira.sky.com.br/browse/SKYIT-801916" xr:uid="{A99BD995-D0E4-47BC-82FD-A424BFDAEECF}"/>
+    <hyperlink ref="A535" r:id="rId534" display="https://jira.sky.com.br/browse/SKYIT-811068" xr:uid="{19736C6A-4998-4CF6-A463-76C4370978D1}"/>
+    <hyperlink ref="A536" r:id="rId535" display="https://jira.sky.com.br/browse/SKYIT-811938" xr:uid="{CAE36177-49CA-403F-82BD-F1189E158C8B}"/>
+    <hyperlink ref="A537" r:id="rId536" display="https://jira.sky.com.br/browse/SKYIT-812097" xr:uid="{6083E305-84A9-4608-B163-B243CE6B6896}"/>
+    <hyperlink ref="A538" r:id="rId537" display="https://jira.sky.com.br/browse/SKYIT-814154" xr:uid="{41194B7D-D89E-45E9-B9F9-C2B134377F23}"/>
+    <hyperlink ref="A539" r:id="rId538" display="https://jira.sky.com.br/browse/SKYIT-815896" xr:uid="{7B3BFFA3-14F1-450B-BD46-E3E8C3E19E24}"/>
+    <hyperlink ref="A540" r:id="rId539" display="https://jira.sky.com.br/browse/SKYIT-821278" xr:uid="{5E1DFF51-E01E-4AEC-A76B-12CDA1172768}"/>
+    <hyperlink ref="A541" r:id="rId540" display="https://jira.sky.com.br/browse/SKYIT-841840" xr:uid="{AB2E2FDF-4D16-4C09-83BA-C3C3D10F02D9}"/>
+    <hyperlink ref="A542" r:id="rId541" display="https://jira.sky.com.br/browse/SKYIT-843892" xr:uid="{983701C4-09D0-446A-A2F0-BF721F4E59C7}"/>
+    <hyperlink ref="A543" r:id="rId542" display="https://jira.sky.com.br/browse/SKYIT-844396" xr:uid="{690DD495-0195-4516-B369-D003CB5D0987}"/>
+    <hyperlink ref="A544" r:id="rId543" display="https://jira.sky.com.br/browse/SKYIT-845532" xr:uid="{6E00ED14-E9E7-46BA-ADA2-604AFDCB982D}"/>
+    <hyperlink ref="A545" r:id="rId544" display="https://jira.sky.com.br/browse/SKYIT-846749" xr:uid="{4F82D313-6BD7-4243-A34D-227BF6FC2376}"/>
+    <hyperlink ref="A546" r:id="rId545" display="https://jira.sky.com.br/browse/SKYIT-846773" xr:uid="{F5BC107E-197D-4A7F-ADA9-163791928064}"/>
+    <hyperlink ref="A547" r:id="rId546" display="https://jira.sky.com.br/browse/SKYIT-846850" xr:uid="{FB8A7BC5-19C0-426D-9192-018B6D52E787}"/>
+    <hyperlink ref="A548" r:id="rId547" display="https://jira.sky.com.br/browse/SKYIT-858753" xr:uid="{0E3E1512-7501-4BE2-B774-3C368F0AFFBD}"/>
+    <hyperlink ref="A549" r:id="rId548" display="https://jira.sky.com.br/browse/SKYIT-858946" xr:uid="{E787F044-F0F5-4D43-920A-0A4B548F0F46}"/>
+    <hyperlink ref="A550" r:id="rId549" display="https://jira.sky.com.br/browse/SKYIT-859326" xr:uid="{9D86E84A-D408-4D7A-AF0B-C91B6FCF91E1}"/>
+    <hyperlink ref="A551" r:id="rId550" display="https://jira.sky.com.br/browse/SKYIT-861332" xr:uid="{AF768ABE-542C-45D7-98AA-DAC56FF0A5F0}"/>
+    <hyperlink ref="A552" r:id="rId551" display="https://jira.sky.com.br/browse/SKYIT-870927" xr:uid="{40318B21-CED6-4A5D-A7CD-8057E5CE86C5}"/>
+    <hyperlink ref="A553" r:id="rId552" display="https://jira.sky.com.br/browse/SKYIT-880452" xr:uid="{15910781-FCC6-433A-8C40-EC6957813F39}"/>
+    <hyperlink ref="A554" r:id="rId553" display="https://jira.sky.com.br/browse/SKYIT-880820" xr:uid="{E7D5534A-4CDC-4941-99D4-9F320520ABFB}"/>
+    <hyperlink ref="A555" r:id="rId554" display="https://jira.sky.com.br/browse/SKYIT-881583" xr:uid="{46BAFDC7-3177-4E1A-BDEC-A2C30F18781F}"/>
+    <hyperlink ref="A556" r:id="rId555" display="https://jira.sky.com.br/browse/SKYIT-882651" xr:uid="{A3B12F5E-269C-40F1-B969-A5C8BBE453B7}"/>
+    <hyperlink ref="A557" r:id="rId556" display="https://jira.sky.com.br/browse/SKYIT-882838" xr:uid="{78242429-501B-4B93-AC3E-4E210EDD2A7E}"/>
+    <hyperlink ref="A558" r:id="rId557" display="https://jira.sky.com.br/browse/SKYIT-883513" xr:uid="{9EFF97E9-5B3D-42B1-969D-E8BE04AA358A}"/>
+    <hyperlink ref="A559" r:id="rId558" display="https://jira.sky.com.br/browse/SKYIT-884149" xr:uid="{E5C5FC17-2012-4E25-94E1-5F809338C7CD}"/>
+    <hyperlink ref="A560" r:id="rId559" display="https://jira.sky.com.br/browse/SKYIT-888743" xr:uid="{CFE5841A-07A0-470B-B02B-B7ACE6628AE6}"/>
+    <hyperlink ref="A561" r:id="rId560" display="https://jira.sky.com.br/browse/SKYIT-890358" xr:uid="{456FD11F-5700-4629-B4F4-E84E0929CAF8}"/>
+    <hyperlink ref="A562" r:id="rId561" display="https://jira.sky.com.br/browse/SKYIT-895479" xr:uid="{5D3BF7E3-70E2-47FC-9A17-D8FAFD16EE25}"/>
+    <hyperlink ref="A563" r:id="rId562" display="https://jira.sky.com.br/browse/SKYIT-899538" xr:uid="{FF76E3FA-8CEE-4A20-8A75-992AAD241905}"/>
+    <hyperlink ref="A564" r:id="rId563" display="https://jira.sky.com.br/browse/SKYIT-899571" xr:uid="{C60C638F-0CBE-432D-8431-643A626426FE}"/>
+    <hyperlink ref="A565" r:id="rId564" display="https://jira.sky.com.br/browse/SKYIT-908582" xr:uid="{9F65200B-7133-4562-9210-1BD73917BB0F}"/>
+    <hyperlink ref="A566" r:id="rId565" display="https://jira.sky.com.br/browse/SKYIT-910700" xr:uid="{F25BDDAB-AC47-4CE4-A57D-D6A2D49861C1}"/>
+    <hyperlink ref="A567" r:id="rId566" display="https://jira.sky.com.br/browse/SKYIT-915320" xr:uid="{AFAD18BF-77A8-4E01-BE01-4E03AAE61A5D}"/>
+    <hyperlink ref="A568" r:id="rId567" display="https://jira.sky.com.br/browse/SKYIT-917983" xr:uid="{E73628C4-3A6E-4270-984F-3F0FE15C95FC}"/>
+    <hyperlink ref="A569" r:id="rId568" display="https://jira.sky.com.br/browse/SKYIT-918841" xr:uid="{C255B032-7089-446F-B8B7-B0D653AACB7D}"/>
+    <hyperlink ref="A570" r:id="rId569" display="https://jira.sky.com.br/browse/SKYIT-1813908" xr:uid="{266C55BC-3F25-4D1A-A648-4F4384B419D7}"/>
+    <hyperlink ref="A571" r:id="rId570" display="https://jira.sky.com.br/browse/SKYIT-1814058" xr:uid="{F47E1813-43E3-4087-8A1E-E5A4CB906B67}"/>
+    <hyperlink ref="A572" r:id="rId571" display="https://jira.sky.com.br/browse/SKYIT-1817456" xr:uid="{4393EFDD-08E6-417A-BFBA-45157A42B2BC}"/>
+    <hyperlink ref="A573" r:id="rId572" display="https://jira.sky.com.br/browse/SKYIT-1820365" xr:uid="{3C8DB5CB-3693-4E4E-9B85-2AEFF9A2A807}"/>
+    <hyperlink ref="A574" r:id="rId573" display="https://jira.sky.com.br/browse/SKYIT-1825366" xr:uid="{5CC66818-BC08-4D52-85E4-F48A4E7C4149}"/>
+    <hyperlink ref="A575" r:id="rId574" display="https://jira.sky.com.br/browse/SKYIT-1827010" xr:uid="{E8672060-249B-480A-BCBF-4435E3481809}"/>
+    <hyperlink ref="A576" r:id="rId575" display="https://jira.sky.com.br/browse/SKYIT-1832556" xr:uid="{FE1F68A7-FBBD-499F-8818-EE08B189C02B}"/>
+    <hyperlink ref="A577" r:id="rId576" display="https://jira.sky.com.br/browse/SKYIT-1884947" xr:uid="{C1D0F482-3036-40FE-8374-E0423482903A}"/>
+    <hyperlink ref="A578" r:id="rId577" display="https://jira.sky.com.br/browse/SKYIT-1884996" xr:uid="{28B0E7C5-F743-439C-AB1E-D1B0B214935B}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.5" footer="0.25"/>

</xml_diff>